<commit_message>
refactor: deleted unwanted activities
</commit_message>
<xml_diff>
--- a/Products.xlsx
+++ b/Products.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kishor Balgi\OneDrive\Documents\UiPath\Flipkart Product Review Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BD43DFD-A8AE-4EF6-B883-A9642EC0B047}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC36A771-0647-4556-8783-EFF21816D995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="15375" windowHeight="7785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,66 +25,57 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
-  <si>
-    <t>https://www.flipkart.com/micromax-x778/p/itm372cb161da595?pid=MOBG6XZB4WJJ6MRJ&amp;lid=LSTMOBG6XZB4WJJ6MRJRXTLJF&amp;marketplace=FLIPKART&amp;q=micromax+keypad&amp;store=tyy%2F4io&amp;srno=s_1_1&amp;otracker=search&amp;iid=22496617-e0d2-4a7c-a8ac-eaf50879265c.MOBG6XZB4WJJ6MRJ.SEARCH&amp;ssid=hptaldccc00000001688580884943&amp;qH=26e55ddeaa2e42a6</t>
-  </si>
-  <si>
-    <t>Micromax X778</t>
-  </si>
-  <si>
-    <t>₹1,455</t>
-  </si>
-  <si>
-    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAcAAAAFQCAYAAAAoQ64wAAAAOXRFWHRTb2Z0d2FyZQBNYXRwbG90bGliIHZlcnNpb24zLjYuMSwgaHR0cHM6Ly9tYXRwbG90bGliLm9yZy/av/WaAAAACXBIWXMAAArEAAAKxAFmbYLUAABGZ0lEQVR4nO3deVxU9f7H8dew7yCiKKviviEqqAjmrrlVLmippW33Wpr1y8x7s7LbvnjLtMzS0rTcLculmzdLw11T3DJxQ0BUFAXZYZjv7w9uU6TggAxnmPk8H48eCXPOdz5zgHnP+X7P93t0SimFEEIIYWPstC5ACCGE0IIEoBBCCJskASiEEMImSQAKIYSwSRKAQgghbJIEoBBCCJskASiEEMImSQAKIYSwSRKAQgghbJIEoBBCCJskASiEEMImSQAKIYSwSRKAQgghbJIEoBBCCJskASiEEMImSQAKIYSwSRKAQgghbJIEoBBCCJskASiEEMImSQAKIYSwSRKAQgghbJIEoBBCCJskASiEEMImSQBauZ49e/LFF1+YpW2dTkdqaqpZ2q6K5ORkfHx8tC7Don355ZcMHTq0yo9bmpdeeolHHnmk3Mc9PDxIS0urwYoqZs6/R1F5EoA1rFGjRri5ueHh4UFAQABTpkyhpKSkRp578eLF9O3b16Rtk5OT8fDwwMPDA3d3d3Q6nfFrDw8PM1daNSEhIWRmZmpdhkUbO3Ys69evN3791w8xf33c0lT2Q1dOTg4BAQFmrKjmSYhWHwlADWzevJmcnBzi4+NZu3Ytn376qdYl3SAkJIScnBxycnI4ffo0gPHrnJwcsz2vXq83W9uWwNpfny1RSmEwGLQuQ9wGCUANNWnShJiYGBISEozfW7NmDW3atMHX15e77rqL9PR0AC5fvszAgQPx8fHBz8+P++67D4CtW7fStGnTMu3e7FPymTNnmDhxIlu3bsXDw4M2bdpUy2tYv349jRs3xs/PjzfeeMP4/ZKSEmbOnEloaCj+/v5MnTq13Df/nj178sILLxAZGYm7uzvFxcVs27aNTp064ePjQ8+ePY0h/Mgjj/Cvf/2rzP5hYWFs376dpKQkHBwcjN+/evUqY8aMoX79+oSFhfH5558DcPLkyTJnBf3796d3797GrwMCAjh58mS5x/yvTp8+zR133IGPjw8BAQE899xzxscWL15Mr169+Pvf/463tzeLFi0qt66b0el0zJ07l5CQEBo0aMA777xjfKygoIBJkybRoEEDQkJCePnll41vyLt376ZDhw54eXkRGBjIe++9Z6zn916A/v37A9CiRQs8PDyIj48v83hFxxoo92d0M/PmzSMsLIx69eoxbtw4srKygD9+f19++WV8fX1p1KgR33///U3buFm9APn5+cTFxeHp6UmXLl04e/ZsmeP3+9/CZ599RmhoKJ6enrRo0YKtW7dW+phPmDCByZMn07t3b9zc3Dh9+jTx8fF06NABHx8fevTowfHjx43b79u3j/DwcLy8vJg4cWKZwJwwYQKvvvqq8eu/9tD8+OOPREZG4uXlRbNmzYiPj+eVV14hPj6eRx55BA8PD15//fVyj7kwgRI1KjQ0VMXHxyullDpx4oRq0KCBmjVrllJKqT179qjAwEB1+PBhVVRUpKZNm6ZGjBihlFJq+vTp6rHHHlPFxcWqoKBA7dixQyml1E8//aSaNGlS5jkAlZKSopRSqkePHmrp0qVKKaUWLVqk+vTpU2bbN954Qw0ePLjCmi9cuKBu9qsCqJEjR6rs7Gx15MgR5ezsrE6dOqWUUurtt99WvXr1Uunp6eratWuqZ8+eau7cuTdtv0ePHqpJkybq5MmTKj8/XyUnJys/Pz/1888/K71er+bMmaMiIyOVUkpt3rxZtW7d2rjvnj17VFBQkDIYDOrs2bPK3t7e+NigQYPU1KlTVUFBgTp+/Lhq2LChOnTokFJKKX9/f3Xq1Cml1+tVcHCwCgwMVEVFRerUqVPK39+/wmP+V6dOnVJbt25VxcXFKjExUQUHB6uvv/7aeMzt7e3VokWLVElJicrLy6uwrpsd4/79+6usrCx1/Phx1aBBA/XDDz8opZR67rnnVI8ePdTVq1fVuXPnVLNmzdSiRYuUUkp16dJFffHFF0oppa5evaoOHDhgrOfPvwN//l356+MVHeuKfkZ/tXnzZtWgQQN17NgxlZOTo4YPH67Gjx+vlCr9/bW3t1dvvvmmKi4uVh9//LEKCQm5aTs3q3fmzJnK1dVV/fjjj6q4uFjdf//96oEHHrhh+5ycHOXp6akSExOVUkolJSWpM2fOVPqYjx8/XtWtW1ft379fFRcXq4sXLyofHx+1du1aVVRUpN5++23VtGlTVVxcrAoLC1VQUJCaN2+eKioqUnPmzFH29vbGv8fx48erV1555abH/vTp08rT01OtX79e6fV6de7cOXXy5EmlVNm/aXF75AxQAwMHDsTDw4MWLVrQrVs3Jk2aBJR+Qn388cdp164djo6OvPDCC3zzzTfo9XocHR25cOECKSkpODs7061bt2qp5R//+AcbNmy4rf09PDxo27Yt4eHhHDlyBIBPP/2UV199lXr16uHj48PUqVNZs2ZNue08/PDDNG3aFBcXF7788kuGDRtG9+7dsbe354knniApKYmkpCR69+7N5cuXOXbsGACrVq0iLi4OnU5Xpr2LFy+ydetW3njjDZydnWnZsiVjxozhq6++AqB79+78/PPPHDx4kPDwcCIiIjhw4ADx8fHExsYCmHzMmzRpQo8ePXBwcKBZs2aMHTvWeJb0++MTJkzAzs6OrKysCuu6mX/+8594eXnRsmVLHn74YVauXAnAihUrmDlzJnXq1CEkJISpU6eyfPlyY+2nTp3i6tWr1KlThw4dOlT4c7yZio51RT+jv1qxYgV/+9vfaN26Ne7u7rz++uusXLkSpRQA7u7uTJs2DQcHB8aNG0dycnKlxnL79OlDr169cHBw4N577+XQoUM33U6n03Hs2DEKCwsJDQ2lcePG5bZZ3jEHGDFiBJ06dcLBwYHNmzcTHh7O8OHDcXR0ZOrUqeTl5bFv3z527dqFg4MDjz32GI6OjkyePJmGDRua9JqWL1/O0KFDGTJkCPb29oSEhNzQ0yNunwSgBr777juys7NZt24d+/fvN46pJScn89prr+Hj44OPjw/BwcE4ODhw8eJFpk2bRkhICD169KBly5YWM27o7+9v/Lebm1uZ1/J796GPjw9jx441dufeTFBQkPHfycnJLF261Livj48Pubm5nD9/Hnt7e0aOHGl8A129ejWjR4++ob3k5GQKCgqMAezj48PHH3/MxYsXgdIAjI+PNwben7/u3r07gMnH/Pz58wwbNowGDRrg7e3N7NmzycjIKPe1VVTXzQQHB5f594ULFwBIS0sjJCTE+FhoaKjxiseFCxdy7NgxmjZtSmxsLLt27Sq3/fJUdKwr+hn91c3qLCgo4OrVqwDUq1cPO7vStyI3NzeASo0zl/c7+Gfu7u4sX76cOXPm4O/vT1xcXIVXh5Z3zKHsz/Ovr83Ozo7g4GDS0tK4cOFCmW11Ol2ZryuSmppaYUCL6iEBqBGdTsfdd99N3759jeMAgYGBvPLKK2RmZhr/y8/PJygoCC8vL95//32Sk5NZvHgxTzzxBGfOnMHd3Z38/Hxju5cuXarwOWtKYGAgP/30k/F1ZGVl8euvv5pUW2BgII8++miZ45CXl0dMTAwAo0ePZtWqVezevRs7Ozu6dOly0+f38PDg2rVrxjays7OZP38+8McZ4Pbt2+nevTvdu3dn+/btbN++3XgGWN4x/6vnn3+eOnXqkJiYSFZWFk899ZTx7OZmr62ium4mJSWlzL9/P4sICAggOTnZ+FhycrJxbLNFixasWrWK9PR07r333nLHL2+lvGN9q5/Rn92sThcXF3x9fatUU1UNGjSIH3/8kdTUVJydncuM1f5Vecccyv48//ralFKkpKQQEBBAw4YNbxiL//PXFf3tBgcH3/Rs+q/PL26PBKDGnnnmGRYuXMiVK1d48MEH+eCDD4xdOFevXuWbb74BYOPGjZw5cwalFN7e3uh0Ouzt7WnevDnXrl1j27ZtFBYW8sorr5T7XPXr1yc1NbVGrkR86KGHeP7557lw4QJKKZKSkti2bZtJ+44ZM4bVq1cTHx+PwWAgOzu7TPdp9+7dyc7O5vnnn2fUqFE3bSMwMJDo6Gief/558vLy0Ov1HDhwwBjC7du35/Lly8THxxMVFUVkZCS7du3iwoULREREAOUf87/Kzs7G09MTDw8Pjh49WuEl6req62beeustrl+/zokTJ/jss8+Mr3n06NG88sorXLt2jZSUFN59913uvfdeoHQ+X0ZGBg4ODnh6et60bij9nSjvjRbKP9a3+hn92ejRo1mwYAHHjx8nNzeXGTNmMGrUqCq9kd+q3vJcunSJDRs2kJ+fj7OzM25ubuUeEyj/mP/VwIEDOXTokHGo4r333sPV1ZXIyEiio6MpLi7mk08+obi4mA8//LDMmWT79u3ZuHEj169f58yZM2V6GO677z7Wr1/Ppk2bMBgMpKSkGC8yquoxEDeSANRYq1at6NGjB++//z7dunVj1qxZPPDAA3h5edGxY0d27NgBQGJiIr169cLT05PBgwcze/ZsQkND8fb25v3332fUqFE0btyYqKiocp+rd+/eNGrUiHr16hEeHg7A66+/zsCBA6v9dU2bNo3o6GhiYmLw9vZm6NChZT5VV6Rx48asWLGCadOm4evrS8uWLY0fBKC0mykuLo4ff/yx3DcmKA2B1NRUwsLCqF+/Pk899ZTxE7ednR3dunWjZcuWODk54eTkROvWrenatavxjbG8Y/5XL774Ij/99BNeXl5MmTKFESNGVPj6KqrrZgYNGkTbtm254447mDJlivFKwRdeeIEWLVrQsmVLoqOjuffeexk/fjwAmzZtokWLFnh6ejJnzhyWLFly07ZffPFFRowYgY+PT5lxy9+Vd6xv9TP6s/79+/PPf/6TQYMGERoaiqOjI7Nnz67wGJXnVvWWx2Aw8Pbbb+Pv70/9+vU5f/58mSsw/6q8Y/5Xfn5+rFu3jpkzZ1K3bl2+/vpr1q1bh6OjI05OTqxdu5a5c+dSt25dDh8+XGYc+f7776dJkyYEBQVx3333lTlLb9y4MWvXrmXGjBl4e3vTp08fY3g+8cQTLF68GB8fH958802Tj4G4kU79ua9GCGFRdDodKSkpJo8didsnx9x2yBmgEEIImyQBKIQQwiZJF6gQQgibJGeAQgghbJIEoBBCCJskASiEEMImSQAKIYSwSRKAQgghbJIEoBBCCJskASiEEMImSQAKIYSwSRKAQgghbJIEoBBCCJskASiEEMImSQAKIYSwSRKAQgghbJIEoBBCCJvkoHUBQtRWGTmFXMgqIC0zn0vXC7icU8Tl7EIycgrJLdJTWGygUG+goLiEQr2BQn3p/3WAi6M9ro72ODva4+poh6uTPS4O9ni6OODv5UIDbxcaervg7+VCQ29X6nk6Y2+n0/olC2FV5H6AQtzCxawCTlzK5sTF65y4mMOJS9c5nZ5LfnFJjdVgb6ejgZcLzfw9aNHAk1YNvGjZ0JMm9TxwtJeOHCGqQgJQiD/JKdSzP+kqe85e5cC5a5y4lE1mXrHWZZXLyd6OsHrutG7oRWQjX7qG+RJWz0PrsoSoFSQAhU27XlBcGnhnrrL7TAZH065TYqjdfxINvFzoEuZLdFhduobVpZGfu9YlCWGRJACFzbmQlc/3Ry/y3dGL7D93rdYH3q0EeLvQt7U/A9s2pEtjX+xkLFEIQAJQ2IhzGbl897/QO5yaia3+1vt5ONGvdQMGtWtAdFhdHGT8UNgwCUBhtbLyill7IJXVv6Ry/MJ1rcuxOD5ujgxo3YDRnYPpGFJH63KEqHESgMLq7Eu6yvI9yWw8coFCvUHrcmqF1g29GNMlhHs6BOLhLLOjhG2QABRW4fezvRX7kkm8lKN1ObWWu5M9d0UEMq5rCG0CvLUuRwizkgEAEzg4OBAREUHbtm2Ji4sjLy+vUvvPnz+flStXArB48WLS09ONjw0aNIj8/PxqrbeyHnnkEU6fPq1pDVWVnl3Aaxt/JfrNLby84VcJv9uUW1TC8r3JDJ6znREf7eSHXy8hn5GFtZIzQBP4+flx5coVAMaOHUunTp14+umnq9RWz549+eCDD2jbtm11lmhUUlKCvb29Wdq2JOcz85m/9TSr9qdIN6eZtWzgyeO9mjKkXUO5glRYFTkDrKTu3btz6tQprly5wtChQwkPD6dnz54kJSUBsGLFClq1akX79u25++67AXjppZf44IMP+Prrr9m/fz8jR44kMjISgEaNGpGTk8P06dP57LPPjM/z0EMP8fXXX1NSUsLUqVOJioqiffv2fPnllzfUtHXrVnr37s2gQYOIiYkhNzeXCRMmEBUVRadOnfjvf/+LwWCgSZMm5ObmApCfn09oaCh6vZ6ePXty9OhRAL7//nuio6Pp0KED48aNo6ioiGXLljFjxgwAnnvuOfr06QPAt99+y5QpUygpKWHcuHG0bt2adu3asWjRIvMcfCDpSi7PrjlEz3d+YunucxJ+NeC3i9lMWX6QAbN/Zv2hNAxWPm1E2A4JwErQ6/V89913tGvXjpdeeonu3btz+PBhHnvsMaZMmQLAa6+9xrfffsuhQ4dYsmRJmf2HDRtGZGQka9asYf/+/WUei4uLY/Xq1cbn2bJlCwMHDuTTTz+lYcOG7Nu3j927d/P222+TkZFxQ22//PILCxcuZPfu3bz22msMGTKEffv28f333/PEE0+g0+kYOHAgGzZsAGDTpk30798fB4c/Lni4cuUK77zzDj/++CMHDx4kLCyMBQsWEBsby/bt2wHYt28fubm56PV6tm/fTmxsLAkJCZw9e5Zff/2VI0eOMHz48Oo76L/XllPIP786TJ93t7FqfyrFJfImXNNOpufwxPKD3Pn+z/z0W/qtdxDCwkkAmiAzM5OIiAgiIyMJDQ3l4YcfZvv27YwbNw6AUaNGsXfvXgBiYmL429/+xsKFCys1dhIZGcmZM2e4du0aW7ZsISYmBhcXFzZv3szChQuJiIggOjqarKwszpw5c8P+MTExBAQEALB582ZefvllIiIi6Nu3L7m5uVy6dKlMyK5Zs4a4uLgybezevZvDhw8THR1NREQEq1ev5uzZs4SEhHDp0iVycnIoKSkhOjqagwcPsmPHDmJiYggLCyMtLY1JkyaxefNmvL2r7+KJIr2Bj7edptc7W1m+N8XqJ63XBomXcnhw8T4mLNrL6csy5ipqL7ne2QQ+Pj4kJCRUuI1OVzo28tFHH7F7927Wr19PZGQkR44cMfl57rnnHtatW8fOnTuN4WQwGPj444/p0aNHhfu6ubkZ/20wGFi/fj2hoaFltqlfvz4PPfQQGRkZ7N69m6VLl5Z53GAwMHjw4Jt2YXbs2JFPPvmETp060bVrV7Zs2cKVK1cIDAwE4MiRI2zatIn33nuPzZs3M2vWLJNfd3m+P3aR1zcd51xG5S46EjVj64nL7Dj1M+OjG/Fk32Z4ujhqXZIQlSJngFUUGxvLsmXLgNKzqc6dOwNw5swZoqOjee2113Bycrqhu9LT05Ps7OybthkXF8fy5cv54YcfGDhwIAD9+/dn3rx5lJSU3nng6NGjxn+Xp3///syZM8f49e/hbWdnx8CBA3niiSfo27dvme5PgOjoaH766SfOnTsHwPXr1zl79qzx9b733nvExMQQGxvLhx9+SFRUFFDadWowGBg1ahQvvfTSLT8s3EripWzGLNjN35f+IuFn4YpLFAu3n6XXrK2s3Jcs44OiVpEzwCp66aWXmDBhAkuWLMHX15fFixcD8Mwzz3Dq1CmUUgwbNoygoKAy+02YMIEJEybg6el5wzhgZGQkp06dIjo6GhcXFwAeffRRzp49S4cOHTAYDDRs2JDvvvuuwtpeeOEFnnzyScLDw9Hr9XTs2JEvvvgCKA3Znj178v3339+wX7169ViwYAEjRoygqKgIOzs7Zs+eTePGjYmNjSU1NZVu3bpRv359XF1diYmJAeD8+fNMmDABg8GAg4MDs2fPrsohpcSg+GjrKeZsOUVRiVzcUptcySli+tojrNqfyqy49jSWBbhFLSDTIIRFSLyUzTOrD3E4NUvrUsRtcnW059k7WzChWyPj0IAQlkgCUGiqxKCYv+007285SZFMabAq0WF1eXtkOMG+brfeWAgNSAAKzZxKz2Hq6kMcSsnUuhRhJh7ODjw3qBVjuoRoXYoQN5AAFJr46kAqz687Sl5RxRf0COvQr7U//x7VHi+5UlRYEAlAUaMKikt46dtjrNiXonUpooY19nPn4/s70dzfU+tShAAkAEUNSr2Wx9+X/sKxNLk3n61yc7LnzRHh3NU+QOtShJAAFDVj+8krPLH8ANfyirUuRViAh2Ia89yglnJHeqEpCUBhdkt2JfGv9b/KMmaijM6NfZk/rhO+7k5alyJslASgMBulFG/95wTzt9XOew0K8wvzc+fzhzrLVAmhCQlAYRbFJQamrznMVwfPa12KsHD1PZ35/KHOtGropXUpwsZIAIpql1uo57EvD/Bz4mWtSxG1hKeLAwseiKRrWF2tSxE2RAJQVKsrOYU8uGgfR87Lkmaicpwc7Hh/dAQD2zXUuhRhIyQARbVJv17A6E92c/ZKrtaliFrKTgevDWvHfZ1l5RhhfnINsqgWV3IKGbNwj4SfuC0GBc99fYS1v6RqXYqwARKA4rZdyy1i3MI9nEqXu4OL26cUPLv2MBsOp2ldirByEoDitmTlFzPu0z38dvHmN/kVoipKDIqnViSw+dhFrUsRVkwCUFRZdkExD3y2V5Y2E2ahNygmLzvI1hPpWpcirJQEoKiSQn0JDy/eL7cyEmZVVGJg4he/sOt0htalCCskASiq5B9rj7A36arWZQgbUFBcGoJnLssYs6heEoCi0uZuOcnXssKLqEFZ+cU8/Pl+smQxdVGNJABFpWw4nMa7PyRqXYawQWev5PLYl7+gLzFoXYqwEhKAwmQJKZk8s/oQsnSC0MrO0xm8+O0xrcsQVkICUJgkLTOfR5fsp6BYPn0LbS3bk8xn289qXYawAhKA4pb0JQYe//IAl7MLtS5FCABe23ScnaevaF2GqOUkAMUtzdqcSIJMdxAWpMSg+L+VCVzLLdK6FFGLSQCKCsWfvMzHP8sNbYXluXS9kGlrDmtdhqjFJABFuS5nF/J/K+WiF2G5fjh+iSW7krQuQ9RSEoDippRSPL0qgSs5Mu4nLNtrG4/z20VZjk9UngSguKkF8WeIPykXGQjLV6g38MSygxQUl2hdiqhlJADFDc5eyeXfm2Wyu6g9Tqbn8NZ/ftO6DFHLSACKGzz31REK9TLfT9Qun+9M4mDyNa3LELWIBKAoY9X+FHadkZX3Re1jUKWLtBfLUmnCRBKAwigjp5DXNx3XugwhquzEpWw+3ibTdoRpHLQuQFiOVzb8SqaFr7ZfnJHK5W/fMn6tv3oev6HTKLpyjpyE71H6QoKnLDM+fnXLAgqSEnAN60SdXg8BkBn/BS4h4biEhtd4/cL8PvjpFHdHBBLs66Z1KcLCyRmgAEonvK9LSNO6jFtyrBtEwINzCXhwLg3Gvo3O0QWXRh1wbdyRBg/8u8y2hoIcii6dJuDhDym8kIihMBd9dgbFV89L+FmxgmID/1ovC2aLW5MAFJQYFC+v/1XrMiot/9QeXELbY+fkgnPD5jh4+JbdQGcHOh1KGUCnA3Rk7VyOT8wYTeoVNeeH4+n8dCJd6zKEhZMAFKz9JZWT6bXvbtu5v23HvWX3ch+3c3bDtVEHLiyagmujDuivp4POHke/4BqsUmjlre9+Q8kyRqICEoA2rqC4hPdq4Q1uDYV5FJ4/jmuTyAq3844eRcBDH+AdPYqsnSvxibmXzO3LuPz16+Ql7qyhaoUWfruYzbeHLL9bX2hHAtDGfb4ziQtZBVqXUWl5J3fj2qgDOgcnk7bPT0rA0S8EQ2Ee+uuX8bvnH1zf/62ZqxRae/e/iTItQpRLAtCGZeUXM29r7bxkPO+3eNxald/9+WdKKbL3f4NX52Go4kIw6AEdhoLa1+0rKudcRh4r9iZrXYawUBKANmze1lNk5Vv2tIebMRTmUnjhJK6NOxq/l/nzUlI/HI+hIIfUD8dzfe/Xxsdyj/2EW/No7BxdcKzfGKUv4sKnk3Bv01uL8kUNm/PjKfKLZJ1QcSOdklFim3Qlp5DYt36koFi6h4T1mzagBZN6NdW6DGFh5AzQRi3ZdU7CT9iMRTvOyt0ixA0kAG1QQXEJX+w+p3UZQtSYKzlFrDt4XusyhIWRALRBaw+kcjW3SOsyhKhRn24/q3UJwsJIANoYpRSfxssbgbA9J9Nz2JZ4WesyhAWRALQxPxxP58yVXK3LEEITC+PPaF2CsCASgDZmgbwBCBsWf/IKiZeytS5DWAgJQBuSeCmbvWeval2GEJpatCNJ6xKEhZAAtCGr9qVoXYIQmttwOE2mRAhAAtBmFJcY+FouAxeC7AI9W47LrZKEBKDN+Om3dDJk6oMQAHx9MFXrEoQFkAC0EesS5OxPiN9tS7wsc2GFBKAtyC4oli4fIf6kuESxXu4VaPMkAG3Ad0cvUqiXdT+F+LOvZEzc5kkA2oDNxy5pXYIQFudQSibJGXlalyE0JAFo5Qr1Jew8fUXrMoSwSFsTZWjAlkkAWrk9Z66SJzcDFeKmtp6QtUFtmQSglfvxN/mEK0R5dp3OkEnxNkwC0MptPSEBKER58otL2CPLA9osCUArduZyDkkyyC9EheRDou2SALRiMr4hxK1tk78TmyUBaMX2nM3QugQhLN6ZK7mcz8zXugyhAQlAK3YwOVPrEoSoFRLkb8UmSQBaqbTMfNKzC7UuQ4haISHlmtYlCA1IAFopOfsTwnSHUrK0LkFoQALQSsknWiFMd+R8FiUGpXUZooZJAFopOQMUwnT5xSWcuJitdRmihkkAWiF9iYGjadKlI0RlJKRkal2CqGESgFYoKSOPgmK5/ZEQlSEfGm2PBKAVSrqSq3UJQtQ6Zy/L342tkQC0QmclAIWotHMZ8ndjayQArdBZ+UMWotIuXC+QO0PYGAlAKyRdoEJUnlKQclUWj7clEoBWSAJQiKqRu6fYFglAK1NQXMKF6wValyFErSTjgLZFAtDKXMgqQMmCFkJUSbJ0gdoUCUArcy2vSOsShKi1MnLl78eWSABamWvyByxElWXlFWtdgqhBEoBW5pr8AQtRZZn58gHSlkgAWplM6QIVosoy5QOkTZEAtDIyBihE1UkXqG2RALQy0gUqRNVlF+rRl8hC8rZCAtDKZBfotS5BiFotK18+RNoKCUArY5C7WgtxWwr1cgZoKyQArYxCAlCI21EiHyJthgSglTHIh1chbotBllKyGQ5aFyCql5wBWrbm/h70b91A6zJEBbxcHLUuQdQQCUArIx9eLdvwjkFM7NFE6zKEEEgXqNWR4QvL1q1JXa1LEEL8jwSgldHptK5AlMfLxYG2Ad5alyGE+B8JQCvj7mSvdQmiHF3C6mJnJ59QhLAUEoBWxttVBvAtVXSYdH8KYUkkAK2MlwSgxerWVAJQCEsiAWhl5AzQMtV1d6KFv6fWZQgh/kQC0MrIGaBl6hpWF51coSSERZEAtDIyidcyRcv0ByEsjgSglZEuUMsk8/+EsDwSgFamobeL1iWIv2jg5UJYPQ+tyxBC/IUEoJUJrOOKvcw1syjS/SmEZZIAtDKO9nZyFmhhJACFsEwSgFYoxNdN6xLEn8j4nxCWSQLQCoXWlQC0FCG+bgTVkZ+HEJZIAtAKBcsZoMWQ5c+EsFwSgFYo1Ndd6xLE/8jyZ0JYLrkhrhVqWl8uubcU5roA5kr+FXam7TRL2+L2Ods7M6DRAK3LELcgAWiFmtb3wMXRjoJig9al2LSm9T2o72meK3L9XP1QSvH6ntfJ0+eZ5TlE1fm5+kkA1gLSBWqF7O10tGjgpXUZNs/c4393N72bVUNX0bpua7M+j6g8O528tdYG8lOyUu0CJQC1VhPTH0K9Qvli4Bc80PoBdMgCCJbCQSeda7WBBKCVah/ko3UJNk2nK70DRE1wtHdkWtQ05vWdh6+Lb408p6iYvZ291iUIE0gAWqkOIXW0LsGmtWzgRR13pxp9ztjAWNbetZZuAd1q9HnFjTwc5UK02kAC0Eo1qecud4bQkFarv/i5+jG/73ye7vQ0DnbSDaeVOi7yAbQ2kAC0UjqdjshQ+SPUipbLn+l0Oh5s+yBfDPyCEM8QzeqwZT7OPlqXIEwgAWjF7mheT+sSbJK9nY7Ojc04FldSbNJmbfzasGroKoaEDTFfLeKm5AywdpAAtGI9JAA10TbQG08XM3U/Z6bAgt5w5ZRJm7s7uvNG9zd4PfZ13B1lhaCaImeAtYMEoBVr5OcuC2NrwKzdn0nxcPEwfHwHHPzC5N2GNhnKqiGraFO3jflqE0Z1nOUMsDaQALRychZY88wagGd/Lv1/cS58MwnWPAwF103aNcQrhKWDljKhzQSZM2hmPi4+WpcgTCABaOUkAGuWk70dUY3MOP53Nr7s10fXwPxYSN1v0u6Odo5MjZzK/L7zqesiC3Wbi5wB1g4SgFYuukldnBzkx1xTIoJ9cHE00yTojNNwPfXG72eeg88GQPy/wWDa+q/dArux9q61xATGVHORAiDQM1DrEoQJ5J3Ryrk5OcgdyWuQue7+APzR/XkzBj1seRmW3gPZF01qrq5rXT7q8xHPRD6Do53MGa0uLvYuBLgHaF2GMIEEoA24O0L+GGtKjYz/VbjNNvioGyR+b1KTOp2O8W3Gs3TQUkK9Qm+zwMo7N+ccvz7+K8kfJBu/l3cmj5PPnSTx2UTSv0kHQClFyrwUTs44ScZ/M4zbpn6aSuHFwhqvuyKNvBuh08kYa20gAWgDBrRpgJuTrE1obi6OduZdgi4p/tbbAORlwLJR8N100JsWDm3qtmHVkFXc1eSu2yiw8ur2q0vQo0Flvndh6QWCHwum2ZvNyD6UTUFKAQUpBegcdDR9tSnX4q8BkH8uH3sXe5wbONdozbfS2Kux1iUIE0kA2gA3Jwf6t/bXugyrFxnqa77x1vTjkHu5cvvsmQ8L+8DlRJM2d3N047XY13ij+xs1NmfQo5UHdi5/HLPia8WoEoVLsAs6Ox3eXbzJPpSNzl6HUgpKQOdQenZ1+dvL1LvL8i7yauwjAVhbSADaiLs7yKC8uWk2/leRi0fgkx5wYInJuwwJG8Lqoatp59euas95G/SZehzr/DEe6VjHkeJrxbgEumDvZs/pf53Gt5cv2YezcW3sioOn5a132thbArC2kAC0EXc0q4efR83encDWaD7+V57iPPj2CVj9IBRkmbRLsGcwnw/8nAfbPmgxcwYD7g+g6StN8YnxIeOHDOr2q0vaF2kkz00mNzFX6/KMwrzDtC5BmEgC0EbY2+kYEi4Xw5iLp7MD4ea6B6PBAEnbb7+dY1+VzhlM2WvS5o52jjzd6Wnm95uPn6vf7T+/CRx8HCi+9sdap8XXinHwKXuWdy3+Gt5dvMk9mYuDpwNBfwvi8reV7B42EzudHY28GmldhjCRBKANGR0VrHUJViuqsS/2dmY6U7p4GAoyq6etzGRYNBB+fsf0OYMBpXMGYwNjq6eGCjjWcQQ7KEgpQBkUWXuy8IrwMj5uKDSQfSAbn24+qEKF0isASvJKzF6bKZr4NMHJXnpaagsJQBvSqqEX0TV0l3JbY7Hdnzdj0MOPr8KSu+B6mkm7+Lr4Mq/PPKZFTqvWOYNn3z5LyrwUsg9n89v//UbeqTwCxgWQ8lEKidMT8WjngUuwi3H7K/+5Qt0BddHpdHi08yDvVB6n/3Wauv0t4/e6Y/2OWpcgKkGnlFJaFyFqzg+/XuKRJaYtmyVMt3FKLG0CvM3T+Bcj4dR/zdO2qy/c/SG0HGTyLsczjvPsz8+SdD3JPDXVYu/c8Q53Nr5T6zKEieQM0Mb0aVWfRnKHiGrl4+ZI64Zet96wKkr0kLzLPG0D5F+FFffBpmkmzxlsVbcVK4es5O4md5uvrlqqo7+cAdYmEoA2RqfTMaFbI63LsCpdG9c138ofaQegKMc8bf/Z3k9K7zN4+YRJm7s5uvFq7Ku81f0tPBw9zFxc7RDsGUx9t/palyEqQQLQBsVFBuPpYnnzp2qrbk3NOf63zXxt/9Wlo/BJT/hlscm7DAobxOqhqwn3CzdbWbWFjP/VPhKANsjd2YH7OodoXYbVqFUXwNxKcR6sfxJWjYf8TJN2CfIM4vOBn/Nw24ex09nuW0on/05alyAqyXZ/W23co93DZH3QalDP05mm9T3N07i+0OQ5e9Xu13Uwvzsk7zFpcwc7B57q9BQf9/uYeq6WtzxZTZAArH0kAG1UPU9nGQusBmadVpKyF/QF5mv/VrL+N2dw29smzxns2rAra+9ayx1Bd5i5OMsS7BlMiJf0qtQ2EoA27O89muAlY4G3xaq6P29GlcBPr8HnQ02eM1jHpQ4f9vmQ6VHTcbKzjUnhvYJ7aV2CqAIJQBvm7erI33s00bqMWq1bEzMuEWYJAfi7c9vhoxj4baPJu4xrPY4vB39pE0uDVSYAdTodzz//vPHrZ555hsWLF1fpebdu3crevZXvJp8wYQIbNmy46ffDwsJo37494eHhbNmypUp1zZ8/n5UrV1Zp35okAWjjHoxphJ+HZd1PrbYI9HElxFxzKoty4fwv5mm7qvKvwooxsHEqFJvWNdvStyUrh6xkWNNhZi5OO3Wc69ChfgeTt/fw8ODLL78kOzv7tp+7ogAsKana8nBz5szh0KFDvPvuu0ycOLFKbUycOJHRo0dXad+aJAFo49ycHJjcS84Cq8Kstz9K3gWG4ltvp4V9C0vnDKb/ZtLmbo5uvBzzMu/c8Q6ejma6YEhDvUN6Y29n+gVlzs7OjB07lnnz5t3w2OnTpxkwYACRkZH07t2bpKQkAHr27MnRo0cBOHr0KD179iQlJYX58+fz5ptvEhERQUJCAhMmTOCxxx6jc+fOvPnmm6xbt47OnTvToUMHBg8eTGZmpsl1xsbGkpqaavz6rbfeIioqivDwcGbNmgXA6NGj+fHHH/84Fr17c/DgQV566SU++OCDcl9TWloaMTExAGzevBlXV1eKiorIzMykQ4fSDxOzZ8+mRYsWtG/fnscee8zkuitDAlAwpksoYfVq5gao1sTqx/8qkn6sdM7g/s9M3uXOxney+q7VtK/X3nx1aaAqS589+eSTfPLJJxQUlD2Tfvzxx/n444/Zv38/zz//PNOmTSu3jeDgYCZOnMg//vEPEhISiIiIACAjI4M9e/YwY8YMevTowZ49ezh48CADBgzgww8/NLnGjRs3ctdddwGlIZWamsrevXs5ePAgmzZt4ujRo8TFxbF69WoA0tPTSUtLMwZYRa8pICCAa9euUVhYyPbt22ndujW//PILO3fuJDo6GoCXX36ZAwcOcOjQId58802T664MuQJC4ORgx6t3t2XMQtMueRelzHsD3HjztV1d9Pmw4f/g9E9w1xxwrXPLXQI9All852LmJczj06OfYlCmXV1qqXxdfInyj6r0fvXq1WPIkCF89tkfHyBycnKIj4/nnnvuAUAphbt75T+Yjhw50rgyUXJyMnFxcVy6dIn8/Hy6dOlyy/2nTJnC008/TXJyMjt27ABKA3Djxo3Ex5f+XmZnZ5OYmMigQYN49tlnKSkp4euvv2b48OFl2qroNUVGRrJ371727NnD1KlT2b59O9euXTOeGXbu3Jlx48YRFxdn3L+6yRmgAKBbUz/ujpD7BZqqsZ87Db1dzdN4QRZcOGSets3h+LfwUSyc22nS5g52DkzpOIUF/RZQ37V2Lx3WL7Rfpbo//+yZZ57h/fffR6/XA2AwGPD39ychIYGEhAQOHTrEzp2lx9TBwQHD/6aiFBZWvGarm9sf49JTpkzh2Wef5ciRI8yePfuW+0LpGGBiYiJvvPEGjz76qLG2mTNnGms7ffo0w4cPx83NjaioKH7++WfWrFlDXFxcmbYqek2xsbFs27aNwsJC+vfvz86dO9mxY4cxADdu3MjkyZPZtWsXPXr0MOWQVpoEoDB6fnBrmRZhIrOe/SXtKJ1+UJtcT4XFQ+CnN8BgWu2dG3Zm7V1r6RnU07y1mdGIZiOqvG9wcDAxMTGsXbsWAC8vL/z9/Vm/fj1QehHL7+N+oaGhJCQkAPDVV18Z2/D09KzwYprr168TGBiIUoolS5ZUqr6nnnoKvV7P5s2b6d+/PwsXLiQvLw+ApKQksrKyAIiLi+Ojjz4iNTX1hu7Pil5TbGwsH3/8MREREfj5+XHlyhXS0tJo1KgRBoOBlJQU+vTpw6xZs0hOTq7yRT0VkQAURvU8nZl2Z0uty6gVbHr8rzyqBLa9WTpnMCv11tsDPi4+zO0zl390/ketmzMYXi+cVnVb3VYb06dPJy3tj/mVy5YtY+7cubRv35527doZpyE8/fTTvP3223Tq1ImioiLj9kOHDmX58uXGi2D+aubMmQwdOpSoqCiCgyt3Q2ydTseLL77IrFmzuPPOOxk2bBhdu3albdu2jBs3zjh+OWjQIDZt2sSwYTe/0re819SqVSvy8/ONZ3ytWrWiY8fS9VRLSkoYO3Ys4eHhREZG8uKLL2JvX/0rV8n9AEUZBoNi+Ec7SUjJ1LoUi6XTwb4Zfc03feSjmNKFqWszFx+4ay60vsvkXU5cPcGzPz/Lmawz5qurGr0e+zpDmwzVugxxG+QMUJRhZ6fjjeHtcLKXX43yNK/vab7wy82AS8fM03ZNKsiEVffD+qegON+kXVr4tmDFkBW31a1YU+o412FAowFalyFuk7zLiRu0aujFs3e20LoMi2Xe8b+fASvqlPllEXzSCy79atLmrg6uvNTtJWb1mIWnk+XOGbyn2T042deuLltxIwlAcVMPxzamezMzLvNVi8n4XyVdPl46cX7fQpN3GdBoAGuGriGiXoT56qoiO50do5qP0roMUQ0kAMVN6XQ6/j2qPXXd5VPun9npoIs57wBRG+b/VYU+v3QJtRVjIe+qSbsEeASw+M7F/C38bxZ1n8GYgBiCPIO0LkNUA8v5rRIWp76nC2+PlDt9/1mbAG+8XR3N0/j1C5Bx0jxtW4rfNpTeZzBph0mb29vZ80SHJ1jYfyH13SxjzuC4VuO0LkFUEwlAUaE+rfx5IDpU6zIshnR/VoPrqaVTJX563eQ5g1ENolg7dK3mtx3qUL8D3QK7aVqDqD4SgOKWnhvUinaB3lqXYRG6SgBWD1UC296CRYMgM8WkXXxcfJjTew7PdXkOZ3tt7mDyeMTjmjyvMA8JQHFLLo72LHggkvqetn3bJEd7HZ0b+ZrvCZJsKAB/l7Ib5sfCr9+YvMt9Le9j2eBlNPGu2buYRPpH0rVh1xp9TmFeEoDCJA28XfjkgUicHWz3VyY8yAd3ZzMtFXctCTKTzdO2pSvIhFUPwPonTZ4z2LxOc1YMWcHI5iPNW9ufTIqYVGPPJWqG7b6biUqLCPbhrRG2e1GMjP+Z2S+LS2+xZOJCAC4OLsyMnsm7Pd/Fy8nLrKV1adiFyAaRZn0OUfMkAEWl3NMhkMd62uYNdKNl+oP5Xf6tdM7gnk9M3qVfaD/WDF1Dx/odzVbW5IjJZmtbaEcCUFTaswNa0K+1v9Zl1ChnBzs6ht76fndVliQBaKQvgO+mwfL7TJ4z2NCjIZ8N+IyJ7Sdir6veRZO7B3Ynon5EtbYpLIMEoKg0nU7HnHs7EGnOQLAwHUPq4OJY/avRA3A5EbIvmKft2uzEptKFwU08O7a3s2dSxCQW9l9IA/cG1VKCk50T0ztPr5a2hOWRABRV4upkz6cTomjV0LxjL5bCvON/28zXdm2XnQZL7oItr0CJ3qRdIhtEsmboGvqE9Lntp3+o3UOEesk8WGslASiqzNvVkSUPdaaxn7vWpZideRfAlu7PCikDxM+CxYNMvlLW29mb2b1m83yX56s8ZzDYM5hH2j1SpX1F7SABKG5LPU9nlj3ahRBfN61LMRt3J3vaB/uYp3GlIGm7edq2Nil7SucMHvva5F1GtxzN8sHLaerTtNJPN6PLDM0m3IuaIQEobltDb1eWPdqFQB9XrUsxi8hGvjia6/6Il45CXoZ52rZGBVmwegJ8MxmK8kzapVmdZiwfvLxSd3DoF9qPmMCYKhYpagsJQFEtguq4seJvXa2yO1Tm/1mgg0vhkx5w8YhJm7s4uPBC9AvM7jn7lnMG3R3dmR4lF77YAglAUW2Cfd1YPTGatoHWdWGMWcf/ZP5f1V1JhAV9YM/HJu/SJ7QPa+9aSyf/TuVuMyliEv7utjXNx1ZJAIpq5efhzIq/RRPT1IyhUYO8XBxoG2CmhcANJXBup3nathUlhfDds7DsXsg1rSu5gXsDPu3/KY+3f/yGOYOdG3RmbKux5qhUWCAJQFHtPJwdWDShM4PbNdS6lNvWJawudnY68zSelgCFWeZp29YkfgfzY0zuUra3s+exiMf4bMBnNHQv/T31cvLitdjXLOrmu8K85CctzMLJwY6593VgXNcQrUu5LWZd/swW7/5gTtkXYMndsOVlk+cMdvTvyOqhq+kX2o8Xol+otgn0onbQKaWU1kUI67bg5zO8+Z/fKDHUvl+1/zzVnZYNzDSmuXQYnP7RPG3buqAoGPEp1JFJ7KJ8cgYozO7RO8JY+nBn6ro7aV1Kpfh5ONHC39M8jZcUQ/Ju87T9F8NW5lHnreuMXPXHtIEvDxfTdl4OrT/M4Z0dhQAopbh3TR5t5+UwZ0+hcduHv8knMcO0O7dbjNR9ML87HF2rdSXCgkkAihrRrYkf65+IpX1Q7bmzfJewuuh0Zhr/S90HxabNY7tdT3ZxYsk9f8zRvJJn4IWfCoh/0J0jj7nzY5KeE1dKOHzJgJO9jiOPubMooRiAgxdK8HDS0byumdZBNafCLFjzEKybBEW5WlcjLJAEoKgxAT6urJoYzajIIK1LMYm13P6oZyMHPJ3/CPIz1xSt6tlTx1WHvZ2OO0Ic+Po3PY72oAC9AZztS7d/Nb6QF3rUrjP3GyR8AR/3gAuHta5EWBgJQFGjnB3seXtke14f1g4XR8v+9bPWCfBNfe04ml7C+esGCvSK707pOX/dQOt69ng7Q9SCXCZGOvLdyWKiAuzxc7Psn5NJMk7Cwr6wa57WlQgL4qB1AcI2jekSQpcwX55edYhDKZlal3ODht4uhNXzME/jxfmlXaAa8XXV8f6dLtyzMg9nex3t/e2w/99Ujw8GlXaVGpRi6PJ8Vo10Zcp3BZzPNvB/XZ2IDanFbxklhfD9P+HMVrhnHrj7aV2R0JgVfLQTtVWTeh589Vg3pvZrjqO9mcbaqsis3Z/Ju0vfjDV0T0tH9j3qwfaH3GnoaUcz37JvBYsOFnNvGwd2pJRQz03H0mGuvPKztjVXm5Pfl95n8MxWrSsRGpMAFJqyt9PxRJ9mfP14jPmuuKyCrlZ++6P0XAMAF3MMrDxWzH3tHI2P5RUr1p3QMy7ckbxiRVGJQinIKtCqWjPIuVg6DeW/M02eMyisj8wDFBajUF/Cu/9N5NP4s+g1njO4fXovguqY6RZPC/vWaBdo3yW5HLpkILdI4euqY3WcK+/uLuJYugF7O5jVz4UBTf/o2nxlWyExIfb0buxAfrFiyPI8LmQrXuzhzL1tHSt4plpq7Bpo1k/rKoQGJACFxUm8lM1L3x5j52ltbhMU4uvGz8/2Mk/jhdnwViMwyFmHRej0IAydrXUVQiPSBSosTnN/T5Y92pWPxnbU5B6DZr3689wuCT9L4d8O7nxT6yqEhiQAhcUa2K4hW6b24Mk+zWp0yoR5b3+0zXxtC9O5eEPcYnB00boSoSEJQGHRXBzt+b9+zfnh6R4M7xhovFzfnMwbgLIAtubsHGDUEvBrqnUlQmMSgKJWCKrjxrujItjydA9GdgrCwUxB2LS+B/U9zXRWkHcVLh01T9vCdIP/DWE9ta5CWAAJQFGrNPJzZ1Zce7ZM7cGoyOoPQrPO/zu3A5TBfO2LW4ueDJ0maF2FsBASgKJWCq3rztsj2/PTMz25r3NItY0RWuvyZwJoMRj6vaJ1FcKCyDQIYRWy8otZ80sqX+45x5nLVVv5X6eDgy/0w8fNTIs/f9gFLv9mnrZFxRqEw0P/ASd3rSsRFkQCUFidHaeusHTXOX44fqlSE+pbN/Ri05PdzVNUTjrMamaetkXF6jSCB78DrwCtKxEWphavbCvEzcU09SOmqR+Xrhew5pdU1h9K47eL2bfcT67+tEI+ITB+g4SfuCkJQGG1/L1cmNSrKZN6NeXM5Rw2HbnAxiMXOX7h+k23l/E/K+MdDOPXg0+w1pUICyVdoMLmnL2Sy8bDaWz+9RJHz2dhUOBgpyNhZn88nM30mfD9CLh21jxtixt5BcKEjeDbWOtKhAWTABQ27VpuETtPZ5CUkcukXmaaGJ2ZArPbmqdtcSPPhqXhV7eJ1pUICyddoMKm1XF3YnB4Q/M+iQXc/shmeDQoHfOT8BMmkAAUwtxk/K9m+DUvvbVRnVCtKxG1hASgEOZ2Vs4AzS6kG9y3DFzraF2JqEUkAIUwp4zTcD1V6yqsW9sRcM9H4OCsdSWilpGl0IQwJ+n+NK+YJ2HEpxJ+okrkDFAIc5IANA+dPQx6G6Ie0boSUYtJAAphTnIFaPXz8IcRC6HxHVpXImo5CUAhzCX9OORe1roK6xLWE4YvAI/6WlcirIAEoBDmIt2f1UdnBz3+AXdMAzu5dEFUDwlAIcxFArB6SJenMBMJQCHMwWCApO1aV1H7NekDw+ZLl6cwCwlAIczh4mEoyNS6itrLtQ4MeB0ixmhdibBiEoBCmIN0f1Zd2xFw51vgUU/rSoSVkwAUwhwkACvPKwiGvAvNB2hdibAREoBCVLcSPSTv0rqK2kNnD1EPQ5+Z4OyhdTXChkgAClHd0g5AUY7WVdQOzQdC35lQv5XWlQgbJAEoRHU7u03rCixfUGfo9y8I7aZ1JcKGSQAKUd1k/K98fs2hz4vQaqjWlQghAShEtdIXQsperauwPHUaQ+xT0OF+sLPXuhohAAlAIapXyl7QF2hdheUIiYboSdBisCxhJiyOBKAQ1Um6P0uv6mx9N3SbDIGdtK5GiHJJAApRnWw5AF3rQMRY6PJ38AnRuhohbkkCUIjqUpQL53/RuoqaZedQul5nxBhoMQgcnLSuSAiTSQAKUV2Sd4GhWOsqaoAOgjuXLlnWZpgsVC1qLQlAIaqLNXd/OriUztlr0gda3yVdnMIqSAAKUV3OxmtdQfWq17I08Jr2htAYcHTVuiIhqpVOKaW0LkIIq3D9ApzbAed2lv535QQog9ZVmcbOEeq3hIbtS1dpadoHvIO0rkoIs5IAFMJcivIg/TikH4NLf/ov/6q2ddk5gn/r0rBrGAEBEeDfFhycta1LiBomAShETbt+AdJ/hevnIfsiXE8r/X/2hdL/514GVVLFxnXg5FF6YYpPcOlYnXdI6b+9//e1V4BZV2PR6XTMmDGDV199FYBnnnmGtm3bMmHChGp7jnXr1tG6dWuaN28OwCOPPMI///lPmjRpclvtOjg40LZtW4qLiwkLC2Pp0qX4+PhUup1Bgwaxdu1aXF2l29iSSQAKYWkMJZB/rXRFGX1h6X8lhaAv+uP/OkqDzsn9f//979+ObqDTaVq+p6cnfn5+HD58GE9PT7ME4IQJExg5ciRDhgyptjYB/Pz8uHLlCgD3338/LVu2ZMaMGdX6HMJyyNpEQlgaO3tw9ysdg6vbpLS7MqADhHSBxndAs77QtC+EdIUG7cA3rPSMz8ld8/ADcHZ2ZuzYscybN++Gx06fPs2AAQOIjIykd+/eJCUlAbBr1y7atGlDhw4dmDRpEiNHjgRKz/Q6d+5Mhw4dGDx4MJmZmezZs4dvv/2WKVOmEBERQXp6Oj179uTo0aN89NFHvPjii8bne/nll3nvvfcAeOutt4iKiiI8PJxZs2bd8nXExMSQmpoKwOXLlxk+fDiRkZFER0dz8OBBsrKyaNasmXH7c+fOERERAUCjRo3IySm9JdbSpUuJioqiffv2PP300wC8/vrrLFiwAIAxY8bw8MMPAzBnzhzeffddcnJyuPPOO2nXrh3t2rXj+++/N/n4i0pQQghRjerWravS09NVWFiYys/PV1OnTlWLFi1SSinVv39/dfbsWaWUUlu2bFEjR45USinVpk0b9csvvyillBo7dqwaMWKEUkqpq1evKoPBoJRS6v3331evvvqqUkqp8ePHq/Xr1xufs0ePHurIkSPq4sWLqk2bNsbvh4eHq5SUFPX999+ryZMnK4PBoPR6verVq5c6cuTITWtXSim9Xq+GDx+uNmzYoJRSasyYMWrv3r1KKaUSExNV586dlVJKDR48WO3evVsppdSsWbOM9YWGhqrs7Gz166+/qhEjRqji4mKllFL333+/2rBhg9q2bZt64IEHlFJKdevWTcXGxiqllIqLi1N79uxRa9asUWPGjFFKKWUwGFRWVlZlfwzCBDINQghR7erVq8eQIUP47LPPjN/LyckhPj6ee+65BwClFO7u7mRmZlJcXEzHjh0BGD16NJ9//jkAycnJxMXFcenSJfLz8+nSpUuFz+vv70+9evU4evQoTk5OuLu7ExQUxOzZs9m4cSPx8aVTVbKzs0lMTKRt27Zl9s/MzCQiIoLU1FSaNWvGgAEDAPjhhx84duyYcbtr164BEBcXx+rVq+nSpQtr165l8eLFZdrbsmULu3fvJjIyEoC8vDw6derE3//+dyZOnEhycjIhISEUFhZy+fJlDhw4QIcOHfDx8eGpp57i2WefZdiwYURHR1fm8AsTSQAKIczimWeeoW/fvgwcOBAAg8GAv78/CQkJZbb7PUxuZsqUKcyYMYP+/fuzYcOGGwLmZkaNGsXq1atxcnIiLi7O+NwzZ85k/PjxFe7r4+NDQkICubm59OvXj3nz5jFlyhQA9u/fj4ND2bfMe+65h9dee40nn3yS/Px840U5vzMYDDz66KPMnDnzhueqU6cOa9asITY2loKCApYuXUpQUBCOjo40b96chIQENmzYwNNPP83YsWOZPHnyLV+7qBwZAxRCmEVwcDAxMTGsXbsWAC8vL/z9/Vm/fj0AJSUlHD16lDp16uDg4GAMxtWrVxvbuH79OoGBgSilWLJkifH7np6eZGdn3/R5hw8fzldffcXatWuNAdi/f38WLlxIXl4eAElJSWRlZZVbu7u7O3PmzOHf//43er2eXr168dFHHxkfP3ToEADe3t40b96c6dOnG8ct/6xPnz6sXLmSjIwMANLT07lw4QJQOsb43nvvERMTQ2xsLO+99x6xsbEApKWl4e7uzvjx43nqqadu+NAgqocEoBDCbKZPn05aWprx62XLljF37lzat29Pu3bt2LJlCwCffPIJY8eOpWPHjjg7O+Pl5QXAzJkzGTp0KFFRUQQHBxvbuffee3nllVeMF8H8mb+/P35+fri4uBAUVDqZ/84772TYsGF07dqVtm3bMm7cOAoKKr5vY2RkJO3atWPVqlXMnTuXrVu30r59e1q1asWyZcuM28XFxbF8+XJj2P5ZmzZtmDFjBn369CE8PJzBgwdz9WrpPNDY2FiysrJo164dHTt25OrVq8TExABw5MgRoqKiiIiIYPbs2caLZ0T1kmkQQgjN5ebm4u7uDsDkyZNp2bKldPkJs5MzQCGE5r755hsiIiJo3bo1GRkZxmkBQpiTnAEKIYSwSXIGKIQQwiZJAAohhLBJEoBCCCFskgSgEEIImyQBKIQQwiZJAAohhLBJEoBCCCFskgSgEEIImyQBKIQQwiZJAAohhLBJEoBCCCFskgSgEEIImyQBKIQQwiZJAAohhLBJEoBCCCFskgSgEEIImyQBKIQQwiZJAAohhLBJEoBCCCFskgSgEEIImyQBKIQQwiZJAAohhLBJEoBCCCFskgSgEEIImyQBKIQQwiZJAAohhLBJEoBCCCFskgSgEEIImyQBKIQQwiZJAAohhLBJEoBCCCFskgSgEEIImyQBKIQQwiZJAAohhLBJEoBCCCFskgSgEEIImyQBKIQQwiZJAAohhLBJEoBCCCFs0v8DehH99LUNmqYAAAAASUVORK5CYII=</t>
-  </si>
-  <si>
-    <t>https://www.flipkart.com/micromax-j22/p/itm3ff6023b66779?pid=MOBGGBQY9QZJGHHR&amp;lid=LSTMOBGGBQY9QZJGHHRFCEBSX&amp;marketplace=FLIPKART&amp;q=micromax+keypad&amp;store=tyy%2F4io&amp;srno=s_1_2&amp;otracker=search&amp;iid=22496617-e0d2-4a7c-a8ac-eaf50879265c.MOBGGBQY9QZJGHHR.SEARCH&amp;ssid=hptaldccc00000001688580884943&amp;qH=26e55ddeaa2e42a6</t>
-  </si>
-  <si>
-    <t>Micromax J22</t>
-  </si>
-  <si>
-    <t>₹1,152</t>
-  </si>
-  <si>
-    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAcAAAAFQCAYAAAAoQ64wAAAAOXRFWHRTb2Z0d2FyZQBNYXRwbG90bGliIHZlcnNpb24zLjYuMSwgaHR0cHM6Ly9tYXRwbG90bGliLm9yZy/av/WaAAAACXBIWXMAAArEAAAKxAFmbYLUAABII0lEQVR4nO3deVxU9f7H8dewy66CIAgq7qK44YKg4hK5ZLmhlZW2Xi3Tfql1b5uW7XnTtDTT0mwxt3L3amoWmvu+5a6AO4LIvs339we3uZGCMMKcYc7n+Xj0SJiZ8/3MmRnec77ne75fg1JKIYQQQuiMndYFCCGEEFqQABRCCKFLEoBCCCF0SQJQCCGELkkACiGE0CUJQCGEELokASiEEEKXJACFEELokgSgEEIIXZIAFEIIoUsSgEIIIXRJAlAIIYQuSQAKIYTQJQlAIYQQuiQBKIQQQpckAIUQQuiSBKAQQghdkgAUQgihSxKAQgghdEkCUAghhC5JAAohhNAlCUAhhBC6JAEohBBClyQAbVx0dDTffvtthWzbYDCQmJhYIds2R3x8PN7e3lqXYdW+++47+vbta/bt1mbixIk89dRTxd7u7u7OxYsXLVhRySry8yjKTgLQwurUqYOrqyvu7u4EBAQwevRoCgoKLNL2vHnz6NGjR6nuGx8fj7u7O+7u7ri5uWEwGEw/u7u7V3Cl5gkODubGjRtal2HVhg4dysqVK00///1LzN9vtzZl/dKVnp5OQEBABVZkeRKi5UcCUAPr168nPT2duLg4li5dypdffql1SbcIDg4mPT2d9PR0Tp8+DWD6OT09vcLazc/Pr7BtWwNbf356opTCaDRqXYa4CxKAGqpXrx6RkZHs37/f9LslS5YQGhpKtWrVuP/++7l69SoA165do1evXnh7e+Pj48NDDz0EwObNm6lfv36R7d7uW/KZM2cYMWIEmzdvxt3dndDQ0HJ5DitXrqRu3br4+Pjw3nvvmX5fUFDAhAkTqF27Nn5+fowdO7bYP/7R0dG8/vrrhIeH4+bmRl5eHr/++itt2rTB29ub6OhoUwg/9dRTvPnmm0UeHxISwpYtWzh37hwODg6m3ycnJ/Pwww9To0YNQkJC+PrrrwE4efJkkaOCmJgYunXrZvo5ICCAkydPFrvP/+706dN07twZb29vAgICeOWVV0y3zZs3j65du/KPf/wDLy8v5s6dW2xdt2MwGJg+fTrBwcH4+/vz0UcfmW7Lzs7mueeew9/fn+DgYN566y3TH+Tt27fTqlUrPD09CQwMZMqUKaZ6/uwFiImJAaBRo0a4u7sTFxdX5PaS9jVQ7Gt0OzNmzCAkJARfX18eeeQRUlNTgf+9f9966y2qVatGnTp1WLdu3W23cbt6AbKysoiNjcXDw4P27dtz9uzZIvvvz8/CV199Re3atfHw8KBRo0Zs3ry5zPt8+PDhjBo1im7duuHq6srp06eJi4ujVatWeHt706VLF44dO2a6/65duwgLC8PT05MRI0YUCczhw4fz9ttvm37+ew/Npk2bCA8Px9PTkwYNGhAXF8ekSZOIi4vjqaeewt3dnXfffbfYfS5KQQmLql27toqLi1NKKXX8+HHl7++vJk+erJRSaseOHSowMFAdPHhQ5ebmqvHjx6uBAwcqpZR6+eWX1ciRI1VeXp7Kzs5WW7duVUop9csvv6h69eoVaQNQCQkJSimlunTpor755hullFJz585V3bt3L3Lf9957T/Xp06fEmi9duqRu91YB1KBBg1RaWpo6dOiQcnZ2VqdOnVJKKfXhhx+qrl27qqtXr6qUlBQVHR2tpk+fftvtd+nSRdWrV0+dPHlSZWVlqfj4eOXj46N+++03lZ+fr6ZNm6bCw8OVUkqtX79eNW3a1PTYHTt2qFq1aimj0ajOnj2r7O3tTbf17t1bjR07VmVnZ6tjx46pmjVrqgMHDiillPLz81OnTp1S+fn5KigoSAUGBqrc3Fx16tQp5efnV+I+/7tTp06pzZs3q7y8PHXixAkVFBSkfvrpJ9M+t7e3V3PnzlUFBQUqMzOzxLput49jYmJUamqqOnbsmPL391cbNmxQSin1yiuvqC5duqjk5GR1/vx51aBBAzV37lyllFLt27dX3377rVJKqeTkZLV3715TPX99D/z1vfL320va1yW9Rn+3fv165e/vr44cOaLS09PVgAED1LBhw5RShe9fe3t79f7776u8vDw1a9YsFRwcfNvt3K7eCRMmqCpVqqhNmzapvLw89eijj6rHHnvslvunp6crDw8PdeLECaWUUufOnVNnzpwp8z4fNmyYql69utq9e7fKy8tTly9fVt7e3mrp0qUqNzdXffjhh6p+/foqLy9P5eTkqFq1aqkZM2ao3NxcNW3aNGVvb2/6PA4bNkxNmjTptvv+9OnTysPDQ61cuVLl5+er8+fPq5MnTyqlin6mxd2RI0AN9OrVC3d3dxo1akTHjh157rnngMJvqM8++yzNmzfH0dGR119/neXLl5Ofn4+joyOXLl0iISEBZ2dnOnbsWC61/POf/2TVqlV39Xh3d3eaNWtGWFgYhw4dAuDLL7/k7bffxtfXF29vb8aOHcuSJUuK3c6TTz5J/fr1cXFx4bvvvqN///506tQJe3t7nn/+ec6dO8e5c+fo1q0b165d48iRIwAsWrSI2NhYDAZDke1dvnyZzZs389577+Hs7Ezjxo15+OGH+fHHHwHo1KkTv/32G/v27SMsLIyWLVuyd+9e4uLiiIqKAij1Pq9Xrx5dunTBwcGBBg0aMHToUNNR0p+3Dx8+HDs7O1JTU0us63b+9a9/4enpSePGjXnyySdZuHAhAD/88AMTJkygatWqBAcHM3bsWBYsWGCq/dSpUyQnJ1O1alVatWpV4ut4OyXt65Jeo7/74YcfeOaZZ2jatClubm68++67LFy4EKUUAG5ubowfPx4HBwceeeQR4uPjy3Qut3v37nTt2hUHBwcefPBBDhw4cNv7GQwGjhw5Qk5ODrVr16Zu3brFbrO4fQ4wcOBA2rRpg4ODA+vXrycsLIwBAwbg6OjI2LFjyczMZNeuXWzbtg0HBwdGjhyJo6Mjo0aNombNmqV6TgsWLKBv377cd9992NvbExwcfEtPj7h7EoAaWLt2LWlpaSxbtozdu3ebzqnFx8fzzjvv4O3tjbe3N0FBQTg4OHD58mXGjx9PcHAwXbp0oXHjxlZz3tDPz8/0b1dX1yLP5c/uQ29vb4YOHWrqzr2dWrVqmf4dHx/PN998Y3qst7c3GRkZXLhwAXt7ewYNGmT6A7p48WKGDBlyy/bi4+PJzs42BbC3tzezZs3i8uXLQGEAxsXFmQLvrz936tQJoNT7/MKFC/Tv3x9/f3+8vLyYOnUq169fL/a5lVTX7QQFBRX596VLlwC4ePEiwcHBpttq165tGvE4Z84cjhw5Qv369YmKimLbtm3Fbr84Je3rkl6jv7tdndnZ2SQnJwPg6+uLnV3hnyJXV1eAMp1nLu49+Fdubm4sWLCAadOm4efnR2xsbImjQ4vb51D09fz7c7OzsyMoKIiLFy9y6dKlIvc1GAxFfi5JYmJiiQEtyocEoEYMBgMPPPAAPXr0MJ0HCAwMZNKkSdy4ccP0X1ZWFrVq1cLT05NPPvmE+Ph45s2bx/PPP8+ZM2dwc3MjKyvLtN0rV66U2KalBAYG8ssvv5ieR2pqKkePHi1VbYGBgTz99NNF9kNmZiaRkZEADBkyhEWLFrF9+3bs7Oxo3779bdt3d3cnJSXFtI20tDQ+//xz4H9HgFu2bKFTp0506tSJLVu2sGXLFtMRYHH7/O9ee+01qlatyokTJ0hNTeWFF14wHd3c7rmVVNftJCQkFPn3n0cRAQEBxMfHm26Lj483ndts1KgRixYt4urVqzz44IPFnr+8k+L29Z1eo7+6XZ0uLi5Uq1bNrJrM1bt3bzZt2kRiYiLOzs5FztX+XXH7HIq+nn9/bkopEhISCAgIoGbNmreci//rzyV9doOCgm57NP339sXdkQDU2Lhx45gzZw5JSUk8/vjjfPrpp6YunOTkZJYvXw7A6tWrOXPmDEopvLy8MBgM2Nvb07BhQ1JSUvj111/Jyclh0qRJxbZVo0YNEhMTLTIS8YknnuC1117j0qVLKKU4d+4cv/76a6ke+/DDD7N48WLi4uIwGo2kpaUV6T7t1KkTaWlpvPbaawwePPi22wgMDCQiIoLXXnuNzMxM8vPz2bt3rymEW7RowbVr14iLi6Nt27aEh4ezbds2Ll26RMuWLYHi9/nfpaWl4eHhgbu7O4cPHy5xiPqd6rqdDz74gJs3b3L8+HG++uor03MeMmQIkyZNIiUlhYSEBD7++GMefPBBoPB6vuvXr+Pg4ICHh8dt64bC90Rxf2ih+H19p9for4YMGcLs2bM5duwYGRkZvPrqqwwePNisP+R3qrc4V65cYdWqVWRlZeHs7Iyrq2ux+wSK3+d/16tXLw4cOGA6VTFlyhSqVKlCeHg4ERER5OXl8cUXX5CXl8dnn31W5EiyRYsWrF69mps3b3LmzJkiPQwPPfQQK1euZM2aNRiNRhISEkyDjMzdB+JWEoAaa9KkCV26dOGTTz6hY8eOTJ48mcceewxPT09at27N1q1bAThx4gRdu3bFw8ODPn36MHXqVGrXro2XlxeffPIJgwcPpm7durRt27bYtrp160adOnXw9fUlLCwMgHfffZdevXqV+/MaP348ERERREZG4uXlRd++fYt8qy5J3bp1+eGHHxg/fjzVqlWjcePGpi8CUNjNFBsby6ZNm4r9wwSFIZCYmEhISAg1atTghRdeMH3jtrOzo2PHjjRu3BgnJyecnJxo2rQpHTp0MP1hLG6f/90bb7zBL7/8gqenJ6NHj2bgwIElPr+S6rqd3r1706xZMzp37szo0aNNIwVff/11GjVqROPGjYmIiODBBx9k2LBhAKxZs4ZGjRrh4eHBtGnTmD9//m23/cYbbzBw4EC8vb2LnLf8U3H7+k6v0V/FxMTwr3/9i969e1O7dm0cHR2ZOnVqifuoOHeqtzhGo5EPP/wQPz8/atSowYULF4qMwPy74vb53/n4+LBs2TImTJhA9erV+emnn1i2bBmOjo44OTmxdOlSpk+fTvXq1Tl48GCR88iPPvoo9erVo1atWjz00ENFjtLr1q3L0qVLefXVV/Hy8qJ79+6m8Hz++eeZN28e3t7evP/++6XeB+JWBvXXvhohhFUxGAwkJCSU+tyRuHuyz/VDjgCFEELokgSgEEIIXZIuUCGEELokR4BCCCF0SQJQCCGELkkACiGE0CUJQCGEELokASiEEEKXJACFEELokgSgEEIIXZIAFEIIoUsSgEIIIXRJAlAIIYQuSQAKIYTQJQlAIYQQuiQBKIQQQpckAC3AwcGBli1b0qxZM2JjY8nMzCzT4z///HMWLlwIwLx587h69arptt69e5e4mrglPPXUU5w+fVrTGoQQoqxkOSQL8PHxISkpCYChQ4fSpk0bXnzxRbO2FR0dzaeffkqzZs3Ks0STgoIC7O3tK2Tbtii/wMil1Gwu3MgiMSWLizeySM7IJS07n/ScvP/+P5+07HwycvIxKoVSoAA7gwFHewMO9gZcHOzxdnXE29WJqq6OVHV1wtvVCW9XR/y9XKhdzZWgaq442st3ViHKi4PWBehNp06dOHjwIElJSTz++OOcP3+eatWqMW/ePOrUqcMPP/zAm2++iZOTE3Xq1GH58uVMnDgRHx8fAgMD2b17N4MGDcLd3Z3du3dTp04dDh8+zKRJk2jUqBFPPPEEAE888QR9+/bl/vvv56WXXuK3334jNzeXl156iaFDhxapafPmzbz11lu4uLiQnJzMxo0bee655zhy5AhGo5H333+f7t2706BBAw4ePIibmxtZWVk0btyY06dP06NHD1Mor1u3jokTJ5KdnU1oaChfffUVS5Ys4ciRI7zzzju88sor7Nixg40bN7JixQo2bNjAlClTGDZsGHv37sXe3p4XX3yRxx9/XIuXp1jZeQUcu3STIxdvcvTSTU5dTedCShaXb2ZTYLTMd0h7OwMB3i7Uqe5GcDVX6vq4ERrgRfNaXrg7y0dZiLKST40F5efns3btWnr27MnEiRPp1KkTK1euZOHChYwePZoVK1bwzjvvsGLFCho0aEBqamqRx/fv35/w8PDbHgHGxsby+uuv88QTT5Cfn8/GjRuZMWMGX375JTVr1mTXrl1kZWXRoUMHevbsSfXq1Ys8fs+ePRw7doyAgABeeeUV7rvvPubNm0dSUhJRUVEcO3aMXr16sWrVKoYMGcKaNWuIiYnBweF/b6GkpCQ++ugjNm3aRJUqVXjjjTeYPXs2ffv2ZdasWQDs2rWLjIwM8vPz2bJlC1FRUezfv5+zZ89y9OhRgFuet6UZjYpDF1LZeTaZQxdSOXIxlXPXMy0WdMUpMCoSkrNISC7a5W0wQIiPGy1qeRNWy4uwIG9CAzxxdpAjeSFKIgFoATdu3KBly5YAdO7cmSeffJJ27dqxZs0aAAYPHsyYMWMAiIyM5JlnnmHo0KEMGjSo1G2Eh4dz5swZUlJS2LlzJ5GRkbi4uLB+/XoOHz7Mt99+CxSGy5kzZ24JwMjISAICAgBYv349q1at4u233wYgIyODK1euEBsby/Tp0xkyZAhLliy55Sht+/btHDx4kIiICABycnLo06cPwcHBXLlyhfT0dAoKCoiIiGDfvn1s3bqVMWPG4OrqysWLF3nuued44IEHiImJKeMevjtKKY5fSeP3U9f5/fR1dp69zs3sfIvWcDeUgtPXMjh9LYMf910AwMXRjrZ1qtG5gS+dG/rSyN9D4yqFsD4SgBbg7e3N/v37S7yPwWAAYObMmWzfvp2VK1cSHh7OoUOHSt1Ov379WLZsGb///juxsbEAGI1GZs2aRZcuXUp8rKurq+nfRqORlStXUrt27SL3qVGjBk888QTXr19n+/btfPPNN0VuNxqN9OnTh7lz596y/datW/PFF1/Qpk0bOnTowMaNG0lKSiIwMBCAQ4cOsWbNGqZMmcL69euZPHlyqZ+3OXLyC4g7kcTaw5f59cRVktJzK7Q9S8vOMxJ3Mom4k0m8s+YYfp7OdGrgS5eGvnRtXEO6TIVARoFqJioqiu+//x6AJUuW0K5dOwDOnDlDREQE77zzDk5OTly/fr3I4zw8PEhLS7vtNmNjY1mwYAEbNmygV69eAMTExDBjxgwKCgoAOHz4sOnfxYmJiWHatGmmn/8Mbzs7O3r16sXzzz9Pjx49inR/AkRERPDLL79w/vx5AG7evMnZs2dNz3fKlClERkYSFRXFZ599Rtu2bYHCrlOj0cjgwYOZOHHiHb8smCs7r4D/HL7MmB/2ET5pA0/N383SvYk2F363c+VmDkv2JPL8gn2Ev/0zz363h7WHLpGdV/J7QQhbJl8DNTJx4kSGDx/O/PnzTYNgAMaNG8epU6dQStG/f39q1apV5HHDhw9n+PDheHh4sHv37iK3hYeHc+rUKSIiInBxcQHg6aef5uzZs7Rq1Qqj0UjNmjVZu3ZtibW9/vrrjBkzhrCwMPLz82ndurWpCzU2Npbo6GjWrVt3y+N8fX2ZPXs2AwcOJDc3Fzs7O6ZOnUrdunWJiooiMTGRjh07UqNGDapUqUJkZCQAFy5cYPjw4RiNRhwcHJg6dao5u7RY205f54dd8Ww4eoWMXPmDn51nZM2hy6w5dBkPZwfuCfWjb4sAOtX3wUFGmQodkcsghE1KychlyZ5EFuyM50xShtblVAo1vVx4uF0wD7YLxtfDWetyhKhwEoDCpuw8m8x3O86z9vBlcvONWpdTKTnZ29GruT+PRdShTe2qWpcjRIWRABSVnlKKjceu8tnmU+yLv6F1OTaleaAXT0bVpW+LAOztDFqXI0S5kgAUlZbRqFh16BIzfjnFH5dvPzBIlI8QHzdGdavPAy0DJQiFzZAAFJVOfoGRH/ddYObm05yV83sWJUEobIkEoKhU1h+5zAf/+YPT1yT4tBTi48aYHg24v0WA6RpWISobCUBRKRy+kMpbK4+y81yy1qWIv2gV7M0b9zWlVbAMlhGVjwSgsGrX0nL4aN0fLNmTiMZTcYpiGAzQv2Ug/+rdRC6fEJWKBKCwSkopFuxM4L21x0irRPNy6pmHiwP/16MhwzrWkfODolKQABRWJ/56Ji8vPci2M9fvfGdhdcJqefHv2BY08JMJuIV1kwAUVsNoVMz9/RyT1x0nS+aorNScHOx48Z6GPNMpBDs5GhRWSgJQWIVTV9N5ackB9sqF7DaldbA3/x7ckro+blqXIsQtJACF5pbsSeSN5YfJlImqbZKLox0v92zM45F1tS5FiCIkAIVmsnILeG3ZYZbuTdS6FGEBMU39+PfgFni4OGpdihCABKDQyMkraTz73V5OXk3XuhRhQXV93Jj5SGsa+3tqXYoQEoDC8pbuSeS1ZYdloItOVXG0590Bzejfqtad7yxEBZIAFBZjNCreW3uM2XFntS5FWIFHOgTzxn2hODnIIrxCGxKAwiKycgt4YeE+1h25onUpwopEhFRn1mNt8JTzgkIDEoCiwl1Ny+bpr3dzIDFV61KEFWrs78Hcx9tS06uK1qUInZEAFBXq+OU0npi3iws3srQuRVixml4uzHu8HY38ZfYYYTkSgKLC7D6XzONzd5GWI3N5ijvzcHFg1qNt6FjPR+tShE5IAIoKsf3MdZ6Yt0subhdl4mRvx7SHWtGzmb/WpQgdkOFXotxtOZnE43Ml/ETZ5RYYeX7BXtYduax1KUIHJABFufrl+FWe/HqXXOMnzJZXoBj1/V5+PiojhkXFkgAU5WbD0Sv8Y/4ecvKNWpciKrm8AsVz3+1lg4SgqEASgKJc/H46iWe/30tugYSfKB+5BUae/W4vm/6QEBQVQwJQ3LWjF2/yj/l7yJUjP1HOcguMjPh2LztkcWRRASQAxV1JSM5k+NydcqmDqDC5+Uae+WYPp2TidFHOJACF2ZIzchn21U6upuVoXYqwcalZeTw+bydJ6fJeE+VHAlCYJSu3gMfn7eJMUobWpQidSEjO4smvd5Mll9eIciIBKMwyfskBDiTc0LoMoTMHEm4w+od9GI0yf4e4exKAosxm/3aGVQcvaV2G0Kmfj17hw3XHtS5D2AAJQFEmv59O4v3//KF1GULnZv12Wq4RFHdNAlCU2qXULJ7/fh8F0v0kNKYUjF18gITkTK1LEZWYBKAolZz8AkZ8u5frGblalyIEUDgy9Lnv95KTL4NihHkkAEWpvLfmDxn0IqzOwcRU3l51TOsyRCUlASjuaMvJJL7edk7rMoS4rW+2n2fVwYtalyEqIVkPUJQoNSuPnlN/41JqttallEnejctcX/sJxowbYLDD/9F/owpyub7mE/KSL2AwGPAd+AYO3v4krfiQvKTzuLfoiWf4/QAkrfkErw6DcKwWqO0TEaVS1dWR9f/XBV8PZ61LEZWIg9YFCOs2ccWRShd+ANfXTMW70yO4BDWjICsNg4Mjyes+xa1JJ9yaRmPMywYFedfOYrB3oOYTn3Fp3hg8w+8n98pp7JxcJPwqkZTMPF5bdohZj4ZrXYqoRKQLVBRr7aFL/LTvgtZllFnutfMY7OxxCWoGgH0VD1ReNjmXT+HWNBoAO0cX7JxcwO6/3wGNBRjsHQFI/X0hXh0f1KJ0cRfWHbnCigPSFSpKT7pAxW0lpecQM+U3kivhqM/ME9tIP7wRjAUUpCfj2iiSKiHhJP/8OfZevuQlJeAS3JyqXZ/AYGdP8s8zyU48imf4A9i7epN77SxeHWK1fhrCDNXcnFj/f53xcZeuUHFncgQobuvtVUcrZfgBKGMBOQlHqBbzLP6PTCbr3D6yzu0j59IJvNoNpObwqRgzU0k/+DMA1e4ZScDj03Fr1o20vavwaN2X5A2zuPbTu2QnHtH42YiySM7I5fVlh7UuQ1QSEoDiFttOX2fZ/srbleTgUR0n//o4ePpicHCkSkg4Kj8XB28/nPxCMBjsqNKgA7lXzxZ5XPrBDbg26UzOhaPYVfGk+n0vkrr1B42ehTDX2sOXWX/kstZliEpAAlAUkVdg5PXllfsbtFPNhhRkplKQnY5SRnISDuPkVw97Vy/ybhT+YcyOP4Rj9Vqmxxjzssk6uQ230K6ovBwoyAcFxhyZaaQymrT6KNl5coG8KJmMAhVFfP37uUq/8KjBzp6qnR/jyncvAwqXOq1wrd8Oe7eqJC17D1WQj5NfCB4tepoec3PnT3i07YfBYMClbmvS9q7k8vz/k8EwlVRCchZf/HaG0d0baF2KsGIyCEaYJKXn0HXyZtKyZXV3UflVcbTnl3HR+Hu5aF2KsFLSBSpM/r3+uISfsBlZeQV8JMsmiRJIAAoAziVlsHh3otZlCFGuftyXyOELqVqXIayUBKAAYNrGk+TLMkfCxigFk9fLUaC4PQlAwamr6SyXGTSEjdp8/BoHE29oXYawQhKAgk82npRFboVNm7bxlNYlCCskAahzxy+nyVIywuZtOHaFoxdval2GsDISgDo3beNJ5EIYoQfTN53UugRhZSQAdSwhOZP/yJRRQif+c+QyJ66kaV2GsCISgDr2zfbzcu5P6IZS8MVvZ7QuQ1gRCUCdysotYOGuBK3LEMKiVh28yI3MyrnKiSh/EoA6tXRvIqlZeVqXIYRFZecZWbJHJnwQhSQAderr389pXYIQmvhuRzwyBbIACUBd2nIyiZOVfMUHIcx1NimDraeua12GsAISgDq0eI+c+xP69s32c1qXIKyABKDOZObm8/PRK1qXIYSmNhy7yrW0HK3LEBqTANSZ9UeukJkrK2ULfSswKtYevqR1GUJjEoA6s2z/Ba1LEMIqrDooAah3EoA6cj09hy0nk7QuQwirsPtcMlduZmtdhtCQBKCOrDp4Sdb8E+K/jArWHJKjQD2TANQROechRFHSDapvEoA6kZ6Tz57zKVqXIYRV2RufwqXULK3LEBqRANSJLSeTyCuQ7k8h/kop+PX4Na3LEBqRANSJX09c1boEIazSllMyMEyvJAB1YrN8yxXitradvi5zg+qUBKAOHL+cxqVUGe4txO1cz8jl6KWbWpchNCABqAO/nZCjPyFKslW6QXVJAlAHZPSnECWLkwkidEkCUAf2J9zQugQhrNqe8ykYZZII3ZEAtHGXU7O5LNM9CVGizNwCTl+TNTL1RgLQxu1PkO5PIUrj0IVUrUsQFiYBaOP2SfenEKUiAag/EoA2bn/8Da1LEKJSOHJBLoXQGwlAGyfXNwlROkcupspAGJ2RALRh19JySMvO17oMISqFjNwCziRlaF2GsCAJQBt2Vj7MQpTJGRkJqisSgDbsbJJ8mIUoi/jkTK1LEBYkAWjDpDtHiLJJTJG1AfVEAtCGnb0mAShEWcgRoL5IANqwc9clAIUoCwlAfZEAtGGXZQkkIcokMUUCUE8kAG1UfoGRm3IJhBBlkp1n5FpajtZlCAuRALRRyZm5WpcgRKV0Qz47uiEBaKOSM+RDLIQ5UrPytC5BWIgEoI1KTpcAFMIcN7MlAPVCAtBGXZcjQCHMIkeA+iEBaKPkPIYQ5knNlADUCwlAG5WVV6B1CUJUSqlZMnpaLyQAbVRuvlHrEoSolDJzJQD1QgLQRkkACmGeAlkTUDckAG1UvnyIhTBLgZLPjl44aF2AqBiSf9bL2cGO3s1ral2GKEbzQC+tSxAWIgFooxSSgNZqZHQ9XujRUOsyhNA96QK1UXYGg9YliNuoU92VEV3qaV2GEAIJQJvl5mSvdQniNibeH4qLo7w2QlgDCUAb5eokvdvWpmeoP9GNamhdhhDivyQAbZS7swSgNXF1smfC/U21LkMI8RcSgDbKTQLQqozu3oCaXlW0LkMI8RcSgDbK1VnOM1mLBjXceTKqrtZlCCH+RgLQRkkXqPWY1K8ZjvbyURPC2sin0kZVdXXSugQB9GsZQIeQ6lqXIYS4DQlAGxXg7aJ1Cbrn4eLAq31k4IsQ1koC0Ea5OjngVcVR6zJ0bew9DfH1cNa6DCFEMSQAbViAt4w61EpogCePRtTRugwhRAkkAG1YgJd0g2rBYCgc+GJvJ9PRCWHNJABtWE05D6iJIeFBtA6uqnUZQog7kAC0YYHerlqXoDtVXR15uWdjrcsQQpSCBKANq+frpnUJuvNyz8ZUdZNLUISoDCQAbViTmp5al6ArrYO9GdI2SOsyhBClJAFow2pVrYKHzAhjEfZ2Bib1a4ZB1mEUotKQALRhBoOBRv4eWpehC492qE1ogJfWZQghykAOD2xc45oe7D6fonUZNs3Xw5mxMQ0t1t7R60f5YOcHHL1+1GJtitJpX7M9n3b/VOsyRClJANq4xv5yHrCivdq7CR4ulpt1p2n1psztOZelJ5cyfe90UnLkC461yFf5WpcgykC6QG1c80DplqtIESHV6dcq0OLt2hnsiG0Yy6oBqxjaZCgOBvkuaw3sDbIMWWUiAWjjQgM8cXOSD2VFcLQ3MKlfqKY1eDp58s92/2Rx38W0r9le01oE8kWkkpEAtHEO9na0qVNN6zJs0pNRIdSvYR2DjOpXrc+cmDlMiZ5CoLvlj0hFIXcnd61LEGUgAagDHUIkAMtboHcVRnevr3UZt+hRuwfL+y3n2ZbPUsVBJkO3NE8nOedemUgA6oAsyFr+Xr+vKa5O1tnd5WzvzMgWI1nRbwX31rlX63J0xdNZArAykQDUgbBALzkPWI6iG/nSs5m/1mXckb+bP5O7TOare7+iYVXLXaahZ3IEWLlIAOqAnAcsP84Odrx5vwYDXzKug9Fo1kPb+rdl0X2LeLX9q3g5y6jgiiQBWLlIAOpE10a+WpdgE0ZG16N2dQ0mGV/0GHzRGc7/btbD7e3sebDxg6zuv5ohjYbIcP0KIl8wKhcJQJ24N9T6u+ysXZ3qrozoUs/yDR9cBOe3wOVDMLcXLHkCUi+YtSkvZy9e6/AaC+9bSLhfeDkXKqo6yzqQlYkEoE4EeFchrJZ8O70bE+8PxcXRwkdO2amw/rWivzu8FD4Nh18/gvwcszbbqFoj5vacy0ddPsLfzTq+HCWtS+LkKyc5+cpJLn57EWOukbMfneXkKydJ3ZVqut/5T86Tn26dM64EesglKJWJBKCOyFGg+XqG+hPdqIblG970DqRfufX3eZnwy9vwWTs4tsrszfes05MV/Vbwj7B/4GzvfBeF3p38m/lc33CdehPrUf/t+mSfyyZpTRKu9VypN6EeSeuSALi59yZuDd1wcLe+Ebhujm5Uc5Fz7ZWJBKCOVIaRi9bI1cmeCfc3tXzDlw7Arjkl3yflHCwcCvP7wbXjZjVTxaEKo1qNYnm/5fQI7mHWNsqFEVSeQuUrVIHC3t0eFKgChZ2jHapAkfxLMtV6WGfIyAQElY8EoI7U83Wnfg2ZqaKsRndvQE0vC19UrhSsHguqoHT3P/MLzOwIa/9Z2G1qhkD3QKZ0ncLsmNnU97bsRf4Ong749PTh+NjjHP+/47iFulEtuho5V3I4+8FZfHr5kPxrMt6R3tg5WuefrVrutbQuQZSRdb6TRIW5L6ym1iVUKg1quPNkVF3LN7z3a0jcVbbHGPNhx0yY1hr2fG32ZRMdanZgcd/F/LPdP/FwssxUbwUZBaQdSKPh5IY0mtKIzJOZZJ7OJPjZYOq/WR/XBq6kH0jHo4UHiV8mEv9pPNkXsy1SW2kFeQRpXYIoIwlAnYkND8JOFi0vtUn9muFob+GPSWYybHjzLh6fBCtHw5xukLDTrE042DkwtMlQVvdfzcAGA7EzVOw+SD+SjlMNJxzcHbBzssOjhQeZpzNNtyetScKntw+pO1Jxa+yG/0P+XFtxrUJrKqtaHnIEWNlIAOpMoHcVohrINYGl0a9lgDbTyG2YAFnJd7+di/vgyxj48RlIu2zWJqq6VGVix4ks6LOAVjVa3X1NxXCs5kjmqUyMuUaUUZHxRwbO/oWDcvJS8si9lotbIzeMOUbTOUJjjnlHuBUlxCtE6xJEGRmUUkrrIoRlrT10iZHf7dW6DKvm4eLAprHR+HpYeGRkwi748h6gnD+WTu7QaSxEjAIHJ7M3s/rMaj7e8zFXM6+WY3GFriy5ws09N8EAbk3dqDm0JgaDgQvzLuBzrw/ONZ3Ju5FH/LR4jDlGaj5SE/cm1nFO24CBrQ9ttViXsSgfEoA6lFdgJOK9jSSl52pditWa2LcpwyMtfO7PWABfdCm84L2iVAuBe9+DRj3N3kRmXiazD81m/pH55BrlPQRQ27M2q/qbfzmK0IZ0geqQo70dA1rL+YrihAZ48mhEHcs3vHN2xYYfQPIZWDAEvh0ESafM2oSroytjWo9h2QPLiK4VXb71VVJNq2lwmYy4axKAOvVg2yAMMhjmFgZD4cAXe0uPFEq7Ar+8Y7n2Tv0MMzoUzjKTk2bWJoI8g5jefTqf9/icul4ajJS1IqE+GkyQLu6aBKBOhfi606OJn9ZlWJ0h4UG0DtZgPsf1r0LOTcu2acyD36fD9Daw77vCaw/NEBkYydL7lzIufBzujtZxTs7SmlaXI8DKSAJQx56N1mBiZytW1dWRl3s2tnzDZ3+DQ4st3+6f0q/A8mdhTg+4sMesTTjaOTIsdBgr+6+kX/1+GNBP94IBA02qNdG6DGEGCUAdaxVclQ4h1jmtlBZe7tmYqm7mj5A0S0EerB5n2TaLc2E3zO4Oy56FdPNGefpU8WFS5CS+7/M9Yb5h5VygdWpcrTHuTvo88q3sJAB1bmS0Zae8slatg70Z0laDmTy2fQpJ5s3hWTEU7P+usFv09+mFAW2GZj7N+LbXt7wd+TY+VXzKuUbr0s6/XanvazAYeO21/63uMW7cOObNm2dWu5s3b2bnzrJPdDB8+HBWrbp1xOrw4cMJCQmhRYsWhIWFsXHjRrPq+vzzz1m4cKFZj7U0CUCd69LQl9AAfa9ibW9nYFK/ZhgsPSooNbFwSSNrlHOzcIDMzI5waoNZmzAYDDxQ/wFW9V/F46GP42jnWM5FWof2NduX+r7u7u589913pKWZN/Dor0oKwIKCUs4h+zfTpk3jwIEDfPzxx4wYMcKsbYwYMYIhQ4aY9VhLkwAUPKvzo8BHO9QmNECDtRLXvgx5GZZvtyySTsC3A+H7BwsvoTCDm6MbL4a/yI/3/0hUYFQ5F6gtRztH2vi1KfX9nZ2dGTp0KDNmzLjlttOnT3PvvfcSHh5Ot27dOHfuHADR0dEcPnwYgMOHDxMdHU1CQgKff/4577//Pi1btmT//v0MHz6ckSNH0q5dO95//32WLVtGu3btaNWqFX369OHGjRulrjMqKorExETTzx988AFt27YlLCyMyZMnAzBkyBA2bdpkuk+3bt3Yt28fEydO5NNPPy32OV28eJHIyEgA1q9fT5UqVcjNzeXGjRu0alU429DUqVNp1KgRLVq0YOTIkaWuu6ysb1EtYXG9m/sTGuDJkYsWHoVoBXw9nBkb09DyDZ/8Gf6oRBdOn1gLpzdBxLPQeTw4uZV5E3W86jCzx0x+S/yND3d9yPmb5yugUMtqXaM1ro6uZXrMmDFj6NChA2PGjCny+2effZZZs2ZRp04dNm3axPjx41m8+PaDo4KCghgxYgQ+Pj6MGjXK9Pvr16+zY8cODAYDKSkpPPDAAxgMBqZNm8Znn33Gq6++WqoaV69ezf333w8UhlRiYiI7d+7EaDRyzz330LNnT2JjY1m8eDHdunXj6tWrXLx4kVatWrF8+fI7PqeUlBRycnLYsmULTZs2Zc+ePaSkpBAREQHAW2+9RUJCAm5ubqSmmre6SWlIAAoMBgMv92zMY1+ZN3FyZfZq7yZ4uFi4ay4vG9aMt2yb5aEgB7ZMgQML4Z43IWywWZvpXKszETUjmH90Pl8c/ILM/Mw7P8hKRQZGlvkxvr6+3HfffXz11Vem36WnpxMXF0e/fv0AUErh5lb2LxmDBg0ydeXHx8cTGxvLlStXyMrKon37O3fVjh49mhdffJH4+Hi2bt0KFAbg6tWriYuLAyAtLY0TJ07Qu3dvXnrpJQoKCvjpp58YMGBAkW2V9JzCw8PZuXMnO3bsYOzYsWzZsoWUlBTTkWG7du145JFHiI2NNT2+IkgXqACgc0NfIutrMPGzhiJCqtOvlQaLmG6ZAilnLd9ueUm7CD8+DV/eCxf3m7UJR3tHnmz+JKv6r6JvSN9Ke9lE51qdzXrcuHHj+OSTT8jPzwfAaDTi5+fH/v372b9/PwcOHOD3338HwMHBAeN/l7bKyckpcbuurv87Gh09ejQvvfQShw4dYurUqXd8LBSeAzxx4gTvvfceTz/9tKm2CRMmmGo7ffo0AwYMwNXVlbZt2/Lbb7+xZMkSYmNji2yrpOcUFRXFr7/+Sk5ODjExMfz+++9s3brVFICrV69m1KhRbNu2jS5dupRml5pFAlCYvNq7qW6WSnK0NzCpnwazdySfga1TLd9uRUjYDrO7worRkHHdrE34uvrybqd3md9rPqHVK9dsKvW961PP27xraYOCgoiMjGTp0qUAeHp64ufnx8qVK4HCQSx/nverXbs2+/fvB+DHH380bcPDw6PEwTQ3b94kMDAQpRTz588vU30vvPAC+fn5rF+/npiYGObMmUNmZuGR+rlz50zdkrGxscycOZPExETT+bs/lfScoqKimDVrFi1btsTHx4ekpCQuXrxInTp1MBqNJCQk0L17dyZPnkx8fLzZg3ruRAJQmDQN8CS2jT4W9XwyKoT6NTSYuX/NeMi3roVc74oyFi7eO70VbJ8JBflmbaZljZZ83+d73uz4JtVcKse1qb3q9rqrx7/88stcvHjR9PP333/P9OnTadGiBc2bNzddhvDiiy/y4Ycf0qZNG3Jz/zf5eN++fVmwYIFpEMzfTZgwgb59+9K2bVuCgsr2uTYYDLzxxhtMnjyZnj170r9/fzp06ECzZs145JFHyM4ufA/37t2bNWvW0L9//9tup7jn1KRJE7KyskxHfE2aNKF169ZAYVAOHTqUsLAwwsPDeeONN7C3ty9T/aV+nrIahPira2k5dJu8mbQc8/6QVQYBXi5sGNsFVycLnwI/ugIWPWrZNi3Ntwn0eh9Cos3eRFpuGjP2z+CHP34gX1nv+3BN/zUEeerjC6OtkiNAUYSvhzMv9dJgOjALeqNvU8uHX24G/Odflm1TC9eOwfwH4IehkGLeKE8PJw9ebvcyS+9fSkTNiHIusHyEVg+V8LMBEoDiFo+0D6ZtHQ0mhLaA6Ea+9GxW0/IN//oB3Ey88/1sxR+r4LN2sOltyDVvlGeIdwhfxHzBJ10/oZa7dS3fdbfdn8I6SBeouK1TV9PpPS2O3Hyj1qWUG2cHO9b/X2dqVy/78PK7cvUP+DyqcPUFPfKsBTFvQbOBZm8ityCXeUfmMefQHLLys8qxuLIzYGD9oPX4u/lrWoe4e3IEKG6rfg13RnW1rRliRkbXs3z4AawZp9/wg8Ij3yVPwNw+cPmwWZtwsnfimbBnWNFvheZHXx0DO0r42QgJQFGskdH1aOSnwUjJClCnuisjumiw/NPBRXAuzvLtWqPzW2BWZ1j1ImQmm7UJfzd/Puz8IfN6zqNxNW3OVT/U6CFN2hXlT7pARYkOJt5g4MzfySuo3G+TeY+3JbpRDcs2mp0Kn7YtXG9PFFWlKnR9FcKfADvzhrgblZElJ5bw6b5PSclJKecCby/QPZA1A9ZgZ5BjB1sgr6IoUVgtb8bf20jrMu5Kz1B/y4cfwKZ3JPyKk5VS2DU8qzOc22LWJuwMdgxuNJiV/VfyUOOHsDdUzLVifzWk0RAJPxsiR4DijpRSPDFvF78cv6Z1KWXm6mTPhhe7EOBdxbINXzoAX3QFVTEzWNic0P4Q8zZ4mT/a82TKST7Y+QE7Lu8ox8L+x9nemQ2DNuDt4l0h2xeWJ19lxB0ZDAYmx7bAz9NZ61LKbHT3BpYPP6Vg9VgJv7I48lNhd/HmDwonCzdDg6oNmHPvHP7d5d8EuAWUc4HQs05PCT8bIwEoSqW6uzNThrSsVHOFNqjhzpNRdS3f8N75kLjL8u1WdnmZsPld+KwtHF1+5/sXI6ZODMv7LefZFs/iYu9SLqUZMPBoUxufxUeHJABFqXWs58Pz3RpoXUapTerXDEd7C7/FM5Nhw0TLtmlrbsTDosfg6/vh6jGzNuHi4MLIliNZ0W8F99S+565L6hbcjUbVKve5cHErCUBRJi/0aMC9oX5al3FH/VoG0CFEg+WdNkyALPOG+Iu/Oftr4QQCa16CrBtmbaKme00+jv6Yr+79igZVzfvyZsDAyBYVtyq50I4MghFllpVbQOys3zl8wTpXkPdwcWDj2C7U8Cif7q9SS9gFX94DyEeq3LlWh26vQ+thYGfe9/YCYwGLTizis/2fkZpT+lXGuwd3Z2rXqWa1KaybHAGKMqviZM+cx9pa7aCYsfc0tHz4GQtg9f8h4VdBMq/DqhdgdjTEbzdrE/Z29jzU+CFW9VvF4IaDS3U5gwEDI1qMMKs9Yf0kAIVZ/L1cmP1YOC6O1vUWCg3w5NGIOpZveOdsuHzI8u3qzaUD8NW9sPQpuHnxzve/DW8Xb16PeJ2F9y2kdY3WJd63a1BXzWacERVPukDFXVlz6BLPfb8Xa3gXGQywdGRHWgdbeCWLtCvwaTjkWGeXsM1ydINOL0LH58HB/N6ItWfX8u/d/+ZKZtFJC+wMdiy6b5EMfrFh1vX1XVQ6vZvX5K0HmmldBgBDwoMsH34A61+T8NNCXgZsmgSftYc/1pi9mV51e7Gy/0qeCXsGZ/v/BWn/+v0l/GycHAGKcjEn7gxvrzZvyHp5qOrqyKax0VR1c7Jsw2fj4Ov7LNumuL163aHn++Db0OxNJKYl8tGuj9h5eSer+q+iehUNRhILi5EAFOVm2saTfPzzCU3afn9Acx5sF2zZRgvyYGYkJB23bLuieHaO0P4f0OVlcPE0ezOXMy7Lkkc6IF2gotyM7t6AkdGWX3KoVbA3Q9oGWbxdtn0q4WdtjHmFr8v0NrD3G8w9OS3hpw9yBCjK3ZsrjzB36zmLtGVvZ2DFqEhCA7ws0p5JaiJ82q7wPJSwXgGtofdHUCtc60qEFZIjQFHuJvQNZXR3y0yZ9miH2pYPP4C1L0v4VQYX98KcHvDTyMLRukL8hRwBigrz9e/nmLjySIVdIuHr4cymsV3wcHGsmAaKc/Jn+G6QZdsUd8/JA7qMh/YjwcHCg6WEVZIjQFFhhnWswycPtsLRvmKWkHi1dxPLh19eNqwZb9k2RfnITYOf34CZEYVfYoTuSQCKCnV/iwC+HNYWV6fyXa07IqQ6/VoFlus2S2XLFEg5a/l2Rfm5fqrwCP67wXD9tNbVCA1JF6iwiIOJN/jHN3u4lGreYqd/5WhvYO2YTtSv4VEOlZVB8hmYEQH5d/8chJWwd4IOI6HzS+DsrnU1wsLkCFBYRFgtb1aMiqJtnbufqeWJqLqWDz8o7PqU8LMtBbmw9ZPCyyYO/GD2ZROicpIAFBbj6+HM90934JEO5l+wHuDlwhgLjTAt4ugKOLXB8u0Ky0i/DNtnSgDqjASgsChHezve7tecDwY2x8mh7G+/N/o2xdXJoQIqK0FuBvznX5ZtU1iWwQ76fGz2WoOicpJXW2hiSNtgFj7TgVpVq5T6MdGNfOnZrGYFVlWMXz+Am4mWb1dYTuthUKuN1lUIC5NBMEJTadl5TFhxhB/3Xijxfs4Odqz/v87Uru5mocr+6+of8HlU4RRbVigh1cijP2VxNUPhYAevd3YmNtSR4cuy+O18Pp7OhZegLB3sSr1qdkzZlsOX+/II87Pj+4GuAHy1LxcD8HgrnV4b5+oDo3aBazWtKxEWZuG+JCGK8nBx5OPBLenRxI9XfjrEjczbB83I6HqWDz+ANeOsNvwAHOxgak8XWvrbczndSJsvMujdoPBjPa2XC/c1LHqd5NcH8jg00o1hy7I5eKWA+tXsWHI0n1UPl/5I3Obc+66En05JF6iwCr2b12TdC53p1MDnlttqV3dlRBfLT7LNwUVwLs7y7ZZBTQ87WvoXXmPp726Hj6uB5KziO3VcHAzkG0FRGJ4fb8vlhQ5O2BkqZrICq9d8MLQYonUVQiMSgMJq+Hm6MP+Jdkx6IBQP5/91Trx5fygujuV7If0dZacWLnRbiey5WECBEYK8Cj/W49bn0OLzdP61IZsCY2Eojgh3pO3sDLycwcfVwIErBcTU02lHUNW6cN/HWlchNCTnAIVVunIzmzdXHsFohM8f1WBwwpqXYOcsy7drpuQsRae5Gczu60LHIAcupRnxdzeQUwDDlmXROdiB59oVPcf3/JosnmnjxJb4AjaezadHiAMjwnVyHtDOEZ5cB4Ey8EXP5AhQWCU/TxdmDG3DtIdaWb7xSwdg1xzLt2umnHxFvx8y+WekEx2DCo/manrYYTAYcHEw8FiYI7suFhR5zPGkAnILIKSqHcuP57FksCvL/sgjI1cn34e7vSbhJyQAhXUz51rBu6IUrB4LquDO97UCSimGL8+iW117Hm3xv6O3S2lGAIxKseJ4PqG+RffjW7/lMCHamdwC+HPcUUYe5FaOp313QrpC5BitqxBWQKed/0IUY+98SNyldRWltjWhgIWH8wnzs2PZH+kAfNO/CmP+k01SpsKooEMte0a3/184xp3Pp15VOwI8CkOxlb89zWak0yPEgapVbHwwjJsv9J8Feh30I4qQc4BC/CkzuXBOyKxkrSsRFcIAQ5dAgx5aFyKshHSBCvGnDRMk/GxZx1ESfqIICUAhABJ2wd5vtK5CVJTG90GPt7SuQlgZCUAhjAWw+v8ovDxc2JygDjDwS5noWtxC3hFC7JoDlw9pXYWoCD4N4aEF4OiidSXCCkkACn1LuwKb3tG6ClER3P3hkaUyz6colgSg0Lf1r0FOqtZViPLm7AmPLAFv8xdfFrZPAlDo19k4OLRI6ypEebNzhCHfgH9zrSsRVk4CUOhTQV7hjC/Cxhig3wwIida6EFEJSAAKfdr2KSQd17oKUa4M0OsDCBusdSGikpCp0IT+pCbCrx9pXYUoT3YO8MBn0OJBrSsRlYgEoNCf//wT8jK0rkKUF4cqEDsPGvXUuhJRyUgACn05+TMcW6l1FaK8OHvBwz9A7Y5aVyIqIQlAoR952bBmvNZViPLiVgMe/VFGewqzSQAK/dgyBVLOal2FKA/eteGxZVAtROtKRCUmASj0IfkMbJ2qdRWiPNQILTzy8/DXuhJRyUkACn1Y8xLkZ2tdhbhb9brBoLlQxVvrSoQNkAAUtu/oCjj1s9ZViLtigM7jIfpfsqqDKDcSgMK25WbAf/6ldRXibrh4wYDZ0PBerSsRNkYCUNi2Xz+Am4laVyHMVbNl4TV+1epqXYmwQRKAwnZd/QO2zdC6CmEWA0Q8B90ngIOT1sUIGyUBKGzXmnFgzNO6ClFWbjWg/0yo30PrSoSNkwAUtungIjgXp3UVoqwa9YG+U8G9htaVCB2QABS2Jzu1cKFbUXl414ZeH8p8nsKiJACF7dn0DqRf0boKURr2zhA5GjqNBccqWlcjdEYCUNgeJ9fCVcHl/J91q9cNek+G6vW0rkTolEEppbQuQohyl3SycNmjUxu0rkT8nUcA9HwXQvtrXYnQOQlAYduOr4V1r0Lyaa0rEfZO0O6ZwtlcnN21rkYICUChA8YCOLwU4j6Ga8e0rkZ/HF2h9WPQcTR4BWpdjRAmEoBCP5SCP1ZD3L/h4l6tq7F9zl7Q9snCC9rdfLSuRohbSAAKfTq9qfCIUK4VLH+u1aHDyMLuThcvrasRolgSgELf4ncUHhGeXKd1JZWfRwB0fB7aDC8ciSuElZMAFALg8mHY903hucKMa1pXU3kY7KBuF2jxUOGoTpm3U1QiEoBC/FVBfmH36MEf4I81kJ+ldUXWya85tBgCzWNlZXZRaUkAClGcnLTCxXQP/gDntoAyal2RtjwCICwWwh4Ev6ZaVyPEXZMAFKI0Ui/AocVw5Ee4fEg/YVilGjTqBWGDoU5nWY1d2BQJQCHKKisFzm0tHEF6Ng6uHgVs5GNk7wzB7SGkK9TrCv4tJPSEzZIAFOJuZVyH81sKw/BcHFz7Q+uKSs/JHWqFQ3BE4X+12soITqEbEoBClLf0q5CwA64eK/zv2nG4fhIKcrWryd4JqoVA9fqFk09XbwB+oeAfBvYyJ77QJwlAISyhIB9SzkHK2f/+/7//pSZA9k3ITYecdPNGnRrsC+fWdPIo/L+H/3+Drn5h0FWvB97BYGdfvs9JiEpOAlAIa2Is+F8Y/vX/uRmFR3HO7uDkVth16exR+H9HF62rFqJSkgAUQgihSzK8SwhRLIPBwGuvvWb6edy4ccybN69c21i2bBknTpww/fzUU09x+vTdL1/l4OBAy5YtCQ0NpW/fvty4ccOs7fTu3ZusLJkQwRZJAAohiuXu7s53331HWlpahbXx9wCcM2cO9erd/Srx3t7e7N+/nyNHjuDt7c1nn31m1nbWrFlDlSpV7roeYX0kAIUQxXJ2dmbo0KHMmDHjlttOnz7NvffeS3h4ON26dePcuXMAbNu2jdDQUFq1asVzzz3HoEGDgMKga9euHa1ataJPnz7cuHGDHTt2sGLFCkaPHk3Lli25evUq0dHRHD58mJkzZ/LGG2+Y2nvrrbeYMmUKAB988AFt27YlLCyMyZMn3/F5REZGkpiYCMC1a9cYMGAA4eHhREREsG/fPlJTU2nQoIHp/ufPn6dly5YA1KlTh/T0dAC++eYb2rZtS4sWLXjxxRcBePfdd5k9ezYADz/8ME8++SQA06ZN4+OPPyY9PZ2ePXvSvHlzmjdvzrp1MvG61VBCCFGM6tWrq6tXr6qQkBCVlZWlxo4dq+bOnauUUiomJkadPXtWKaXUxo0b1aBBg5RSSoWGhqo9e/YopZQaOnSoGjhwoFJKqeTkZGU0GpVSSn3yySfq7bffVkopNWzYMLVy5UpTm126dFGHDh1Sly9fVqGhoabfh4WFqYSEBLVu3To1atQoZTQaVX5+vuratas6dOjQbWtXSqn8/Hw1YMAAtWrVKqWUUg8//LDauXOnUkqpEydOqHbt2imllOrTp4/avn27UkqpyZMnm+qrXbu2SktLU0ePHlUDBw5UeXl5SimlHn30UbVq1Sr166+/qscee0wppVTHjh1VVFSUUkqp2NhYtWPHDrVkyRL18MMPK6WUMhqNKjU1tawvg6ggcgGQEKJEvr6+3HfffXz11Vem36WnpxMXF0e/fv0AUErh5ubGjRs3yMvLo3Xr1gAMGTKEr7/+GoD4+HhiY2O5cuUKWVlZtG/fvsR2/fz88PX15fDhwzg5OeHm5katWrWYOnUqq1evJi6ucC3HtLQ0Tpw4QbNmzYo8/saNG7Rs2ZLExEQaNGjAvffeC8CGDRs4cuSI6X4pKSkAxMbGsnjxYtq3b8/SpUtvOde5ceNGtm/fTnh4OACZmZm0adOGf/zjH4wYMYL4+HiCg4PJycnh2rVr7N27l1atWuHt7c0LL7zASy+9RP/+/YmIiCjL7hcVSAJQCHFH48aNo0ePHvTq1QsAo9GIn58f+/fvL3K/P8PkdkaPHs2rr75KTEwMq1atKtVgmsGDB7N48WKcnJyIjY01tT1hwgSGDRtW4mP/PAeYkZHBPffcw4wZMxg9ejQAu3fvxsGh6J+/fv368c477zBmzBiysrJo2LBhkduNRiNPP/00EyZMuKWtqlWrsmTJEqKiosjOzuabb76hVq1aODo60rBhQ/bv38+qVat48cUXGTp0KKNGjbrjcxcVT84BCiHuKCgoiMjISJYuXQqAp6cnfn5+rFy5EoCCggIOHz5M1apVcXBwMAXj4sWLTdu4efMmgYGBKKWYP3++6fceHh7FDrIZMGAAP/74I0uXLjUFYExMDHPmzCEzMxOAc+fOkZqaWmztbm5uTJs2jX//+9/k5+fTtWtXZs6cabr9wIEDAHh5edGwYUNefvll03nLv+revTsLFy7k+vXrAFy9epVLly4BhecYp0yZQmRkJFFRUUyZMoWoqCgALl68iJubG8OGDeOFF1645UuD0I4EoBCiVF5++WUuXrxo+vn7779n+vTptGjRgubNm7Nx40YAvvjiC4YOHUrr1q1xdnbG09MTgAkTJtC3b1/atm1LUFCQaTsPPvggkyZNMg2C+Ss/Pz98fHxwcXGhVq1aAPTs2ZP+/fvToUMHmjVrxiOPPEJ2dnaJtYeHh9O8eXMWLVrE9OnT2bx5My1atKBJkyZ8//33pvvFxsayYMECU9j+VWhoKK+++irdu3cnLCyMPn36kJycDEBUVBSpqak0b96c1q1bk5ycTGRkJACHDh2ibdu2tGzZkqlTp5oGzwjtyYXwQohylZGRgZubGwCjRo2icePG0uUnrJIcAQohytXy5ctp2bIlTZs25fr166bLAoSwNnIEKIQQQpfkCFAIIYQuSQAKIYTQJQlAIYQQuiQBKIQQQpckAIUQQuiSBKAQQghdkgAUQgihSxKAQgghdEkCUAghhC5JAAohhNAlCUAhhBC6JAEohBBClyQAhRBC6JIEoBBCCF2SABRCCKFLEoBCCCF0SQJQCCGELkkACiGE0CUJQCGEELokASiEEEKXJACFEELokgSgEEIIXZIAFEIIoUsSgEIIIXRJAlAIIYQuSQAKIYTQJQlAIYQQuiQBKIQQQpckAIUQQuiSBKAQQghdkgAUQgihSxKAQgghdEkCUAghhC5JAAohhNAlCUAhhBC6JAEohBBCl/4fohYZYImkEsYAAAAASUVORK5CYII=</t>
-  </si>
-  <si>
-    <t>https://www.flipkart.com/micromax-x412/p/itm1d1df2e8a9012?pid=MOBFJXFH6QUFHXKV&amp;lid=LSTMOBFJXFH6QUFHXKVEQFVJO&amp;marketplace=FLIPKART&amp;q=micromax+keypad&amp;store=tyy%2F4io&amp;srno=s_1_3&amp;otracker=search&amp;iid=22496617-e0d2-4a7c-a8ac-eaf50879265c.MOBFJXFH6QUFHXKV.SEARCH&amp;ssid=hptaldccc00000001688580884943&amp;qH=26e55ddeaa2e42a6</t>
-  </si>
-  <si>
-    <t>Micromax X412</t>
-  </si>
-  <si>
-    <t>₹906</t>
-  </si>
-  <si>
-    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAcAAAAFQCAYAAAAoQ64wAAAAOXRFWHRTb2Z0d2FyZQBNYXRwbG90bGliIHZlcnNpb24zLjYuMSwgaHR0cHM6Ly9tYXRwbG90bGliLm9yZy/av/WaAAAACXBIWXMAAArEAAAKxAFmbYLUAABH0ElEQVR4nO3deVxU9f7H8dfAsK8qiwuI+y6LgorgvpSalQuaWy5ZN29m/tSW22bpbTNvmpbmzdRbmZVa7l29aRqaa+ZuqbgAoqJsssMw398f1BQKOChwBubzfDx8CMyZM+85MPOes351SimFEEIIYWVstA4ghBBCaEEKUAghhFWSAhRCCGGVpACFEEJYJSlAIYQQVkkKUAghhFWSAhRCCGGVpACFEEJYJSlAIYQQVkkKUAghhFWSAhRCCGGVpACFEEJYJSlAIYQQVkkKUAghhFWSAhRCCGGVpACFEEJYJSlAIYQQVkkKUAghhFWSAhRCCGGVpACFEEJYJSlAIYQQVkkKUAghhFWSAhRCCGGVpACrue7du/P5559XyLx1Oh3x8fEVMu+7ERsbi6enp9YxLNrKlSsZOHDgXd9uaV577TUmTpxY4u2urq4kJCRUYqLSVeTrUZSdFGAla9CgAc7Ozri6ulK3bl2mTJlCQUFBpTz2ihUr6N27t1nTxsbG4urqiqurKy4uLuh0OtP3rq6uFZz07tSvX5/U1FStY1i0UaNGsXHjRtP3t36IufV2S1PWD10ZGRnUrVu3AhNVPinR8iMFqIFt27aRkZFBdHQ0a9eu5ZNPPtE60m3q169PRkYGGRkZxMTEAJi+z8jIqLDHNRgMFTZvS1Ddn581UUphNBq1jiHugRSghho3bkxERARHjhwx/WzNmjW0bt2amjVr8uCDD5KYmAjA9evX6devH56ennh5eTFixAgAdu7cSZMmTYrMt7hPyefPn+fJJ59k586duLq60rp163J5Dhs3bqRhw4Z4eXnx1ltvmX5eUFDAzJkzCQgIwNfXl+nTp5f45t+9e3deeeUVQkNDcXFxIT8/n127dtG+fXs8PT3p3r27qYQnTpzI66+/XuT+jRo1Yvfu3Vy8eBG9Xm/6eXJyMiNHjsTHx4dGjRrxn//8B4CzZ88WWSvo27cvPXv2NH1ft25dzp49W+Iyv1VMTAxdu3bF09OTunXr8uKLL5puW7FiBT169OBvf/sbHh4eLF++vMRcxdHpdCxcuJD69etTu3Zt3n33XdNtOTk5PPXUU9SuXZv69esza9Ys0xvyvn37CAkJwd3dnXr16jFv3jxTnj+2AvTt2xeA5s2b4+rqSnR0dJHbS1vWQIm/o+IsWrSIRo0a4e3tzejRo0lLSwP+/PudNWsWNWvWpEGDBmzdurXYeRSXFyA7O5uoqCjc3Nzo2LEjFy5cKLL8/ngtLFu2jICAANzc3GjevDk7d+4s8zIfN24ckydPpmfPnjg7OxMTE0N0dDQhISF4enrSrVs3Tp8+bZr+4MGDBAYG4u7uzpNPPlmkMMeNG8c///lP0/e3bqHZsWMHoaGhuLu707RpU6Kjo5k9ezbR0dFMnDgRV1dX3nzzzRKXuTCDEpUqICBARUdHK6WU+u2331Tt2rXV3LlzlVJK7d+/X9WrV08dO3ZM5eXlqWeffVYNGTJEKaXU888/ryZNmqTy8/NVTk6O2rNnj1JKqR9++EE1bty4yGMAKi4uTimlVLdu3dRnn32mlFJq+fLlqlevXkWmfeutt9SAAQNKzXzlyhVV3J8KoIYOHarS09PV8ePHlYODgzp37pxSSqk5c+aoHj16qMTERJWSkqK6d++uFi5cWOz8u3Xrpho3bqzOnj2rsrOzVWxsrPLy8lI//vijMhgMasGCBSo0NFQppdS2bdtUq1atTPfdv3+/8vPzU0ajUV24cEHZ2tqabuvfv7+aPn26ysnJUadPn1Z16tRRR48eVUop5evrq86dO6cMBoPy9/dX9erVU3l5eercuXPK19e31GV+q3PnzqmdO3eq/Px8debMGeXv76++/fZb0zK3tbVVy5cvVwUFBSorK6vUXMUt4759+6q0tDR1+vRpVbt2bfX9998rpZR68cUXVbdu3VRycrK6dOmSatq0qVq+fLlSSqmOHTuqzz//XCmlVHJysjp8+LApz1//Bv76t3Lr7aUt69J+R7fatm2bql27tjp58qTKyMhQgwcPVmPHjlVKFf792traqrffflvl5+erJUuWqPr16xc7n+Lyzpw5Uzk5OakdO3ao/Px8NWbMGPXoo4/eNn1GRoZyc3NTZ86cUUopdfHiRXX+/PkyL/OxY8eqWrVqqUOHDqn8/Hx19epV5enpqdauXavy8vLUnDlzVJMmTVR+fr7Kzc1Vfn5+atGiRSovL08tWLBA2draml6PY8eOVbNnzy522cfExCg3Nze1ceNGZTAY1KVLl9TZs2eVUkVf0+LeyBqgBvr164erqyvNmzenc+fOPPXUU0DhJ9S///3vtG3bFjs7O1555RXWr1+PwWDAzs6OK1euEBcXh4ODA507dy6XLC+88AKbNm26p/u7urrSpk0bAgMDOX78OACffPIJ//znP/H29sbT05Pp06ezZs2aEufz2GOP0aRJExwdHVm5ciWDBg2iS5cu2Nra8vTTT3Px4kUuXrxIz549uX79OidPngTg66+/JioqCp1OV2R+V69eZefOnbz11ls4ODjQokULRo4cyTfffANAly5d+PHHH/nll18IDAwkODiYw4cPEx0dTWRkJIDZy7xx48Z069YNvV5P06ZNGTVqlGkt6Y/bx40bh42NDWlpaaXmKs4//vEP3N3dadGiBY899hhfffUVAF9++SUzZ86kRo0a1K9fn+nTp7Nq1SpT9nPnzpGcnEyNGjUICQkp9fdYnNKWdWm/o1t9+eWXPPHEE7Rq1QoXFxfefPNNvvrqK5RSALi4uPDss8+i1+sZPXo0sbGxZdqX26tXL3r06IFer+eRRx7h6NGjxU6n0+k4efIkubm5BAQE0LBhwxLnWdIyBxgyZAjt27dHr9ezbds2AgMDGTx4MHZ2dkyfPp2srCwOHjzI3r170ev1TJo0CTs7OyZPnkydOnXMek6rVq1i4MCBPPDAA9ja2lK/fv3btvSIeycFqIHvvvuO9PR01q1bx6FDh0z71GJjY3njjTfw9PTE09MTf39/9Ho9V69e5dlnn6V+/fp069aNFi1aWMx+Q19fX9PXzs7ORZ7LH5sPPT09GTVqlGlzbnH8/PxMX8fGxvLZZ5+Z7uvp6UlmZiaXL1/G1taWoUOHmt5AV69ezfDhw2+bX2xsLDk5OaYC9vT0ZMmSJVy9ehUoLMDo6GhT4f31+y5dugCYvcwvX77MoEGDqF27Nh4eHsyfP5+kpKQSn1tpuYrj7+9f5OsrV64AkJCQQP369U23BQQEmI54XLp0KSdPnqRJkyZERkayd+/eEudfktKWdWm/o1sVlzMnJ4fk5GQAvL29sbEpfCtydnYGKNN+5pL+Bv/KxcWFVatWsWDBAnx9fYmKiir16NCSljkU/X3e+txsbGzw9/cnISGBK1euFJlWp9MV+b408fHxpRa0KB9SgBrR6XQ89NBD9O7d27QfoF69esyePZvU1FTTv+zsbPz8/HB3d+f9998nNjaWFStW8PTTT3P+/HlcXFzIzs42zffatWulPmZlqVevHj/88IPpeaSlpXHq1CmzstWrV4/HH3+8yHLIysoiIiICgOHDh/P111+zb98+bGxs6NixY7GP7+rqSkpKimke6enpfPTRR8Cfa4C7d++mS5cudOnShd27d7N7927TGmBJy/xWL7/8MjVq1ODMmTOkpaUxdepU09pNcc+ttFzFiYuLK/L1H2sRdevWJTY21nRbbGysad9m8+bN+frrr0lMTOSRRx4pcf/lnZS0rO/0O/qr4nI6OjpSs2bNu8p0t/r378+OHTuIj4/HwcGhyL7aW5W0zKHo7/PW56aUIi4ujrp161KnTp3b9sX/9fvSXrv+/v7Frk3f+vji3kgBamzGjBksXbqUGzduMH78eD744APTJpzk5GTWr18PwObNmzl//jxKKTw8PNDpdNja2tKsWTNSUlLYtWsXubm5zJ49u8TH8vHxIT4+vlKORJwwYQIvv/wyV65cQSnFxYsX2bVrl1n3HTlyJKtXryY6Ohqj0Uh6enqRzaddunQhPT2dl19+mWHDhhU7j3r16hEeHs7LL79MVlYWBoOBw4cPm0o4KCiI69evEx0dTVhYGKGhoezdu5crV64QHBwMlLzMb5Weno6bmxuurq6cOHGi1EPU75SrOO+88w43b97kt99+Y9myZabnPHz4cGbPnk1KSgpxcXG89957PPLII0Dh+XxJSUno9Xrc3NyKzQ2FfxMlvdFCycv6Tr+jvxo+fDgff/wxp0+fJjMzk5deeolhw4bd1Rv5nfKW5Nq1a2zatIns7GwcHBxwdnYucZlAycv8Vv369ePo0aOmXRXz5s3DycmJ0NBQwsPDyc/P59///jf5+fl8+OGHRdYkg4KC2Lx5Mzdv3uT8+fNFtjCMGDGCjRs3smXLFoxGI3FxcaaDjO52GYjbSQFqrGXLlnTr1o3333+fzp07M3fuXB599FHc3d1p164de/bsAeDMmTP06NEDNzc3BgwYwPz58wkICMDDw4P333+fYcOG0bBhQ8LCwkp8rJ49e9KgQQO8vb0JDAwE4M0336Rfv37l/ryeffZZwsPDiYiIwMPDg4EDBxb5VF2ahg0b8uWXX/Lss89Ss2ZNWrRoYfogAIWbmaKiotixY0eJb0xQWALx8fE0atQIHx8fpk6davrEbWNjQ+fOnWnRogX29vbY29vTqlUrOnXqZHpjLGmZ3+rVV1/lhx9+wN3dnSlTpjBkyJBSn19puYrTv39/2rRpQ9euXZkyZYrpSMFXXnmF5s2b06JFC8LDw3nkkUcYO3YsAFu2bKF58+a4ubmxYMECPv3002Ln/eqrrzJkyBA8PT2L7Lf8Q0nL+k6/o7/q27cv//jHP+jfvz8BAQHY2dkxf/78UpdRSe6UtyRGo5E5c+bg6+uLj48Ply9fLnIE5q1KWua38vLyYt26dcycOZNatWrx7bffsm7dOuzs7LC3t2ft2rUsXLiQWrVqcezYsSL7kceMGUPjxo3x8/NjxIgRRdbSGzZsyNq1a3nppZfw8PCgV69epvJ8+umnWbFiBZ6enrz99ttmLwNxO53667YaIYRF0el0xMXFmb3vSNw7WebWQ9YAhRBCWCUpQCGEEFZJNoEKIYSwSrIGKIQQwipJAQohhLBKUoBCCCGskhSgEEIIqyQFKIQQwipJAQohhLBKUoBCCCGskhSgEEIIqyQFKIQQwipJAVoQvV5PcHAwbdq0ISoqiqysrDLd/6OPPjKNXL1ixYoiA9D279+/1BEHKsPEiRNNQ7oIIYTW5FJoFsTLy4sbN24AMGrUKNq3b8+0adPual7du3fngw8+oE2bNuUZ0aSgoKDU8dSEEMLSyRqgherSpQvnzp3jxo0bDBw4kMDAQLp3724aCPPLL7+kZcuWBAUF8dBDDwHw2muv8cEHH/Dtt99y6NAhhg4dSmhoKAANGjQgIyOD559/nmXLlpkeZ8KECXz77bcUFBQwffp0wsLCCAoKYuXKlbdl2rlzJz179qR///5ERESQmZnJuHHjCAsLo3379vzvf//DaDTSuHFjMjMzAcjOziYgIACDwUD37t05ceIEAFu3biU8PJyQkBBGjx5NXl4eX3zxBS+99BIAL774Ir169QJgw4YNTJkyhYKCAkaPHk2rVq1o27Yty5cvr5iFL4SwClKAFshgMPDdd9/Rtm1bXnvtNbp06cKxY8eYNGkSU6ZMAeCNN95gw4YNHD169LbBTgcNGkRoaChr1qzh0KFDRW6Liopi9erVpsfZvn07/fr145NPPqFOnTocPHiQffv2MWfOHJKSkm7L9vPPP7N06VL27dvHG2+8wQMPPMDBgwfZunUrTz/9NDqdjn79+rFp0yagcGDWvn37otfrTfO4ceMG7777Ljt27OCXX36hUaNGfPzxx0RGRpoGOT148CCZmZkYDAZ2795NZGQkR44c4cKFC5w6dYrjx48zePDg8lvoQgirIwVoQVJTUwkODiY0NJSAgAAee+wxdu/ezejRowEYNmwYBw4cACAiIoInnniCpUuXUpat2KGhoZw/f56UlBS2b99OREQEjo6ObNu2jaVLlxIcHEx4eDhpaWmcP3/+tvtHRERQt25dALZt28asWbMIDg6md+/eZGZmcu3atSIlu2bNGqKioorMY9++fRw7dozw8HCCg4NZvXo1Fy5coH79+ly7do2MjAwKCgoIDw/nl19+Yc+ePURERNCoUSMSEhJ46qmn2LZtGx4eHne1nIUQAkB/50lEZfH09OTIkSOlTqPT6QBYvHgx+/btY+PGjYSGhnL8+HGzH+fhhx9m3bp1/PTTT6ZyMhqNLFmyhG7dupV6X2dnZ9PXRqORjRs3EhAQUGQaHx8fJkyYQFJSEvv27eOzzz4rcrvRaGTAgAHFbsJs164d//73v2nfvj2dOnVi+/bt3Lhxg3r16gFw/PhxtmzZwrx589i2bRtz5841+3lXlDyDkWs3c0hIzeZKWg4JadlcS8vhZo6BjFwDmb//K/y6gPwCIzY2OvQ2Omx0OmxtCv/pbXS4Oepxd7LDw8mOGs72eLna4+XqQB1PJwJqOuNXwwm9rXxuFaI8SAFauMjISL744gtmzJjBmjVr6NChAwDnz58nPDycTp06sW7duts2V7q5uZGenl7sPKOionjxxRc5e/YsCxcuBKBv374sWrSIyMhIbG1tOXHiBC1btiz1QJe+ffuyYMEC/vWvfwFw5MgRgoODsbGxoV+/fjz99NP07t27yOZPgPDwcKZMmcKlS5cICAjg5s2bJCUl0bBhQyIjI3nrrbdYuHAh4eHhTJ061VTKN27cwN7enmHDhhEQEGDaX1hZsvIM/HY1nd+upvPr7//HXM/gekYulXUomd5GR11PJwJqOVO/pjONvV1p6+dB67ruONvLy1mIspBXjIV77bXXGDduHJ9++ik1a9ZkxYoVAMyYMYNz586hlGLQoEH4+fkVud+4ceMYN24cbm5ut+0HDA0N5dy5c4SHh+Po6AjA448/zoULFwgJCcFoNFKnTh2+++67UrO98sorPPPMMwQGBmIwGGjXrh2ff/45UFiy3bt3Z+vWrbfdz9vbm48//pghQ4aQl5eHjY0N8+fPNxVgfHw8nTt3xsfHBycnJyIiIgC4fPky48aNw2g0otfrmT9//t0sUrMopThzLYMDF5I4cDGFY/GpxCZnVVrRlcRgVMQmZxGbXPQUGRsdpjIMrOdBkL8nbet5yNqiEKWQ0yCE+N2phJv8FHOD/ReSOXQxmZSsfK0j3RM3Bz0dG9WiS1MvIpp40cTHVetIQlgUKUBhtfILjOw/n8z/Tl3l+9OJXE7V9kIBFa2uhyMRTbzo27o23Zp5Y6+XtUNh3aQAhVXJNRSw/XQi/z1xlZ2/JXIzx6B1JE24Oerp09KXAYF16NJUylBYJylAYRWOx6ex+uc4NhxNILWKb9osb+6Oevq2rk1Uez86NqqldRwhKo0UoKi2kjJy+faXy6z5OZ5frxZ/RKwoqqmPKyM71mdwOz88nOy0jiNEhZICFNXOqYSbfLL7AhuPJZBnMGodp0pysrPlgcA6jO4UQJC/p9ZxhKgQUoCi2th15jpLdsXwU8ztl3ATd69jw5o83bMpkU29tI4iRLmSAhRVmlKKLcev8uEP5zh15abWcaq1IH9PJvdoQu+WPqYrEglRlUkBiipr52+JzN32GycuS/FVpha13ZjcswkD2taRIhRVmhSgqHJ+vpTCnP/+yv4LyVpHsWrB/p688kBL2gfU1DqKEHdFClBUGeevZ/DmltN8fzrxzhOLStO/bW1euL8l9Ws533liISyIFKCweDn5BXz4wzmW7DpPXoEc1WmJ7G1tGNs5gKd7NcXdUU6fEFWDFKCwaD/8msjMDSdvu/izsEw+bg7MHNiaAYF1tI4ixB1JAQqLdCUtm9c3nOK/J69qHUXchV4tfPjnoDbU8XDSOooQJZICFBbnm8PxzFx/kvRc67xOZ3Xh5qDnxQEtGdGhvtZRhCiWFKCwGGlZ+by47jibj13ROoooR12aevGvYUH4uDlqHUWIIqQAhUXYffYGM1Yf5erNHK2jiArg5erAvOFBdGnqrXUUIUykAIWm8guMvP3dryzbc0Hz0dZFxdLpYFK3xkzr00xGqhcWQQpQaOZ6ei5/X/kzBy+maB1FVKL2ATVYMCKEep5ygIzQlhSg0MQvsSlM+vywbPK0Up7Odiwa1Y7OjeUC20I7UoCi0n15IJZX15+Uk9qtnJ2tjlkPtZGjRIVmpABFpTEUGJm54SQr98dqHUVYkAkRDXl5QEtsbOTC2qJySQGKSpGTX8BTKw+z/Ve5jqe4Xc8WPiwYEYKrg17rKMKKSAGKCpealceEFQc5HJuqdRRhwVrUduPTxzrI+YKi0kgBigqVkJrN2GUHOJuYoXUUUQU09HLh84kd5QhRUSmkAEWFOXstnUeXHeBKmhzpKcxXz9OJlRM70sDLResoopqTAhQV4uy1dB759z6SMvO0jiKqIG83B1ZO7EgzXzeto4hqTC7HIMrd+esZjFy6X8pP3LXr6bkMX7KXE5fTtI4iqjEpQFGuLiVlMvLj/VxPz9U6iqjiUrLyeXTZAc7J/mNRQaQARbmJS85i5Mf75eouotwkZ+Yx5pP9XE7N1jqKqIakAEW5SLyZw8il++SNSpS7K2k5jFm6nxsZslVBlC8pQHHPsvIMTPjPQeKSpfxExTh/I5Oxyw6QnpOvdRRRjUgBintiNCqmrDrCics3tY4iqrmTCTeZ+J9D5Ms1ZEU5kQIU92T25lN8f/qa1jGEldh/IZlX15/UOoaoJqQAxV1bsecCy/dc1DqGsDKrDsTy6d6LWscQ1YAUoLgrO39LZPbm01rHEFZq1sZT/BRzQ+sYooqTAhRlFp+SxdSvjlBglIsICW0YjIqnVh4mLjlL6yiiCpMCFGWSayjg7ysPk5olR+MJbaVk5fP4p4fIyS/QOoqooqQARZm8sfk0x+Ll8lTCMvx6NZ03t8imeHF3ZPRJYbb/nrjCp3svaR3jnuWnXiXpu/cxZqaCzobaY/5F4uqZGHMzwViAc8uueEaMQCnFjQ1zyL9xCdeg+3EPfRCAG1vex6PTUOxq1tP2iQgAPt17ia5NvendylfrKKKKkQIUZklIzea5Nce0jlEukrbMx7PLaBz921CQnY5Ob4fP0JnYODijjAVc/fw5nJt0AJ0Ona2eOhM+5MqKZ3APfZC8azHY2DtK+VmY59Ye479+XfBxl8F0hflkE6gwy/Nrj3Ezx6B1jHuWd/0SOhtbHP3bAGDr5IbOxhYbB2cAVIEBjAZABza/fz40FqCztQMg7aev8Oj8iBbRRSmSM/OY9vVRZHQ3URayBiju6KuDsUSfrR6HnBtSEtDZO5G45nUKMpJxbh6BR/gwAK5+NoO8G5dwC+mPvW8jAGwcnLny6f/hHvoQ2TGHsK/TFFtnDy2fgijB7nM3WBp9gce7NtI6iqgiZEBcUaqraTn0mbeL9Gqw9geQ+etukrd+SJ3xC7B19uTa6lfx6DQMp4YhABhzs7i+7i1q9HwMe+8GpvspZeT6mll4PfQCqT/+h4L0JNzCHsLRr7VGz0QUx8nOlq1Tu1K/lrPWUUQVIJtARan+8c2xalN+AHq3WtjXboLe3Rud3g6nRqHkJZ433W7j4IxjgyCyzx8ucr+MY9/j3LIruZdPYePkTq0HppG258vKji/uIDu/gJfWHdc6hqgipABFidb8HM8Pv13XOka5sq/TjIKsNApyMlDKSG7cCexq1qMgq/DUDmXIJ+fCYexq+ZnuY8zPIfvsXlxa90Dl50KBAVTh2qKwPNFnb7D+yGWtY4gqQDaBimKlZefTY+5OkjPztI5S7rJjDpGyczmgcGwQgnvoQ1xf92bhATDKiHOLLnhGjDBNn7pnFQ5+rXAKCMKYn8v1ta9TkJGCR+dHcGnVTbsnIkrk5WrP9mnd8XC20zqKsGBSgKJYszaeYtmeC1rHEOKuDQ/1552hgVrHEBZMNoGK25xLzOCzfRe1jiHEPfn65ziOxKVqHUNYMClAcZvZm06RXyAbBkTVphS8KSOWiFJIAYoidvx6jV1nqteBL8J6HbiYzH9PXNU6hrBQUoDCpMCoeEM+MYtqZs7WX2XoLlEsKUBhsuHoZWKuZ2odQ4hydf56JqsPxWkdQ1ggKUABgNGoWLjjnNYxhKgQ728/S65Bxg0URUkBCgA2HkvgvKz9iWrqSloOa36O1zqGsDBSgAKjUbFg+1mtYwhRoT7+8TxG2Rco/kIKULDxWILs+xPV3sWkLL6TI0LFX0gBChbvjNE6ghCV4qNd8rcu/iQFaOX2n0/i16vpWscQolIcv5zG7moytqW4d1KAVu7TvZe0jiBEpVryo6wFikJSgFbs2s0ctp6UfSLCuuw+d4O4ZBnKSkgBWrWV+y5hkKPihJVRCr46KCfGCylAq5VnMPLFAXkTENZp9c9xcnk0IQVorXb8msiNjFytYwihiWs3c/nh10StYwiNSQFaqQ1HL2sdQQhNfXkwVusIQmNSgFYoI9fA9tPy6VdYtx9+u871dNkKYs2kAK3Q1hNXyTUYtY4hhKYKjEqOgrZyUoBWaMPRBK0jCGERZLBc6yYFaGWSMnLZc06uhCEEwL7zSaRm5WkdQ2hECtDKfH/6mpz7J8TvDEbF/05d0zqG0IgUoJXZ+dt1rSMIYVFkP6D1kgK0IoYCI7tl86cQRfx49gZZeQatYwgNSAFakV/iUknPkRe6EH+VZzBy8GKK1jGEBqQArcgu2fwpRLF+ipEtI9ZICtCK7DojBShEcfbFJGkdQWhACtBKpGblcSIhTesYQlikEwk3Sc/J1zqGqGRSgFbiSFwqSs5+EKJYBUbFgQvJWscQlUwK0EociUvVOoIQFm2vbAa1OlKAVuKX2FStIwhh0Y7Gp2odQVQyKUArIS9uIUp3+ko6SvYTWBUpQCtw4UYmqVmyg1+I0mTkGriUlKV1DFGJpACtwFHZ/yeEWU4m3NQ6gqhEUoBW4Ldr6VpHEKJKOHVFThWyJlKAVuBcYobWEYSoEmQN0LpIAVqBGClAIcxy9pq8VqyJFGA1ZygwEpciO/aFMMfVmzkYCoxaxxCVRAqwmrucmk1+gRzaLYQ5CoyKK2k5WscQlUQKsJqTw7qFKJv4lGytI4hKIgVYzV1JkxezEGUhuwyshxRgNXcjI0/rCEJUKbIGaD2kAKu5Gxm5WkcQokpJSJUCtBZSgNVckqwBClEmctlA6yEFWM3JGqAQZXNTBsa1GlKA1ZysAQpRNjezpQCthRRgNZeSJQUoRFmk5xi0jiAqiRRgNZdrkKtaCFEWsgZoPaQAq7l8uayTEGWSkWfAaJSrJ1kDKcBqLk/WAIUoE6UgTz44WgUpwGpMKYVBPskKUWYF8rqxClKA1Zh8ihXi7hiVFKA10GsdQFQcg4wCYbHua+3Li/1bah1DlMDFXt4arYH8lqsxWxud1hFEMdoH1OD9R0JwtLPVOooQVk02gVZjjna26KQDLUojLxeWPhoq5SeEBZACrOYc9PIrthRervasGN+BGi72WkcRQiAFWO05yZqGRXC2t2XZuDDq13LWOooQ4ndSgNWcFKD2bG10fDAyhEA/T62jCCH+QgqwmpN9Tdqb/VAberbw1TqGEOIWUoDVnJujHOirpck9mjCyY32tYwghiiEFWM15uzlqHcFqDW5Xjxn3Ndc6hhCiBFKA1Zyvu4PWEaxSZBMv3hkSqHUMIUQppACrOR9ZA6x0LWq7sXh0O+xs5eUlhCWTV2g1J2uAlauuhyMrxnfAzdFO6yhCiDuQAqzmfN1lDbCyuDvqWTGhA7U9ZJkLURVIAVZzUoCVw97WhiVjQmnm66Z1FCGEmaQAq7mGXi5yPdAKptPBu1GBhDeupXUUIUQZSAFWc072ttTzdNI6RrX23H0teCi4ntYxhBBlJAVoBWSzXMV5NDyASd0bax1DCHEXpACtQFMfV60jVEt9Wvny2sDWWscQQtwlKUAr0EQKsNyF1Pdk4YgQbGTQYSGqLClAKyCbQMtXQy8XPhkbJhcaF6KKkwK0As1ru2FnK2sq5aGWiz0rxodRUwa1FaLKk6ECrICjnS2t6npwNC5V6yhVmpOdLZ+MCyOglotmGdafW88b+99AKaVZBlG8j/t+TLBPsNYxRBlIAVqJ0IAaUoD3wNZGx8IRIQT7e2qa46EmD3Eh7QKfnPhE0xzidjY62aBW1chvzEq0D6ihdYQq7fUHW9O7lWUMavtMu2d4oNEDWscQt9DbyPpEVSMFaCVCpQDv2qTujRndKUDrGCY6nY5ZEbPoWLuj1lHEX0gBVj1SgFbCx90RvxpyRZiyeji4Ls9Z4KC2djZ2zOsxj6Y1mmodRfxOr5MCrGqkAK1IeCO5VmVZdG5cizlDg9BZ6MVU3ezdWNRrEb7OlrFp1trZ2coQWFWNFKAV6dHCR+sIVUZzXzc+GtMee71lv0Rqu9Rmce/FuNnJuZ5a83by1jqCKCPLfnWLctWlqZecD2iG2u6OrJgQhnsVGdS2aY2mzOsxDzubqpG3OnK3d8dRL0OPVTVSgFbEzdGOsAY1tY5h0dwc9KyYEEYdD433lxbkw645UGAwa/KOdTryeufX0SEfcLTg4yxbV6oiKUAr01M2g5bIzlbHkjHtaVHbXesosOFp+OEN2DTV7LsMbDyQKe2mVFwmUSLZD1s1SQFaGSnAks0ZGkjnJl5ax4Ad/4Sjqwq//uUz2PmO2Xed2HYiw5oNq6BgoiS+LlKAVZEUoJVp5O1KY2/tLuVlqZ69rzmDQvy0jgE/r4Af3y36s51vwi8rzZ7Fix1fpLtf93KNJUonm0CrJilAK/RgkIxe/lejOtbnqR5NtI4BZ7bCpmnF37ZxCpzbbtZsbG1smdNtDm292pZjOFEaKcCqSQrQCj0UXFfrCBajd0sfZj3URusYcPkwrB4PqqD4240G+HosXDlq1uyc9E580OsD/N38yzGkKInsA6yapACtUAMvF80v6mwJgvw8WDiiHbZaD2qbchG+GA75maVPl5cOK4dBaqxZs63pWJPFvRdTw0Eug1fRpACrJilAKzWkvQXs79JQQC1nPhkXhpO9xoPaZiXD50MgM9G86TOuwsooyE4xa/IA9wAW9lqIo62co1aRZBNo1SQFaKUeDKqLg4Vf5aSi1HSxZ8X4Dni5OmgbJD8HVj0CSefKdr/rv8KXo8CQa9bkQd5BvN31bRmup4I4652p4Shr2VWRvCKslIeTHfe3qa11jErnaGfDx4+G0tBL4yNhjUb4ZiLE7b+7+1/aA98+CWYOjNurfi9e6PDC3T2WKFUbLwvYhyzuihSgFRsf0VDrCJXKRgfvPxJiGWMjbv0HnN54b/M4+Q1se9nsyUe0GMH41uPv7THFbeRo26pLCtCKBft7ElLfU+sYlWbmwNbc19oC1np/Wgj7Pyqfee39APaZP6//a/9/9GvYr3weWwDQ1lsKsKqSArRyE6xkLfCJro0Y27mB1jHgxFrY9kr5znPrP+DUBrMm1el0vBHxBmG1w8o3gxkuLbjEqb+fIvaDokexKqMiZlaM6edKKeIWxXH2pbMk/S/JNF38J/HkXjVvv2dlCvQK1DqCuEtSgFauX5va1PGo3kcIDgyqyz/6tdA6BlzcA99OAszbb2c2ZYRvHodY8/Yn2tnaMb/HfJp4Vu7J/7X61MLv8duPPk75MQU7rz9HssiJy0Gn19Hkn01IiS482jX7Uja2jrY41Nb4wKVb1HapjbezDINUVUkBWjm9rQ1jwgO0jlFhOjWqyb+iLGBQ2+u/wZcjoaCC1mAMvx9ResO8I0rd7d1Z3HsxPk6Vd/i+a0tXbByLvuUYMgyk7U+jZvc/RynR2epQSkEB6PSFv7frG67j/aDlFY3s/6vapAAFozoE4Oag1zpGuWvm68qSMaHaD2qbfhU+Hwo5qRX7ONnJ8PlgyDDvnMLaLrVZ1HsRLnbaHRGbuDaxsNj+8vnEsZ4jts62xLweQ80eNUk/lo5TQyf0bpb3NyqbP6s2KUCBh7Md4yOr175AX3cHlo/vgIeTxoPE5mYUnrieZt7VW+5Z6iX4Yhjk3eGqMr9rXrM573V/D71N5ZdL9qVsCjILcG3petttdcfUpcnsJnhGeJL0fRK1+tQi4fMEYhfGknnGvOdWGeQAmKpNClAAMLFLQ+3Lopy4OuhZPq4D9Ty1HtTWAF8/ClePVe7jJvxSeF1RYwnXFb1F57qdeb3z6xUc6nZZMVlknsnkt+m/Eb84nvRj6VxefrnINCnRKXh09CDzbCZ6Nz1+T/hxfcP1Ss9aHL1OT6tarbSOIe6BFKAAwN3Rjie6NtI6xj2zs9WxeHQ7WtW1gEFtNz4DMeaN4FDuzm6FzSWMLFGMBxs/yOTgyRUY6Ha1etaixfwWNP9Xc/wm+eEW6Ea98X+OVGLMNZJ+OB3Pzp6oXIUyFB48VJBlXrFXtCY1muCk1/hDlrgnUoDCZFznBtRysdc6xj15a3AgXZpawMESP7wFRz7XNkNxYwuW4m9Bf2NI0yEVFufCnAvELYoj/Vg6v/7fr2Sdyyp1+hv/vUGt+2qh0+lwbetK1rksYl6PoVbfWhWWsSw61emkdQRxj3RKmXktJWEVPv7xPG9sOa11jLsyrU8zpvRqqnUMOPwZbKjctalSPfwRBI8wa9ICYwFTfpjCj/E/VnCoqu+L/l/IPsAqTtYARRFjwgPwr1n1NuuM6OBvGeV39nvYNFXrFEVteBpifjBrUlsbW97t+i6ta7Wu4FBVWx2XOlJ+1YAUoCjC0c6WVx+oWm9+PZp7M9sSBrVNOAKrxxYOXmtJjPm/H4xz3KzJne2c+aDXB9RzrXfnia1U74DeWkcQ5UAKUNymTytfejS3gP1oZmhbz4MPR7VDb6vxn3LKH6cfZGiboyS5N38/HSPerMm9nLz4qPdHeDp4VmyuKqpvQF+tI4hyIAUoijVzYGvtTyC/A/+aTiwbF4azvcYnSGenwMqhkHFN2xx3kn6l8IT87FSzJm/g0YCFPRfiYGtZlx/Tmq+zL0HeQVrHEOXAst/hhGYaeLnweBfLPTne09mOFeM74O2m8ZuzIRdWjYAbZ7TNYa7rp+Gr0WDIM2vyYJ9g3u4ig+n+Ve+A3tpfWk+UC/mrFiWa3KMpfjUs74AYB70NSx8NpbH37VcQqVRKwTdPQOxebXOU1cVoWDfJ7MF0ewf05rmw5yo4VNUhmz+rDylAUSIne1vmDA3Ekj7sFg5qG0xog5p3nriibX0JTq3TOsXdObEGvp9p9uSjWo7i0VaPVmCgqsHHyYcQnxCtY4hyIgUoStW5sRdjwxtoHcPk5QGtuL9NHa1jwN5FsO9DrVPcmz3vw4GPzZ58RugM7mtwXwUGsny9AnrJ5s9qRApQ3NEL/VrQyFu7EQP+8FhkQyZYwkW7T62HbS9pnaJ8fPcc/LrZrEl1Oh1vRr5JO592FRzKcvVv2F/rCKIcSQGKO3K0s+VfUUHY2mj3yXdAYB1eHtBSs8c3id1XuN9PGbVOUj6UEdY8BnEHzZrc3taeBT0X0Mij6l83tqxa1mxJsE+w1jFEOZICFGYJqV+DJ7tp86bXoUFN3htmAYPa3jhbOOisIUfbHOXNkA2rhkNSjFmTezh4sLj3Yrydqsa5ouVlRAvzLicnqg4pQGG2/+vdjA6VfPBJEx9XPn40FAe9baU+7m0yEgsHm81O0TZHRclKgs+HQOYNsyav61qXD3t9iLPeuYKDWYaajjUZ0GiA1jFEOZMCFGbT29rwwagQfCrp3DsfNwdWjA/Dw1njcQrzMguvopJaSYPaaiXlwu9Xsyl9lIY/tKzVsnAwXZ3ljdRe3oY0HYK9bdUeKUXcTgpQlImPm2PhpccqeH+gi70ty8aF4VdD4zWMAgN8PRauHNE2R2W5/DOsmWD2YLoR9SJ4NfzVCg6lLb2NnuHNh5s9vU6n4+WXXzZ9P2PGDFasWHFXj71z504OHDhQ5vuNGzeOTZs2FfvzRo0aERQURGBgINu33914lR999BFfffXVXd3XkkgBijILa1CTF/q1qLD56210LBrdnjb1PCrsMcy2+f/g3P+0TlG5znwHW2aYPfmgpoOYFDSpAgNpa2Cjgfi6+Jo9vaurKytXriQ9Pf2eH7u0AiwouLuBgRcsWMDRo0d57733ePLJJ+9qHk8++STDh5v/ocBSSQGKuzKxSyMGBFbM+XhvDmpLt2YWcIDFrjlw+FOtU2jj0DKIfs/syf8e/HcGNRlUgYG0YaOzYUKbCWW6j4ODA6NGjWLRokW33RYTE8N9991HaGgoPXv25OLFiwB0796dEydOAHDixAm6d+9OXFwcH330EW+//TbBwcEcOXKEcePGMWnSJDp06MDbb7/NunXr6NChAyEhIQwYMIDU1FSzc0ZGRhIf/+fF0d955x3CwsIIDAxk7ty5AAwfPpwdO3aYpunZsye//PILr732Gh988EGJzykhIYGIiAgAtm3bhpOTE3l5eaSmphISUnghgfnz59O8eXOCgoKYNEmbD1DVf+O9qDBzhwZxOSWbI3Gp5TbPZ3o1ZViYf7nN764d+QJ+eEPrFNraPgs8/CBwmFmTvxr+KonZiey5vKeCg1WeXvV70cCjQZnv98wzz9CpUyeeeeaZIj//+9//zpIlS2jQoAE7duzg2WefZfXq1cXOw9/fnyeffBIvLy8mT/5zgOWkpCT279+PTqcjJSWFhx56CJ1Ox4IFC/jwww956SXzzlHdvHkzDz74IFBYUvHx8Rw4cACj0UifPn24//77iYqKYvXq1fTs2ZPExEQSEhIICQlh/fr1d3xOKSkp5Obmsnv3blq1asXPP/9MSkoK4eHhAMyaNYu4uDhcXFxIS0sr0/ItL1KA4q452dvyydhQhiz+iYtJ5h04UZphoX78X59m5ZDsHp3bDhumaJ3CAihY/xS4+kKjbnecWm+j571u7zHuv+M4nXy6EvJVvMfbPn5X9/P29uaBBx5g2bJlpp9lZGQQHR3Nww8/DIBSCheXsl9gYujQoaZTgmJjY4mKiuLatWtkZ2fTsWPHO95/ypQpTJs2jdjYWPbsKfywsm3bNjZv3kx0dDQA6enpnDlzhv79+/Pcc89RUFDAt99+y+DBg4vMq7TnFBoayoEDB9i/fz/Tp09n9+7dpKSkmNYMO3TowOjRo4mKijLdv7LJJlBxT2q5OrBifAdqudzbEXJdm3nz5iALGGH7yrHCg16M+VonsQwFefDVGLh2yqzJne2cWdR7EXVd6lZwsIrXza8bLWvd/cUXZsyYwfvvv4/BUDhAstFoxNfXlyNHjnDkyBGOHj3KTz/9BIBer8doLLy4Qm5ubqnzdXb+88CwKVOm8Nxzz3H8+HHmz59/x/tC4T7AM2fO8NZbb/H444+bss2cOdOULSYmhsGDB+Ps7ExYWBg//vgja9asISoqqsi8SntOkZGR7Nq1i9zcXPr27ctPP/3Enj17TAW4efNmJk+ezN69e+nW7c4fsCqCFKC4Zw28XFg6NhQnu7s7V691XXcWW8Kgtqlxv58GcO8HL1QruWmF4x3eTDBrci8nLxb3WYy7vXsFB6s4djZ2zAg1/0Cg4vj7+xMREcHatWsBcHd3x9fXl40bNwKFB7H8sd8vICCAI0eOAPDNN9+Y5uHm5lbqwTQ3b96kXr16KKX49NOy7a+eOnUqBoOBbdu20bdvX5YuXUpWVuGWnIsXL5o2S0ZFRbF48WLi4+NN++/+UNpzioyMZMmSJQQHB+Pl5cWNGzdISEigQYMGGI1G4uLi6NWrF3PnziU2NvauD+q5F1KAolyE1K/BghEhZT49op6nE8vHh+HioPWgtqmFb/LpV7TNYaluXi4cTDfnplmTN/JoxMKeC7G3qZrnzo1uOfqu9v3d6vnnnych4c8PDl988QULFy4kKCiItm3bmk5DmDZtGnPmzKF9+/bk5f05VuPAgQNZtWqV6SCYW82cOZOBAwcSFhaGv3/Z9p3rdDpeffVV5s6dy/3338+gQYPo1KkTbdq0YfTo0eTkFF7xqH///mzZsoVBg4o/yKmk59SyZUuys7NNa3wtW7akXbvC68gWFBQwatQoAgMDCQ0N5dVXX8XWtvIvdqFTysxBwYQww6ZjCUz98ggG453/rDyc7Fg7qTNNfDQe18+QC58Nhku7tc1RFTTsCqO/AVvzLk6w9eJWnt31LIqq8zbj7eTNxkEbcbHT/gLwomLJGqAoVw8E1mX+I8F3XBO019vw8aOh2pefUvDtk1J+5rrwY+GBMWa6r8F9TA+dXoGByt/U9lOl/KyEFKAod3cqQZ0O5g0LpkNDCxjU9n+vwMlv7jyd+NOxr+D7182efGzrsYxuOboCA5WfIO8gBjYaqHUMUUmkAEWFKK0EX+rfssJOoi+T/Uvgp4Vap6iadr8HBz8xe/Jnw56lT0CfCgx072x0Nvyj4z+0H3VEVBopQFFhHgisywcj22Gv//PPbHxEAyZ2sYCx5E5vhP++oHWKqm3Ls/Dbd2ZNaqOz4a0ubxHiE3LniTUyqMkgWtdqrXUMUYnkIBhR4fafT2Lip4eIbOLFhyPbYaPhwLoAxB2A/zxYOA6euDd2zjBuE9Rrb9bkablpjN4ymos3L1ZsrjJys3dj06BN1HS0gM3yotJIAYpKcS4xA78aTjje5bmC5ebGOfikD2Qna5ujOnHxhse2QU3z1uzj0+MZvWU0STlJFRzMfC90eIFRLUdpHUNUMtkEKipFEx9X7csv4zqsHCLlV94yrxeeI5hpXqH5ufnxYe8PcdI7VXAw83Ss01FGe7dSUoDCOuRlFV7lJeWi1kmqp+QYWDUc8s3brNy6VmvmdpuLrU7bD0U1HWvydpe3sdHJW6E1kt+6qP6MBbBmPCQc1jpJ9RZ/ENZOhN+vaXknXf268nKnl+88YQXRoeOtyLfwcvLSLIPQlhSgqP42T4Mz/9U6hXX4dRN895zZkw9tNpQnAp+owEAlm9BmAp3rddbksYVlkAIU1duPc+HnFVqnsC4HP4Y975s9+dMhT/Ng4wcrMNDtgr2DmRwy+c4TimpNjgIV1dfRL+Hbv2mdwkrpYMhSaDvUrKnzjfk89f1T7L2yt4Jzgbu9O2sGrqGOqwVcjEFoStYARfUU8wOsl0/42lGwbhJciDZrajsbO+b1mEfzGs0rOBfM6jxLyk8AUoCiOrp6Ar5+VAa11VpBHnw1ChLNGx3exc6FRb0XUcel4sppRIsR9AroVWHzF1WLbAIV1UvaZVjaG9LNG7xVC3FpRsZ8m01ipkJvA690dSCqtR0j1mZx6rqRAiN0qW/LhwMcsdHpmLY1h/+dN3B/Yz3v9nUE4NUfcujRQE+PhhqPo2gOD3947H/gbl6xxaTGMOa7MaSX88DErWu15tN+n2JvWzXHKBTlT9YARfWR8/vI5RZcfgB6G5h/vyOnnnJl2xhnpm7NITNPseQBJ44+6crxSS7cyFas/9VAao7i5ysFHJ/kyoGEAtJyFAnpRs4kGatG+QGkxcHKKMg1r9Aaezbm/R7vY2dj3piD5mjg3oBFvRdJ+YkipABF9WDIgy9HQeIprZPcUR03G4JrF54AXtvVBi9nHcnZCneHwmukFijINRQOG2WrAxsdGJXC5vevZ+3KZWY3By2fQtldOw5fjYEC8zZLh9UO443IN9Bx79eN9XHyYUmfJXKdT3EbKUBR9SkF6/8OF8074MKS/JxQQIER/D0KX4pDv87Cd24GrvbwYHM9bg46+jTSE7Ikkz6N9FxKM2Krg5beGl9W7m6c/wE2TDF78n4N+/F/7f/vnh7S3d6dJX2WUNe17j3NR1RPsg9QVH3/mwl75mudosySsxVdlmfy8UBHOvv/uTkzr0Axdl02E4Lt6dO46GbO4WuyWHC/Ix8dyud4YgGj2toxqGX5bSqsFF2fhZ7mXwHmzf1vsurXVWV+GCe9E//u82+CfYLLfF9hHWQNUFRtBz6ukuWXa1A8/GUWL0TYFyk/AHtbHYNa2LH+t6KbC7efN9DG25a0XEVsmpGvo5yYvz+vMmOXjx/fLdPFCV7o8AI9/XuW6SH0Oj1zu82V8hOlkgIUVdevW+C757VOUWZKKcatz6ZnQ1vGBBUelJFfoLiUWngNzQKjYtMZAy28bIvcZ/7+PKZ3ticrH/KMoANSsqvoBpxN0+DMNrMmtdHZ8E7XdwjyDjJreh06ZkfOpqtf13tJKKyAbAIVVVP8IfjPQMjP0jpJme2ONdB1eRaBvn9+/vzPw048uTmHjDyFUtC9gS3z73dE//vgwZ8dzSPfCBNC7FFKMWxNNqeuGxkfbMeMzlXsgJg/2LnA+M1Q17xR4lNyUhjz3Rgu3bxU6nTPhz3P6FajyyOhqOakAEXVkxQDn/SFrBtaJxH3ysUHJv4PajQwa/K49DhGbxlNck7xYzr+LfBvco1PYTbZBCqqlswbhef6SflVD5mJhYPpZpk3SLG/mz8f9rp9MF0dOqa1nyblJ8pEClBUHfnZ8MVwSD6vdRJRnpLOwqoRkJ9j1uRtvNrwbtd3TYPp6nV6ZkfMZnyb8RWZUlRDUoCiajAWwJoJcPmQ1klERYjbB9+YP5huN/9uvNjxRRxtHZnfYz4PNXmoggOK6kj2AYqqYfN0OLhU6xSionV8Evq9Y/bkVzOvUtuldgUGEtWZrAEKy7d7npSftdj/Efz0gdmTS/mJeyFrgMKyHVsN3zwOyJ+p9dDB0GXQZrDWQUQ1J2uAwnJd+LHwGp9SflZGwbdPwqWftA4iqjkpQGGZrp2CL0cXDqoqrE9BbuGRodd/0zqJqMakAIXluZnw+/hxaVonEVrKSS08RzD9qtZJRDUlBSgsS87NwvK7Ga91EmEJ0mJ//zCUoXUSUQ1JAQrLUZAPX4+Baye0TiIsydVj8PWjUGDQOomoZqQAheU4/Cmc36l1CmGJYrbD0S+0TiGqGSlAYTlCJ0CXGVqnEJao2wvQ7lGtU4hqRs4DFJbnl5Ww8Rkw5t95WlG92drDgwsh6BGtk4hqSApQWKYL0bBmPGRe1zqJ0IqLD0StgAYRWicR1ZQUoLBc6dfg2ydkv6A1atwTBi0BVx+tk4hqTApQWDajEfbMgx/eBKMcBVjt2dhBz5ch4hnQ6bROI6o5KUBRNcQdgLWPQWqs1klERfEMgKHLwa+91kmElZACFFVHThpsmAKn1mmdRJS3NkPggfng6K51EmFFpABF1XNoOfz3H2DI1jqJuFd2ztBvDrQbo3USYYWkAEXVlBQDW2ZAzA6tk4i71aRP4eC3tRprnURYKSlAUbWdWg//fVGuHVqVeNSH+9+Clg9onURYOSlAUfXlZcGPc2DvhzJ8kiWzdYDOT0PXGWDnpHUaIaQARTVy4yxseRbO/6B1EnGrxr2g/7uyuVNYFClAUf2cXAdbX5LNopbAoz7c9wa0elDrJELcRgpQVE+GXPjlc9gzX84d1IJnAET+HwSPAr291mmEKJYUoKjeCgxw7CvY/R4kndM6TfXn1Qwip0HbKLDVa51GiFJJAQrrYDTCyW8g+l+QeErrNNWPbxvoMh1aPQw2MsqaqBqkAIV1UQp+3QzRcyHhF63TVH312heO4di8n1y7U1Q5UoDCel0+DEdWwvE1kJOqdZqqw6lG4SbO4FFQN1jrNELcNSlAIQy5hWuFR74ovLKMKtA6keXR2UKTXoWl17y/HNgiqgUpQCH+6uYVOLqqsAyTzmqdRntezSF4ZOGI7G61tU4jRLmSAhSiJJd/hrPfQ8x2iD9kHWuGOlvwCytc22vaB+qGaJ1IiAojBSiEObJTC0emP/d94WbSm5e1TlR+PPwLR2Bv0gsadQdHD60TCVEppACFuBuJvxauGZ7fBVePQ3qC1onM514PareFht0KS8+7udaJhNCEFKAQ5SErubAIr52Aqyfg2nG4/pu2F+e2dSgst9ptC8/Tq92m8H/nmtplEsKCSAEKUVEKDHDjTOGJ9+lXICMRMq9DxjXIuA6ZiZB54+72LepswcULXHzA9fd/Lt7g6lt4sIpPq8KrssjVWIQokRSgEFoyGiErqbAM87PBaPjLvwKwsQUb/Z//7JwKS8+5llxxRYh7JAUohBDCKslHSCGEEFZJClAIIYRVkgIUQghhlaQAhRBCWCUpQHHPdDodL7/8sun7GTNmsGLFinJ9jHXr1nHmzBnT9xMnTiQmJuae56vX6wkODqZ169YMHDiQ1NTUu5pP//79yc7Ovuc8QojKIwUo7pmrqysrV64kPT29wh7j1gJcunQpjRs3vuf5enp6cuTIEU6ePImnpycffvjhXc1ny5YtODk53XMeIUTlkQIU98zBwYFRo0axaNGi226LiYnhvvvuIzQ0lJ49e3Lx4kUA9u7dS+vWrQkJCeGpp55i6NChQGHRdejQgZCQEAYMGEBqair79+9nw4YNTJkyheDgYBITE+nevTsnTpxg8eLFvPrqq6bHmzVrFvPmzQPgnXfeISwsjMDAQObOnXvH5xEREUF8fDwA169fZ/DgwYSGhhIeHs4vv/xCWloaTZs2NU1/6dIlgoODAWjQoAEZGRkAfPbZZ4SFhREUFMS0adMAePPNN/n4448BGDlyJI899hgACxYs4L333iMjI4P777+ftm3b0rZtW7Zu3Wr28hdC3CUlxD2qVauWSkxMVI0aNVLZ2dlq+vTpavny5Uoppfr27asuXLiglFJq+/btaujQoUoppVq3bq1+/vlnpZRSo0aNUkOGDFFKKZWcnKyMRqNSSqn3339f/fOf/1RKKTV27Fi1ceNG02N269ZNHT9+XF29elW1bt3a9PPAwEAVFxentm7dqiZPnqyMRqMyGAyqR48e6vjx48VmV0opg8GgBg8erDZt2qSUUmrkyJHqwIEDSimlzpw5ozp06KCUUmrAgAFq3759Siml5s6da8oXEBCg0tPT1alTp9SQIUNUfn6+UkqpMWPGqE2bNqldu3apRx99VCmlVOfOnVVkZKRSSqmoqCi1f/9+tWbNGjVy5EillFJGo1GlpaWV9dcghCgjuU6SKBfe3t488MADLFu2zPSzjIwMoqOjefjhhwFQSuHi4kJqair5+fm0a9cOgOHDh/Of//wHgNjYWKKiorh27RrZ2dl07Nix1Mf19fXF29ubEydOYG9vj4uLC35+fsyfP5/NmzcTHR0NQHp6OmfOnKFNmzZF7p+amkpwcDDx8fE0bdqU++67D4Dvv/+ekydPmqZLSUkBICoqitWrV9OxY0fWrl17277O7du3s2/fPkJDQwHIysqiffv2/O1vf+PJJ58kNjaW+vXrk5uby/Xr1zl8+DAhISF4enoydepUnnvuOQYNGkR4eHhZFr8Q4i5IAYpyM2PGDHr37k2/fv0AMBqN+Pr6cuTIkSLT/VEmxZkyZQovvfQSffv2ZdOmTWYdTDNs2DBWr16Nvb09UVFRpseeOXMmY8eOLfW+f+wDzMzMpE+fPixatIgpU6YAcOjQIfT6oi+Rhx9+mDfeeINnnnmG7OxsmjVrVuR2o9HI448/zsyZM297rBo1arBmzRoiIyPJycnhs88+w8/PDzs7O5o1a8aRI0fYtGkT06ZNY9SoUUyePPmOz10IcfdkH6AoN/7+/kRERLB27VoA3N3d8fX1ZePGjQAUFBRw4sQJatSogV6vNxXj6tWrTfO4efMm9erVQynFp59+avq5m5tbiQfZDB48mG+++Ya1a9eaCrBv374sXbqUrKwsAC5evEhaWlqJ2V1cXFiwYAH/+te/MBgM9OjRg8WLF5tuP3r0KAAeHh40a9aM559/3rTf8q969erFV199RVJSEgCJiYlcuXIFKNzHOG/ePCIiIoiMjGTevHlERkYCkJCQgIuLC2PHjmXq1Km3fWgQQpQ/KUBRrp5//nkSEv4cG++LL75g4cKFBAUF0bZtW7Zv3w7Av//9b0aNGkW7du1wcHDA3d0dgJkzZzJw4EDCwsLw9/c3zeeRRx5h9uzZpoNg/srX1xcvLy8cHR3x8/MD4P7772fQoEF06tSJNm3aMHr0aHJyckrNHhoaStu2bfn6669ZuHAhO3fuJCgoiJYtW/LFF1+YpouKimLVqlWmsv2r1q1b89JLL9GrVy8CAwMZMGAAycnJAERGRpKWlkbbtm1p164dycnJREREAHD8+HHCwsIIDg5m/vz5poNnhBAVRy6GLTSRmZmJi4sLAJMnT6ZFixayyU8IUalkDVBoYv369QQHB9OqVSuSkpJMpwUIIURlkTVAIYQQVknWAIUQQlglKUAhhBBWSQpQCCGEVZICFEIIYZWkAIUQQlglKUAhhBBWSQpQCCGEVZICFEIIYZWkAIUQQlglKUAhhBBWSQpQCCGEVZICFEIIYZWkAIUQQlglKUAhhBBWSQpQCCGEVZICFEIIYZWkAIUQQlglKUAhhBBWSQpQCCGEVZICFEIIYZWkAIUQQlglKUAhhBBWSQpQCCGEVZICFEIIYZWkAIUQQlglKUAhhBBWSQpQCCGEVZICFEIIYZWkAIUQQlglKUAhhBBWSQpQCCGEVZICFEIIYZX+H1bhyOE0L7LMAAAAAElFTkSuQmCC</t>
-  </si>
-  <si>
-    <t>https://www.flipkart.com/micromax-x513/p/itmbe37b321587ec?pid=MOBG6XZBFNDXXSHC&amp;lid=LSTMOBG6XZBFNDXXSHC1JYNVJ&amp;marketplace=FLIPKART&amp;q=micromax+keypad&amp;store=tyy%2F4io&amp;srno=s_1_4&amp;otracker=search&amp;iid=22496617-e0d2-4a7c-a8ac-eaf50879265c.MOBG6XZBFNDXXSHC.SEARCH&amp;ssid=hptaldccc00000001688580884943&amp;qH=26e55ddeaa2e42a6</t>
-  </si>
-  <si>
-    <t>Micromax X513+</t>
-  </si>
-  <si>
-    <t>₹1,050</t>
-  </si>
-  <si>
-    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAcAAAAFQCAYAAAAoQ64wAAAAOXRFWHRTb2Z0d2FyZQBNYXRwbG90bGliIHZlcnNpb24zLjYuMSwgaHR0cHM6Ly9tYXRwbG90bGliLm9yZy/av/WaAAAACXBIWXMAAArEAAAKxAFmbYLUAABE/klEQVR4nO3deVxUZf//8dew7yCiKAi47yIqLggGLmmuuaGVlt4td1amfVNbLa1u225/ZW6puWWW5b6k3VG5BLnfCi5Z7gLihuz7Muf3B3eTKOCIA2eY83k+Hj50nDlnPnNg5j3Xda5zXTpFURSEEEIIjbFSuwAhhBBCDRKAQgghNEkCUAghhCZJAAohhNAkCUAhhBCaJAEohBBCkyQAhRBCaJIEoBBCCE2SABRCCKFJEoBCCCE0SQJQCCGEJkkACiGE0CQJQCGEEJokASiEEEKTJACFEEJokgSgEEIITZIAFEIIoUkSgEIIITRJAlAIIYQmSQAKIYTQJAlAIYQQmiQBKIQQQpMkAIUQQmiSBKCFi4iIYPXq1VWyb51OR2JiYpXsuzLi4+Px8PBQuwyz9vXXXzN48OBK329uZs6cydNPP13u/S4uLiQlJVVjRRWryvejuHcSgNWsYcOGODk54eLigo+PD5MmTaK4uLhannvlypX06dPHqMfGx8fj4uKCi4sLzs7O6HQ6w20XF5cqrrRy/P39SUtLU7sMszZmzBi2bdtmuH37l5jb7zc39/qlKysrCx8fnyqsqPpJiJqOBKAKoqKiyMrKIjo6mg0bNrBs2TK1S7qDv78/WVlZZGVlce7cOQDD7aysrCp73qKioirbtzmw9NenJYqioNfr1S5D3AcJQBU1adKE0NBQYmNjDf+3fv162rRpg6enJ0OGDOH69esA3Lhxg/79++Ph4YGXlxePPvooALt376Zp06al9lvWt+Tz588zYcIEdu/ejYuLC23atDHJa9i2bRuNGjXCy8uLDz74wPD/xcXFzJgxg4CAALy9vZkyZUq5H/4RERG89dZbBAcH4+zsTGFhIXv27KFTp054eHgQERFhCOGnn36ad955p9T2jRs3JiYmhosXL2JjY2P4/5SUFB577DHq1q1L48aN+fLLLwE4c+ZMqVZB37596dWrl+G2j48PZ86cKfeY3+7cuXM88MADeHh44OPjwxtvvGG4b+XKlfTs2ZNnn30Wd3d3VqxYUW5dZdHpdMybNw9/f3/q1avHv//9b8N9eXl5vPDCC9SrVw9/f3/effddwwfy/v376dChA25ubvj6+vLpp58a6vmrF6Bv374AtGjRAhcXF6Kjo0vdX9GxBsr9GZVl4cKFNG7cmDp16jB27FjS09OBv39/3333XTw9PWnYsCE//vhjmfsoq16A3NxcIiMjcXV1pWvXrly4cKHU8fvrvbB8+XICAgJwdXWlRYsW7N69+56P+fjx45k4cSK9evXCycmJc+fOER0dTYcOHfDw8CA8PJxTp04ZHn/o0CECAwNxc3NjwoQJpQJz/Pjx/Otf/zLcvr2HZufOnQQHB+Pm5kazZs2Ijo7mvffeIzo6mqeffhoXFxfef//9co+5MIIiqlVAQIASHR2tKIqi/Pnnn0q9evWU2bNnK4qiKAcOHFB8fX2VY8eOKQUFBcq0adOUESNGKIqiKK+++qry3HPPKYWFhUpeXp7y22+/KYqiKLt27VKaNGlS6jkAJSEhQVEURQkPD1e++uorRVEUZcWKFUrv3r1LPfaDDz5QBg4cWGHNV65cUcr6VQGUkSNHKpmZmcrx48cVe3t75ezZs4qiKMrHH3+s9OzZU7l+/bqSmpqqREREKPPmzStz/+Hh4UqTJk2UM2fOKLm5uUp8fLzi5eWl/Prrr0pRUZEyd+5cJTg4WFEURYmKilJat25t2PbAgQNKgwYNFL1er1y4cEGxtrY23DdgwABlypQpSl5ennLq1Cmlfv36SlxcnKIoiuLt7a2cPXtWKSoqUvz8/BRfX1+loKBAOXv2rOLt7V3hMb/d2bNnld27dyuFhYXK6dOnFT8/P2XTpk2GY25tba2sWLFCKS4uVnJyciqsq6xj3LdvXyU9PV05deqUUq9ePeXnn39WFEVR3njjDSU8PFxJSUlRLl26pDRr1kxZsWKFoiiK0rVrV2X16tWKoihKSkqKcuTIEUM9t/4O3Pq7cvv9FR3rin5Gt4uKilLq1aunnDx5UsnKylKGDx+ujBs3TlGUkt9fa2tr5cMPP1QKCwuVxYsXK/7+/mXup6x6Z8yYoTg6Oio7d+5UCgsLlccff1x54okn7nh8VlaW4urqqpw+fVpRFEW5ePGicv78+Xs+5uPGjVNq166tHD58WCksLFSuXr2qeHh4KBs2bFAKCgqUjz/+WGnatKlSWFio5OfnKw0aNFAWLlyoFBQUKHPnzlWsra0N78dx48Yp7733XpnH/ty5c4qrq6uybds2paioSLl06ZJy5swZRVFKv6fF/ZEWoAr69++Pi4sLLVq0oHv37rzwwgtAyTfU559/nnbt2mFra8tbb73Fli1bKCoqwtbWlitXrpCQkIC9vT3du3c3SS2vvfYa33///X1t7+LiQtu2bQkMDOT48eMALFu2jH/961/UqVMHDw8PpkyZwvr168vdz1NPPUXTpk1xcHDg66+/ZtiwYfTo0QNra2tefPFFLl68yMWLF+nVqxc3btzg5MmTAKxdu5bIyEh0Ol2p/V29epXdu3fzwQcfYG9vT8uWLXnsscfYuHEjAD169ODXX3/l6NGjBAYGEhQUxJEjR4iOjiYsLAzA6GPepEkTwsPDsbGxoVmzZowZM8bQSvrr/vHjx2NlZUV6enqFdZXl9ddfx83NjZYtW/LUU0/x3XffAfDtt98yY8YMatWqhb+/P1OmTGHNmjWG2s+ePUtKSgq1atWiQ4cOFf4cy1LRsa7oZ3S7b7/9ln/+85+0bt0aZ2dn3n//fb777jsURQHA2dmZadOmYWNjw9ixY4mPj7+nc7m9e/emZ8+e2NjY8MgjjxAXF1fm43Q6HSdPniQ/P5+AgAAaNWpU7j7LO+YAI0aMoFOnTtjY2BAVFUVgYCDDhw/H1taWKVOmkJOTw6FDh9i3bx82NjY899xz2NraMnHiROrXr2/Ua1qzZg2DBw9m0KBBWFtb4+/vf0dPj7h/EoAq+OGHH8jMzGTz5s0cPnzYcE4tPj6eWbNm4eHhgYeHB35+ftjY2HD16lWmTZuGv78/4eHhtGzZ0mzOG3p7exv+7eTkVOq1/NV96OHhwZgxYwzduWVp0KCB4d/x8fF89dVXhm09PDzIzs7m8uXLWFtbM3LkSMMH6Lp16xg9evQd+4uPjycvL88QwB4eHixevJirV68CJQEYHR1tCLxbb/fo0QPA6GN++fJlhg0bRr169XB3d2fOnDncvHmz3NdWUV1l8fPzK/XvK1euAJCUlIS/v7/hvoCAAMOIx6VLl3Ly5EmaNm1KWFgY+/btK3f/5anoWFf0M7pdWXXm5eWRkpICQJ06dbCyKvkocnJyArin88zl/Q7eytnZmTVr1jB37ly8vb2JjIyscHRoecccSv88b39tVlZW+Pn5kZSUxJUrV0o9VqfTlbpdkcTExAoDWpiGBKBKdDodDz/8MH369DGcB/D19eW9994jLS3N8Cc3N5cGDRrg5ubGZ599Rnx8PCtXruTFF1/k/PnzODs7k5uba9jvtWvXKnzO6uLr68uuXbsMryM9PZ3ff//dqNp8fX155plnSh2HnJwcQkNDARg9ejRr165l//79WFlZ0bVr1zKf38XFhdTUVMM+MjMzWbRoEfB3CzAmJoYePXrQo0cPYmJiiImJMbQAyzvmt5s+fTq1atXi9OnTpKen89JLLxlaN2W9torqKktCQkKpf//VivDx8SE+Pt5wX3x8vOHcZosWLVi7di3Xr1/nkUceKff85d2Ud6zv9jO6VVl1Ojg44OnpWamaKmvAgAHs3LmTxMRE7O3tS52rvV15xxxK/zxvf22KopCQkICPjw/169e/41z8rbcreu/6+fmV2Zq+/fnF/ZEAVNnUqVNZunQpycnJ/OMf/2D+/PmGLpyUlBS2bNkCwPbt2zl//jyKouDu7o5Op8Pa2prmzZuTmprKnj17yM/P57333iv3uerWrUtiYmK1jER88sknmT59OleuXEFRFC5evMiePXuM2vaxxx5j3bp1REdHo9fryczMLNV92qNHDzIzM5k+fTqjRo0qcx++vr6EhIQwffp0cnJyKCoq4siRI4YQbt++PTdu3CA6OprOnTsTHBzMvn37uHLlCkFBQUD5x/x2mZmZuLq64uLiwokTJyocon63usry0UcfkZGRwZ9//sny5csNr3n06NG89957pKamkpCQwCeffMIjjzwClFzPd/PmTWxsbHB1dS2zbij5nSjvgxbKP9Z3+xndavTo0XzxxRecOnWK7Oxs3nzzTUaNGlWpD/K71Vuea9eu8f3335Obm4u9vT1OTk7lHhMo/5jfrn///sTFxRlOVXz66ac4OjoSHBxMSEgIhYWFLFmyhMLCQhYsWFCqJdm+fXu2b99ORkYG58+fL9XD8Oijj7Jt2zZ27NiBXq8nISHBMMiossdA3EkCUGWtWrUiPDyczz77jO7duzN79myeeOIJ3Nzc6NixI7/99hsAp0+fpmfPnri6ujJw4EDmzJlDQEAA7u7ufPbZZ4waNYpGjRrRuXPncp+rV69eNGzYkDp16hAYGAjA+++/T//+/U3+uqZNm0ZISAihoaG4u7szePDgUt+qK9KoUSO+/fZbpk2bhqenJy1btjR8EYCSbqbIyEh27txZ7gcTlIRAYmIijRs3pm7durz00kuGb9xWVlZ0796dli1bYmdnh52dHa1bt6Zbt26GD8byjvnt3n77bXbt2oWbmxuTJk1ixIgRFb6+iuoqy4ABA2jbti0PPPAAkyZNMowUfOutt2jRogUtW7YkJCSERx55hHHjxgGwY8cOWrRogaurK3PnzmXVqlVl7vvtt99mxIgReHh4lDpv+ZfyjvXdfka36tu3L6+//joDBgwgICAAW1tb5syZU+ExKs/d6i2PXq/n448/xtvbm7p163L58uVSIzBvV94xv52XlxebN29mxowZ1K5dm02bNrF582ZsbW2xs7Njw4YNzJs3j9q1a3Ps2LFS55Eff/xxmjRpQoMGDXj00UdLtdIbNWrEhg0bePPNN3F3d6d3796G8HzxxRdZuXIlHh4efPjhh0YfA3EnnXJrX40QwqzodDoSEhKMPnck7p8cc+2QFqAQQghNkgAUQgihSdIFKoQQQpOkBSiEEEKTJACFEEJokgSgEEIITZIAFEIIoUkSgEIIITRJAlAIIYQmSQAKIYTQJAlAIYQQmiQBKIQQQpMkAIUQQmiSBKAQQghNkgAUQgihSRKAQgghNEkCUAghhCbZqF2AEDVRem4h1zPyuJ6Zz7Xb/k7LKSC/UE9BsZ6CopI/+UUltwuL9dhY6XCys8HJzhonO2uc7W1wtC3529XBhnruDvh6OOLj4YivhyPebg5YW+nUfslCWBxZD1CICiSl5XLqSgZ/XM3k3PUszlzP4vyNLLILiqutBhsrHd5uJaHYpK4zrX3caePjRuv6bjjYWldbHUJYGglAIf4nt6CYQxdTOHDhJkcupXHqagZpOYVql1Uuaysdjb2caePjRhsfdwIbuNPBvxZ2NnJmQwhjSAAKzcotKObwpRT2n7/J/vMpHEtMo7C4Zr8dHG2t6dzIkx5NvQhr5kXLeq7odNJ9KkRZJACFplxNz2PH8Sv85+RVjsan1vjAuxsvF3tCm9YmrKkXfVp5U8vZTu2ShDAbEoDC4l1Oy+WH41fYcfwKRxPS0OpvvK21jrCmXgwJ8qFv63o428sYOKFtEoDCIt3Mymfjkct8f/wKxxK1G3rlcbC1ondLb4YE+RDRog72NjKYRmiPBKCwKIcupvDVvkv858RVCor1apdTI7g62DCkvQ9PhDSkRT1XtcsRotpIAIoaLzu/iI1HL/P1/kv8cTVT7XJqtC6NPBkX0pCH2taTaw+FxZMAFDVWQkoOS349z6ajl8nKL1K7HIvi6+HIP0IbMrqzH64OtmqXI0SVkAAUNU5CSg7zd55l49FEix/FqTZXexseDwng2Qea4O4kQSgsiwSgqDEk+NTj5mDDPx9ozJNhjXCyk9GjwjJIAAqzJ8FnPrxc7Hguoilju/nLyFFR40kACrOVW1DMvJ1nWBpzgYIiGdFpTnzcHZjcpxkjO/nJYBlRY0kACrO0/dgVZm3/naT0PLVLERVo6+vGrKHtaO/noXYpQtwzCUBhVs5ez2TG1pP8dvam2qUII1npYGy3AKb1ayEjRkWNoulp421sbAgKCqJt27ZERkaSk5NzT9svWrSI7777DoCVK1dy/fp1w30DBgwgNzfXpPXeq6effppz586pWoOxsvOL+Nf3v9P/s2gJvxpGr8CqfZfo/f/2sC0uSe1yhDCapluAXl5eJCcnAzBmzBg6derEyy+/XKl9RUREMH/+fNq2bWvKEg2Ki4uxtrbMQQeHL6bw8to44lPu7QuIME8PNK/Dvx5ui39tJ7VLEaJCmm4B3qpHjx6cPXuW5ORkBg8eTGBgIBEREVy8eBGAb7/9llatWtG+fXsefvhhAGbOnMn8+fPZtGkThw8fZuTIkQQHBwPQsGFDsrKyePXVV1m+fLnheZ588kk2bdpEcXExU6ZMoXPnzrRv356vv/76jpp2795Nr169GDBgAKGhoWRnZzN+/Hg6d+5Mp06d+Omnn9Dr9TRp0oTs7GwAcnNzCQgIoKioiIiICE6cOAHAjz/+SEhICB06dGDs2LEUFBTwzTff8OabbwLwxhtv0Lt3bwC2bt3KpEmTKC4uZuzYsbRu3Zp27dqxYsUKkx7zwmI9H/3nD0Yt3ifhZ0F+PX2D/p/9yrrDCWqXIkSFJACBoqIifvjhB9q1a8fMmTPp0aMHx44d47nnnmPSpEkAzJo1i61btxIXF8eqVatKbT9s2DCCg4NZv349hw8fLnVfZGQk69atMzzPL7/8Qv/+/Vm2bBn169fn0KFD7N+/n48//pibN+/s+vvvf//L0qVL2b9/P7NmzWLQoEEcOnSIH3/8kRdffBGdTkf//v35/vvvAdixYwd9+/bFxubva7WSk5P597//zc6dOzl69CiNGzfmiy++ICwsjJiYGAAOHTpEdnY2RUVFxMTEEBYWRmxsLBcuXOD333/n+PHjDB8+3GTH/My1TIYu+I3Pd59Dr9k+CMuVXVDMtPXHmLTmKJl55ruosNA2TQdgWloaQUFBBAcHExAQwFNPPUVMTAxjx44FYNSoURw8eBCA0NBQ/vnPf7J06VLupdc4ODiY8+fPk5qayi+//EJoaCgODg5ERUWxdOlSgoKCCAkJIT09nfPnz9+xfWhoKD4+PgBERUXx7rvvEhQURJ8+fcjOzubatWulQnb9+vVERkaW2sf+/fs5duwYISEhBAUFsW7dOi5cuIC/vz/Xrl0jKyuL4uJiQkJCOHr0KL/99huhoaE0btyYpKQkXnjhBaKionB3d6/Ucb6Voigsi7nAoHkxnEzKuO/9CfO2NS6JAXOjORKfqnYpQtxB01M6eHh4EBsbW+Fj/lpN+/PPP2f//v1s27aN4OBgjh8/bvTzDB06lM2bN7N3715DOOn1ehYvXkx4eHiF2zo5/X0eRa/Xs23bNgICAko9pm7dujz55JPcvHmT/fv389VXX5W6X6/XM3DgwDK7MDt27MiSJUvo1KkT3bp145dffiE5ORlfX18Ajh8/zo4dO/j000+Jiopi9uzZRr/u26XnFjL526Ps/vNGpfchap6ElFxGLdrHS32a8XxEU6zkukFhJjTdAixLWFgY33zzDVDSmurSpQsA58+fJyQkhFmzZmFnZ3dHd6WrqyuZmWWvRBAZGcmaNWv4+eef6d+/PwB9+/Zl4cKFFBcXA3DixAnDv8vTt29f5s6da7j9V3hbWVnRv39/XnzxRfr06VOq+xMgJCSEXbt2cenSJQAyMjK4cOGC4fV++umnhIaGEhYWxoIFC+jcuTNQ0nWq1+sZNWoUM2fOvOuXhYqcvV7S5Snhp01FeoXZUacZu+wAqdkFapcjBKDxFmBZZs6cyfjx41m1ahWenp6sXLkSgKlTp3L27FkURWHYsGE0aNCg1Hbjx49n/PjxuLq63nEeMDg4mLNnzxISEoKDgwMAzzzzDBcuXKBDhw7o9Xrq16/PDz/8UGFtb731FpMnTyYwMJCioiI6duzI6tWrgZKQjYiI4Mcff7xjuzp16vDFF18wYsQICgoKsLKyYs6cOTRq1IiwsDASExPp3r07devWxdHRkdDQUAAuX77M+PHj0ev12NjYMGfOnMocUn7+/RovfRcrKzYI9p67ybCFv7FsfGea1HFRuxyhcZq+DEJULUVRmL/zLJ/8fFpWZBeluDnYsHBMJ8KaealditAwCUBRJXIKipi6Lo4dx6+qXYowUzZWOmYMacPj3QLu/mAhqoAEoDC5m1n5/GPlIY4lpqtdiqgBxndvyFuDWsuk2qLaSQAKk0pMzeGJZQc5n5ytdimiBundsi4Lx3aUJZZEtZIAFCZz5lomjy87yNUMWcFB3Lsezbz44olgHGwlBEX1kAAUJnEyKZ3Hlx0kRYa4i/sQ0rg2y8YHy6rzolpIAIr7djQ+lXHLD5KRJ5c5iPvXuWEtVvyjCy72EoKiakkAivsSl5DGmKUH5Bo/YVId/D348skuuMn6gqIKyUwwotLOXs/iHysPSfgJkzsan8aYLw6QIRNpiyokASgqJSktlyeWHZBzfqLKHL+czrOr/ktBkV7tUoSFkgAU9ywlu4DHlx0gKV1Ge4qqte/8Taasi7unFViEMJYEoLgn2flF/GPFQc7dkOv8RPXYFpfErO2n1C5DWCAJQGG0giI9z371X+JkhhdRzZbGXGBZzAW1yxAWRgJQGG3G1hPEnE1WuwyhUf/a/jvfH0tSuwxhQSQAhVHWHIxnzcEEtcsQGqYo8PLaOI7K6vLCRCQAxV0diU9lxpaTapchBAVFeiZ+c1QW1RUmIQEoKnQjM5/nVx+hoFiGogvzcDktl5e+i0Wvl5Gh4v5IAIpyFRbreeHrIzK5tTA7e07fYN7Os2qXIWo4CUBRrlnbT3HwYoraZQhRps9+OU3MGRmUJSpPAlCU6effr7Fy70W1yxCiXHoFJn97lKsyIYOoJAlAcYfU7AJe33Rc7TKEuKub2QW8uOaInA8UlSIBKO4wffMJbmTmq12GEEY5dDFVLpIXlSIBKErZGpfE9uNX1C5DiHsyO+pPzl7PUrsMUcNIAAqD6xl5vL3lhNplCHHP8ov0TFkXJ12h4p5IAAqDVzccIy1H1l8TNVNcQhrLf5OuUGE8CUABwOajl9n15w21yxDivnzy02kSUnLULkPUEBKAguz8Ij74QZabETVfTkExb26WbnxhHAlAwYJdZ7mWIaM+hWX49fQNfv79mtpliBpAAlDj4m/msFSGkAsL88EPpyiS+WvFXUgAaty/tv9OQZF8UAjLcu5GNmsOxqtdhjBzNmoXINQTcyaZKDPuKiq8mciNrR8ZbhelXMZr8DScmocAcGPT+xRlXKf+uDkApPzyBXkXY3Fs3IlaPZ8EIC16NQ7+gTgEBFZ7/UJdc34+w9AOvrg62KpdijBT0gLUqGK9wrvfm/caf7a1G+Dzj3n4/GMe9cZ8jM7WAYeGHQDIvXAUrKwNj9XnZVFw7Rw+Ty0g/8pp9PnZFGXepDDlsoSfRt3MLmDh7nNqlyHMmASgRm2Nu8zpazVn5ozcswdwCGiPlZ0DSnER6fvX4t599N8P0FmBToei6EGnA3Sk712DR+hjqtUs1Lc85gKX03LVLkOYKQlADdLrFebXsLXUsv+IwbllDwAyDm3GpW1vrOwcDfdb2Tvh2LADV1ZMwrFhB4oyroPOGlsvP7VKFmYgv0jP/4v6U+0yhJmSANSgHSeucO5GttplGE2fn0P+5VM4NgmmKDOZvItHcG7b+47HuYeMwufJ+biHjCJ973d4hD5CWsw33Nj0Pjmn96pQuTAHW2OTSEyVi+PFnSQANUZRal7rL+fMfhwbdkBnY0fB9QsUJidwedFTXF39CgU3LnJt3YxSj8+9GIutlz/6/ByKMm7gNfQ1Mg5vVal6obYivcLSaLnUR9xJAlBjfvr9Gn9czVS7jHuS80c0Tq1Kuj+dmnSmwcSvaPDccuqN/Ri7Og3xjnzH8FhFUcg8vAW3LsNQCvNBXwTo0OfVnPOdwvS+O5RAanaB2mUIMyMBqDHzaljrT5+fTf6VMzg26mjU47NP7sKpeQhWtg7Y1m2EUlTAlWUv4NymVxVXKsxZbmExX+67qHYZwszoFEWR9UM0Ys/pG4xbflDtMoRQRS0nW/a+1htHO+u7P1hogrQANeQr+QYsNCw1p5BvD8nsMOJvEoAacSU9V5Y7Epq3LOaCLJorDCQANeLbgwkUyxtfaFxiai57z91UuwxhJiQANaBYr7D2cILaZQhhFuS9IP4iAagBu/64zpX0PLXLEMIs/HjyKum5hWqXIcyABKAGfCPLwghhkF+kZ1tcktplCDMgAWjhrqTnsue0DH4R4lbrpBtUIAFo8bYfuyKDX4S4TVxiOqev1awZkYTpSQBauKiT5rvgrRBq2vDfRLVLECqTALRgyVn5HL6UonYZQpilqN/ly6HWSQBasKiT15DeTyHKdiE5m/M3ZJJ0LZMAtGA/nryqdglCmLWdf1xXuwShIglAC5WRV8g+mfFCiAr9fEq6QbVMAtBC7Tx1nYJivdplCGHWDl9MlYviNUwC0ELt/lO6doS4myK9ItfJapgEoIXad166P4Uwxk7pBtUsCUALdP5GFtcy8tUuQ4ga4cAFuVRIqyQALdD+8/KGFsJYV9LzuJKeq3YZQgUSgBbo0EUJQCHuxZFLaWqXIFQgAWiB/nspVe0ShKhRjsTLe0aLJAAtzI3MfOJTctQuQ4gaRQJQmyQALUxsQpraJQhR45xMyqCgSK6b1RoJQAvz59UMtUsQosYpKNJzIild7TJENZMAtDBnrsvkvkJUxvFECUCtkQC0MGeuSQAKURkXkrPVLkFUMwlAC6LXK5xPlgAUojLOSwBqjgSgBUlIzSGvUE7kC1EZF+TLo+ZIAFoQ6f4UovKS0vJkJKjGSABaEBkAI0TlFesV4lOkG1RLJAAtSEKqXAAvxP24kCzvIS2RALQgyZmyAoQQ9+OiDITRFAlAC5KcJQEoxP24lpGndgmiGkkAWpAbEoBC3Je03EK1SxDVSALQgiRnFqhdghA1WlqOvIe0RALQQmTnF5FbWKx2GULUaKk50gLUEglACyHn/4S4f6nSAtQUCUALkZwlb1wh7le6tAA1RQLQQuRL96cQ9y0ttxBFUdQuQ1QTCUALUaSXN60Q96tYr5CVX6R2GaKaSABaiCK9zGEohCkUy5dJzZAAtBBFxfKmFcIUJAC1QwLQQkgXqBCmIQGoHTZqFyBMQwLQ/Hm72fPOkDZqlyHuws3RVu0SRDWRALQQRcVyDtDc1XNz4KG29dUuQwjxP9IFaiF0OrUrEHcjLQshzIsEoIVwspPGvLlzc5AAFMKcSABaCFcHCUBz5+YoPyMhzIkEoIVwtZfWhbmTFqAQ5kUC0EK4SAvQ7Mk5QCHMiwSghXCxlwA0d27yJUUIsyIBaCHkHKD5kxagEOZFAtBCONhaY2st10KYMzkHKIR5kQC0IHVc7NUuQVRARoEKYV4kAC1IA08ntUsQFXCXLlAhzIoEoAXxqyUBaM6kC1QI8yIBaEH8PB3VLkFUQAbBCGFeJAAtiLQAzZedjRUOttZqlyGEuIUEoAVpUEtagOZKrgEUwvxIAFoQPxkEY7bk/J8Q5ke+llqQem4O2NtYkV8kawOaG9cqOP8XnxHPBwc/4EL6BZPvW5jG0KZDmdB+gtpliHJIAFoQKysdreq7EZuQpnYp4jZV0QXq7+bPZz0/Y8mxJSw/sZxCfaHJn0Pcn8yCTLVLEBWQLlALE9jAXe0SRBmqagSonbUdEztMZN3gdQTVCaqS5xCVZ62TgU/mTALQwrTzlQA0R1V9DrCJRxNW9V/F9K7TcbF1qdLnEsaz0slHrDmTn46FCWzgoXYJogzVMQuMTqdjdMvRbBm6hd7+vav8+cTdOdnKwDRzJgFoYZrWdcFRrjczO9U5D2hdp7rM6TmHORFzqOtYt9qeV9zJw95D7RJEBSQALYy1lY7WPm5qlyFuo8ZlEL0DerNl6BZGtxiNDlkpRA1u9vJeNGcSgBZIBsKYH7WmQXOxc2F6t+ms6r+Kph5NValBy9zt5L1oziQALVDXRp5qlyBuUyUzwax/EjKuGPXQoLpBrB20lheCXsDOys70tYgyudtLAJozCUALFNrUCxsr6fIyJyZvARbkwIkNsKArHFoKinLXTWytbZnQfgLrh6ynk3cn09YjyiQBaN4kAC2Qq4MtHfw91C5D3MLk5wDz0kv+zk+H7VNg+UNw/Q+jNm3k3ogV/VYwM2Qmrnaupq1LlCKDYMybBKCFCm9eR+0SxC1MPgr0rwD8S8J+WNwDdr0PRfl33Vyn0zGi+Qi2Dt1Kv4b9TFubAMDB2gFnW2e1yxAVkAC0UOHNZfi7OamyFuCtigtgz0ewKAwu7TVqN16OXswOn838XvOp51zPtDVqXAPXBmqXIO5CAtBCtfV1o7azDHYwB1WyFmBZAfiX5NOwYgBsnQS5aUbtLtwvnC0Pb2FMqzFmMXtJ8g/JnHnjDGfePEPa3jT0BXou/PsCZ944Q/qhv1/7pc8uUZRVpGKl5QtwC1C7BHEX6v+miyqh0+no0cxL7TIEVTQLTF7aXR6gwJEvYUEXOLnJqF062TrxWpfXWN1/Nc1rNb/vEisrLyGPtP1pNJnZhCYzmnDz55ukH0zHqYkTTWY0IfnHZAAyjmTg3NwZGxfznNPf39Vf7RLEXUgAWrBerbzVLkFQRZdAVNQCvFXWNVg3Hr55BNITjdqkXZ12fDfoOyZ3nIy9tX3la6yk/Cv5ODVxwsrOCis7Kxz8HdBZ60ABpVjBytYKpVghZVcKnn3M95IffzcJQHMnAWjB+rSqK9OimYEquQj+ri3A25z+ARZ0gwOLQX/39SJtrGx4ut3TbByyka71u1auxkqy97Un+49sirOLKc4uJvuPbApTCsm/ls+Fjy7g1d+LlD0peIR6YGVrvh9h0gI0f+b72yPum5OdDb1byWAYtVXJNGjGtgBvVZAJP7wCyx6EayeN2sTfzZ+lfZfyXuh71Tak38HXgdoP1ubCxxeInxePUxMndDY6/J/3p+k7TXFq5kRWXBau7V1JXJZI/Px48pLyqqW2eyEtQPMnAWjhhrT3UbsEzauaFmAlAvAvlw/D4gfg53eg0LjgGNp0KFuGbmFg44GVf9574NnTk6bvNKXRa43QWeuw9/67KzZ5RzJeA7xIP5COc0tn6j1ajxtbb1RLXcZytHHE20lOQZg7CUALF9GiLh5O6sxDKUqoeg6wPPoiiPkEPg+B83uM2sTTwZMPe3zIoj6L8HXxvb/nv4uijJKRnflX8sk5n4NLu5I1DgtTCym4UYBzC2f0+XqUIgWlWEGff/du3erUyrMVOp3MxmTuJAAtnJ2NlbQCVWZ2LcBbpZyHVUNg8/OQk2LUJqG+oWx6eBPjWo+rshXPL312iTNvnCFxSSINnm5QMggGuL7lOnUfLunWd+/qTuqeVOI/i6d239pVUkdltfNqp3YJwgg6RTFiEkFRox1LTGPI/N/ULkOzXn2oJc9FNDHtTpdEQNJR0+7TuQ70+wACI43e5PebvzNz70xOpZwybS013Ozw2TLDTg0gLUANCGzgQct6MuejWqpkMVxTtQBvlX0DNj4Nq0dA6iWjNmlduzVrBq5havBUHG0cTV9TDRXoFah2CcIIEoAaMb57Q7VL0KwqGQVq5AwvlXL2Z1gYAnvngb74rg+3trJmXJtxbHp4E6E+oVVXVw1Rx7EO9V3qq12GMIIEoEYM7eCLl4tMjaaGKpkJJj/D9Pu8VWE2RE2HL3rBlTijNvF18WXRg4v4oMcHeDqY7wXqVU3O/9UcEoAa4WBrzZiuMjehGkw+CCY/q2QUZ3W4EgtLepaEYUGOUZsMajyILQ9vYUiTIVVbm5lqV0cCsKaQANSQx0MCsLeRH3l1M/llEFVx/q8iSnFJd+jCbnD2F6M28XDwYFbYLL7o+wV+rn5VXKB56Vyvs9olCCPJp6GGeLnYMzSoaq/fEncyeQuwugPwL2mXYPVw2PAMZCcbtUm3+t3YOGQjT7V9ChudeU5abUru9u60rd3WqMfqdDqmT59uuD116lRWrlxZqefdvXs3Bw8evOftxo8fz/fff1/m/zdu3Jj27dsTGBjIL78Y98XndosWLeK7776r1LbVQQJQY57q0UjtEjSnWtYCrE7H18L8zhD7jVEPd7Bx4KVOL/HtoG8t/vxYt/rdsLYy7tpIFxcXvv76azIzM+/7eSsKwOLiuw9kKsvcuXOJi4vjk08+YcKECZXax4QJExg9enSltq0OEoAa09zblYgWslp8dXGwtcLO1N3OagcgQG4KbH4OvhxScjG9EVp4tmD1gNW81uU1nGycqrhAddzLKFh7e3vGjBnDwoUL77jv3Llz9OvXj+DgYHr16sXFixcBiIiI4MSJEwCcOHGCiIgIEhISWLRoER9++CFBQUHExsYyfvx4nnvuObp06cKHH37I5s2b6dKlCx06dGDgwIGkpaUZXWdYWBiJiX+vJPLRRx/RuXNnAgMDmT17NgCjR49m586dhsf06tWLo0ePMnPmTObPn1/ua0pKSiI0tOSYRUVF4ejoSEFBAWlpaXTo0AGAOXPm0KJFC9q3b89zzz1ndN3GkADUoKl9WyCzNFUPs5kIu6pc2AMLu0P0J1B894E5VjorxrQaw5ahWwhvEF4NBVYfHTp6NOhxT9tMnjyZJUuWkJdXek7W559/nsWLF3P48GGmT5/OtGnTyt2Hn58fEyZM4LXXXiM2NpagoCAAbt68yYEDB3jzzTcJDw/nwIEDHD16lH79+rFgwQKja9y+fTtDhpQMaIqKiiIxMZGDBw9y9OhRduzYwYkTJ4iMjGTdunUAXL9+naSkJEOAVfSafHx8SE1NJT8/n5iYGFq3bs1///tf9u7dS0hICADvvvsuR44cIS4ujg8//NDouo1h+Z3y4g5tfd0Z2K4+3x+7onYpFs+sp0EzlaJc+OUdOLERhnwGvp3uukk953rM7z2f/1z8Dx8d/IjkXOPOKZqzdl7t8HK8t0Wo69Spw6BBg1i+fLnh/7KysoiOjmbo0KEAKIqCs7PzPdczcuRIw3yk8fHxREZGcu3aNXJzc+na9e5LXE2aNImXX36Z+Ph4fvutZCapqKgotm/fTnR0NACZmZmcPn2aAQMG8Morr1BcXMymTZsYPnx4qX1V9JqCg4M5ePAgBw4cYMqUKcTExJCammpoGXbp0oWxY8cSGRlp2N5UpAWoUVP7tsDWWpqBVc0sJ8KuKteOw9I+8MNrJZdqGOGhhg+xZegWRjQbgY6a/fsY4RdRqe2mTp3KZ599RlFRSQtar9fj7e1NbGwssbGxxMXFsXfvXgBsbGzQ/289x/z8/Ar36+T0dzfzpEmTeOWVVzh+/Dhz5sy567ZQcg7w9OnTfPDBBzzzzDOG2mbMmGGo7dy5cwwfPhwnJyc6d+7Mr7/+yvr164mMLD2dXkWvKSwsjD179pCfn0/fvn3Zu3cvv/32myEAt2/fzsSJE9m3bx/h4abtNZAA1KiGXs6M7qyt4elqMIvFcKuToocDn5dcMnH6R6M2cbNzY2b3mSzvt5yGbg2rtr4q9GDAg5Xazs/Pj9DQUDZs2ACAm5sb3t7ebNu2DSgZxPLXeb+AgABiY2MB2Lhxo2Efrq6uFQ6mycjIwNfXF0VRWLVq1T3V99JLL1FUVERUVBR9+/Zl6dKl5OSUXBN68eJF0tNLvpBFRkby+eefk5iYeEf3Z0WvKSwsjMWLFxMUFISXlxfJyckkJSXRsGFD9Ho9CQkJ9O7dm9mzZxMfH1/pQT1lkQDUsEm9m+FkJyvGV6UqmQXGnAPwL+kJ8M0oWDcesq4btUlwvWA2DNnAs4HPYmNVs87OBNYJpKF7w0pv/+qrr5KUlGS4/c033zBv3jzat29Pu3btDJchvPzyy3z88cd06tSJgoICw+MHDx7MmjVrDINgbjdjxgwGDx5M586d8fO7ty++Op2Ot99+m9mzZ/PQQw8xbNgwunXrRtu2bRk7dqzh/OWAAQPYsWMHw4YNK3M/5b2mVq1akZuba2jxtWrVio4dOwIlQTlmzBgCAwMJDg7m7bffxtradJ9ZshqExs3+8U/m7zqrdhkW6/FuAbw31Ljrwoz23Vg4tc20+6xKDh7w4LvQ8QmMHX11NvUs7+x7h9gbsVVamqm81e0tRrUYpXYZ4h5JC1Djng1vTF1X+7s/UFRKjVkJoirlpcG2SbByECQb92Wraa2mrOq/iuldp+Ni61K19d0nOys7WfqohpIA1DhXB1tmDG6jdhkWy+Ivg7gXl2Lg8+6w52MoLrzrw3U6HaNbjmbzw5vp5derGgqsnHC/cNzt3dUuQ1SCBKBgYGB9+rSqq3YZFkkTl0Hci+J82DULFvWABOOm7vJ29uazXp8xJ2IOdR3N7/f04SYPq12CqCQJQAHAuw+3xVkGxJictADLceMULO8H26dAnnFLO/UO6M2WoVsY3WK02Vwy4engSaivrIFYU0kACgB8PByZ0reF2mVYnKo5B1jFawFWF0UPh5bCgq5w6s4JmcviYufC9G7TWdV/FU3cm1RxgXc3vNnwGjdiVfxNAlAYjO/ekPYN5FyGKZm8BZifWbI8kSXJTILvxsC3YyDDuNmJguoGsW7wOl4IegE7K3UWera1smVMqzGqPLcwDQlAYWBlpeOD4YEyQ4wJmfwcYG6aafdnTv74vqQ1eGgpGHF1lq21LRPaT2D9kPV08r779GumNrDxwHue+kyYFwlAUUprHzemSleoydT4xXCrW356yXnB5Q/B9T+M2qSReyNW9FvBjJAZuNq5VnGBfxvXely1PZeoGhKA4g7/fKAx4c1lySRTMPlMMJYegH9J2A+Le8DOWVB093krdTodI5uPZOvQrdVyTV6obyhNazWt8ucRVUsCUNxBp9Pxyaj2eLvJBfL3w8nOGhtrC1wLsLoUF8CvH8OiMLi016hNvBy9mB0+m/m95lPPuV6VlSatP8sgASjKVNvFnk9HB2ElpwMrTS6BMJHk07BiAGydZPQ50HC/cLY8vIUxrcZgpTPtx1xLz5aE+ISYdJ9CHRKAolzdm3gxsVcztcuosWQaNFNS4MiXsKALnNxk1BZOtk681uU1VvdfTfNazU1WyQtBL5hsX0JdEoCiQpN7N6NrI0+1y6iRpAVYBbKulaww8c0jkJ5o1Cbt6rTju0HfMbnjZOyt769bv2PdjpVe90+YHwlAUSFrKx0LxnTEz9NR7VJqHJkGrQqd/gEWdIP9i+B/C8RWxMbKhqfbPc3GIRvpWv/uq6GX5/86/V+ltxXmRwJQ3JWXiz0rxneumtXNLZimVoNXQ0Em/OdVWPYgXDtp1Cb+bv4s7buU90Lfu+cJrHv59SKoblAlChXmSgJQGKVpXVc+H9tJLpK/B5pbDV4tlw/D4gfg53egMM+oTYY2HcrWoVsZ0GiAUY+31lkzudPk+6lSmCEJQGG00KZezBraTu0yagw5B1iN9EUQ8wl8HgLn9xi1iaeDJx898BGf9/kcXxffCh87tOlQGrs3NkWlwoxIAIp7MqqzH89FqD8JcU1QNaNA00y/T0uSch5WDYHNz0NOilGbhPmGsenhTYxrPQ5r3Z0rojjbOvN80POmrlSYAQlAcc9e6deCwe191C7D7Jl8FhiQFqCxYr+G+Z3h2DqjHu5o48jUzlP5ZuA3tPJsVeq+iUETqetkfusQivsnASjumU6n49NR7enXxlvtUsyadIGqLCcZNj4Nq0dA6iWjNmlduzVrBq5havBUHG0caeXZikdbPlrFhQq16BTFiGnXhShDYbGe578+wk+/X1O7FLP09dNdCW1qwtUCFAXe9SxZR0/cG1tn6Pk6dHserIxb+Ply1mVyC3Nlzk8LJi1AUWm21lYsHNORPq2kJVgW068FmCHhV1mF2RA1Hb7oBVfijNrE18VXws/CSQCK+/JXCPZuKedIbmfyQTDS/Xn/rsTCkp4lYViQo3Y1QmUSgOK+2dlYsXBsR3q2kCWUbmXyFmAVBuCw73Ko9VEGI9eWhEJmvkLQoizDH/cPM5izv2RZopd/zKPd51lMi/r7mru3d+Wx60JRldVnUkox7J0HC7vB2V/UrkaoSAJQmIS9jTWLHu8ko0NvUZNWg5/c1Y5VQ/+e7s7VXkfsBBdiJ7hw9FlnPBx0PNzClrQ8hf9eKeb4cy4cTComPU8hKVPP6Zt6ejaqYTMFpV2C1cNhwzOQnax2NUIFEoDCZOxtrJn7SBATwuU6QWc7a6xNvZZUFbYAIxra4Gpfdr37Eoup56KjUS0rrHVgpQO9omD1v3+/uyefGeE1eO3I42tLLpmI/UbtSkQ1kwAUJqXT6Xitf0tmDWtr+gCoQSxpIuy1J4sY3abk9bja63iwsQ0dFmfzYGMbLqXrsdZBqzrGjaw0W7kpsPk5+HJIycX0QhMkAEWVGNM1gKXjgnG2q+EfjJVkKdcAKorChlOFjGrz9+t5o4c9cRNceKOHPe/9ms/b4fa8szufkWtz2HSqsNprNKkLe2Bhd4j+BIpryDlNUWkSgKLK9GxRl++eDaGuaw3uHqskS5kFJia+mAB3Kxq43flR8cv5ItrWsSY9XyE+Xc/aSEfmHCio9hpNrigXfnmn5CJ6YdEkAEWVauvrzpaJoXTw91C7lGplKavBrz1ZaOj+vJWiKMw5UMCU7nbkFEKBHnRAaq6FzKuhsyq5aF5YNAlAUeXquzuy9tkQxndvqHYp1aamdYH2WZVN5LpcdpwposEnmexLKEKvKGz6o4iRre8M89XHChnW0gYnWx3tva3IK1Jo+3k2T7Svgtethi7/BL8ualchqphMhSaq1ba4JN7YeJzMfMs+vzK+e0NmDmlj2p2ueQz+3G7afYo7eTaGCTFg56x2JaKKSQtQVKvB7X3YPqkH7Rvc22rcNY2sBl9DWdvByBUSfhohASiqnX9tJ9Y/151nH2iMpV4pIavB11B93gGfILWrENVEAlCowtbaitcHtGL9c91p7u2idjkmV9POAQqg+UMQIgNftEQCUKiqo38ttk/qwf/1aY6dteX8OlrKKFDNcPWBhxeqXYWoZpbziSNqLFtrKyb3acaOyWF0CqildjkmYfIWoF4P+Zmm3acoobOCEV+Ac221KxHVTAJQmI2mdV1ZPyGEdx9ug4t9DZtY+TYmPweYnw7IgO0q0WcmNAxTuwqhAglAYVZ0Oh1PhDRk97QInggJwNa6Zo6SMflMMNL9WTU6jIXQyWpXIVQiASjMkpeLPe8+3Jao/wtnQLt6apdzz2rSWoCaFRAGg+aoXYVQkQSgMGuNvJxZOKYTm57vTpdGnmqXYxSdDlxNfR2gBKBp1WoEo78CawuZuUZUigSgqBE6+Ndi7bMhLH0imEAzv4jexc4Gqxq0FqDmOLjDY2vBqWZ8oRJVp2aPNBCa06e1N31ae7P//E2W/HqeXX9ex9wm87OktQAtjrU9jFoFdZqrXYkwAxKAokbq1rg23RrX5uz1TL749QKbYi9TUKRXuyygCro/AXLTTL9PrbGyhVFfQuMItSsRZkK6QEWN1rSuKx+NDOS3V3vxYq+m1DGDtQelBWiGdNYwfAm06K92JcKMSAtQWIQ6rvZM6duCl/o059czN9h45DJRJ6+Sr0KrUKZBMzc6eHgBtB2udiHCzEgACotibaWjZ4u69GxRl4y8QnYcu8LGI5c5dCml2s4VyjRoZmbQJxD0qNpVCDMkASgslpuDLY908eeRLv7E38xhx4kr7PrjOv+9lEqRvurSUFqA5kIH/T+C4CfVLkSYKQlAoQn+tZ2YEN6ECeFNyMgrJOZMMrv+uM7u0ze4kZlv0ucy+SwwIAF4r6xsYehCCByldiXCjEkACs1xc7BlQLv6DGhXH0VROJmUwa9nbhAbn0ZsQhrX7zMQZRCMymydSy51aNZH7UqEmZMAFJqm0+lo6+tOW9+/L66/kp5LXEIasQnpxCWkcfxyOln5RUbvU1aDV5GjJ4xZBw2C1a5E1AASgELcpr67I/XdHXmobX0A9HqFqxl5XLqZQ3xKNpdu5nApJYf4mzlcuplNRl7pcJQWoErc/WDsRrnIXRhNpyjmNo+GEDVLRl4hKVkFpOYUkJZTSFtfd9Nej6gvhndl2q4K+QaXzO3p5qN2JaIGkRagEPfJzcEWNwdbGuJcNU8grb+KdXgcBv4/sFF/EgRRs0gACmHu8tLUrsA8WdvJZQ7ivkgACmHupAV4J5d6JV2efl3UrkTUYBKAQpg7CcDSAsJg5DJwrXkLJQvzIgEohLmTACxhbQ+934JuL4CVzOMv7p8EoBDmTgIQ6rWDYUvAu7XalQgLIgEohLnTcgDqrCF0MkS8DjZ2alcjLIwEoBDmTqsB6NUchswD/25qVyIslASgEOZOa6vB27lA+CvQ7XmwroJZdYT4HwlAIcydllqAbUdA31ngVl/tSoQGSAAKYe60EIB1WsGAf0OjHmpXIjREAlAIc2fJAehaHx6YCh3Hg7V8HInqJb9xQpg7SwxAR08Iewm6/BNsHdWuRmiUBKAQ5s6SAtCpNnR/ETo/A/YualcjNE4CUAhzZwkBWKthSWuv03iwq6JVM4S4RxKAQpiz4iIozFa7ispr3BO6PgvN+sn0ZcLsSAAKYc5qYuvPzgXaP1LS4qvTQu1qhCiXfCUTwpzVlLUAdVbQ6IGSmVte/r1kgdpKhp9Op2P69OmG21OnTmXlypUmKrTE5s2bOX36tOH2008/zblz5+57vzY2NgQFBdGmTRsGDx5MWlpapfYzYMAAcnNz77seUTEJQCHMmbkHoE9H6PcBvHwKxm2Djk+Ag/t97dLFxYWvv/6azMxMExV5p9sDcOnSpTRp0uS+9+vh4UFsbCwnT57Ew8ODBQsWVGo/O3bswNFRRsdWNQlAIcyZuXWBWtmAfwj0mg4vHoF/7oKQ5026Np+9vT1jxoxh4cKFd9x37tw5+vXrR3BwML169eLixYsA7Nu3jzZt2tChQwdeeOEFRo4cCZQEXZcuXejQoQMDBw4kLS2NAwcOsHXrViZNmkRQUBDXr18nIiKCEydO8Pnnn/P2228bnu/dd9/l008/BeCjjz6ic+fOBAYGMnv27Lu+jtDQUBITEwG4ceMGw4cPJzg4mJCQEI4ePUp6ejrNmjUzPP7SpUsEBQUB0LBhQ7KysgD46quv6Ny5M+3bt+fll18G4P333+eLL74A4LHHHuOpp54CYO7cuXzyySdkZWXx0EMP0a5dO9q1a8ePP/5o9PHXEglAIcyZOQSghz90+geMXg2vnIcn/wMPTIPa999iKs/kyZNZsmQJeXl5pf7/+eefZ/HixRw+fJjp06czbdo0AJ555hm++uorQ7D8JTw8nAMHDnD06FH69evHggUL6Nq1K0OGDGHu3LnExsZSt25dw+OHDx/Oxo0bDbc3bNhAZGQkUVFRJCYmcvDgQY4ePcqOHTs4ceJEufUXFxfz008/MWjQIABeeuklXn/9dQ4fPsyqVauYMGEC7u7utGjRggMHDgCwfv16IiMjS+3n1KlTbNmyhX379hEXF0dycjLbt28nLCyMmJgYoCQ4/2rNxsTEEBYWxo8//kjt2rU5fvw4x44dIyQk5J5/Blogg2CEMGfVHYA6a6jTEnw7lHRvNnoAvJrdfTsTq1OnDoMGDWL58uWG/8vKyiI6OpqhQ4cCoCgKzs7OpKWlUVhYSMeOHQEYPXo0X375JQDx8fFERkZy7do1cnNz6dq1a4XP6+3tTZ06dThx4gR2dnY4OzvToEED5syZw/bt24mOjgYgMzOT06dP07Zt21Lbp6WlERQURGJiIs2aNaNfv34A/Pzzz5w8edLwuNTUVAAiIyNZt24dXbt2ZcOGDXec6/zll1/Yv38/wcHBAOTk5NCpUyeeffZZJkyYQHx8PP7+/uTn53Pjxg2OHDlChw4d8PDw4KWXXuKVV15h2LBhEoDlkAAUwpxVZQDaOIJnI6jbGnw7lgRe/UCzuU5v6tSp9OnTh/79+wOg1+vx9vYmNja21OP+CpOyTJo0iTfffJO+ffvy/fffGzWYZtSoUaxbtw47OztDi0yv1zNjxgzGjRtX4bZ/nQPMzs7mwQcfZOHChUyaNAmAw4cPY2NT+iN36NChzJo1i8mTJ5Obm0vz5s1L3a/X63nmmWeYMWPGHc9Vq1Yt1q9fT1hYGHl5eXz11Vc0aNAAW1tbmjdvTmxsLN9//z0vv/wyY8aMYeLEiXd97VojASiEOatsAFrbgWOtv/+41i8JO8/GUOt/f7vWA53OtPWakJ+fH6GhoWzYsIGgoCDc3Nzw9vZm27ZtDB48mOLiYk6dOkXbtm2xsbEhNjaWoKAg1q1bZ9hHRkYGvr6+KIrCqlWrDP/v6upa7iCb4cOH06dPH2xtbdm6dSsAffv2ZdasWURGRuLk5MTFixepVasW7u5lD/hxdnZm7ty5jBgxgueff56ePXvy+eef8+KLLwIQFxdH+/btcXd3p3nz5rz66quG85a36t27N5GRkUycOJHatWtz/fp1iouLqV+/PqGhoXz66ads27aN/Px8Ro4caQjopKQkPD09GTduHA4ODvz000+V+yFYOAlAIcxZ2MvQcRwUZEF+FugLAd3/gut/4fXXv20d/w48C5lm7NVXXzV0ZwJ88803TJgwgenTp1NYWMizzz5L27ZtWbJkCWPGjMHe3p5OnToZWlozZsxg8ODBeHp6Eh4ezqVLlwB45JFHeOaZZ/joo4+Iiooq9Zze3t54eXmRn59PgwYNAHjooYf4/fff6datG3q9Hg8PDzZs2FBuAAIEBwfTrl071q5dy7x585gwYQJLly6loKCAIUOG0L59e6CkG3T8+PH8+eefd+yjTZs2vPnmm/Tu3Ru9Xo+9vT0rV66kfv36hIWFsWjRItq1a4deryclJYXQ0FAAjh8/ztSpU7G2tsbR0ZFly5bdx0/BcukURVHULkIIIe5HdnY2zs4lXbcTJ06kZcuW0uUn7kpGgQoharwtW7YQFBRE69atuXnzpuGyACEqIi1AIYQQmiQtQCGEEJokASiEEEKTJACFEEJokgSgEEIITZIAFEIIoUkSgEIIITRJAlAIIYQmSQAKIYTQJAlAIYQQmiQBKIQQQpMkAIUQQmiSBKAQQghNkgAUQgihSRKAQgghNEkCUAghhCZJAAohhNAkCUAhhBCaJAEohBBCkyQAhRBCaJIEoBBCCE2SABRCCKFJEoBCCCE0SQJQCCGEJkkACiGE0CQJQCGEEJokASiEEEKTJACFEEJokgSgEEIITZIAFEIIoUkSgEIIITRJAlAIIYQmSQAKIYTQJAlAIYQQmiQBKIQQQpMkAIUQQmiSBKAQQghNkgAUQgihSRKAQgghNEkCUAghhCZJAAohhNAkCUAhhBCaJAEohBBCkyQAhRBCaJIEoBBCCE2SABRCCKFJ/x8dvI7zFR0HoAAAAABJRU5ErkJggg==</t>
-  </si>
-  <si>
-    <t>https://www.flipkart.com/micromax-x818/p/itmf4ecd9e0919ca?pid=MOBG6XZBBGUEFGH5&amp;lid=LSTMOBG6XZBBGUEFGH5EDBWBT&amp;marketplace=FLIPKART&amp;q=micromax+keypad&amp;store=tyy%2F4io&amp;srno=s_1_5&amp;otracker=search&amp;iid=22496617-e0d2-4a7c-a8ac-eaf50879265c.MOBG6XZBBGUEFGH5.SEARCH&amp;ssid=hptaldccc00000001688580884943&amp;qH=26e55ddeaa2e42a6</t>
-  </si>
-  <si>
-    <t>Micromax X818</t>
-  </si>
-  <si>
-    <t>₹1,503</t>
-  </si>
-  <si>
-    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAcAAAAFQCAYAAAAoQ64wAAAAOXRFWHRTb2Z0d2FyZQBNYXRwbG90bGliIHZlcnNpb24zLjYuMSwgaHR0cHM6Ly9tYXRwbG90bGliLm9yZy/av/WaAAAACXBIWXMAAArEAAAKxAFmbYLUAABHL0lEQVR4nO3dd3gU5drH8e8mm16BQIA0eicJEEpI6Bq6SAmooGA9ekDkFRALCopdlKYIisoRAWmCgHhEQTR0kY6FThJCTwjpbZ/3jz2uhhKygWR2d+7PdXlJsjsz906y+e0z8xSDUkohhBBC6IyT1gUIIYQQWpAAFEIIoUsSgEIIIXRJAlAIIYQuSQAKIYTQJQlAIYQQuiQBKIQQQpckAIUQQuiSBKAQQghdkgAUQgihSxKAQgghdEkCUAghhC5JAAohhNAlCUAhhBC6JAEohBBClyQAhRBC6JIEoBBCCF2SABRCCKFLEoBCCCF0SQJQCCGELkkACiGE0CUJQCGEELokASiEEEKXJAAdXOfOnfniiy/KZd8Gg4Hk5ORy2XdZJCYm4u/vr3UZNm3hwoX07du3zI/bmsmTJ/PII4/c8HFvb29SUlIqsKKSlef7UVhPArCC1apVC09PT7y9valZsyajR4+mqKioQo49f/587rjjjlI9NzExEW9vb7y9vfHy8sJgMFi+9vb2LudKyyY0NJTLly9rXYZNGzp0KGvWrLF8ffWHmKsftzXWfujKzMykZs2a5VhRxZMQvX0kADWwfv16MjMzSUhIYMWKFXzyySdal3SN0NBQMjMzyczM5NixYwCWrzMzM8vtuIWFheW2b1vg6K9PT5RSmEwmrcsQt0ACUEN169YlJiaGvXv3Wr63fPlymjZtSuXKlbnrrrs4f/48ABcuXKBnz574+/sTEBDAvffeC8CmTZuoV69esf1e71Py8ePHefzxx9m0aRPe3t40bdr0tryGNWvWULt2bQICAnjjjTcs3y8qKmLSpEmEhYURGBjI2LFjb/jHv3Pnzrz44otERUXh5eVFQUEBP/30E61atcLf35/OnTtbQviRRx7h5ZdfLrZ9nTp12Lx5MydPnsRoNFq+n5qayn333Ue1atWoU6cO//nPfwA4cuRIsVZBXFwcXbt2tXxds2ZNjhw5csNzfrVjx47RsWNH/P39qVmzJs8//7zlsfnz59OlSxf+9a9/4efnx2effXbDuq7HYDAwa9YsQkNDqV69Ou+8847lsdzcXEaOHEn16tUJDQ3llVdesfxB3r59Oy1atMDX15egoCCmTZtmqeevqwBxcXEANGzYEG9vbxISEoo9XtK5Bm74M7qe2bNnU6dOHapWrcqwYcNIT08H/v79feWVV6hcuTK1atXiu+++u+4+rlcvQE5ODvHx8fj4+NC2bVtOnDhR7Pz99V749NNPCQsLw8fHh4YNG7Jp0yarz/mIESMYNWoUXbt2xdPTk2PHjpGQkECLFi3w9/enU6dO/P7775bn//LLL4SHh+Pr68vjjz9eLDBHjBjBq6++avn66is0GzduJCoqCl9fX+rXr09CQgJTpkwhISGBRx55BG9vb15//fUbnnNRCkpUqLCwMJWQkKCUUurPP/9U1atXV1OnTlVKKbVjxw4VFBSk9u/fr/Lz89X48ePVwIEDlVJKTZgwQT3xxBOqoKBA5ebmqi1btiillPrxxx9V3bp1ix0DUElJSUoppTp16qQWLFiglFLqs88+U926dSv23DfeeEP17t27xJrPnDmjrverAqhBgwapjIwMdeDAAeXm5qaOHj2qlFLq7bffVl26dFHnz59XaWlpqnPnzmrWrFnX3X+nTp1U3bp11ZEjR1ROTo5KTExUAQEB6ueff1aFhYVq5syZKioqSiml1Pr161WTJk0s2+7YsUMFBwcrk8mkTpw4oZydnS2P9erVS40dO1bl5uaq33//XdWoUUPt27dPKaVUYGCgOnr0qCosLFQhISEqKChI5efnq6NHj6rAwMASz/nVjh49qjZt2qQKCgrU4cOHVUhIiFq5cqXlnDs7O6vPPvtMFRUVqezs7BLrut45jouLU+np6er3339X1atXVz/88INSSqnnn39ederUSaWmpqpTp06p+vXrq88++0wppVTbtm3VF198oZRSKjU1Ve3evdtSzz9/B/75u3L14yWd65J+Rldbv369ql69ujp06JDKzMxUAwYMUMOHD1dKmX9/nZ2d1ZtvvqkKCgrU3LlzVWho6HX3c716J02apDw8PNTGjRtVQUGBuv/++9UDDzxwzfMzMzOVj4+POnz4sFJKqZMnT6rjx49bfc6HDx+uqlSponbt2qUKCgrU2bNnlb+/v1qxYoXKz89Xb7/9tqpXr54qKChQeXl5Kjg4WM2ePVvl5+ermTNnKmdnZ8v7cfjw4WrKlCnXPffHjh1TPj4+as2aNaqwsFCdOnVKHTlyRClV/D0tbo20ADXQs2dPvL29adiwIe3bt2fkyJGA+RPqv//9b5o3b46LiwsvvvgiX3/9NYWFhbi4uHDmzBmSkpJwc3Ojffv2t6WWZ599lrVr197S9t7e3jRr1ozw8HAOHDgAwCeffMKrr75K1apV8ff3Z+zYsSxfvvyG+3n44YepV68e7u7uLFy4kP79+9OhQwecnZ158sknOXnyJCdPnqRr165cuHCBQ4cOAbB06VLi4+MxGAzF9nf27Fk2bdrEG2+8gZubG40aNeK+++7jq6++AqBDhw78/PPP7Nmzh/DwcCIjI9m9ezcJCQnExsYClPqc161bl06dOmE0Gqlfvz5Dhw61tJL+enzEiBE4OTmRnp5eYl3X89xzz+Hr60ujRo14+OGHWbJkCQBffvklkyZNolKlSoSGhjJ27FgWL15sqf3o0aOkpqZSqVIlWrRoUeLP8XpKOtcl/Yyu9uWXX/LYY4/RpEkTvLy8eP3111myZAlKKQC8vLwYP348RqORYcOGkZiYaNW93G7dutGlSxeMRiP33HMP+/btu+7zDAYDhw4dIi8vj7CwMGrXrn3Dfd7onAMMHDiQVq1aYTQaWb9+PeHh4QwYMAAXFxfGjh1LdnY2v/zyC9u2bcNoNPLEE0/g4uLCqFGjqFGjRqle0+LFi+nbty99+vTB2dmZ0NDQa670iFsnAaiBb7/9loyMDFatWsWuXbss99QSExN57bXX8Pf3x9/fn5CQEIxGI2fPnmX8+PGEhobSqVMnGjVqZDP3DQMDAy3/9vT0LPZa/rp86O/vz9ChQy2Xc68nODjY8u/ExEQWLFhg2dbf35+srCxOnz6Ns7MzgwYNsvwBXbZsGUOGDLlmf4mJieTm5loC2N/fn7lz53L27FnAHIAJCQmWwPvn1x06dAAo9Tk/ffo0/fv3p3r16vj5+TF9+nQuXbp0w9dWUl3XExISUuzfZ86cASAlJYXQ0FDLY2FhYZYej/PmzePQoUPUq1eP2NhYtm3bdsP930hJ57qkn9HVrldnbm4uqampAFStWhUnJ/OfIk9PTwCr7jPf6Hfwn7y8vFi8eDEzZ84kMDCQ+Pj4EnuH3uicQ/Gf59WvzcnJiZCQEFJSUjhz5kyx5xoMhmJflyQ5ObnEgBa3hwSgRgwGA/369eOOO+6w3AcICgpiypQpXL582fJfTk4OwcHB+Pr6MmPGDBITE5k/fz5PPvkkx48fx8vLi5ycHMt+z507V+IxK0pQUBA//vij5XWkp6fz22+/laq2oKAgHn300WLnITs7m5iYGACGDBnC0qVL2b59O05OTrRt2/a6x/f29iYtLc2yj4yMDObMmQP83QLcvHkzHTp0oEOHDmzevJnNmzdbWoA3OudXmzhxIpUqVeLw4cOkp6czZswYS+vmeq+tpLquJykpqdi//2pF1KxZk8TERMtjiYmJlnubDRs2ZOnSpZw/f5577rnnhvcvb+ZG5/pmP6N/ul6d7u7uVK5cuUw1lVWvXr3YuHEjycnJuLm5FbtXe7UbnXMo/vO8+rUppUhKSqJmzZrUqFHjmnvx//y6pPduSEjIdVvTVx9f3BoJQI2NGzeOefPmcfHiRR588EHef/99yyWc1NRUvv76awC++eYbjh8/jlIKPz8/DAYDzs7ONGjQgLS0NH766Sfy8vKYMmXKDY9VrVo1kpOTK6Qn4kMPPcTEiRM5c+YMSilOnjzJTz/9VKpt77vvPpYtW0ZCQgImk4mMjIxil087dOhARkYGEydOZPDgwdfdR1BQENHR0UycOJHs7GwKCwvZvXu3JYQjIiK4cOECCQkJtG7dmqioKLZt28aZM2eIjIwEbnzOr5aRkYGPjw/e3t4cPHiwxC7qN6vret566y2uXLnCn3/+yaeffmp5zUOGDGHKlCmkpaWRlJTEe++9xz333AOYx/NdunQJo9GIj4/PdesG8+/Ejf7Qwo3P9c1+Rv80ZMgQPv74Y37//XeysrJ44YUXGDx4cJn+kN+s3hs5d+4ca9euJScnBzc3Nzw9PW94TuDG5/xqPXv2ZN++fZZbFdOmTcPDw4OoqCiio6MpKCjgo48+oqCggA8++KBYSzIiIoJvvvmGK1eucPz48WJXGO69917WrFnDunXrMJlMJCUlWToZlfUciGtJAGqscePGdOrUiRkzZtC+fXumTp3KAw88gK+vLy1btmTLli0AHD58mC5duuDj40Pv3r2ZPn06YWFh+Pn5MWPGDAYPHkzt2rVp3br1DY/VtWtXatWqRdWqVQkPDwfg9ddfp2fPnrf9dY0fP57o6GhiYmLw8/Ojb9++xT5Vl6R27dp8+eWXjB8/nsqVK9OoUSPLBwEwX2aKj49n48aNN/zDBOYQSE5Opk6dOlSrVo0xY8ZYPnE7OTnRvn17GjVqhKurK66urjRp0oR27dpZ/jDe6Jxf7aWXXuLHH3/E19eX0aNHM3DgwBJfX0l1XU+vXr1o1qwZHTt2ZPTo0Zaegi+++CINGzakUaNGREdHc8899zB8+HAA1q1bR8OGDfHx8WHmzJl8/vnn1933Sy+9xMCBA/H39y923/IvNzrXN/sZ/VNcXBzPPfccvXr1IiwsDBcXF6ZPn17iObqRm9V7IyaTibfffpvAwECqVavG6dOni/XAvNqNzvnVAgICWLVqFZMmTaJKlSqsXLmSVatW4eLigqurKytWrGDWrFlUqVKF/fv3F7uPfP/991O3bl2Cg4O59957i7XSa9euzYoVK3jhhRfw8/OjW7dulvB88sknmT9/Pv7+/rz55pulPgfiWgb1z2s1QgibYjAYSEpKKvW9I3Hr5Jzrh7QAhRBC6JIEoBBCCF2SS6BCCCF0SVqAQgghdEkCUAghhC5JAAohhNAlCUAhhBC6JAEohBBClyQAhRBC6JIEoBBCCF2SABRCCKFLEoBCCCF0SQJQCCGELkkACiGE0CUJQI0YjUYiIyNp1qwZ8fHxZGdnW7X9nDlzWLJkCQDz58/n/Pnzlsd69epV4vpyFeGRRx6xLOAphBC2SCbD1khAQAAXL14EYOjQobRq1Yqnn366TPvq3Lkz77//Ps2aNbudJVoUFRWVuHq2EELYI2kB2oAOHTpw9OhRLl68SN++fQkPD6dz586cPHkSgC+//JLGjRsTERFBv379AJg8eTLvv/8+K1euZNeuXQwaNIioqCgAatWqRWZmJhMmTODTTz+1HOehhx5i5cqVFBUVMXbsWFq3bk1ERAQLFy68pqZNmzbRtWtXevXqRUxMDFlZWYwYMYLWrVvTqlUrvv/+e0wmE3Xr1iUrKwuAnJwcwsLCKCwspHPnzhw8eBCA7777jujoaFq0aMGwYcPIz89n0aJFvPDCCwA8//zzdOvWDYDVq1czevRoioqKGDZsGE2aNKF58+Z89tln5XPyhRC6ZdS6AL0rLCzk22+/pUePHkyePJkOHTqwZs0alixZwujRo1m9ejWvvfYaq1evpn79+qSnpxfbvn///kRFRV23BRgfH8+LL77IQw89RGFhIRs2bGD27Nl88skn1KhRg19++YWcnBzatWtHjx49qFKlSrHtf/31V37//Xdq1qzJ888/T58+fZg/fz4XL14kNjaW33//nZ49e7J27VqGDBnCunXriIuLw2j8+9fq4sWLvPPOO2zcuBEPDw9eeuklPv74Y/r27cvcuXMB+OWXX8jKyqKwsJDNmzcTGxvL3r17OXHiBL/99hvANa/blpxNz+X05WwuZORzMTPP8t+lzHwuZeWTW1BEfqGJ/CITBUUm8gtNFBQplFK4ODvh5uKEm9EZT1dnvFyNeLkZCfB2JdDXnUBfd6r7uVn+XcXLFYPBoPVLFsIhSABq5PLly0RGRgLQsWNHHn74Ydq0acO6desAGDx4ME899RQAMTExPPbYYwwdOpRBgwaV+hhRUVEcP36ctLQ0du7cSUxMDO7u7qxfv56DBw/yxRdfAOZwOX78+DUBGBMTQ82aNQFYv349a9eu5dVXXwUgKyuLc+fOER8fz6xZsxgyZAjLly/nwQcfLLaP7du3s3//fqKjowHIy8ujd+/ehIaGcu7cOTIzMykqKiI6Opo9e/awZcsWnnrqKTw9PUlJSWHkyJH069ePuLg4K8/w7VVkUhw5n8GRc5kcv5DFsQuZHL+YyYkLWWTlF1VYHe4uTtSt6k2DQB/qB3rToJoPDQJ9CKnsIcEohJUkADXi7+/P3r17S3zOX3/QPvzwQ7Zv386aNWuIioriwIEDpT7O3XffzapVq9i6dSvx8fEAmEwm5s6dS6dOnUrc1tPT0/Jvk8nEmjVrCAsLK/acatWq8dBDD3Hp0iW2b9/OggULij1uMpno3bv3dS9htmzZko8++ohWrVrRrl07NmzYwMWLFwkKCgLgwIEDrFu3jmnTprF+/XqmTp1a6td9qy5m5rH7VBp7ki6zJzGNA8npFRp0N5JbYOJQyhUOpVwp9n1PV2eaBfnRulYlompVplVYJXzdXTSqUgj7IAFoQ2JjY1m0aBHjxo1j+fLltGnTBoDjx48THR1Nu3btWLVqFZcuXSq2nY+PDxkZGdfdZ3x8PM8//zxHjhxh1qxZAMTFxTF79mxiY2Nxdnbm4MGDNG7cuMSOLnFxccycOZN3330XgL179xIZGYmTkxM9e/bkySef5I477ih2+RMgOjqa0aNHc+rUKcLCwrhy5QqXLl2idu3axMbG8sYbbzBr1iyio6MZM2aMJZQvXryIq6srgwcPJiwszHK/sLxk5hWy+cgFNv15ga3HLpGYal2vXK1l5xex80QqO0+kAsdwMkCDQB9a16pM+7pV6NCgKt5u8nYX4p/kHWFDJk+ezIgRI/j888+pXLky8+fPB2DcuHEcPXoUpRT9+/cnODi42HYjRoxgxIgR+Pj4sGvXrmKPRUVFcfToUaKjo3F3dwfg0Ucf5cSJE7Ro0QKTyUSNGjX49ttvS6ztxRdf5KmnniI8PJzCwkJatmxpuYQaHx9P586d+e67767ZrmrVqnz88ccMHDiQ/Px8nJycmD59uiUAk5OTad++PdWqVcPDw4OYmBgATp8+zYgRIzCZTBiNRqZPn16WU1qiw+cy+PGP82z68wK7TqVSUOQ4HaJNCv44m8EfZzNYsP0Urs5OtK1TmTubBNKtcSBB/h5alyiE5mQYhNCV4xcyWbU3hdV7T3Pykn218m6nxjV8iWsSSP8WQdQK8NK6HCE0IQEoHN6FjDzW7Evh672n2Zdsu71JtRIVVolBrYLpHV4DH7lvKHREAlA4JKUUPx2+wOfbTvHT4QsUmeTX/GY8XJzp3jSQQa1CiKlXRXqVCocnASgcSlZeISt2J/OfrSc5diFL63LsVv1q3jzSoTZ3twjCzSizAAnHJAEoHEJSajbzt55k6a4kMnILtS7HYQR4u/FAdBj3twujkper1uUIcVtJAAq7dvJiFrM2HuXrvacplMuc5cbdxYlBrYL5d+d61JQepMJBSAAKu5SUms30H46wau9pub9XgVyNTtzfLoyRXepRWVqEws5JAAq7cj4jl5kbjrDklySHGrdnb7zdjDwcW5tHO9aRAfbCbkkACrtQUGTik80nmLXhiE1MSSbMKnu5MrJLPYZHh2F0lsVlhH2RABQ27+fDF5i85hDHpVenzapfzZuX+zWlfd0ArUsRotQkAIXNSkrNZsra31j/2zmtSxGldFdETV7s04SqPm5alyLETUkACptjMinmbT7Oe98fJrfApHU5wkp+Hi4827MR97QOkcH0wqZJAAqbcupSFuOW7eOXk2lalyJuUfu6VXh3cAQ1/GTYhLBNEoDCZizYfoo31v1OtnRycRh+Hi681r8ZfcJral2KENeQABSaO5ueyzMr9vPz4QtalyLKyYAWQbzcr6lMti1sigSg0FTCkQuMXryHtOwCrUsR5Sy4kgfThkTSulZlrUsRApAAFBpRSvHBj0d57/vDyEQu+mF0MvB8r8Y8FFtb61KEkAAUFe9KbgFPL9nHD7/L8Aa9GtgymNf6N8PdRVaaENqRABQV6o+zV3h8wa+6Xo1dmEUE+zHn/lbSS1RoRgJQVJgf/zzPyIW7pZensAjwduPDYS3lvqDQhASgqBBLdyXx/FcHZMkicQ1XZyemDYmkd3gNrUsROiMBKMrdjB+OMO2Hw1qXIWyYkwFe7teM+9uFaV2K0BEJQFFuikyKiasOsHhnktalCDvxVLf6/N+dDbQuQ+iEBKAoF/mFJkYu2s33MpG1sNID0WFM7tsUJyeZR1SULwlAcdsVFJl44ovdMsxBlFm/yJq8NzgSZwlBUY5kBUtxWxUUmRi5UMJP3Jqv96bwzPL9yOdzUZ4kAMVtU1hk4slFe2T9PnFbrNidzMRVB7UuQzgwCUBxWxQWmRj95R7+e+is1qUIB7JwRyJT1v6mdRnCQUkAitvi2a8OsO6AhJ+4/T7ZfIKp3/2pdRnCAUkAils244cjLP81WesyhAN7/8ejfLL5hNZlCAcjAShuyYpfk2WQu6gQr33zGxukc5W4jSQARZltPXqRZ7/ar3UZQidMCkYv3sPvZ65oXYpwEBKAokz+PJvBv774lYIi6aYuKk5WfhEPz/+F8xm5WpciHIAEoLBaek4Bj36+i4zcQq1LETqUkp7Lo5//Sm6BrCoibo0EoLDauGX7SEyV9fyEdvYlXea5rw5oXYawcxKAwipzfzom83sKm7Byz2mW7pKJ1kXZSQCKUtt5IpV3ZDyWsCGTvj7E0fMZWpch7JQEoCiVCxl5jFq0Wxa0FTYlp6CIkQv3yP1AUSayGoS4KaUUD3y6k4QjF7UupUwKLp/l0rczMGVdBoMT1e9/l/PLJ1OUdRmD0QWA6sOm4uTiRuqGj8k9uRePOq2o1OUhAC4nfIF7aDjuYeEavgpRkntah/DmQPn5COsYtS5A2L4vtp+y2/ADuLRuOv4dhuEe0oyinAxL6FW9+1lcq9ayPM+Um0n+uWPUfPgDzi56FlNeFqb8XApST+PfYZhG1YvS+PKXJDrUr0rv8BpalyLsiFwCFSU6eTGL19f9oXUZZZZ/4RQGJ2fcQ5oB4Ozhg8HJ+fpPNjiBwYBSJjAYAAPpWxfjH3NfxRUsyuylrw+SlpWvdRnCjkgAihtSSvHM8v3k2PH9lcK0FAyuHpxf/jJn5j9F+rallscurplKymejubJzJQBObp541GrBmc9G41GrBYVXzoPBGZeAEK3KF1a4lJXPy2sOaV2GsCNyD1Dc0OfbTvLS1/b9ByXrj82kfvcBNR6cibOnP+eWvYRfu8G4BIRg9AnAlJfF+RVT8G07EM+6rYtte+Hrt6h8x2Nk7PmWggsn8WraGc8G7TV6JaK0PhvRmi6NqmldhrAD0gIU13X6cg5vfWu/lz7/YvSpgmv1ehh9q2IwuuBRJ4r888cx+gQA4OTmhVejWPLPFJ/QO+fkXlwCQjHlZVN45QIBdz/LlV2rtXgJwkovrDxAZp7MUiRuTgJQXNera38jK99+L33+xbVGA4qy0ynKzUQpE3lJB3GpEkJRdjoAqqiAnOO/4hIQZtlGKUXGrq/xbdMfVZAHpkLAgCk3U6NXIayRkp7rEB/eRPmTXqDiGtuOXeLbg46xuK3ByZlKHR/g3MIJgMK9VgvcQ8M5t2gCylQEJhMe9drg2TDGsk3WoR/xbBCNk4s7LtVqowrzOfPJSLya36HdCxFW+WLHKeKjggkP9te6FGHD5B6gKKbIpOgza7MsOSPsXlRYJZY/IfdsxY3JJVBRzOKdiRJ+wiHsOpXG6n0pWpchbJgEoLBIzy7gve9ldXfhON7+7x/kFdr/vWxRPiQAhcWsjUdIlYHEwoEkp+Xw+dZTWpchbJQEoADgfEYuC7bLHwrheN7/8Sjp2QValyFskASgAGDOpuPkFZq0LkOI2y49p4DPtp7QugxhgyQABeczclm0U1p/wnHN33qSLBkcL64iASj46Kfj5BZI6084rsvZBSzcIR/yRHESgDp3ISOPhTsStS5DiHL3ccIJ6REqipEA1LlPNp+w69UehCitCxl5LN2VrHUZwoZIAOpYbkERS36R1p/Qj7k/HaOwSC73CzMJQB1bvS+FNOkeLnQkOS2HDX+c17oMYSMkAHVswTbpFCD0Z5Hc8xb/IwGoU7sT0zhwOl3rMoSocAlHLpCUmq11GcIGSADqlLT+hF6ZFHwp974FEoC6dDk7n28OnNG6DCE0s2xXsnSGERKAerTuwFnyZdozoWPnM/L44fdzWpchNCYBqEOr953WugQhNLdyj7wP9E4CUGfOXcll54lUrcsQQnOb/rwg84PqnASgzqzZl4JJaV2FENrLKzSxUcYE6poEoM6s2S+dX4T4yzrpDKZrEoA6kpSazb6ky1qXIYTN2PTnBXLyZS5cvZIA1JEf/5TLPUL8U05BkVwG1TEJQB35+fAFrUsQwuZskOEQuiUBqBMFRSa2HbukdRlC2Jwtxy5qXYLQiASgTuw6mUaW3OsQ4hrnruRx9Hym1mUIDUgA6sTPR+TypxA3slVagbokAagTCRKAQtzQlqMSgHokAagDGbkF/JZyResyhLBZ24+nYpIZInRHAlAHDpxOl9lfhChBek4Bv52RD4l6IwGoA/uSZOFbIW5GFojWHwlAHZDZX4S4uYMSgLojAagD+5Mva12CEDbvkNwn1x0JQAd3PiOXlPRcrcsQwub9cfYKRXKzXFckAB3codPyqVaI0sgtMMmAeJ2RAHRwxy7IG1qI0jqUIvcB9UQC0MGdvJSldQlC2A35wKgvEoAO7uTFbK1LEMJuJKXmaF2CqEASgA5OWoBClF5Smnxg1BMJQAeWV1hEymX5RCtEaUkLUF8kAB1YUmqOTIEmhBUuZuaRI8uG6YYEoAOT1p8Q1kuWy6C6IQHowC5m5mldghB2J1k+OOqGBKADkwAUwnrp2QValyAqiASgA7uUla91CULYnfQcCUC9kAB0YPJJVgjrXZEA1A0JQAd2WQJQCKtdyZX3jV5IADqwjDx5IwthLbkEqh8SgA4sv9CkdQlC2J0rOYValyAqiASgAyuUUfBCWC2nQAbC64UEoAMzSQAKYTWTkveNXkgAOjBpAQphPVkVXj+MWhcgyo+8kW3Xk13rEVrZU+syxHVU83XXugRRQSQAHZi0AG3TgBZBjI1rqHUZQuieXAJ1YM4Gg9YliKvUDvBiyt3NtC5DCIEEoEPzcHXWugTxDy7OBmbe0wIvN7nwIoQtkAB0YN7yh9amjO/ekObBflqXIYT4HwlAB+blJi1AW9GxQVUe7VBH6zKEEP8gAejAvFylBWgLArzdeDc+AoPckxXCpkgAOjC516Q9gwHeHRxBVR83rUsRQlxFAtCBebtLAGrtkdjadGpQVesyhBDXIQHowKp6S6tDS+HBfjzTo5HWZQghbkAC0IHV9JcZLbTi5erMzHta4OIsbzEhbJW8Ox1YDT8PrUvQrVf6NaNWgJfWZQghSiAB6MBqSAtQE/1bBDGwVbDWZQghbkIC0IFV9XbDVS7BVaiwKp4y1ZkQdkL+Ojowg8FAoJ90hKkof011JjPwCGEfJAAdXEglWXKnooyNa0hEiL/WZQghSkkC0ME1rO6jdQm60KF+AP/qKFOdCWFPJAAdXOPqvlqX4PACvF15d7BMdSaEvZEAdHDSAixfBgO8Ex9BNR/pcSuEvZEAdHANq/vgJA2TcvNQTG26NKymdRlCiDKQ7moOzt3FmVpVvDh+MUvrUhxOsyBfJlTwVGcFpgI+OfAJyRnJFXpcUTqT2k/CxclF6zJEKRmUUkrrIkT5+vfCX1l34KzWZTgUL1dn1o7uQG0NZnvJzM/klW2v8O3Jbyv82KJku4ftxsVZAtBeyCVQHWgZWknrEhzO5LuaahJ+AN6u3rzd6W1eaf8KHkaZ7s6WODvJItT2RAJQB9rVqaJ1CQ6lX2RN4qNCtC6D/vX7s7TPUhpXbqx1KeJ/nAzyJ9WeyE9LB5rU8MVH1ga8LUIre/KqDU11VsuvFgt7LWRY42EYkN5OWpJ7f/ZHAlAHnJwMRIXJZdBb5eJsYOa9LfBxt60/dC7OLkxoM4H3u71PZffKWpejW35uflqXIKwkAagTbeUy6C37vzsbEGnDU511DO7IirtW0K5GO61L0SV/N3+tSxBWkgDUiba1pWVwK2LrBfBEp7pal3FTAR4BfHTnR4xpOQajk1z2rkiV3OUqi72RANSJ5kF++Hva1qU7e1HFy5X37GiqM4PBwMPNH+bzHp8T7C3rElYUaQHaHwlAnTA6O9FVZiyxmsEAU+MjqOar0VRnuVfgk+5w/CerN21etTnL+i6jV+1e5VCYuJrcf7U/EoA6Etc0UOsS7M6I9rXo0kjDDw5rx0DSdlhwN/zwMhQVWrW5t6s3b3V8i1djXsXTKEtjlSdpAdofCUAd6dSgGu4u8iMvraY1fXmup4Zj7PZ8AQdXmP+tTLD5Pfi0O6SdtHpX/er1Y2lfGTNYnuQeoP2Rv4Y64uHqTGy9qlqXYRc8XZ2ZeW8LXI0avUUuHoV1z1z7/dO7YE4HOLDc6l2G+YaxsNdCHmjygIwZLAdV3KWntb2RANQZuQxaOpP7NqVuVW9tDl6YD8sfhIIbTGCedwVWPAyrRkK+dZOcuzi7ML71eGbfMVvuWd1mob6hWpcgrCQBqDN3Ng7ExVk+/Zekb0RNBrfWcKqzHybB2f03f97eL2BuRzizz+pDxAbFsuKuFbSv2b4MBYqrGTBQ26+21mUIK0kA6kwlL1fuaCytwBsJqezBa/01nOrs8HrY/mHpn3/pKMy7A7bNtvpQAR4BzLljDk+3errCxwyemnmK3/79G4nvJ1q+l308myPPH+HwM4c5//V5AJRSJM1O4sgLR7j0/SXLc5M/SSbvbF6F1lySGl41ZGJyOyQBqEODbWAiZ1tkdDIw454W+Go11VnGOVj1BGDlCmVF+fDdc7AwHrIuWrWpwWDgwWYP8kXPLwj1qbhLeFXurELwo8XHKJ5ZcIaQJ0Ko/2Z9MvZlkJuUS25SLgajgXqv1iMtIQ2AnFM5OLs741bdrcLqvRlp/dknCUAd6tigKtW1Gtdmw/7vzgbaLR2lFKx8DLKtC7BijqyHD9vDsR+t3rRpQFOW9l1Knzp9yn58K3g39sbJ/e8/PwVpBagihXuIOwYnA35t/cjYl4HB2YBSCorAYDRfur+w+gJV77KtzlwSgPZJAlCHnJ0MDGolM4T8U/u6VbSd6mzLdDi+6db3k3kOFvSH71+CogKrNvVy8eKNDm/weuzreLlU7FqHhZcLcan0d8vbpZILBWkFuAe54+zpzLGXj1G5S2Uy9mfgUdsDo49tTfMmAWifJAB1anBUCHYys1e5q+zlyrQhkTg5aXRCkn+Fja/dxh0q2DLDPGYw9YTVW/et25elfZbStErT21hT2dW8vyb1ptTDP8afSz9cosqdVUj5IoXEWYlkHbauF2x5qeNXR+sSRBlIAOpUaBVPomWFCADeGRROoJZTna14CEzWtdZK5fSv5l6i+5dZvWmobygLei1gRNMRFTJm0OhvpCDt73NQkFaA0b94Ky8tIQ2/tn5kHcnC6GMk+LFgLqy+UO61lUZdf9ufKF1cSwJQxx6Mkcs2I9rXopuWvWK/ebpMM7uUWt4V+OoRWPk45GVatamLkwtjo8Yy54455T7I26WSCzhBblIuyqRI35GOb6Sv5XFTnomM3Rn4t/dH5SlUobmjUFF2UbnWVRq1fGvJLDB2SgJQx+5oXI06ARV7r8eWNK7hy3O9GmlXwN5FcMD61lmZ7Ftsbg2m7LV60/ZB7Vlx1wpigmJuWzkn3j5B0uwkMvZn8Mf//UH20WxqDqtJ0odJHJ5wGO/m3riH/N0qv/jfi1TpXgWDwYB3c2+yj2Zz7OVjVInT/ipGq8BWWpcgysiglLKyz7VwJAt3nOKFlQe1LqPCebg4s+bJWOpV02i2l0vHzIGUb12r7JY5u0K3lyB6FNbeBFZK8flvnzNj9wwKyuOSrZ16LfY17qp7l9ZliDKQFqDODWwZTFUf2xlPVVEm9W2iXfj9NdVZRYcfmMcMrp8ICwdBpnX3zwwGA8ObDmdBrwWE+YaVU4H2p2W1llqXIMpIAlDn3F2ceThWX/cCe4fX4J42Gs7buOHlMk1fdlsd/cE8ZvDoBqs3bVqlKUv7LJVWDxDoGUiwjwwpslcSgIJh7cJ0s1p8cCUP3hjQXLsCjvwA2z7Q7vj/lHUevhhobhFaOWbQ08WT12Jf440Ob1T4mEFb0jJQWn/2TAJQ4O1m1HYQeAXRfKqzzPOw6nGsnuqsXCnYOgs+iTPfl7RSnzp9WNZnGc0DNPxQoaFW1aQDjD2TABQADG9fi5p+jj092lPd6tMqTMupzv4FWbYxbu0aKbthbifYt8TqTUN8Q/hPz//wYLMHdbfOYOsarbUuQdwCCUABmO8F/t+dDbQuo9y0q1OZkV3qaVfA1plwbKN2xy+N/AzzfKRfPVamMYNPt3qaOXfOIcAjoJwKtC1hvmEyA4ydkwAUFgNbBtOouo/WZdx2lTxdmD6khXZTnZ3eDRumaHPssti/BOZ2MNdtpfY1zWMGY4Niy6Ew29IlpEupn2swGJg4caLl63HjxjF//vwyHXfTpk3s3LnT6u1GjBjB2rVrr/v9OnXqEBERQXh4OBs2WN8xCmDOnDksWWL9FQQtSQAKCycnA8/0aKh1Gbfd24MiqK7V5d28DPPq7fY2bi71uPm+4JYZ5su3VqjsXpnZ3WYzPmo8Lk6O27mqa2jXUj/X29ubhQsXkpGRccvHLSkAi4rKNjPOzJkz2bdvH++99x6PP/54mfbx+OOPM2TIkDJtqxUJQFFM10aBxNTTfnaN2+WB6DDubKLlVGdjzWFij0wF5lUlvhhg7sBjBYPBwANNH2Bhr4XU8q1VPvVpKMAjgIiqEaV+vpubG0OHDmX27GsXLj527Bjdu3cnKiqKrl27cvLkSQA6d+7MwYPmSSoOHjxI586dSUpKYs6cObz55ptERkayd+9eRowYwRNPPEGbNm148803WbVqFW3atKFFixb07t2by5cvl7rO2NhYkpOTLV+/9dZbtG7dmvDwcKZOnQrAkCFD2Ljx78v5Xbt2Zc+ePUyePJn333//hq8pJSWFmBjzbELr16/Hw8OD/Px8Ll++TIsWLQCYPn06DRs2JCIigieeeKLUdZeVBKC4xpR+zXA12v+vRqPqPjzfq7F2Bez70nw50d4d22geM3jkB6s3bVylMUv6LKFf3X7lUJh27gy7EyeDde+Rp556io8++ojc3Nxi3//3v//N3Llz2bVrFxMnTmT8+PE33EdISAiPP/44zz77LHv37iUyMhKAS5cusWPHDl544QU6derEjh072LNnD927d+eDD0o/7Oabb77hrrvM4zvXr19PcnIyO3fuZM+ePaxbt46DBw8SHx/PsmXmKfzOnz9PSkqKJcBKek01a9YkLS2NvLw8Nm/eTJMmTfj111/ZunUr0dHRALzyyivs3r2bffv28eabb5a67rKyrUW1hE2oU9WbkZ3rMe2Hw1qXUmYeLs68f18L3F2ctSng0jH4Zpw2xy4PWRfMs8dEj4Ruk8DoWupNPV08eTX2VdrXbM+U7VPILNBgBpzbrEetHlZvU7VqVfr06cOnn35q+V5mZiYJCQncfffdgHm6OS8v68dVDho0CMP/prZLTEwkPj6ec+fOkZOTQ9u2bW+6/ejRo3n66adJTExky5YtgDkAv/nmGxISEgDIyMjg8OHD9OrVi2eeeYaioiJWrlzJgAEDiu2rpNcUFRXFzp072bFjB2PHjmXz5s2kpaVZWoZt2rRh2LBhxMfHW7YvT/b/MV+Uiyc619VuqrDb4MU+TahXTaMOPUUF5vt++bd+v8e2KNj2PnxyZ5nGDPaq04tlfZcRHhBeDrVVnEDPQFpUa3HzJ17HuHHjmDFjBoWFhQCYTCYCAwPZu3cve/fuZd++fWzduhUAo9GIyWQCIC8vr8T9enp6Wv49evRonnnmGQ4cOMD06dNvui2Y7wEePnyYN954g0cffdRS26RJkyy1HTt2jAEDBuDp6Unr1q35+eefWb58OfHx8cX2VdJrio2N5aeffiIvL4+4uDi2bt3Kli1bLAH4zTffMGrUKLZt20anTp1Kc0pviQSguC5XoxOv929ul4vm9mpenfvaajzVWcoe7Y5f3s7sNU/kvXeR1ZsG+wTzn57/4eFmD1t9CdFW9KnTx9LaslZISAgxMTGsWLECAF9fXwIDA1mzZg1g7sTy132/sLAw9u7dC8BXX31l2YePj0+JnWmuXLlCUFCQefLyzz+3qr4xY8ZQWFjI+vXriYuLY968eWRnZwNw8uRJ0tPTAYiPj+fDDz8kOTn5msufJb2m2NhY5s6dS2RkJAEBAVy8eJGUlBRq1aqFyWQiKSmJbt26MXXqVBITE8vcqae07PM3UFSINrUrM7hViNZlWCXI34M3BmjYwji6Aba+r93xK0p+Jqx6AlY8au7pagWjk5ExrcYw9865VPWoWk4Flg8ngxPxDeNv/sQSTJgwgZSUFMvXixYtYtasWURERNC8eXPLMISnn36at99+m1atWpGfn295ft++fVm8eLGlE8zVJk2aRN++fWndujUhIda9fw0GAy+99BJTp06lR48e9O/fn3bt2tGsWTOGDRtmuX/Zq1cv1q1bR//+/a+7nxu9psaNG5OTk2Np8TVu3JiWLc3TyRUVFTF06FDCw8OJioripZdewtm5fG9hyHJIokRXcgvoOT2B05dztC7lppydDCx5rB1RtSprU0DmBXNnkSzrekzavUq1YeAnEGz9tGBpuWlM3DKRn5N/LofCbr+OwR35oJuNzOUqbpm0AEWJfN1dmHFPJM5aDSK3wuiu9bULP6XM83zqLfwA0k7Ap91h8zSrxwxWcq/EB90+YELrCbg6lb5jjVaGNLSvcW6iZBKA4qaialVmlJbTiJVCm9qVGdVVwxq3vW9eYkivTAXww2RY0B8yzlm9+bAmw1jY27bHDAZ7B+tihhs9kQAUpTK6W32itJpI+ib8PV2YPkTDVmrKHtjwijbHtjXHf/zfmMHvrd60UeVGLOmzhP71rn9fSWuDGw6224474vrkpylKxdnJwPR7IvFxt72ho28OCKemv4c2B8/LhOUPm1daF2bZF2FhPPz3OSi07rx4unjySswrvNPxHXxcbGdeWjdnN5sNZlF2EoCi1IIrefL2wHCbGhoxtG0oPZpV166AdeMg1foxcY5PwfbZMK8bXDxq9dY9avdg2V3LrJpurDx1r9Udf3d/rcsQt5kEoLBKz+Y1eLJrfa3LAKBhoA8v9mmiXQH7l8K+xdod3x6c3W8eM7jnC6s3DfIOYn6P+Tza/FFNLz06G5x5tPmjmh1flB8JQGG1/7ujPj2aatjqAtxdnJh5r4ZTnaWegLVPa3Nse1OQBV+PNF8qzr1i1aZGJyOjW47m4zs/pppHtXIqsGS96/Smll8tTY4typcEoLCawWDgvSERmq4d+ELvJjTU6vgOO9VZOTu4HObEQvIuqzdtU6MNK+5aQefgzre/rhIYDUYejyjb8kDC9kkAijLxdDUyb3gUVbwqfuxW96aB3N8urMKPa7FxCpz+Vbvj27PLp8xjBhPehf/Nc1la/u7+zOo2i2fbPFthYwb71etHiI99zYYkSk9mghG35JeTqQybt4O8Quv+mJVVTT93vn2qI36eGi20emwjLBgAyNvmltXuBAM+Ah/rL6f/mfonz/z8DMfTy2+tRRcnF77p/w01vGuU2zGEtqQFKG5J61qVmT20JcYKGIPn7GRg2pBI7cIv6yKsfBwJv9vkxE/mMYOHv7N604aVG/Jlny8ZWH9gORRmNqD+AAk/BycBKG5Zt8aBvDs4gvLOwJFd6tG2jkar1StlDr9M62c5ESXIvgSLBsO3E6Dw5sv2/JOH0YPJ7ScztdNUfFxv7/1gN2c36fmpAxKA4rboFxnEy/2aldv+W9eqxFPdNBx+sX02HLV+dhNRSjvm/G/M4BGrN+1eqzvL+y4nsmrkbSvnoWYPEegVeNv2J2yT3AMUt9X7G48wdf3tXUnez8OFdU91IEir2V7O7IN5d8hsLxXBxQt6vgktH7B60yJTEbP3zWbegXmYVNnvSYf6hLKy30pcnW1/cm5xa6QFKG6rUV3rM/o2T0r95oDm2oVffhYsf0jCr6IUZMHqJ2HZg5CbbtWmzk7OPNniSebFzaOaZ9nHDL7Q9gUJP52QABS33dNxDXmuZ6Pbsq9724TSs7mGHRHWjYdL1k/lJW7Roa/MYwaTdlq9aevqrVnRdwVdQrpYvW33Wt1pH9Te6u2EfZJLoKLcLNxxihdXHcRUxt+w+tW8WfNkrHazvRxYbh7wLrTjZITOz0LsWHCy/vP64j8W8+6ud8krunkHGy8XL1bfvfqWWo/CvkgLUJSboW3DmDYkskxDJNyMTsy6T8OpztJOwtr/0+bY4m+mQtj4Knx+F1w5Y/Xm9za6l0W9F1HXr+5NnzsqcpSEn85IAIpy1S8yiA+HtcLdxbpftRd6N6ZRdd9yquomigrN81bmWTdvpShHJxPMYwb//NbqTRtUasCXfb5kUINBN3xO48qNubfRvbdSobBDcglUVIh9SZd5bMEuzl25+aWoO5sE8vEDURVQ1Q38MBk2T9Pu+KJkbR6DuFfB6Gb1pt+f+p7JWydzJf/vDzduzm4s7r2Y+pVsY5UTUXGkBSgqRESIP6tHxRIe7Ffi82r4ufPOoPAKquo6jm+CLTO0O764uZ0fwcdd4cKfVm96Z9idLO+7nJbVWlq+N6blGAk/nZIWoKhQuQVFjF++nzX7Uq55zMkAix5tRzutZnvJumS+zJZ5VpvjC+u4eEKPN6DVCKs3LTIVMWf/HA5ePMjsbrMx2NIqz6LCSAAKTczacIT3fjjMP3/7nuxaj7FxDbUrauFgOGL9vJRCY03uhr4zwMPf6k1NyqTpYrtCWxKAQjOb/jzP2KX7uJSVT6uwSiz9VzTOFTCp9nVt/xD++6w2xxa3zi8UBs6D0LZaVyLsiASg0NS5K7lMXHWQSX2bEFzJU5sizuz/31Rn1k3GLGyMwdk8ZrDDuDKNGRT6IwEo9C0/C+Z2gkvWT8IsbFStDuZ1Bn1ral2JsHESgELfvh4Je77QuooSJaWbuH9lDuezFEYneLGjG/FNXRixKoefTxXi62a+bLxisCd1KzsxbVsen+wpIDzQiUUDza3qT/fkYwAebKGTOS49KkO/96FRb60rETbMqHUBQmjm4AqbDz8AoxNM7+FOZHVnzmaaaPVRFr3qm9+6M3u606dB8QWC/7OvgANPeDF8VS77zxVRr7ITy38rZO19Gk0oroWcVPjyPmj9CMS9Bi7uWlckbJBcKBf6lHYK1tjHVGc1fJyIrG6eEq66txMBngZSc2584cbdaKDQZF633ugE723LZ0w7V5z02NX/l3nmMYPn/9C6EmGDJACF/hQVwopHIM+65XZswa8pRRSZIMTP/NYdtz6PiDmZPPdDLkX/m3X88SgXWn+chZ8bBHga2HeuiLi6Or7Yc/4QfNQZdn2qdSXCxsg9QKE/G16BhHe1rsJqqTmKDp9l8XFfd9qHGDmTYaK6t4G8Ihi+KoeOoUZGtil+j+/JdTk81sqVzYlFbDhRyB11jDwepZP7gNfTfDAM/FjrKoSNkBag0JcTP9vlPJ95hYq7v8zm2RhX2oeYW3M1fJwwGAy4Gw08EO7CLylFxbb582IR+UVQp5ITX/9ZwPLBnqz6o4CsfB1/5pVxguIfJACFfmSnwlePgTJpXYlVlFKM+DqHrrWduT/i79bbmQzz6zApxeo/C2latfjb+ZWf85jU2Y38IsguMH8vqwDyi+ekfjQbaO4UI8T/6PjGgNCdVf+GDOvXlNPalqQilhwsJDzQiVV/ZAKwoL8HT/03l4vZCpOCdsHOjG77dzgmnCqkbiUnavqYQ7FFdWeazc7kjjpGKnnosDNM5brm6dKE+Ae5Byj0Ycdc+PYZrasQWjC6w8PfQw0NVxkRNkkugQrHd/YgrH9R6yqEFgxOMPATCT9xXRKAwrHlZ8Pyh2SeT73q+TY07qN1FcJGSQAKx/bfCXDR+oVThQOIfRraPKp1FcKGSQAKx3VoJez+XOsqhBYi7oU7JmldhbBxEoDCMV1OhDVPaV2F0ELdrnDXLK2rEHZAAlA4HlOReaqzXPub6kzcohoRMHgBOLvc/LlC9yQAhePZ9CYk7dC6ClHR/MNg6HJw89a6EmEnJACFYzm5GRKmal2FqGg+NWHYV+BdTetKhB2RmWCE47DTqc7ELapSD+5fCf6hWlci7IwEoHAcq5+EK6e1rkJUpBoR5pafV4DWlQg7JAEoHMPOj+GPtVpXISpSrQ5wzyJw99W6EmGnZC5QYf/O/QYfd4HCXK0rERWlYW+I/wyMblpXIuyYdIIR9q0gxzzVmYSffkQOhSELJPzELZMAFPbtv8/Bhd+1rkJUlOhR0O8DcHLWuhLhAOQeoLBfv62GXz/TugpREZxcoPtr0PZfWlciHIgEoLBP6cnmXp/C8fmFQvx8CG6ldSXCwUgACvtjKoIVj0LuZa0rEeWtQU/o/yF4VNK6EuGAJACF/fnpbUjcqnUVojw5GaHbS9B+NBgMWlcjHJQEoLAv2amw/UOtqxDlyTcIBn0Koe20rkQ4OOkFKuyLZ2X41yYIbq11JaI81O0G/0qQ8BMVQgbCC/tkKoKfp8LPb4OpUOtqxK1y8YIuz5mHOcglT1FBJACFfUv+FdaMhnMHta5ElFWjPtDzLfAL1roSoTMSgML+mYpg16fw42uQk6Z1NaK0/MOg1zvQoLvWlQidkgAUjiM7FTa+Cr/OB1WkdTXiRpxdof2T0HE8uHhoXY3QMQlA4XjOHoRvJ8CpzVpXIq5WqwP0fg+qNtC6EiEkAIUDO7gC1r8EV5K1rkT4hUDXFyFiiNaVCGEhASgcW342bJluHjuYd0XravSnch2IfRoi7gFnF62rEaIYCUChD7lXzBNnb58DGSlaV+P4qjaCDmOh2UBZuUHYLAlAoS+F+XBgGWydJcsolYfqzaHDOGjST8bzCZsnASj0SSk4/B1snQmntmhdjf0LamXu1dmwp9aVCFFqEoBCJO+CLTPgz3Uyq4w1PCqZL3FG3AvBUVpXI4TVJACF+EvWRTi0Eg5+BYnbAHlrXMPJCPXjzJ1aGvQEo6vWFQlRZhKAQlxP+mk49BUcWA5n9mpdjfZqRJhbes3jwStA62qEuC0kAIW4mUvHzGMKDyyHi39qXU0FMZg7tNTtCuFDILCJ1gUJcdtJAAphjfN/wMkEOLXVfJk044zWFd0+letCnU5QuxPU7mheekoIByYBKMStSD0Op7b9LxC3mr+2F97V/w68Op1kNQahOxKAQtxOGWfNYXj6V3MYpp6AtJNQmKNdTQYn84ws1ZqY/wtsAoHNoEpd7WoSwgZIAApR3pSCKymQduLvUEw9bv7vSgoUZENBDmXqderiCW6+4O5r/r+Hv3mZocp1/vFfbTC63e5XJYTdkwAUwhYoZQ7Bgpz/BWL238FYkA1FBeDmYw45Nx9w9zP/29modeVC2C0JQCGEELrkpHUBQgghhBYkAIUQQuiSBKAQOmIwGJg4caLl63HjxjF//vzbeoxVq1Zx+PBhy9ePPPIIx44du+X9Go1GIiMjadq0KX379uXy5ctl2k+vXr3IydGwV66wGRKAQuiIt7c3CxcuJCMjo9yOcXUAzps3j7p1b33Ihb+/P3v37uXQoUP4+/vzwQcflGk/69atw8PD45brEfZPAlAIHXFzc2Po0KHMnj37mseOHTtG9+7diYqKomvXrpw8eRKAbdu20bRpU1q0aMHIkSMZNGgQYA66Nm3a0KJFC3r37s3ly5fZsWMHq1evZvTo0URGRnL+/Hk6d+7MwYMH+fDDD3nppZcsx3vllVeYNm0aAG+99RatW7cmPDycqVOn3vR1xMTEkJycDMCFCxcYMGAAUVFRREdHs2fPHtLT06lfv77l+adOnSIyMhKAWrVqkZmZCcCCBQto3bo1ERERPP300wC8/vrrfPzxxwDcd999PPzwwwDMnDmT9957j8zMTHr06EHz5s1p3rw53333XanPv7AxSgihG1WqVFHnz59XderUUTk5OWrs2LHqs88+U0opFRcXp06cOKGUUmrDhg1q0KBBSimlmjZtqn799VellFJDhw5VAwcOVEoplZqaqkwmk1JKqRkzZqhXX31VKaXU8OHD1Zo1ayzH7NSpkzpw4IA6e/asatq0qeX74eHhKikpSX333Xdq1KhRymQyqcLCQtWlSxd14MCB69aulFKFhYVqwIABau3atUoppe677z61c+dOpZRShw8fVm3atFFKKdW7d2+1fft2pZRSU6dOtdQXFhamMjIy1G+//aYGDhyoCgoKlFJK3X///Wrt2rXqp59+Ug888IBSSqn27dur2NhYpZRS8fHxaseOHWr58uXqvvvuU0opZTKZVHp6urU/BmEjZBCREDpTtWpV+vTpw6effmr5XmZmJgkJCdx9990AKKXw8vLi8uXLFBQU0LJlSwCGDBnCf/7zHwASExOJj4/n3Llz5OTk0LZt2xKPGxgYSNWqVTl48CCurq54eXkRHBzM9OnT+eabb0hISAAgIyODw4cP06xZs2LbX758mcjISJKTk6lfvz7du3cH4IcffuDQoUOW56WlpQEQHx/PsmXLaNu2LStWrLjmXueGDRvYvn07UVHmtQyzs7Np1aoV//rXv3j88cdJTEwkNDSUvLw8Lly4wO7du2nRogX+/v6MGTOGZ555hv79+xMdHW3N6Rc2RAJQCB0aN24cd9xxBz17mldwN5lMBAYGsnfv3mLP+ytMrmf06NG88MILxMXFsXbt2lJ1phk8eDDLli3D1dWV+Ph4y7EnTZrE8OHDS9z2r3uAWVlZ3HnnncyePZvRo0cDsGvXLozG4n/O7r77bl577TWeeuopcnJyaNCgQbHHTSYTjz76KJMmTbrmWJUqVWL58uXExsaSm5vLggULCA4OxsXFhQYNGrB3717Wrl3L008/zdChQxk1atRNX7uwPXIPUAgdCgkJISYmhhUrVgDg6+tLYGAga9asAaCoqIiDBw9SqVIljEajJRiXLVtm2ceVK1cICgpCKcXnn39u+b6Pj88NO9kMGDCAr776ihUrVlgCMC4ujnnz5pGdnQ3AyZMnSU9Pv2HtXl5ezJw5k3fffZfCwkK6dOnChx9+aHl83759APj5+dGgQQMmTJhguW/5T926dWPJkiVcunQJgPPnz3PmjHl1j5iYGKZNm0ZMTAyxsbFMmzaN2NhYAFJSUvDy8mL48OGMGTPmmg8Nwn5IAAqhUxMmTCAlJcXy9aJFi5g1axYRERE0b96cDRs2APDRRx8xdOhQWrZsiZubG76+vgBMmjSJvn370rp1a0JCQiz7ueeee5gyZYqlE8w/BQYGEhAQgLu7O8HB5tUnevToQf/+/WnXrh3NmjVj2LBh5Obmllh7VFQUzZs3Z+nSpcyaNYtNmzYRERFB48aNWbRokeV58fHxLF682BK2/9S0aVNeeOEFunXrRnh4OL179yY1NRWA2NhY0tPTad68OS1btiQ1NZWYmBgADhw4QOvWrYmMjGT69OmWzjPC/shUaEKIEmVlZeHl5QXAqFGjaNSokVzyEw5BWoBCiBJ9/fXXREZG0qRJEy5dumQZFiCEvZMWoBBCCF2SFqAQQghdkgAUQgihSxKAQgghdEkCUAghhC5JAAohhNAlCUAhhBC6JAEohBBClyQAhRBC6JIEoBBCCF2SABRCCKFLEoBCCCF0SQJQCCGELkkACiGE0CUJQCGEELokASiEEEKXJACFEELokgSgEEIIXZIAFEIIoUsSgEIIIXRJAlAIIYQuSQAKIYTQJQlAIYQQuiQBKIQQQpckAIUQQuiSBKAQQghdkgAUQgihSxKAQgghdEkCUAghhC5JAAohhNAlCUAhhBC6JAEohBBClyQAhRBC6JIEoBBCCF2SABRCCKFL/w8Ff7PL0XFZUQAAAABJRU5ErkJggg==</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+  <si>
+    <t>https://www.flipkart.com/oneplus-y1-80-cm-32-inch-hd-ready-led-smart-android-tv-dolby-audio/p/itme650a6bb8cee3?pid=TVSFVWD2ENXYGEJY&amp;lid=LSTTVSFVWD2ENXYGEJY9U6ROG&amp;marketplace=FLIPKART&amp;q=tv&amp;store=ckf%2Fczl&amp;srno=s_1_5&amp;otracker=search&amp;iid=19bade9d-3b9f-4a13-aed0-8b222b07eaf3.TVSFVWD2ENXYGEJY.SEARCH&amp;ssid=f7bg2wadtc0000001688654484751&amp;qH=c9a1fdac6e082dd8</t>
+  </si>
+  <si>
+    <t>OnePlus Y1 80 cm (32 inch) HD Ready LED Smart Android TV with ...</t>
+  </si>
+  <si>
+    <t>₹14,999</t>
+  </si>
+  <si>
+    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAcAAAAFQCAYAAAAoQ64wAAAAOXRFWHRTb2Z0d2FyZQBNYXRwbG90bGliIHZlcnNpb24zLjYuMSwgaHR0cHM6Ly9tYXRwbG90bGliLm9yZy/av/WaAAAACXBIWXMAAArEAAAKxAFmbYLUAABG6klEQVR4nO3deVxU9f7H8dfAsK8qiAKCa26siguCueZu5YJ609J2KzN/qdUty5bber25tZlmZpmZWppbUm5h7ikqZilugLgh+w4z5/cHt7mhqAMOnFk+z8fDhwwz5zufOQy853u+3/M9GkVRFIQQQggbY6d2AUIIIYQaJACFEELYJAlAIYQQNkkCUAghhE2SABRCCGGTJACFEELYJAlAIYQQNkkCUAghhE2SABRCCGGTJACFEELYJAlAIYQQNkkCUAghhE2SABRCCGGTJACFEELYJAlAIYQQNkkCUAghhE2SABRCCGGTJACFEELYJAlAIYQQNkkCUAghhE2SABRCCGGTJACFEELYJAlAIYQQNkkC0Mr17NmTr776qlba1mg0pKWl1UrbNZGSkoK3t7faZZi1ZcuWMXTo0Brfb25effVVHnnkkRve7+7uTnp6eh1WdHO1+fsoqk8CsI41bdoUV1dX3N3d8ff3Z/Lkyeh0ujp57iVLltC3b1+jHpuSkoK7uzvu7u64ubmh0WgMt93d3Wu50poJCgoiOztb7TLM2tixY1m3bp3h9rUfYq6939xU90NXfn4+/v7+tVhR3ZMQNR0JQBXEx8eTn59PQkICq1ev5rPPPlO7pOsEBQWRn59Pfn4+p06dAjDczs/Pr7XnLS8vr7W2zYG1vz5boigKer1e7TLEbZAAVFGLFi2IiYkhMTHR8L1Vq1bRvn176tevz913383ly5cBuHLlCgMHDsTb2xsfHx/+8Y9/ALB9+3ZatmxZqd2qPiWfPn2aiRMnsn37dtzd3Wnfvr1JXsO6deto1qwZPj4+vP3224bv63Q6Zs6cSXBwMH5+fkydOvWGf/x79uzJyy+/TFRUFG5ubpSVlbFjxw46duyIt7c3PXv2NITwI488wmuvvVZp++bNm7Nz507Onj2LVqs1fD8zM5P77ruPhg0b0rx5c7744gsATp48WalX0K9fP3r37m247e/vz8mTJ2+4z6916tQp7rzzTry9vfH39+fFF1803LdkyRJ69erF448/jpeXF59//vkN66qKRqNh/vz5BAUF0ahRI/79738b7isuLuapp56iUaNGBAUF8frrrxv+IO/Zs4fIyEg8PT0JCAhg9uzZhnr+OgrQr18/AFq3bo27uzsJCQmV7r/ZvgZu+DOqykcffUTz5s3x9fVl3Lhx5OTkAP97/77++uvUr1+fpk2bsnnz5irbqKpegKKiIuLi4vDw8KBLly6cOXOm0v7763dh8eLFBAcH4+HhQevWrdm+fXu19/mECROYNGkSvXv3xtXVlVOnTpGQkEBkZCTe3t706NGD48ePGx6/f/9+wsLC8PT0ZOLEiZUCc8KECfzrX/8y3L72CM3WrVuJiorC09OTVq1akZCQwBtvvEFCQgKPPPII7u7uvPXWWzfc58IIiqhTwcHBSkJCgqIoivLnn38qjRo1UmbNmqUoiqLs3btXCQgIUI4cOaKUlpYq06dPV0aMGKEoiqI8//zzyhNPPKGUlZUpxcXFyq+//qooiqJs27ZNadGiRaXnAJTU1FRFURSlR48eypdffqkoiqJ8/vnnSp8+fSo99u2331YGDx5805ovXLigVPVWAZSRI0cqeXl5ytGjRxUnJyclOTlZURRFee+995RevXoply9fVrKyspSePXsq8+fPr7L9Hj16KC1atFBOnjypFBUVKSkpKYqPj4/yyy+/KOXl5cq8efOUqKgoRVEUJT4+XmnXrp1h27179yqBgYGKXq9Xzpw5o9jb2xvuGzRokDJ16lSluLhYOX78uNK4cWPl8OHDiqIoip+fn5KcnKyUl5crTZo0UQICApTS0lIlOTlZ8fPzu+k+v1ZycrKyfft2paysTDlx4oTSpEkT5fvvvzfsc3t7e+Xzzz9XdDqdUlhYeNO6qtrH/fr1U3JycpTjx48rjRo1Un7++WdFURTlxRdfVHr06KFkZmYq586dU1q1aqV8/vnniqIoSpcuXZSvvvpKURRFyczMVA4ePGio5+/vgb+/V669/2b7+mY/o2vFx8crjRo1Uo4dO6bk5+crw4cPV8aPH68oSsX7197eXnnnnXeUsrIyZcGCBUpQUFCV7VRV78yZMxUXFxdl69atSllZmXL//fcrDzzwwHWPz8/PVzw8PJQTJ04oiqIoZ8+eVU6fPl3tfT5+/HilQYMGyoEDB5SysjLl4sWLire3t7J69WqltLRUee+995SWLVsqZWVlSklJiRIYGKh89NFHSmlpqTJv3jzF3t7e8Ps4fvx45Y033qhy3586dUrx8PBQ1q1bp5SXlyvnzp1TTp48qShK5d9pcXukB6iCgQMH4u7uTuvWrenWrRtPPfUUUPEJ9cknnyQ0NBQHBwdefvll1q5dS3l5OQ4ODly4cIHU1FScnJzo1q2bSWp54YUXWL9+/W1t7+7uTkhICGFhYRw9ehSAzz77jH/961/4+vri7e3N1KlTWbVq1Q3befjhh2nZsiXOzs4sW7aMYcOG0b17d+zt7Xn66ac5e/YsZ8+epXfv3ly5coVjx44B8O233xIXF4dGo6nU3sWLF9m+fTtvv/02Tk5OtGnThvvuu4/vvvsOgO7du/PLL79w6NAhwsLCiIiI4ODBgyQkJBAbGwtg9D5v0aIFPXr0QKvV0qpVK8aOHWvoJf11/4QJE7CzsyMnJ+emdVXln//8J56enrRp04aHH36YFStWAPDNN98wc+ZM6tWrR1BQEFOnTmX58uWG2pOTk8nMzKRevXpERkbe9OdYlZvt65v9jK71zTff8Nhjj9GuXTvc3Nx46623WLFiBYqiAODm5sb06dPRarWMGzeOlJSUao3l9unTh169eqHVahkzZgyHDx+u8nEajYZjx45RUlJCcHAwzZo1u2GbN9rnACNGjKBjx45otVri4+MJCwtj+PDhODg4MHXqVAoLC9m/fz+7d+9Gq9XyxBNP4ODgwKRJk2jcuLFRr2n58uUMHTqUIUOGYG9vT1BQ0HVHesTtkwBUwaZNm8jLy2PNmjUcOHDAMKaWkpLCm2++ibe3N97e3jRp0gStVsvFixeZPn06QUFB9OjRgzZt2pjNuKGfn5/ha1dX10qv5a/Dh97e3owdO9ZwOLcqgYGBhq9TUlL48ssvDdt6e3tTUFDA+fPnsbe3Z+TIkYY/oCtXrmT06NHXtZeSkkJxcbEhgL29vVmwYAEXL14EKgIwISHBEHh/v929e3cAo/f5+fPnGTZsGI0aNcLLy4s5c+Zw9erVG762m9VVlSZNmlT6+sKFCwCkp6cTFBRkuC84ONgw43HRokUcO3aMli1bEhsby+7du2/Y/o3cbF/f7Gd0rarqLC4uJjMzEwBfX1/s7Cr+FLm6ugJUa5z5Ru/Bv3Nzc2P58uXMmzcPPz8/4uLibjo79Eb7HCr/PK99bXZ2djRp0oT09HQuXLhQ6bEajabS7ZtJS0u7aUAL05AAVIlGo+Gee+6hb9++hnGAgIAA3njjDbKzsw3/ioqKCAwMxNPTk7lz55KSksKSJUt4+umnOX36NG5ubhQVFRnavXTp0k2fs64EBASwbds2w+vIycnh999/N6q2gIAAHn300Ur7obCwkJiYGABGjx7Nt99+y549e7Czs6NLly5VPr+7uztZWVmGNvLy8vjkk0+A//UAd+7cSffu3enevTs7d+5k586dhh7gjfb5tWbMmEG9evU4ceIEOTk5TJkyxdC7qeq13ayuqqSmplb6+q9ehL+/PykpKYb7UlJSDGObrVu35ttvv+Xy5cuMGTPmhuOXt3KjfX2rn9HfVVWns7Mz9evXr1FNNTVo0CC2bt1KWloaTk5OlcZqr3WjfQ6Vf57XvjZFUUhNTcXf35/GjRtfNxb/99s3+91t0qRJlb3pa59f3B4JQJVNmzaNRYsWkZGRwYMPPsgHH3xgOISTmZnJ2rVrAdiwYQOnT59GURS8vLzQaDTY29tzxx13kJWVxY4dOygpKeGNN9644XM1bNiQtLS0OpmJ+NBDDzFjxgwuXLiAoiicPXuWHTt2GLXtfffdx8qVK0lISECv15OXl1fp8Gn37t3Jy8tjxowZjBo1qso2AgICiI6OZsaMGRQWFlJeXs7BgwcNIRweHs6VK1dISEigU6dOREVFsXv3bi5cuEBERARw431+rby8PDw8PHB3dycpKemmU9RvVVdV3n33XXJzc/nzzz9ZvHix4TWPHj2aN954g6ysLFJTU3n//fcZM2YMUHE+39WrV9FqtXh4eFRZN1S8J270hxZuvK9v9TP6u9GjR7Nw4UKOHz9OQUEBL730EqNGjarRH/Jb1Xsjly5dYv369RQVFeHk5ISrq+sN9wnceJ9fa+DAgRw+fNgwVDF79mxcXFyIiooiOjqasrIyPv30U8rKyvjwww8r9STDw8PZsGEDubm5nD59utIRhn/84x+sW7eOjRs3otfrSU1NNUwyquk+ENeTAFRZ27Zt6dGjB3PnzqVbt27MmjWLBx54AE9PTzp06MCvv/4KwIkTJ+jVqxceHh4MHjyYOXPmEBwcjJeXF3PnzmXUqFE0a9aMTp063fC5evfuTdOmTfH19SUsLAyAt956i4EDB5r8dU2fPp3o6GhiYmLw8vJi6NChlT5V30yzZs345ptvmD59OvXr16dNmzaGDwJQcZgpLi6OrVu33vAPE1SEQFpaGs2bN6dhw4ZMmTLF8Inbzs6Obt260aZNGxwdHXF0dKRdu3Z07drV8IfxRvv8Wq+88grbtm3D09OTyZMnM2LEiJu+vpvVVZVBgwYREhLCnXfeyeTJkw0zBV9++WVat25NmzZtiI6OZsyYMYwfPx6AjRs30rp1azw8PJg3bx5Lly6tsu1XXnmFESNG4O3tXWnc8i832te3+hn9Xb9+/fjnP//JoEGDCA4OxsHBgTlz5tx0H93Ireq9Eb1ez3vvvYefnx8NGzbk/PnzlWZgXutG+/xaPj4+rFmzhpkzZ9KgQQO+//571qxZg4ODA46OjqxevZr58+fToEEDjhw5Umkc+f7776dFixYEBgbyj3/8o1IvvVmzZqxevZqXXnoJLy8v+vTpYwjPp59+miVLluDt7c0777xj9D4Q19Mofz9WI4QwKxqNhtTUVKPHjsTtk31uO6QHKIQQwiZJAAohhLBJcghUCCGETZIeoBBCCJskASiEEMImSQAKIYSwSRKAQgghbJIEoBBCCJskASiEEMImSQAKIYSwSRKAQgghbJIEoBBCCJskASiEEMImSQAKIYSwSRKAQgghbJIEoBBCCJskASiEEMImadUuQAhLk1NYRlp2IenZxZzPKiQ9p5jMglKKSnUUlpZTVKb779cV/4rLdJTq9DjY26G10+Bgb4eT1g4XR3vcHLW4Odnj4eyAn6cTjbxc8PdyprF3xf8+7k7Y2WnUfslCWCUJQCGqoNMrJF/OJ+l8DknpOZzNKOB8dhHp2cXkl5TXWR0O9hoaejgT4O1CKz932vt70d7fk9aNPHB2sK+zOoSwRnJBXGHzynV6Tv4VdudzOHo+h+MX8igq06ld2g1p7TS08HWnnb8n7f09aefvSWSTerg4SigKYSwJQGGT/riYy86TGfyanMG+M5kUlJpv2BnLUWtHVHA9Ylv5cGcrX9r7e6LRyOFTIW5EAlDYhIKSchJOZrDtj8ts+/Myl/NK1C6p1jVwc6RbSx+6t/Sh+x0+NPZyUbskIcyKBKCwWkWlOuJ/v8j3h86zK/kqpTq92iWpKjzQiyFh/gwJbyxhKAQSgMLK6PUKu09f5buD59l87GKdTlixFBoNRAXX497IAIaE+ePl4qB2SUKoQgJQWIUTl/L47uB51iae50JOsdrlWAwnrR192/kxsmMgPe/wlTFDYVMkAIXF0usV4n+/xKKE0xw4l6V2ORavua8bD8Y0I65joJxiIWyCBKCwOMVlOlb9lsZnO89wJqNA7XKsTj1XB+7rEsT46KY09HRWuxwhao0EoLAYmQWlfLHrLF/tOcfVglK1y7F6jvZ2DAlvzCOxzWnn76l2OUKYnASgMHuX84qZvyWZlb+lUlxm2zM51dK7TUOeG9CaNo0kCIX1kAAUZquwtJwFO06zMOE0hVZworqls9PAsMhApva7A39vOY1CWD4JQGF2dHqFFftTmf3zCa7YwAnrlsZJa8f4bk15qmdLvFzlFAphuSQAhVn5+fdLvPPjHyRfzle7FHELns5anujZkgdjmsqsUWGRJACFWThxKY9X1iax53Sm2qWIagqs58Jbw0K58w5ftUsRolokAIWqSsp1fLA1mU92nKJMJ29FSza8QwCvDGmHt6uj2qUIYRQJQKGafWcyeeG7I5y+IufyWQsfd0dmDm3P0HB/tUsR4pYkAEWdKy7T8e6Pf7Bk11nk3Wed+rZtyL/uDaWRl5xIL8yXBKCoU7+dy2L6ysOclhVcrJ6Hk5YZQ9oyulOQ2qUIUSUJQFEnFEXh4x2n+E/8CXR6ecvZkiFhjXl7eCgeznLKhDAvEoCi1uUUlTH120R+Pn5Z7VKESoIbuDL/H5GEBXqrXYoQBhKAolYdS8/hia8OkpJZqHYpQmWO9na8MrQd47oGq12KEIAEoKhFK/an8MraY5SUy/qd4n9GdAjkzWEhcvK8UJ0EoDC54jIdr6xN4tsDaWqXIsxU28aeLBofRYCsKSpUJAEoTCqroJSHvtjPoZRstUsRZs7P04klD3ambWO5woRQhwSgMJm0rEIeWLxPTmwXRvNw0rLg/o50a+mjdinCBkkACpM4fiGX8Yv3cVmu3iCqydHejn/HhXFPRIDapQgbY6d2Aaai1WqJiIggJCSEuLg4CgurN+vwk08+YcWKFQAsWbKEy5f/N2V/0KBBFBUVmbTe6nrkkUc4deqUqjXcyO5TVxm1YLeEn6iRUp2eKSsS+WSHeb6/hfWymh6gj48PGRkZAIwdO5aOHTvy7LPP1qitnj178sEHHxASEmLKEg10Oh329tYxA27j0QtMWZFIqcz0FCYwoVtTXhnSDjs7jdqlCBtgNT3Av+vevTvJyclkZGQwdOhQwsLC6NmzJ2fPngXgm2++oW3btoSHh3PPPfcA8Oqrr/LBBx/w/fffc+DAAUaOHElUVBQATZs2JT8/n+eff57Fixcbnuehhx7i+++/R6fTMXXqVDp16kR4eDjLli27rqbt27fTu3dvBg0aRExMDAUFBUyYMIFOnTrRsWNHfvrpJ/R6PS1atKCgoGIMraioiODgYMrLy+nZsydJSUkAbN68mejoaCIjIxk3bhylpaV8/fXXvPTSSwC8+OKL9OnTB4AffviByZMno9PpGDduHO3atSM0NJTPP//8tvfzsr3nmPT1QQk/YTJLdp1l+qojWMnncmHmrC4Ay8vL2bRpE6Ghobz66qt0796dI0eO8MQTTzB58mQA3nzzTX744QcOHz7M0qVLK20/bNgwoqKiWLVqFQcOHKh0X1xcHCtXrjQ8z5YtWxg4cCCfffYZjRs3Zv/+/ezZs4f33nuPq1evXlfbb7/9xqJFi9izZw9vvvkmQ4YMYf/+/WzevJmnn34ajUbDwIEDWb9+PQAbN26kX79+aLVaQxsZGRn8+9//ZuvWrRw6dIjmzZuzcOFCYmNj2blzJwD79++noKCA8vJydu7cSWxsLImJiZw5c4bff/+do0ePMnz48Nvaz98eSGXGmiRkVTNhaqsPpjFjTZLaZQgbYDUBmJ2dTUREBFFRUQQHB/Pwww+zc+dOxo0bB8CoUaPYt28fADExMTz22GMsWrSoWp80o6KiOH36NFlZWWzZsoWYmBicnZ2Jj49n0aJFREREEB0dTU5ODqdPn75u+5iYGPz9Ky4TEx8fz+uvv05ERAR9+/aloKCAS5cuVQrZVatWERcXV6mNPXv2cOTIEaKjo4mIiGDlypWcOXOGoKAgLl26RH5+PjqdjujoaA4dOsSvv/5KTEwMzZs3Jz09naeeeor4+Hi8vLxqtJ8B1h9J54XVR+RKDqLWLNubwuvrfle7DGHltLd+iGXw9vYmMTHxpo/RaCrGFT7++GP27NnDunXriIqK4ujRo0Y/z7333suaNWvYtWuXIZz0ej0LFiygR48eN93W1dXV8LVer2fdunUEB1deFqphw4Y89NBDXL16lT179vDll19Wul+v1zN48OAqD2F26NCBTz/9lI4dO9K1a1e2bNlCRkYGAQEVs+uOHj3Kxo0bmT17NvHx8cyaNcvo1/2XLccv8X8rEqXnJ2rd4l/P4ORgx/MD2qhdirBSVtMDrEpsbCxff/01UNGb6ty5MwCnT58mOjqaN998E0dHx+sOV3p4eJCXl1dlm3FxcSxfvpyff/6ZgQMHAtCvXz8++ugjdDodAElJSYavb6Rfv37MmzfPcPuv8Lazs2PgwIE8/fTT9O3bt9LhT4Do6Gi2bdvGuXPnAMjNzeXMmTOG1zt79mxiYmKIjY3lww8/pFOnTkDFoVO9Xs+oUaN49dVXb/lhoSq7kjN4ctlBuXK7qDMfbz/FnJ9PqF2GsFJW0wOsyquvvsqECRNYunQp9evXZ8mSJQBMmzaN5ORkFEVh2LBhBAYGVtpuwoQJTJgwAQ8Pj+vGAaOiokhOTiY6Ohpn54qLfT766KOcOXOGyMhI9Ho9jRs3ZtOmTTet7eWXX+aZZ54hLCyM8vJyOnTowFdffQVUhGzPnj3ZvHnzddv5+vqycOFCRowYQWlpKXZ2dsyZM4dmzZoRGxtLWloa3bp1o2HDhri4uBATEwPA+fPnmTBhAnq9Hq1Wy5w5c6q1L387l8UjSw/Iup6izs35+STODvZM7NFC7VKElbGa0yBE7Tl+IZfRC3aTW1yudinChs0dEyEnywuTsupDoOL2Xckr4ZEvDkj4CdU9t+oIianZapchrIgEoLihknIdj315gPPZ6q6CIwRASbmex5Ye4GJOsdqlCCshAShu6PlVR+SqDsKsXM4r4dGlByguu/kkMyGMIQEoqrTwl9OsSUxXuwwhrnP0fA7TVh5WuwxhBSQAxXV2JWfwzo9/qF2GEDe0/sgF5m05qXYZwsJJAIpKzmcXMWn5IXRyprswc7N/PsGW45fULkNYMAlAYaDXKzyz/BCZBaVqlyLELSkKTF91hEu5MilG1IwEoDD4eMcpDpzLUrsMIYyWWVBasTSfHLEQNSABKAA4lp4jS04Ji7Tr1FU+lovpihqQABSUlOv4vxWJssansFhzfj7BsfQctcsQFkYCUPDej39y4lK+2mUIUWNlOoVnVxympFzODxTGkwC0cbuSM1j86xm1yxDitv15KY//xMthfGE8CUAblldcxrSVh+XCtsJqLEo4zdE0ORQqjCMBaMNm/3SSdFlXUVgRvQKv/JCEXORGGEMC0EadvJTH0t1n1S5DCJM7lJLNygNpapchLIAEoI16bd3vlMu5U8JKvfvjH+QUlaldhjBzEoA26Meki+xMzlC7DCFqzdWCUt6P/1PtMoSZkwC0McVlOt7c+LvaZQhR677am8Lv6blqlyHMmASgjVmw4zSpmXKBW2H9dHqFV9YmqV2GMGMSgDYkPbuIT2TJKGFDDpzLYsORC2qXIcyUBKANmb/1JEVyJW1hY+ZtOSmnRYgqSQDaiPTsIlb/dl7tMoSoc39eyuPHpItqlyHMkASgjfhkxylKdXq1yxBCFXOlFyiqIAFoAy7nFbNif6raZQihmj8u5rH5mFw9XlQmAWgDPt1xmpJy6f0J2yZjgeJaWrULELXran4Jy/amqF1GlcqupnHlh3cNt8szz+MzdDoaRxeyti0GRY+9Wz187n4OexcPMrcspPhsIi7NO1Kv10MAZCd8hXNQGM7BYWq9DGEhfr+Qy0+/X6Jf+0ZqlyLMhPQArdyinWfMduanQ4NA/B+cj/+D82k09j00Ds44N40ka8tCfO9+Dv+HPsDRrwX5iZvQF+dTeukU/g9/SMmFE+hLCijPu0pZ5nkJP2G0+VuT1S5BmBEJQCuWX1LOl7vPqV2GUYqS9+IcHI6dozNoNOhLK07W15cWYu9eHzR2oNGgKHrQaAANObuW4x1zn7qFC4ty9HwOB1Oy1C5DmAk5BGrFvj90nvyScrXLMErBHztxb98bgPr9nuTyyplo7LVovRtRv+/jaOzscWkayYXPJ+PW9k7Kcy+Dxh4HnyYqVy4szdd7U+gQVE/tMoQZ0CgyKmy1Bsz5hT8u5qldxi3pSwo5/+mjBD7xORqtI1e+fwuvbqNx9GtB1rbFaJxc8e42ptI2V9a+S/2+j5F3aBNlV87i1r4nrnd0U+kVCEvi7GDH3hf74uXioHYpQmVyCNRKHTibaRHhB1B4cg8uTSPRaB3RFeZQdjUNR78WALi2iaXk/PFKjy86m4iDTxD6kkLKc6/gc+8L5B74QY3ShQUqLtPz3UG5XqCQALRaX+8zz5mfVSn8IwHXtt0BsHN2R1eUQ1l2xcodxecO41A/0PBYRVHIO7AWz87DUMpKQF8OaNAX56tRurBQX5vpzGhRtyQArVB+STmbjlrG0k/6kgJKLpzEpVkHADR29tS/6wmurH6d9MWTKE5Nwit6lOHxBce24XpHNHYOzjg0bIZSXsqFz57C7b/jh0IY4+TlfPadyVS7DKEyGQO0Qt/sS+GF746qXYYQZu2eCH/mjolUuwyhIukBWqGVv8n4hhC3sinpIrnFZWqXIVQkAWhlzmcX8ds5Oc9JiFspLdfz8++yPqgtkwC0Mj8ds4yxPyHMwUYLGSsXtUMC0Mr8dFw+0QphrF9OXiFPDoPaLAlAK5JTVMbe0zKzTQhjlZbr2frHZbXLECqRALQi2/64TLleJvUKUR0/H5cAtFUSgFbkJxnQF6Ladvx5mXKdXC/TFkkAWonScj07TlxRuwwhLE5ucbmcFG+jJACtxK5TGRZz5QchzM2Ok/Lh0RZJAFqJX5Mz1C5BCIt14KycO2uLJACthJz8LkTNHU3LobhMp3YZoo5JAFqBknIdSem5apchhMUq1ek5nJqtdhmijkkAWoGk8zmUlsssNiFuxwE5imJzJACtgBz+FOL27T8rM0FtjQSgFZAAFOL2HTyXhV4WkrApEoBW4GBKttolCGHxcovL+fNSntpliDokAWjhUjMLuZJXonYZQlgFmQhjWyQALdyx9By1SxDCapy6kq92CaIOSQBauDMZhWqXIITVOH2lQO0SRB2SALRwZzLkE6sQpiI9QNsiAWjhzmTIJ1YhTCU1q0jOqbUhEoAWTg6BCmE6Or3CuavyodJWSABasLziMjLyZQaoEKZ0SsYBbYYEoAWTw59CmJ6MA9oOCUALJgEohOnJIVDbIQFowc5nF6ldghBWJ7OgVO0SRB2RALRgV/PlF1UIU5MAtB0SgBZMflGFML3swjK1SxB1RALQgl2VABTC5DIL5ffKVkgAWrBs+UUVwuRyi8rQyWWRbIIEoAXLLZJDNUKYml6RD5e2QgLQguWXlKtdghBWKUvGAW2CBKAFyy2WABSiNkgP0DZIAFoonV6RRXuFqCWlOvndsgUSgEIIcQ295J9NkAC0UHYatSsQwnrpFJkFagu0ahcgakajkQS0JD7ujrTwdVe7DGEkT2f502gL5KdswTQakA+qliGwnisrHo9WuwwhxN/IIVALZie9QItx/EIuZTKxQgizIgFowWQc0HKUlOv582Ke2mUIIf5GAtCCyTigZTmSlqN2CUKIv5EAtGBa6QJalCNp2WqXIIT4GwlAC+bp7KB2CaIapAcohHmRALRgDdwd1S5BVMOJS3kUl+nULkMI8V8SgBasvpsEoCUp1yscS89VuwwhxH9JAFowH3cntUsQ1STjgEKYDwlAC9ZAeoAWR8YBhTAfEoAWrL6MAVoc6QEKYT4kAC2Yj5scArU0pzMKyCuWi60KYQ4kAC2YzAK1PIoCR8/LYVAhzIEEoAULrOeqdgmiBmQcUAjzIFeDsGDNfNzQ2mko18slISzJURMGYFF5EZvObCK7JNtkbYraM7jZYPzc/NQuQ/yXBKAFc9TaEdTAldNXCtQuRVTDYRNOhHHRujCg6QC+/fNblv6+lCtFV0zWtjC9Dg07SACaETkEauFaykVWLU5aVhGZBaUma8/VwZUJIRP4ccSPvNz1ZQLdA03WtjAtBztZvtCcSABauFZ+EoCWyJS9wL842jsyqvUo1g9bzzvd36Gld0uTP4e4PVo7OehmTiQALVyrhh5qlyBqwJTjgNeyt7NncPPBfHf3d8zrNY8w37Baey5RPfYae7VLEH8jAWjhWjaUHqAlqosT4jUaDb2CerFs0DI+6/cZ0Y2ja/05xc1JD9C8yE/DwrVs6I6dBmQiqGU5XMenQnRu3JnOjTtzLOMYC48uZGvKVhTkTVPXHO3l3F1zIj1AC+fsYE8zHze1yxDVdCWvhAs5RaZrsLzEqIe192nPnF5zWHPPGu5ucTdajXwGrisaNPi6+KpdhvgbCUAr0DG4ntoliBow6Qnxnw+EXfOh1LhTYpp7N+fN2DfZMHwDY1qPwcleltWrbfWc6+FgL7NAzYkEoBWICq6vdgmiBkw6DujeCOJnwOz2sO1tKMw0ajN/d39e6voSP474kYdDHsbdQcaUa0sjt0ZqlyCuIcc/rEAH6QFaJJP2AAMi4c8NUJQFO96B3R9AxwkQPQk8G99ycx8XH6Z0nMLDoQ+z/I/lLDu+jMxi40K0tpVcKCH1o9T/3b5YQpOJTcjZm0Px+WLq96xPg7saAJD2WRq+g31xamR+PVo/VzkB3txID9AKtGzojo8sjG1xTBqA/h0q3y7NrwjBueGw7hnIPGNUMx6OHjwW9hg/jviRFzq/YBa9FqfGTrR8oyUt32hJs5eaYedkh4OvAxqthpb/aklWQhYAReeKsHe2N8vwA+kBmiMJQCvRpXkDtUsQ1ZRTVMa5qyZaxs4/surv60rgtyUwvyOsehguHTOqORetC2PbjmXj8I283u11mno2NU2dtynvUB5u7dzQ2GtQFAV0oNFqALjywxV87zbfSSbSAzQ/EoBWIloC0CKZ7HQI1/pQr+mN71d0kLQKPo6Br8dA6n6jmnWwc2BYq2GsvXct/+nxH9rWb2uaemsoZ18OXp29cA5wxt7VnlOvnaJ+r/rkHcnDpZkLWg/zHdWRHqD5kQC0Et1aSABaoiOp2aZr7NrDoFVS4MQm+KwvLBkCyVuMatpOY0e/pv34dui3fNL3Ezr6dby9WmtAV6SjMLkQj7CK1Y/87/en5Rst8Y7x5urPV2lwVwPSv0onZX4KBSfMb4F46QGaHwlAK9Hc152g+nJ9QEtj2okwxgTg35xNgK+Gw6c94fcfKq7Wa4SYgBiWDFjC0oFLuTPwzurXWUO5B3NxD3HHzrHyn62shCy8unhRcLIArYeWwMcCufKD+V0VQ3qA5kcC0IoMCJFfMEuTlJ6D3lTL+BjVA6xC+iH49n74sAskfg26cqM2i2wYyYd9PmTV0FUMbDqw1te5zN2Xi1dnr0rf05foyTuYh3c3b5QSBaW8Yl/qCnW1Wkt1adBID9AMSQBakYESgBansFRH8pV80zTWOBw0t/ErnfEnrHkC5kXC3k+hrNiozVrXb817Pd7jh3t/YESrEbVyyR9doY7CM4W4h1Y+TzHjxwwa9G+ARqPBPdSdwuRCTr12igb9zGtIoL5zfTkJ3gxpFMXI4x7C7CmKQsw7W0nPMe4PlzAP/x4ZRlxUE9M09mEXuPKHadpyawhdn4BOj4Czp9GbXSq4xBe/f8GqE6soKjfhcm8WLMw3jGWDlqldhriG9ACtiEajob/0Ai1OrZ4PeDsKLsOW12B2CGx5HQoyjNrMz82P5zo9R/yIeCaGT8TT0fjwtFbtG7RXuwRRBQlAKzMw5NarfgjzYtIl0ao7EcYYJTmQ8J+KINz4HGSn3nobwNvZm6ciniJ+ZDzPdnwWHxcf09dmISQAzZMEoJWJCq6Hr4d5roQhqnb8Yh5lOr1pGrvRCfGmUF4E+xZUjBGueRIyThq1mZuDGw+GPMjmEZt5uevLBLgH1F6NZirEJ0TtEkQVJACtjJ2dhv7tZbaZJSkt1/PHhTzTNNYoFGphEkol+jJIXAYfdoYV90N6olGbOdo7Mqr1KDYM28Db3d+mpXfL2q3TTLhqXWnm1czox2s0GmbMmGG4PW3aNJYsWVKj596+fTv79u2r9nYTJkxg/fr1VX6/efPmhIeHExYWxpYtxp1Heq1PPvmEFStW1GhbU5IAtEIjOgSqXYKopsOmOgyqdQK/dqZp61YUPRz/AT7tAV8Oh7M7jdrM3s6eIc2H8N3d3zGv1zzCfMJquVB1tWvQDrtqzM51d3dn2bJl5OXd/oeimwWgTlezU0XmzZvH4cOHef/995k4cWKN2pg4cSKjR4+u0bamJAFohSKD6hESIBMPLIlJxwFNORHGWKe2wJLB8Fl/OLHZqE00Gg29gnqxbPAyPuv3GV0bd63lItUR6htarcc7OTkxduxYPvroo+vuO3XqFP379ycqKorevXtz9uxZAHr27ElSUhIASUlJ9OzZk9TUVD755BPeeecdIiIiSExMZMKECTzxxBN07tyZd955hzVr1tC5c2ciIyMZPHgw2dnZRtcZGxtLWlqa4fa7775Lp06dCAsLY9asWQCMHj2arVu3Gh7Tu3dvDh06xKuvvsoHH3xww9eUnp5OTEwMAPHx8bi4uFBaWkp2djaRkRWH+efMmUPr1q0JDw/niSeeMH4H/435Lpwnbsu4LsG88N1RtcsQRjLtTNBI+O1z07VXHal74OtR4BcKsVOg/TCwu/UJ8p0bd6Zz484kZSSx8MhCtqVuQ8E6ztCK8ouq9jbPPPMMXbt25Zlnnqn0/SeffJIFCxbQtGlTtm7dyvTp01m5cmWVbTRp0oSJEyfi4+PDpEmTDN+/evUqe/fuRaPRkJWVxT333INGo2HevHl8+OGHvPTSS0bVuGHDBu6++26gIqTS0tLYt28fer2eu+66iwEDBhAXF8fKlSvp3bs3ly9fJj09ncjISNauXXvL15SVlUVJSQk7d+6kXbt2/Pbbb2RlZREdHQ3A66+/TmpqKm5ubuTk1Oz3RwLQSt0TEcBbG4+TW2zcqh5CXScv51NUqsPF0QSrqdTGTNDqunQUVj8M296EmGcg/D7Q3vqSXSE+IcztPZdT2af47OhnbDqziXLFct/Ddho7OjSs/s/D19eXIUOGsHjxYsP38vPzSUhI4N577wUqzvt1c3OrdtsjR45Eo6m4gkZKSgpxcXFcunSJoqIiunTpcsvtJ0+ezLPPPktKSgq//vorUBGAGzZsICEhAYC8vDxOnDjBoEGDeO6559DpdHz//fcMHz68Uls3e01RUVHs27ePvXv3MnXqVHbu3ElWVpahZ9i5c2fGjRtHXFycYfvqkkOgVsrF0Z7hMhZoMXR6hWPpJuoF+rYFrYtp2rpdmacrrkc4Nxx2fQClxi1S3cK7BW91f4v1w9czuvVonOwtc2Zz63qtcXd0v/UDqzBt2jTmzp1LeXnFBwC9Xo+fnx+JiYkkJiZy+PBhdu3aBYBWq0Wvr5hJXFJSctN2XV3/t2bw5MmTee655zh69Chz5sy55bZQMQZ44sQJ3n77bR599FFDbTNnzjTUdurUKYYPH46rqyudOnXil19+YdWqVcTFxVVq62avKTY2lh07dlBSUkK/fv3YtWsXv/76qyEAN2zYwKRJk9i9ezc9evQwZpdeRwLQit0fHax2CaIaTHZpJHstNDaziSV56RD/UsW5hNvfrbhyvREC3AOY0XUGP474kYdCHsLdoWZhopbbuWpGkyZNiImJYfXq1QB4enri5+fHunXrgIpJLH+N+wUHB5OYmAjAd999Z2jDw8PjppNpcnNzCQgIQFEUli5dWq36pkyZQnl5OfHx8fTr149FixZRWFgIwNmzZw2HJePi4vj4449JS0szjN/95WavKTY2lgULFhAREYGPjw8ZGRmkp6fTtGlT9Ho9qamp9OnTh1mzZpGSklKjST0SgFasha+7XCbJghy19IkwxijKhO1vwexQiJ8BeZeM2szHxYf/6/h/bB65macjn6a+c/1aLtQ0ohpVf/zv755//nnS09MNt7/++mvmz59PeHg4oaGhhtMQnn32Wd577z06duxIaWmp4fFDhw5l+fLlhkkw15o5cyZDhw6lU6dONGlSveX4NBoNr7zyCrNmzWLAgAEMGzaMrl27EhISwrhx4ygurliScdCgQWzcuJFhw4ZV2c6NXlPbtm0pKioy9Pjatm1Lhw4V72udTsfYsWMJCwsjKiqKV155BXv76g8fyFqgVu7HpAtM/Oqg2mUIIzT3cWPrtJ6maezwCvj+MdO0VZvsnSDivooJMze7oO81isqL+O7kdyw5toSLBRdrrbzb4WTvxI7RO3BzqP44nagb0gO0cv3bN6K1n4faZQgjnLlaQG5xmWkaM4eJMMbQlVTMWJ3XAVY/Apd+N2ozF60LY9uOZePwjbze7XWaejat3TproHtAdwk/MycBaOU0Gg3P9G2ldhnCCIoCR001DtigJTh53fpx5kLRwdGV8HE3WP4PSDtg1GYOdg4MazWMtfeuZVaPWbSt37aWCzXewGYD1S5B3IIEoA0YGNKINo2kF2gJTHY+oEYD/uGmaatOKfDnRljUB5YMgVPbjNrKTmNH/6b9+Xbot3zc9+ManXpgSm4ObtwZeKeqNYhbkwC0ARqNhil971C7DGEE064IU4sLY9eFswnw5b3waS84vq6ii2yE2IBYvhj4BV8M+ILuAd1rt8Yb6NWkF85aZ1WeWxhPAtBG9G/vR3t/WR7N3JnttQHVlH4QVoyDj7pC4nLQGXdifAe/DnzU9yNWDl3JgKYDqrUe5+2Sw5+WQQLQRkgv0DKczy4iI//WJyMbxVImwhjryh+wZiLMj4R9C6Gs2KjN2tRvw797/Jsf7v2B4a2G41DLV8vwcvIi2j+6Vp9DmIYEoA25q50foQEWNDHCRplsIox3ELha4UVos1Ng4zSYEwoJ70NxrlGbBXsG81q319g0fBPj2o7DpZZWy+kb1LfWQ1aYhgSgjfnnoDZqlyBuwWSXRgLLHwe8mYLLsOU1mBMCW96AgqtGbebn5sfznZ8nfkQ8j4c9jqejaYcGBjUbZNL2RO2RALQx3Vr4MDi0sdpliJsw6TigtR0GrUpxDiTMqgjCTc9DznmjNvN29mZS5CTiR8bzbMdn8XG5/d6yr4vvba/+IuqOBKANenFwW1wcTHDVAVErLP7agGopK4S9n1QsvL3mKchINmozNwc3Hgx5kB9H/MiMLjMIcA+ocQn9m/av08k24vbIT8oGBXi78GTPFmqXIW4gI7+U89lFpmnMFnqA19KXQeJX8GEn+HY8XDhs1GZO9k6MbjOa9cPW81bsW7T0blntp767xd3V3kaoRwLQRj3eowUtfGWZJnNlsoWx3RuCZ817NBZN0cPva2DBnfDVCDj7q1Gbae20DG0xlO/u/o65veYS5mPclTU6NepE2wbmsxKNuDUJQBvlqLXjrWGh/Pe6mMLMmOzSSGDdE2GMlfwzLBkEiwfAiXijNtFoNPQO6s2ywctY1G8RXRrf/GKxE9pPMEGhoi5JANqwLs0bMFIummuWTDoOaIuHQW8kZTd8HQefxELSavjvRWRvpUvjLizqt4jlg5fTu0lvNFT+5NjCq4Vqq86ImpMAtHEzBrfD30uWbDI3R9NyMNmVymxpIoyxLh6FVQ/BB1Hw2xdQXnrrbYAQnxDm9p7L9/d8z9DmQ9FqtAA80P4BNHI4xeLI9QAFe05f5b6Fe9DLO8GsbJvWk2Y+JhinLcqGd4Nvvx1r5hkA0ZOg4wRwdDV6s/P55/nmj294OvJpHO0da68+USskAAUA/978Bx9uO6V2GeJv5o6J4J4IE01gmRcJmadN05Y1c20AXSZC50fBpZ7a1YhaJodABQD/1/cOwpt4q12G+JvDqbIwdp0rvArb3oTZoRD/MuRdUrsiUYskAAUAWns75o2JwN1Jq3Yp4r9kIoyKSvNg1zyYGwbr/w+yzqpdkagFEoDCILiBG6/e3V7tMsR/HUvPRWeqgVk5FaJmyovhwGKY3xG+ewwuH1e7ImFCEoCikpEdA7k73F/tMgRQVKbj5OU80zTWOBw0svxdjenL4cgK+Cgalt8Hab+pXZEwAQlAcZ13RoTSrrFcPNccHDHVOKCjG/i2Nk1bNk2BPzfAot7wxVA4vV3tgsRtkAAU13F11PLZhCgaejipXYrNM+2lkWQc0KTO/AJL74GFveH4epAJ9RZHAlBUqbGXCwsfiMLZQd4iajp63pSXRjL9OOCwFYXUezeXkd8WGr7Xc0kBbT7IJ+KTin9FZRXB8OzmYkI/zmd6/P+u5P7KtmK2nSk3eV116vxvsPYpKDHR4WpRZ+Svm7ih8CbezIoLl/VCVfTHhTxKy41bruuWamEizDNdHFl67/VXVl81yoXEie4kTnTHxUFDdrHCbxd0HH3CnX3pOnKKFdLz9Jy4qqdXMyuYeRz9FDjLsIGlkQAUNzUkzJ8pfe5QuwybVarTc/xCrmka8wsFE69W0rOpFg+nW39CsteAnQb0ioLdf79+fUcJM3tYwWF2Z++Kk+eFxZEAFLf0TN9WMjNURSY7H1DrCH51c5rLfauLiFyQz/u7SwDwcNJwV3MtkQsKuKu5lnM5euw10NbXCmamSu/PYlnBsQdRF94bGUZmQSk7kzPULsXmHDHppZE6QPoh07VXhWXDXQjwtCOnWOHubwpp3cCOwXc48GJ3J17sXtHjG72qkHkDnHltewlHL+sYG+rAsLYOtVpXrZDen0WTHqAwirODPYvGR9G1eX21S7E5pg3A2j8hPsCz4s+Kl7OGUe0c2J+uq3T/ltPlhPjak1OikJKj59s4F+bsNe5qDGan29PS+7NgEoDCaM4O9iye0InOTSUE61LylXwKS000U7KWl0Qr1ytkFFZM2inVKWxKLqf93w5zKorCnL2lTO3mSGEZlOpBA2QVWeApBA1aVQSgsFgSgKJaXB21fP5gJzoGy0r5dUWnV0g6b6KJML5twMH4y/3cSt+lBcStLGLjyXIC389jb5qO/l8VEvZxPpELCghpaMfIdv8bafnqSBnD2mhxddAQ7mdHcblCyMcFPBBugYc/h8wGrRVM4rFhcjkkUSN5xWXc/9k+ElOz1S7FJswY3JZHujc3TWOLB1RcGV3UXPh9MOxjtasQt0l6gKJGPJwdWPpwZ0IDvNQuxSZY2jigVXOpD/3+pXYVwgQkAEWNeTo78NUjXejcTMYEa5tJL40kS6Ldnv5vglsDtasQJiABKG6Ll4sDXz7cmYEhjdQuxaqdvVpITmGZaRqTawPWXNPuEHGf2lUIE5EAFLfNSWvPh/d14IHoYLVLsWpHzmebpqH6zcFZDl1Xm70TDJmjdhXChCQAhUnY2Wl4/Z4QZgxui52sHVorTDYOqNFA4wjTtGVLuj8LPi3VrkKYkASgMKlHujfn0/ujcHW0giWuzIxJxwHlMGj1NGgFsc+qXYUwMQlAYXJ92/mxcmI0Tepff5UAUXMmXxJNGEkDQ+dUrKUqrIoEoKgV7f29WP90d/q391O7FKtxIaeYy3nFt36gMaQHaLyuT0LTWLWrELVAAlDUGi8XBxbcH8WrQ9vhaC9vNVM4aqpeoFcguDU0TVvWrNmd0O8NtasQtUT+KolaNyGmGaueiCaovumW4LJVh+WE+LrjFQQjl4CdjGdbKwlAUSfCAr1ZPzmWQaFyvuDtkIkwdUTrAmO+khPerZwEoKgzns4OfDS2I28OC8HdSS5FWRMmOwQKMhHmZu6eB43D1a5C1DIJQFHnxnYJ5qdn7+SudjJBprquFpSSllVomsakB1i1rk9C2Ci1qxB1QAJQqKKxlwsLH4jik3Ed8POUS8pUh8lOh3DzAa8mpmnLWjTtDnfJpBdbIQEoVDUgpDE/PduDsV2C0MgKMkY5bNKFsWUijIFXEMR9AfZyeN5WSAAK1Xk6O/DmsFBWPh7NHX7uapdj9o6kmnAcUA6DVpBJLzZJAlCYjaim9dn0zJ28MzyUxl7OapdjtpLSczDZdaxlIkyFoXNl0osNkgAUZsXeTsOYzkFsm9aTFwe1wdvVQe2SzE5ecTmnMwpM05h/BGDjx54H/hvCR6tdhVCBBKAwS84O9jx2Zwt+ea4Xk3q1lMW1r2Gy8wGdvaBBC9O0ZXE0MGgWdHlM7UKESiQAhVnzdHZgWv/W7Jjei/HRwThp5S0LcNiU44A2eRhUA4NnQedH1S5EqEj+mgiL4OvhxGv3hPDrC72Z3KcV9d1se2X+o+dlIkzNaWDIbOj0iNqFCJVpFJONpgtRd4rLdKw+mMbSXef481Ke2uXUOWcHO5Je7Y/WFIuMp+yBxf1vvx2LoKmY8NJxvNqFCDMgASgs3u5TV1m6+yw//X6Jcr3tvJ03Tu5OO3/P22+otBDeDgRFd/ttmTUN3D0fOtyvdiHCTMgZn8LiRbdoQHSLBlzOK2bDkQv8cDidQynZapdV646kZZsmAB1doWFbuJR0+22ZK41dRfhFjlO7EmFGpAcorFJqZiE/HE5n3eF0/rhonYdI/9E5iLeHh5qmsbWT4NCXpmnL3Gjs4J4PIeI+tSsRZkYCUFi9k5fy+OFwOpuSLpJ8OV/tckwmJMCT9U93N01j+z+DDc+api1zYudQEX5ynp+oggSgsCmXcov5NTmDnckZ7Eq+ysXcYrVLqjEHew1Jr/XHSWuCcyTTD8GnPW+/HXPi5gujvoTgaLUrEWZKAlDYtOTL+ew6lcHOkxnsP5tJVmGZ2iVVy/dPdiMyqN7tN6Qrg7cCQFdy+22Zg8bhMOZr8ApUuxJhxiQAhfibiznFHL+Qy/GLuRy/kMfxC7mcyShAZyazSz2ctLT196S9vyft/b3o1dqXBu4mupzUwt5w/jfTtKWmkBEVhz0dXNSuRJg5CUAhbqG4TMeJS3mcuJTP+awi0rOLSM+p+P9KXgm5xeUmey5HrR2B3i4E1HOhSX1XAuu50KTef/+v74qPqcKuKhumwv5Ftdd+bdPYQ+8Z0N0KxzJFrZDTIIS4BWcHe8ICvQkL9K7y/pJyHRn5pVzNL6G4TE9puZ5SnY7Scj0l5X/drvjfwd4Odyctbk5a3BztK/530uLupMXVyR4PJy0atS6MaMlLork3gpGfQdNYtSsRFkQCUIjb5KS1J8DbhQBvCz/kZqlLojXvCcMXgbuv2pUICyMBKISo4NMaHN2h1EJOFdHYQY/n4c7nwE6WNRbVJ+8aIUQFOztoFKZ2FcZp0ArGr4OeL1Qr/DQaDTNmzDDcnjZtGkuWLDFpaWvWrOHEiROG24888ginTp267Xa1Wi0RERG0b9+eoUOHkp2dXaN2Bg0aRFFR0W3XYw0kAIUQ/2Puh0G1LhUTXZ7YVaPxPnd3d5YtW0ZeXu2tDnRtAC5atIgWLW7/move3t4kJiZy7NgxvL29+fDDD2vUzsaNG3FxsfDD9SYiASiE+B//SLUruLFW/eCpPXDndNDW7HJYTk5OjB07lo8++ui6+06dOkX//v2Jioqid+/enD17FoDdu3fTvn17IiMjeeqppxg5ciRQEXSdO3cmMjKSwYMHk52dzd69e/nhhx+YPHkyERERXL58mZ49e5KUlMTHH3/MK6+8Yni+119/ndmzZwPw7rvv0qlTJ8LCwpg1a9YtX0dMTAxpaWkAXLlyheHDhxMVFUV0dDSHDh0iJyeHVq1aGR5/7tw5IiIiAGjatCn5+RWHub/88ks6depEeHg4zz5bMXv2rbfeYuHChQDcd999PPzwwwDMmzeP999/n/z8fAYMGEBoaCihoaFs3rzZ6P1vbiQAhRD/Y449QM+AihVdxq6Eek1vu7lnnnmGTz/9lOLiyqsAPfnkkyxYsIADBw4wY8YMpk+fDsCjjz7Kl19+aQiWv/To0YO9e/dy6NAh+vfvz4cffkiXLl24++67mTdvHomJiTRs2NDw+OHDh/Pdd98Zbq9evZq4uDji4+NJS0tj3759HDp0iI0bN5KUdOOFyXU6HT/99BNDhgwBYMqUKfzzn//kwIEDLF26lIkTJ+Ll5UXr1q3Zu3cvAKtWrSIuLq5SO8ePH2ft2rXs3r2bw4cPk5GRwYYNG4iNjWXnzp1ARXD+1ZvduXMnsbGxbN68mQYNGnD06FGOHDlCdLTlrrQjk2CEEP9Tvzm41IOiLLUrATstdH0CerwATu4ma9bX15chQ4awePFiw/fy8/NJSEjg3nvvBUBRFNzc3MjOzqasrIwOHSo+GIwePZovvvgCgJSUFOLi4rh06RJFRUV06dLlps/r5+eHr68vSUlJODo64ubmRmBgIHPmzGHDhg0kJCQAkJeXx4kTJwgJCam0fXZ2NhEREaSlpdGqVSv696+4huPPP//MsWPHDI/Lyqr42cXFxbFy5Uq6dOnC6tWrrxvr3LJlC3v27CEqKgqAwsJCOnbsyOOPP87EiRNJSUkhKCiIkpISrly5wsGDB4mMjMTb25spU6bw3HPPMWzYMAlAIYQVaRwBp7epW0OTrjDkffBrXyvNT5s2jb59+zJw4EAA9Ho9fn5+JCYmVnrcX2FSlcmTJ/PSSy/Rr18/1q9fb9RkmlGjRrFy5UocHR0NPTK9Xs/MmTMZP/7mF+n9awywoKCAu+66i48++ojJkycDcODAAbTayn/O7733Xt58802eeeYZioqKuOOOOyrdr9frefTRR5k5c+Z1z1WvXj1WrVpFbGwsxcXFfPnllwQGBuLg4MAdd9xBYmIi69ev59lnn2Xs2LFMmjTplq/dHMkhUCFEZWoeBnXzhbs/gId+rLXwA2jSpAkxMTGsXr0aAE9PT/z8/Fi3bh1QcZgxKSmJevXqodVqDcG4cuVKQxu5ubkEBASgKApLly41fN/Dw+OGk2z+Ogz61+FPgH79+rFo0SIKCwsBOHv2bKVDrddyc3Nj3rx5/Oc//6G8vJxevXrx8ccfG+4/fPgwAF5eXtxxxx08//zzhnHLv+vTpw8rVqzg6tWrAFy+fJkLFy4AFWOMs2fPJiYmhtjYWGbPnk1sbMWko/T0dNzc3Bg/fjxTpky57kODJZEAFEJUpsaKMPWaweD3YUpSxRXb62A1nOeff5709HTD7a+//pr58+cTHh5OaGgoW7ZsAeDTTz9l7NixdOjQAScnJzw9Ky5CPHPmTIYOHUqnTp1o0qSJoZ0xY8bwxhtvGCbB/J2fnx8+Pj44OzsTGFixUPeAAQMYNmwYXbt2JSQkhHHjxl03PnmtqKgoQkND+fbbb5k/fz7bt28nPDyctm3b8vXXXxseFxcXx/Lly68b/wNo3749L730En369CEsLIzBgweTmZkJQGxsLDk5OYSGhtKhQwcyMzOJiYkB4OjRo3Tq1ImIiAjmzJljmDxjiWQtUCFEZbnp8H7bunmuxhEQOwXa3mO2J7MXFBTg5uYGwKRJk2jTpo3FHvITlZnnO04IoR5P/4q1NWtT817wwFp4fAe0H2a24Qewdu1aIiIiaNeuHVevXjWcFiAsn/QAhRDX+3oMnNhk2jY19tD+Xoh5puJ6fUKoTGaBCiGuF9DBdAGodYHIcdBtkknO4xPCVCQAhRDXu92JMPZO0LIPtLsHWg8EZy/T1CWECUkACiGuV5Ml0bTO0LIvtLsXWg8AJw+TlyWEKUkACiGu59YAvIMgO+Xmj9O6QKu7Knp6dwww6YotQtQ2CUAhRNX8O1QdgI7uFT299vdWLFDt6FbnpQlhChKAQoiqBXSA39dU9ASbdPnvv87gFwJ29mpXJ8Rtk9MghBBVK7gK+jLwqOVzAoVQiQSgEEIIm2S+yy8IIYQQtUgCUAghhE2SABRCCGGTJACFEELYJAlAIYQQNkkCUAghhE2SABRCCGGTJACFEELYJAlAIYQQNkkCUAghhE2SABRCCGGTJACFEELYJAlAIYQQNkkCUAghhE2SABRCCGGTJACFEELYJAlAIYQQNkkCUAghhE2SABRCCGGTJACFEELYJAlAIYQQNkkCUAghhE2SABRCCGGTJACFEELYJAlAIYQQNkkCUAghhE2SABRCCGGTJACFEELYJAlAIYQQNkkCUAghhE2SABRCCGGTJACFEELYJAlAIYQQNkkCUAghhE2SABRCCGGTJACFEELYJAlAIYQQNkkCUAghhE2SABRCCGGTJACFEELYJAlAIYQQNkkCUAghhE2SABRCCGGTJACFEELYJAlAIYQQNkkCUAghhE2SABRCCGGT/h+WfoYnNMFfUAAAAABJRU5ErkJggg==</t>
+  </si>
+  <si>
+    <t>https://www.flipkart.com/micromax-x512/p/itmfhwvhrwhxq5tu?pid=MOBG8Z47Q9FT9AKJ&amp;lid=LSTMOBG8Z47Q9FT9AKJ1VUFP7&amp;marketplace=FLIPKART&amp;q=micromax+x512&amp;store=tyy%2F4io&amp;srno=s_1_1&amp;otracker=search&amp;iid=e532b5ae-9020-461a-a39a-dca423c959b8.MOBG8Z47Q9FT9AKJ.SEARCH&amp;ssid=0udxp3g2jk0000001689862408205&amp;qH=8aab057c4a7cd0c3</t>
+  </si>
+  <si>
+    <t>Micromax X512</t>
+  </si>
+  <si>
+    <t>₹1,107</t>
+  </si>
+  <si>
+    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAcAAAAFQCAYAAAAoQ64wAAAAOXRFWHRTb2Z0d2FyZQBNYXRwbG90bGliIHZlcnNpb24zLjYuMSwgaHR0cHM6Ly9tYXRwbG90bGliLm9yZy/av/WaAAAACXBIWXMAAArEAAAKxAFmbYLUAABBgklEQVR4nO3deVwU9eMG8Gd3uW/kUi4VPBDlUPEEBY/IO03RyvpppmWXmnmUeZXdX8urMsvKMjPPvE1LpcAzVFS8RREQFDnlXNjd+f3Bt/2KgqLCzO7O8369fMmxM59nF5ZnPzOzMwpBEAQQERHJjFLqAERERFJgARIRkSyxAImISJZYgEREJEssQCIikiUWIBERyRILkIiIZIkFSEREssQCJCIiWWIBEhGRLLEAiYhIlliAREQkSyxAIiKSJRYgERHJEguQiIhkiQVIRESyxAIkIiJZYgESEZEssQCJiEiWWIBERCRLLEAiIpIlFiAREckSC5CIiGSJBSgTUVFR+Pnnn+tl3QqFAunp6fWy7oeRmpoKJycnqWPIwty5czF27FjRxx09ejTef//9ar9niD//Jk2aID4+XuoYdAcWoESaNGkCGxsb2NnZwdPTExMmTIBWqxVl7BUrVqB37961um1qairs7OxgZ2cHW1tbKBQK/ed2dnb1nPTh+Pr6Ij8/X+oYRsHQXrxUJyUlBWZmZrW+van+/FmidY8FKKHdu3ejqKgIcXFx2LBhA7777jupI93F19cXRUVFKCoqQnJyMgDoPy8qKqq3cTUaTb2t2xAYy/0T60WZMTGWnx3dHwvQAPj7+yM8PByJiYn6r61fvx6tW7dGgwYNMGjQIGRlZQEAbt68ib59+8LJyQmurq54+umnAQCxsbFo1qxZlfVW9+r+8uXLGD9+PGJjY2FnZ4fWrVvXyX3YunUrmjZtCldXV3z00Uf6r2u1WsyZMweNGzeGh4cH3nzzzRr/gERFRWHWrFkICwuDra0tKioq8Ndff6F9+/ZwcnJCVFSUvoTHjh2Ld999t8ryfn5+iI+Pv2vGkJubi2eeeQbu7u7w8/PDjz/+CAC4ePEiPD099beLjo5Gz5499Z97enri4sWLNT7md0pOTkb37t3h5OQET09PzJgxQ/+9FStWoEePHnjppZfg6OiIH374ocZc1VEoFFi6dOkDP8Z3bqK8/fckOjoaANCyZUvY2dkhLi4Oc+fOxdNPP42hQ4fCzs4Oe/fuxbZt2xAUFAR7e3s0b94c69atqzHn7XQ6HebMmQMfHx80atQIEyZMgFqt1j8ePXv2xMsvvwwHBwcEBgbi2LFj1a4nOjoaWq1Wv9UhNTUVAJCVlYVevXrB3t4e0dHRyM3NBXD3jPGDDz5Ao0aN4ODggKCgIJw5c+auMf5dZunSpfDw8ICvr2+VXQbV/W5u3LgRrVq1grOzMwYMGIBr167pb79z5040a9YMDRo0uOv39M7dEXf+jNasWYM2bdrA3t4eQUFBOH/+PMaOHYvU1FRER0fDzs4Oq1atqtXPgO5DIEk0btxYiIuLEwRBEM6fPy80bNhQmD9/viAIgnD48GHBy8tLOHnypFBeXi5MnTpVGDp0qCAIgjB9+nTh5ZdfFioqKoSysjJh//79giAIwr59+wR/f/8qYwAQ0tLSBEEQhMjISGHlypWCIAjCDz/8IPTq1avKbT/66COhf//+98ycmZkpVPcrA0AYNmyYUFhYKJw6dUqwtLQULl26JAiCIHz66adCjx49hKysLCEvL0+IiooSlixZUu36IyMjBX9/f+HixYtCaWmpkJqaKri6ugp///23oNFohMWLFwthYWGCIAjC7t27hcDAQP2yhw8fFry9vQWdTidcuXJFUKlU+u/169dPePPNN4WysjLh7NmzQqNGjYQTJ04IgiAIHh4ewqVLlwSNRiP4+PgIXl5eQnl5uXDp0iXBw8Pjno/5nS5duiTExsYKFRUVwoULFwQfHx/ht99+0z/mKpVK+OGHHwStViuUlJTcM1ddPcZz5swRXnjhBf167vw9uf135N/bW1paCrt27RK0Wq1QWloqxMbGCufOnRO0Wq2wfft2wdbWVsjMzKx2/bf75ptvhMDAQCEtLU3Izs4WunbtKsyZM0f/eJiZmQm//PKLoNFohHfeeUfo3r17teu58+cpCIIwatQowcPDQzhx4oRQWloq9OzZU5g9e/Zdtz979qzg7e0tZGZmCjqdTjh79qw++51jABBGjx4tlJaWCvv37xfs7e2F8+fPC4Jw9+/mmTNnBAcHByEuLk4oKysTXn/9dSEqKkoQBEHIysoS7OzshK1btwpqtVqYOnWqoFKp9M/325+Ldz6G8fHxgouLixAfHy9otVrh7NmzQkZGhiAIVf9mUN3gDFBCffv2hZ2dHVq2bImuXbvi1VdfBQB8//33eOWVVxAUFARzc3PMmjULmzdvhkajgbm5OTIzM5GWlgZLS0t07dq1TrK89dZb2LZt2yMtb2dnhzZt2iA4OBinTp0CAHz33Xd4//334ebmBicnJ7z55ptYv359jet54YUX0KxZM1hZWWHVqlUYMmQIunXrBpVKhddffx0pKSlISUlBz549cfPmTZw+fRoAsHbtWsTExEChUFRZ3/Xr1xEbG4uPPvoIlpaWCAgIwDPPPIONGzcCALp164a///4bx48fR3BwMEJDQ3Hs2DHExcUhIiICAGr9mPv7+yMyMhJmZmZo3rw5Ro4cWWWfjb+/P0aPHg2lUomCgoJ75qrPx/h+IiMjER0dDaVSCSsrK0RGRqJly5ZQKpXo168fgoKCkJCQcN/1/Prrr5gyZQq8vb3h4uKC2bNnY/Xq1frvBwQE4Omnn4ZKpcIzzzyDEydOPFDOmJgYBAcHw8rKCkOHDq12eTMzM6jVapw9exZarRYBAQFo2LBhjeucM2cOrKys0LVrVwwaNKjK43j77+b69esxePBgREREwNLSEh9++CHi4+ORmZmJHTt2oH379hgwYAAsLCwwd+5cKJW1+1O7YsUKvPTSSwgPD4dSqURAQAAaNWr0QI8L1R4LUEI7d+5EYWEhNm3ahISEBP0+tdTUVHzwwQdwcnKCk5MTfHx8YGZmhuvXr2Pq1Knw9fVFZGQkAgICDGa/oYeHh/5jGxubKvfl382HTk5OGDlypH5zbnW8vb31H6empmLlypX6ZZ2cnFBcXIxr165BpVJh2LBhWLNmDQRBwLp16zBixIi71peamoqysjJ9OTg5OWHZsmW4fv06gMoCjIuL0xfe7Z9369YNAGr9mF+7dg1DhgxBw4YN4ejoiIULFyInJ6fG+3avXPX5GN/P7TkBID4+HuHh4WjQoAGcnJyQkJBQ5X7VJCMjA76+vvrPGzdujIyMjPven9qqzfLNmjXDZ599hhkzZsDDwwNjx47FrVu3alynj49PlY8zMzP1n9/+uNx53+zs7ODi4oKMjAxkZmZWWY+NjQ1cXFxqdZ/S09PRtGnTWt2WHh0LUGIKhQJPPPEEevfurT+s28vLC/PmzUN+fr7+X2lpKby9veHg4IBFixYhNTUVK1aswOuvv47Lly/D1tYWpaWl+vXeuHHjnmOKxcvLC/v27dPfj4KCgmr3wVSXzcvLC+PGjavyOJSUlCA8PBwAMGLECKxduxaHDh2CUqlEp06dqh3fzs4OeXl5+nUUFhbi66+/BvC/GWB8fDy6deuGbt26IT4+HvHx8foZYE2P+Z1mzpwJZ2dnXLhwAQUFBZg0aRIEQajxvt0r14O412P8IL8X1eUEgOeeew6jRo3C9evXkZ+fj7CwsCr3qyaenp76/XVAZVHfvs+1th719/W5557DwYMHcf78eaSkpODzzz+v8bZpaWlVPr599nV7jjvvW3FxMXJycuDp6YlGjRpVWU9paWmVFwz3+pn4+PggJSWl2mxiPm/lggVoIKZMmYLly5cjOzsbzz//PL744gv9Jp3c3Fxs3rwZALB9+3ZcvnwZgiDA0dERCoUCKpUKLVq0QF5eHv766y+o1WrMmzevxrHc3d2Rnp4uytFsY8aMwcyZM5GZmQlBEJCSkoK//vqrVss+88wzWLduHeLi4qDT6VBYWFhlk1S3bt1QWFiImTNnYvjw4dWuw8vLC126dMHMmTNRUlICjUaDY8eO6QsiJCQEN2/eRFxcHDp06ICwsDAcPHgQmZmZCA0NBVDzY36nwsJC2Nvbw87ODklJSfd83+X9cj2Iez3GISEhiI2NxfXr15GVlYVFixZVWdbd3b3GP7i33y8XFxeYm5tjw4YNOHr0aK1yjRgxAp999hmuXbuG3NxczJs3D0899dQD3z9XV1fodLqHervG+fPnERsbi/LyctjY2MDS0rLan92/5s2bh7KyMhw6dAhbtmzB0KFDq73dsGHDsGnTJhw4cADl5eWYOXMmunbtikaNGqFfv344evQoduzYgfLycrz77rvQ6XT6ZUNCQrBx40ao1WokJiZW+Z0eNWoUli1bhoMHD0IQBJw/f14/C63Nz4oeDAvQQLRq1QqRkZFYtGgRunbtivnz5+P//u//4ODggHbt2mH//v0AgAsXLqBHjx6wt7dH//79sXDhQjRu3BiOjo5YtGgRhg8fjqZNm6JDhw41jtWzZ080adIEbm5uCA4OBgB8+OGH6Nu3b53fr6lTp6JLly4IDw+Ho6MjBg4cWOXV8b00bdoUv/76K6ZOnYoGDRogICBA/0IAAJRKJWJiYrB3794aCxAAVq1ahfT0dPj5+cHd3R2TJk3SvwJXKpXo2rUrAgICYGFhAQsLCwQGBqJz5876P5Q1PeZ3mj17Nvbt2wcHBwdMmDChxj+etcn1IO71GD/22GMYMGAAAgIC0KNHj7syzZ49G0OHDoWTk1ON7zFbsmQJJkyYAGdnZ+zatQuRkZG1yvXCCy9gyJAh6NixIwIDAxESEoK33377ge+fra0t3nrrLYSGhsLJyanKzOt+1Go1pk6dChcXF/j6+sLR0RFvvPFGtbdVqVQICwuDr68vYmJisGTJErRs2bLa27Zq1QrLly/H888/Dw8PD5w/f17/gsfNzQ2rV6/G66+/Dg8PD1hbW1fZfPrGG29ArVbD1dUV06ZNq/KiIDw8HIsWLcKYMWPg4OCAmJgY/Sbb6dOn46233oKTkxN++eWXWj8GVDOFUJttGUREJiwlJQXNmjXje/xkhjNAIiKSJRYgERHJEjeBEhGRLHEGSEREssQCJCIiWWIBEhGRLLEAiYhIlliAREQkSyxAIiKSJRYgERHJEguQiIhkiQVIRESyxAIkIiJZYgESEZEssQCJiEiWWIBERCRLLEAiIpIlM6kDEBFws1CNtLwSpOWW4MatMhSUVvz3n0b/8a3SCpSWa6EThP/+A5QKQKlQQKVUwNpcBQdrczhW88/D0Qq+DWzg28AGDWwtpL67D8XMzAxt2rSBRqNBq1at8OOPP8LGxqbWy3/99ddwdnbGiBEjsGLFCvTr1w/u7u4AgH79+mHDhg2wtraur/j3NXbsWLz99tvw9/eXLIPc8HqARCLRaHW4mFWEU9cKcP56Ia7mVBZeWl4JSsq1ouWwszSDt7M1fBvYoLGLDQIaOiDI2xH+bnZQKRWi5XhQrq6uyM7OBgCMHDkS7du3x+TJkx9qXVFRUfjiiy/Qpk2buoyop9VqoVKp6mXdVHc4AySqB4Ig4PyNQpxMK8Cpa5X/zmbeglqjkzoaitQanLteiHPXC6t83dpchUBPBwR5OaKNlyNCvB3R3MNeopT31q1bN5w8eRLZ2dl4/vnncfXqVTRo0AArVqxAkyZN8Ouvv+Ldd9+FhYUFmjRpgs2bN2Pu3LlwdXWFl5cXEhISMGzYMNjZ2SEhIQFNmjRBUlIS5s2bh5YtW2LMmDEAgDFjxmDgwIEYNGgQpk2bhr///hvl5eWYNm0aRo4cWSVTbGws3nvvPVhZWSE3Nxd79uzBq6++itOnT0On0+Hjjz9Gr1690Lx5c5w8eRK2trYoLS1FQEAAkpOT0bt3b30p79q1C3PnzkVZWRlat26N77//HuvXr8fp06fxwQcfYMaMGTh8+DD27NmDLVu24M8//8SCBQswatQoHDt2DCqVCpMnT8bzzz8vxY/HaLAAierItfxSxF+8ibiL2TiYnIOc4nKpIz2Q0gotjl7Nw9GrefqvudlbItzfBRHN3dCtuSs8HKwkTFhJo9Fg586d6NOnD+bOnYtu3bph69atWLNmDSZMmIAtW7bggw8+wJYtW9C8eXMUFBRUWX7IkCEICwurdgYYExODWbNmYcyYMdBoNNizZw+++uorfPfdd2jUqBH++ecflJaWonPnzujTpw9cXFyqLH/06FGcPXsWnp6emDFjBgYMGIAVK1YgOzsbEREROHv2LPr27Ytt27ZhxIgR2LFjB6Kjo2Fm9r8/xdnZ2fjPf/6DvXv3wtraGrNnz8a3336LgQMHYtmyZQCAf/75B8XFxdBoNIiPj0dERAQSExNx5coVnDlzBgDuut90NxYg0UMq1+gQf+km9p7Lwv5LObiSXSx1pDp3s1CNTYkZ2JSYAQBo5m6HiGau6Bngjq7+LjBTiXccXX5+PkJDQwEA3bt3xwsvvICOHTtix44dAIDhw4dj4sSJAIDw8HC8+OKLGDlyJIYNG1brMcLCwnD58mXk5eXhyJEjCA8Ph5WVFXbv3o2kpCT8/PPPACrL5fLly3cVYHh4ODw9PQEAu3fvxrZt2/D+++8DAIqLi3Hjxg3ExMRgyZIlGDFiBNavX3/XLO3QoUM4efIkunTpAgBQq9Xo378/fH19cePGDRQVFUGr1aJLly44fvw49u/fj4kTJ8LGxgYZGRl49dVX8cQTTyA6OvoBH2H5YQESPQCNVof9yTnYdiIDu05fx60yjdSRRHUpqwiXsoqw4kAKGtha4PHWDTEwuBE6+7lAWc/7D52cnJCYmHjP2ygUlRmWLl2KQ4cOYevWrQgLC8OpU6dqPc7gwYOxadMmHDhwADExMQAAnU6HZcuWITIy8p7L3n5Qjk6nw9atW9G4ceMqt3F3d8eYMWOQk5ODQ4cOYeXKlVW+r9Pp0L9/f/zwww93rb9du3b45ptv0L59e3Tu3Bl79uxBdnY2vLy8AACnTp3Cjh07sGDBAuzevRvz58+v9f2WI74Ngug+BEHAgeRsvL3xFDp+uAejvj+CdUfTZVd+d8otLsfqI6l4ZvlhdPxwD2ZvTsI/KbmiZoiIiMAvv/wCAFi/fj06duwIALh8+TK6dOmCDz74ABYWFsjJyamynL29PQoLC+9aH1C5GXT16tX4888/0bdvXwBAdHQ0vvrqK2i1lQcrJSUl6T+uSXR0NBYvXqz//N/yViqV6Nu3L15//XX07t27yuZPAOjSpQv27duHq1evAgBu3bqFK1eu6O/vggULEB4ejoiICHz55Zfo0KEDgMpNpzqdDsOHD8fcuXPv+2KBOAMkqlF+STnWJqRh1eFUXM0pkTqOQcsuUuOng1fx08GraOZuh5GdfDG0vTccrMzrddy5c+di9OjR+Omnn/QHwQDAlClTcOnSJQiCgCFDhsDb27vKcqNHj8bo0aNhb2+PhISEKt8LCwvDpUuX0KVLF1hZVe7zHDduHK5cuYK2bdtCp9OhUaNG2Llz5z2zzZo1CxMnTkRwcDA0Gg3atWun34QaExODqKgo7Nq1667l3Nzc8O2332Lo0KEoLy+HUqnEwoUL0bRpU0RERCA9PR1du3aFu7s7rK2tER4eDgC4du0aRo8eDZ1OBzMzMyxcuPBhHlJZ4dsgiO5wPDUPPx9KxbaTGQZx1KaxsrFQ4YlQTzzXuQkCPR2kjkN0FxYgEQCtTsDWExn4Lv4KTl3j0XN1rZ2vE8Z280PfNg31++mIpMYCJFnTaHX47fg1fBWbbJJHcRqaFh52eK1ncwwIalTvB80Q3Q8LkGSpQqvDhqPp+Co2Gam53L8nNn83W7zWsxkGhXgZ9NlnyLSxAElWdDoB646mYcneS0jPK5U6juw1dbXFxF7N8USoJzeNkuhYgCQb8Rez8f72M3edAoykF+LtiJkDAtGhSQOpo5CMsABJFk6k5eOJL/dLHYPuo39QI7zTvxU8naS7KgPJBwuQZOP5H45g3/mbUseg+7A2V+GVKH+8GOkHSzNeUYHqDwuQZOPyzSI8vvBvVGj5K28M/NxsMT8mBO18naWOQiaKp0Ij2fBzs8P/dWkidQyqpcs3izFs6QF8tOMsyirEu14iyQdngCQrt8oq0OM/sUZ3qSK58//vbLAtZ4NUhzgDJFlxsDLHm9EtpY5BDyj5ZjGGfX0QH+08C7WGs0GqG5wBkuzodAIGLInHmcxbUkehh9DGywFLR7aHTwOb+9+Y6B44AyTZUSoVmDMwUOoY9JCSrt3CgCXx+PPMDamjkJFjAZIsdfJzQb+ghlLHoIdUUFqBcSsT8PHOc9DquBGLHg43gZJspeeVoNdnf/GSR0aus18DLHm6HdzsLaWOQkaGM0CSLW9nG7zY3U/qGPSIDl3OxcAl8TiTwX269GBYgCRrL0f5o6GDldQx6BFdv1WG4csOIu4iz/RDtccCJFmzsTDD9L58W4QpKFJrMGbFP1iXkCZ1FDISLEAyPOUlwN//AdTiXLVhcKgX2vk6iTIW1a8KrYCp609i4Z8XpI5CRoAFSIbl9G/AFx2Ave8DcZ+JMqRCocCcga3By9GZjoV/XsS09Sd4hCjdEwuQDMOtDODnYcC60cCt9MqvHfwKyL0iyvAhPk54sq23KGORONYmpOPNtYksQaoRC5Ckd/xn4MvOwKU/qn5dqwZ2zxQtxvQ+LWFrwcvvmJJNiRksQaoRC5CkcysTWBUDbH4VUBdUf5tz24DLsaLEcXewwis9mokyFomHJUg1YQGSNBJXA191Ai7uvv9tf38b0IlzAuSx3ZrCl+eYNDksQaoOC5DEVV4MbBgLbBoPlNUw67tT1hkg4fv6zfVflmYqzOjXSpSxSFybEjMwZd0J8ORX9C8WIInn5gXg257AqXUPvuy+D4HSvLrPVI0+bRoivJmLKGORuH47fg0f/35O6hhkIFiAJI5T64FvewA3H/KPT2kusO+jus10D7MHtIZKyfdFmKJlf13GyoMpUscgA8ACpPqlKQe2TwE2vACUFz3auhK+A7LEefXesqE9nu7oI8pYJL65W8/gD15OSfZYgFR/SnKBHwcC/3xbN+vTaYBdb9fNumrhzcdawtHaXLTxSDxanYAJq48jMS1f6igkIRYg1Y/cK8B3jwFph+p2vcl7gXM76nadNXC2tcCk3s1FGYvEV1qhxdgf/0FabonUUUgiLECqe9eOVpZfzqX6Wf/udyo3rYrguc6N0dzdTpSxSHzZReV4aeVRlFWI8zYbMiwsQKpb53cCKwYAxfV4WZrcy8DhpfW3/tuYqZSYNSBQlLFIGmcyb2HO5tNSxyAJsACp7iR8D/w6EqgQYZPS3/OBoqz6HwdA9xZu6BXgLspYJI01CWm8jJIMsQCpbhz+Btj2BiCItClJfQvY8644YwGYOSAQFio+XUzZrM1JOJvJq8rLCZ/R9OgOfwPsnCr+uIm/ABnHRRmqqastRoc3EWUskkZZhQ6vrDqGwrIKqaOQSFiA9GikKj8AEHSV5wkVyes9m8HVzlK08Uh8V7KLMXNTktQxSCQsQHp4Upbfv1IPVp5lRgT2VuaY+ngLUcYi6WxOzMDvSdeljkEiUAg8Myw9jH+WA9vflDpFJQdv4PUEwNy63ofS6QQM+jIeSddMd1+RrqwIN9bMhKDTAjot7NsPgn1oH1xfNR06dTGg08KmVXc4hT8NQRCQveVTVGRfhV1IHziEDQIAZO9YBMfOw2DewEvie/NwXO0s8ccb3eFsayF1FKpHnAHSgzuzBdgh8czvdrfSgfiFogylVCowZ2BrUcaSisLCGh7PfAzP55eg4XOfo+DQOmhLb8F92Bx4jvkCjcZ8gdLkBJTfSEbFzStQqMzQaMyXKDr1JwCg/EYylBZWRlt+AJBdpMbsLXxrhKljAdKDSTsCbHyxcv+bIdm/CChIF2WoDk0aYEBwI1HGkoJCqYLS3AoAIGgrAEEABAFKS5v/fk1TeVo6KAClWeVCOi0UqsrTxhUcWAPHrk9JEb1ObT2Rgd+TMqWOQfWIBUi1l5MMrH4K0JRKneRumlLgj9miDTejXytYmZvu00dXVoSM71/Dta9Gw7HTk1DZOAIArq+cgvQvnoVVk1BYePjBwtUXSksbZP70Buzb9kVpcgIsGjXX397YzdyUhNxicc46ROLjPkCqneJsYHlvIO+K1Enu7fnfgcZdRBlqwR8XsGjPRVHGkoq2OA83f/sQbkNmQGXrDADQqUtwc9NHcO75AizcmuhvKwg63Fz/HlyfeAv5f/8IbWEO7Ds8AStv495kPKy9N+bHhEgdg+qB6b6EpbpTUVY58zP08gOA36cDOnE2z46P9Ieno5UoY0lFZesMc/emKEv73/4wpaUNrJqEoPTysSq3LTr5J2xadYf62hkorR3gMmAyCvb/KnbkOrfhWDqOpYpzMWYSFwuQ7m/Hm0D6P1KnqJ3ME0Diz6IMZW2hwvS+AaKMJSZtcR506srT2enUxVCnJcG8gSe0JQUAAEFTgbIrx2Du4q1fRldRhtKLB2HbugeECjWg1QAC9OsxZoIAzNl8GjodN5aZGm4CpXs7thLY8prUKR6MrTvw+lHAykGU4WK+PoB/UkxnhqDOOI+cXV9U/uUHYN+uP6ybtsfNTR9WHgAj6GAT0A1O4U/rl8nfvxqW3oGwbhwCXYUaNze8C21RHhy7PgXbwEip7kqd+nRoMIZ34EWSTQkLkGp2/VTlfj9NmdRJHlzXCUD0PFGGSrpWgEFfxIMTBNPmbm+J2KlRsLEwkzoK1RFuAqXqlRUAa54zzvIDgMNfVx61KoI2Xo4Y1t77/jcko5ZVqMbXseL8TpE4DKIAFQoFZs6cqf98ypQpWLFiRZ2OsWnTJly4cEH/+dixY5Gc/Oi/zGZmZggNDUXr1q0xcOBA5OfnP9R6+vXrh9JSA3p7waZXjOOgl5poy4Fd74g23NTHA2BnyZmBqVsefwU5RWqpY1AdMYgCtLOzw6pVq1BYWFhvY9xZgMuXL4e/v/8jr9fJyQmJiYk4ffo0nJyc8OWXXz7Uenbs2AFr6/o/lVetHF4GnNsmdYpHd2EncGmPKEO52VvitZ7NRBmLpFNSrsW3cUb8wpCqMIgCtLS0xMiRI/HVV1/d9b3k5GQ8/vjjCAsLQ8+ePZGSkgIAOHjwIFq3bo22bdvi1VdfxbBhwwBUFl3Hjh3Rtm1b9O/fH/n5+Th8+DC2bNmCCRMmIDQ0FFlZWYiKikJSUhKWLl2K2bP/9wbq9957DwsWLAAAfPLJJ+jQoQOCg4Mxf/78+96P8PBwpKdXno3k5s2bePLJJxEWFoYuXbrg+PHjKCgoQPPmzfW3v3r1KkJDQwEATZo0QVFREQBg5cqV6NChA0JCQjB58mQAwIcffohvv/0WAPDMM8/ghRdeAAAsXrwYn3/+OYqKitCnTx8EBQUhKCgIu3btqvXjX0VOMvDn3Idb1hDtmlF5RKIIxoQ3RRMXG1HGIumsPJiCPL453iQYRAECwMSJE/HNN9+grKzqPqdXXnkFy5YtQ0JCAmbOnImpUyvPQTlu3DisXLlSXyz/ioyMxOHDh3H8+HE8/vjj+PLLL9GpUycMGjQIixcvRmJiItzd/3d17yeffBIbN27Uf75hwwbExMRg9+7dSE9Px5EjR3D8+HHs2LEDSUk1XyZFq9Xijz/+wIABAwAAkyZNwttvv42EhAT89NNPGD9+PBwdHdGyZUscPnwYALB+/XrExMRUWc/Zs2exefNmHDx4ECdOnEB2dja2b9+OiIgIxMfHA6gszn9ns/Hx8YiIiMCuXbvg4uKCU6dO4eTJk+jS5SHeDC4IwObXxLmiu1hunqs8cbcILMyUeKd/oChjkXSKy7X4Lp6zQFNgMDst3NzcMGDAAHz//ff6rxUVFSEuLg6DBw8GAAiCAFtbW+Tn56OiogLt2rUDAIwYMQI//vgjACA1NRUxMTG4ceMGSktL0alTp3uO6+HhATc3NyQlJcHCwgK2trbw9vbGwoULsX37dsTFxQEACgsLceHCBbRp06bK8vn5+QgNDUV6ejqaN2+Oxx9/HADw559/4vTp/715OC+v8jD5mJgYrFu3Dp06dcKGDRvu2te5Z88eHDp0CGFhYQCAkpIStG/fHi+99BLGjx+P1NRU+Pr6Qq1W4+bNmzh27Bjatm0LJycnTJo0CdOmTcOQIUMergAPfw2kHnjw5Qxd7EdA8HDApkG9D/VYoAe6NXdF3MXseh+LpPPjgRSM6+4HR2tzqaPQIzCYGSBQefDLokWLoNFUbrLS6XTw8PBAYmIiEhMTceLECRw4cAD3eufGhAkTMG3aNJw6dQoLFy6EWn3/HdbDhw/HunXrsG7dOv2MTKfTYc6cOfqxk5OT8eSTT9617L/7AK9evQqFQlFlM25CQoJ++atXrwIABg8ejC1btiAtLQ2lpaVo0aLq9eV0Oh3GjRunX+7ChQuYOHEirKys4OzsjPXr1yMiIgLh4eFYuXIlvL29YW5ujhYtWiAxMRGtW7fG5MmT8cUXX9z/Ab9dTjKw570HW8ZYlOUD+z4QbbhZAwJhplSINh6Jr1CtwfecBRo9gypAHx8fhIeHY8OGDQAABwcHeHh4YOvWrQAqNzMmJSXB2dkZZmZmSExMBACsW7dOv45bt27By8sLgiDgp59+0n/d3t6+xoNs/t0M+u/mTwCIjo7G8uXLUVJSuTkwJSWlyqbWO9na2mLx4sX47LPPoNFo0KNHDyxdulT//RMnTgAAHB0d0aJFC0yfPl2/3/J2vXr1wpo1a5CTkwMAyMrKQmZm5Rnpw8PDsWDBAoSHhyMiIgILFixAREQEACAjIwO2trYYNWoUJk2apH9sakWnqzzq05Q2fd4p4QfgxhlRhmrhYY+RnXxFGYuks+JACkrLtVLHoEdgUAUIANOnT0dGRob+819++QVLlixBSEgIgoKCsGdP5VF933zzDUaOHIl27drB0tISDg6VZ/2YM2cOBg4ciA4dOsDH539nbXjqqacwb948/UEwt/Pw8ICrqyusrKzg7V35fq4+ffpgyJAh6Ny5M9q0aYNnn332rv2TdwoLC0NQUBDWrl2LJUuWIDY2FiEhIWjVqhV++eUX/e1iYmKwevXqu/b/AUDr1q3xzjvvoFevXggODkb//v2Rm5sLAIiIiEBBQQGCgoLQrl075ObmIjw8HABw6tQpdOjQAaGhoVi4cKH+4JlaObYCSDtU+9sbI0FbeZ5QkUx+rCWcbbh5zJQVlFZgy4lrUsegR2C0Z4IpLi6Gra0tAOC1115DQEAAXnvNyE7ZZQhKcoEl7YBS0zmV1z2N+BloNVCUoX46mILZm3lRVVPWxssB217vJnUMekgGNwOsrc2bNyM0NBSBgYHIycnRvy2AHtDeefIpPwDYPRPQiPNG5pGdGqOlh70oY5E0kq7dwnFeKcJoGe0MkOrAjdPA190qNw/KSa85QLcH2ET8CPZfysbI5YdFGYukMbSdNz4bzusFGiOjnQFSHdg1Q37lBwBxnwGF10UZKryZKx4L9BBlLJLGtpMZyC/hG+ONEQtQri7sAi7HSp1CGuVFwJ/vijbczP6tYGHGp5qpUmt0WJeQLnUMegh8VsqRIJjue/5q68Rq4NpRUYZq7GKLMeFNRRmLpLGZR4MaJRagHJ3bBtyo+bRu8iAAO98SbbTXejaDm72laOORuJKu3UJKdrHUMegBsQDl6K9PpU5gGNKPACfXijKUnaUZpj7eUpSxSBrbTmbc/0ZkUFiAcnNuB3D9pNQpDMcfc4BycV65x7T3RrC3oyhjkfi2ncyUOgI9IBag3PzN2V8VhRlA/AJRhlIoFJgzsLUoY5H4zl0vxKWs+rumKdU9FqCcXNgNZByXOoXhObAEyE8VZaj2jZ3xRKinKGOR+Lae4CzQmLAA5USkmY7R0ZQBu2eJNtxbfQNgba4SbTwSz67T4ry/lOoGC1Aubpw2zWv91ZUzm4CU/aIM1cjRGuMj/UUZi8R1/kYhbhaKc6o9enQsQLkQ6aroRu336ZWXhhLBS5F+8HKyFmUsEo8gAAeSeTFkY8EClAN1oWiH+xu166eAYz+KMpSVuQpv9wsQZSwSV9xFFqCxYAHKwYlfK0//Rfe3932grOYLH9elAcGe6Ni0gShjkXj2X2IBGgsWoBz8853UCYxHSTYQ+4low80eEAilQrThSASZBWW4lMUXnMaABWjqrh4Abp6VOoVxOfINkH1RlKHaeDlieJiPKGOReDgLNA4sQFNnQPv+hqwpgfMntzBsbQkAoFAtIPTrIv0/x49vYeGhyiPoJu8qQ9DSIkzdXaZffva+Muy7oqn/oLqKyktFiWTK4y1hb2Um2nhU/47xIrlGgQVoyrQa4OwWqVPoTexkgZ8G/+/IR3tLBRLH2yFxvB2Ov2QLJysFnmhpjvwyAUcztTj1sh2OZGhRUCYgo1CHCzk69GgqUlFc3A1c/EOUoVztLDGhZ3NRxiJxnLomzn5kejQsQFN25S+gJEfqFHpRTcxgb1n9Dq+D6Vo0tFOgqbMSKgWgVAA6QYDyvx+/95cacyJFvprCrhmAtkKUoUaHN4Gfq60oY1H9u5JdjCK1CFsr6JGwAE3Z6Y1SJ6i1tac1GNHaHEDlzPAxPzO0XVaMx/zMcLVAB5UCaOUm8tlTsi9U7g8UgblKiXf6txJlLKp/ggCc5izQ4LEATZW2Aji7TeoUtSIIAjacrcDw/xYgAMzoZokT4+0wo5sl5v2txuxIS7wbq8awtSX47aw4szIAwF+fAMXizKJ7tfJAZAs3Ucai+peUcUvqCHQfLEBTlbwPKMuXOkWtxKdq0dhRCW+Hu38d91zWoI2bCgVqAakFOqyNscbCw+XihSsrAPbOE224WQMCYcb3RZiEJM4ADR4L0FSd2yp1glpbe7pCv/nzdoIgYOHhcrzZ1QIlFUC5DlAAyCsVxA147MfKs8SIoJm7HZ7r0liUsah+sQANHwvQVCXHSp3gLr1/KkbMulLsuKiB9+eFOJimgU4Q8Ns5DYYF3n10588nKzAkwAw25gqEeChRphHQZmkx/i/k7rKsV4IO+P1t0Yab1LsFGthaiDYe1Y+ruSUQBJFfrNEDUQj8CZmenGRgSTupU5iemB+B1oNFGWrloauYtSlJlLGo/hx8uycaOfKk54aKM0BTlLxX6gSm6Y9ZQEXZ/W9XB57p6IuAhvaijEX1JzWnROoIdA8sQFN0OVbqBKYpPxU4uESUoVRKBWYPDBRlLKo/qbksQEPGAjQ1Oi1wJU7qFKYrbgFwK1OUobr6u6JP64aijEX1I40FaNBYgKYm4zig5tFn9aaiGPhzjmjDvdO/FSzM+DQ1VpwBGjY+s0xN2mGpE5i+k2uBtH9EGcqngQ3GRjQVZSyqe9fyS6WOQPfAAjQ1GYlSJ5ABAfh9euX5rkTwao9m8HAQ+TyoVCfyS0Q8axE9MBagqclMlDqBPFw7Cpz4VZShbC3NMO3xAFHGorpVUMoCNGQsQFOiLgJyLkmdQj72vFv5mIvgyXZeCPVxEmUsqjssQMPGAjQl109WnrWExFGYCcR9JspQCkXl2yIUPE2oUVFrdCir0Eodg2rAAjQl3P8nvoNfAnkpogzVztcZg0O9RBmL6s4tzgINFgvQlFw/KXUC+dGqgV3viDbcW30DYGMh8nUR6ZFwM6jhYgGaEu7/k8a5bcCVv0UZysPBCq9E+YsyFtWNQl4Z3mCxAE2JSJviqBq/v115Fh4RjO3mB29nnmDZWGh1vN6AoWIBmoryYqD4ptQp5OtGEnD0B1GGsjJXYUa/VqKMRY+OBWi47r4IGxknzv6kt+9DoM1QwNq53ofqF9QI0YEeOJ1xq97HokdjruKhu4aK1wM0Fee2A78+I3UK6jQe6PuJ1CmIqBa4CdRU5F2VOgEBwD/LgZvnpU5BRLXAAjQVBWlSJyAA0GkqD4ghIoPHAjQVJTlSJ6B/Je8Bzv8udQoiug8WoKkozZc6Ad1u1wxAyzdAExkyFqCpKMuXOgHdLjcZOLRU6hREdA8sQFPBGaDh+fs/QBHfm0lkqFiApqKsQOoEdCf1LWDve1KnIKIasABNBTeBGqbjPwOZJ6ROQUTVYAGaAk05oCmTOgVVR9ABO9+SOgURVYMFaAp0PNu8QUs9ACRtkDoFEd2BBWgKBF5x2uD9MQeoKJU6BRHdhifDNhW27lInoHvRqIFjK4FOL0qdhIj+iyfDJiIiWeImUCIikiUWIBERyRILkIiIZIkFSEREssQCJCIiWWIBEhGRLLEAiYhIlliAREQkSyxAIiKSJZ4KTUZ+SPoBRRVFUscgMnrNnJqhb9O+UsegR8QClJFVZ1fhRskNqWMQGb3oxtEsQBPATaAyYqbk6x2iuqBSqqSOQHWABSgjKgWftER1wUzBF5OmgAUoI3zVSlQ3+FwyDSxAGTFXmksdgcgkcHeCaWAByoiTpZPUEYhMgrOls9QRqA6wAGXEzcZN6ghEJoHPJdPAApQRN2s+aYnqAp9LpoEFKCOu1q5SRyAyCXwumQYWoIy427hLHYHIJPC5ZBpYgDLCV61EdYObQE0DC1BG+KqV6NE5WTrBXMW3FJkCFqCM8FUr0aPjlhTTwQKUERtzG9ia20odg8iocUuK6WABygxngUSPhjNA08EClBkfex+pIxAZNV97X6kjUB1hAcpMoEug1BGIjBqfQ6aDBSgzfPISPRo+h0wHC1Bm+OQlengeNh5wsXaROgbVERagzDS0bQgXKz6BiR5Ga5fWUkegOsQClCHOAokeDp87poUFKEN8EhM9HD53TAsLUIb4JCZ6OHzumBYWoAxxPwbRg2to25AHwJgYFqAMedh68EAYogcU2ICzP1PDApSpUPdQqSMQGRU+Z0wPC1CmIr0jpY5AZFT4nDE9LECZ6u7dHUoFf/xEtdHYoTH8nPykjkF1jH8BZcrF2gVBrkFSxyAyCpz9mSYWoIxF+URJHYHIKPC5YppYgDLWw6eH1BGIDJ6jpSPaureVOgbVAxagjPk7+fPaZkT3EeEVATOlmdQxqB6wAGUu0of7NojuhZs/TRcLUOaivKOkjkBksMyUZojwjJA6BtUTFqDMtfNoBwcLB6ljEBmkMI8w2FnYSR2D6gkLUObMlGZ4rPFjUscgMkh9m/aVOgLVIxYgYUTLEVJHIDI49hb2LEATxwIktHJphWDXYKljEBmUJ/yfgLWZtdQxqB6xAAkAMCKAs0Cifymg4JYRGWABEgCgT5M+cLJ0kjoGkUHo1KgTmjg2kToG1TMWIAEALFQWGNJsiNQxiAzCUy2fkjoCiYAFSHoxLWN4hQiSPQ8bD775XSb41470fOx9EO4ZLnUMIkkNazEMKqVK6hgkAhYgVfFUADf9kHyZKc0wrMUwqWOQSFiAVEWEVwS87byljkEkicd8H4OrtavUMUgkLECqQqlQYnzIeKljEIlOpVDxd19mWIB0l4H+A9HMqZnUMYhENch/EPyc/KSOQSJiAdJdlAolJrabKHUMItFYqizxSugrUscgkbEAqVpRPlG8CjbJxlMtn0JD24ZSxyCRsQCpRpPaTZI6AlG9sze3x7jgcVLHIAmwAKlG7TzaIdKbV4wn0za6zWg4WjpKHYMkwAKke5rQbgLPDkMmy9XaFc+2elbqGCQR/mWje2rh3AL9m/aXOgZRvXgp+CXYmNtIHYMkwgKk+3q17auwUFpIHYOoTvnY+2Boi6FSxyAJsQDpvrzsvPgGYTIpCigwp8scmCvNpY5CEmIBUq2MaTMGrV1aSx2DqE7EtIhBp0adpI5BEmMBUq2olCq8H/4+XzGT0fOy88KbYW9KHYMMAAuQaq2ZczO8HPKy1DGIHpoCCrzb9V0e+EIAADOpA5BxGdNmDPak7sHpnNNSRzFK5988D6W1EgqFAipbFZq+1RTqLDXSvkqDrkQH20BbeI7yhEKhQObqTBSdLoJ9G3s0fKryLCU3Nt6AbStb2LWyk/ieGCdu+qTbcQZID0SlVGFe+DxuCn0EfjP90GxeMzR9qykA4MbaG3Af7I4Wn7aAtkiLwhOF0BZrUZpSiubvN0fJlRJoS7SoyKtA+fVylt9D4qZPuhMLkB5Yc+fm3BRaRwRBQMmlEtiH2AMAnLo4oTCxEFACCoUCgk6AQqEAFEDW5iy4DXaTOLFx4qZPqg4LkB4Kjwp9SArgykdXkPxuMvIP5ENbpIXKVlVZcgDMnM2gydNAZa2CbWtbJM9Jhm1rW1TkVEChVMDK00riO2CcuOmTqsN9gPRQVEoVPoj4AE9vfxqlmlKp4xgNv3f8YO5sjor8CqR8mgJzl5o3JbsPdIf7QHcAQOpXqfAc6YmsTVkoSy+DUxcnOLR3ECu2UWvs0JibPqlanAHSQ/N38seHER9CAYXUUYyGuXNl4Zk7mcM+2B7lWeXQFmshCAIAQJOngZlT1delRWeKYOVlBW2pFuU55fB5xQfZu7NFz26M7M3tsbjnYm76pGqxAOmR9G7cm2eJqSWdWgdtqRYAoC3TouhsESy9LGHjb4PCE4UAgPyD+bAPtdcvIwgCcnblwLWPK3RqHQSNACgAbbFWkvtgTJQKJT7p/gn8HHmVd6oeN4HSI3s55GVczLuIP1P/lDqKQdMUaJC6JBUAIOgEOEc6w8bPBh4xHkhbmobMVZmwC7TTHxADAPkH8uHQ3gFKSyWsfK0gVAi49M4lOHdzlupuGI1J7Sahm3c3qWOQAVMI/257IXoEJRUleG7nc7iQd0HqKEQY4DcAH3X7SOoYZOBYgFRnMooy8PT2p5Fblit1FJKxINcg/NDnB1iqLKWOQgaO+wCpznjaeeKzyM9gpuSWdZKGu7U7FvZYyPKjWmEBUp0KaxiGGZ1mSB2DZMhSZYmFPRbC3cZd6ihkJFiAVOdiWsTg2VbPSh2DZOTfM70EuQVJHYWMCAuQ6sW0DtPwZPMnpY5BMjGryyz09+svdQwyMixAqhcKReUVt/lHierbWx3fQkyLGKljkBFiAVK9USqU+CD8AzzW+DGpo5CJeqP9GxjZaqTUMchIsQCpXqmUKnzS/RP09u0tdRQyMa+3fR1j2oyROgYZMb4PkESh0WkwI34Gdl7ZKXUUMgFTwqZgVOtRUscgI8cCJNHoBB1m75+NzcmbpY5CRkoBBd7u9DaeDnha6ihkAliAJCpBEPD+ofex9sJaqaOQkVEqlJjdeTaGthgqdRQyESxAksTyU8ux5PgS6ASd1FHICNia2+KTbp8g0idS6ihkQliAJJm/0v7C9LjpKK4oljoKGTBfe18s7rkY/k7+UkchE8MCJEkl5ydjwt4JSC1MlToKGaDOjTpjfuR8OFo6Sh2FTBALkCRXoC7AlL+m4FDmIamjkAEZ2WokpoZNhUqpkjoKmSgWIBkErU6L/yT8B6vOrpI6CknMXGmOWZ1nYUjzIVJHIRPHAiSDsvHiRrx/6H1U6CqkjkIScLFywcIeCxHqHip1FJIBFiAZnONZxzH97+nILM6UOgqJKNgtGJ9FfoaGtg2ljkIywQIkg1RUXoT5CfOx4eIGqaNQPbNUWeLV0Ffxf4H/x/19JCoWIBm0AxkHMPfAXM4GTVSwWzDmhc+Dn6Of1FFIhliAZPA4GzQ9nPWRIWABktHgbNA0cNZHhoIFSEaFs0HjxVkfGRoWIBmlw5mH8VnCZzibe1bqKFQLUT5RmNx+Mpo6NpU6CpEeC5CMliAI2JWyC0uOL+Gp1AxUO/d2eKP9G3xfHxkkFiAZvQpdBTZe2IivT36N7NJsqeMQgObOzTGp3SR09+4udRSiGrEAyWSUakrx85mf8UPSDyisKJQ6jix52Xnh1dBX0d+vP5QKpdRxiO6JBUgmp0BdgOWnlmP1udVQa9VSx5GFBlYN8GLwixjeYjjMVeZSxyGqFRYgmawbxTew9sJabLiwATllOVLHMUn+jv4Y3nI4BjcbDBtzG6njED0QFiCZvApdBf68+id+PfcrjmUdkzqO0TNTmqGnT088FfAUOjTsIHUcoofGAiRZuZh3EWvOr8G2y9t4JfoH5G7jjmEthmFY82Fws3GTOg7RI2MBkiwVVxRja/JWrDm/BpfyL0kdx2ApoEDHRh3xVMunEOUTBTOlmdSRiOoMC5Bk73T2aexN24vYtFhcyLsgdRzJqRQqtHVviyifKPT07Qkfex+pIxHVCxYg0W0yijKwL20fYtNikXAjARqdRupIorAzt0O4VzgivSPR3bs7HC0dpY5EVO9YgEQ1KCovQnxGPGLTYhGXHodb5bekjlSnPG09EekTiSifKHRo2AHmSr59geSFBUhUCxqdBudyz+FMzhn9v4v5F41mhmhtZo1WDVoh0CUQgS6BaO3SGn5OvBoDyRsLkOghlWvLcSHvgsGVYnVl18SxCc/MQnQHFiBRHSrXliPlVgqySrJws+Qmbpbe/N//pTeRXZKNm6U3UaGreKj1W5tZw83aDW42blX+d7V2hbuNOzxsPODr4MuyI6oFFiCRyARBQIG6ANml2VBr1dAIGmh0Gmh12srZowIwV5pDpVDBTGkGlVIFGzMbuFm7wc7CTur4RCaDBUhERLLE7SRERCRLLEAiIpIlFiAREckSC5CIiGSJBUhkgBQKBWbOnKn/fMqUKVixYsVDrSs2NhZHjhx54OVGjx6Nbdu2Vft1Pz8/hISEIDg4GHv27HmoXF9//TXWrFnzUMsS1QUWIJEBsrOzw6pVq1BYWPjI67pXAWq12oda5+LFi3HixAl8/vnnGD9+/EOtY/z48RgxYsRDLUtUF1iARAbI0tISI0eOxFdffXXX95KTk/H4448jLCwMPXv2REpKCgAgKioKSUlJAICkpCRERUUhLS0NX3/9NT7++GOEhoYiMTERo0ePxssvv4yOHTvi448/xqZNm9CxY0e0bdsW/fv3R35+fq1zRkREID09Xf/5J598gg4dOiA4OBjz588HAIwYMQJ79+7V36Znz544fvw45s6diy+++KLG+5SRkYHw8HAAwO7du2FtbY3y8nLk5+ejbdu2AICFCxeiZcuWCAkJwcsvv1z7B5gIAC/uRWSgJk6ciM6dO2PixIlVvv7KK69g2bJlaNKkCfbu3YupU6di3bp11a7Dx8cH48ePh6urK1577TX913NycnD48GEoFArk5eXhiSeegEKhwOLFi/Hll1/inXfeqVXG7du3Y9CgQQAqSyo9PR1HjhyBTqfDY489hj59+iAmJgbr1q1Dz549kZWVhYyMDLRt2xabN2++733Ky8uDWq1GfHw8AgMDcfToUeTl5aFLly4AgPfeew9paWmwtbVFQUHBAz2+RCxAIgPl5uaGAQMG4Pvvv9d/raioCHFxcRg8eDCAyrPK2NraPvC6hw0bBoVCAQBITU1FTEwMbty4gdLSUnTq1Om+y0+YMAGTJ09Gamoq9u/fD6CyALdv3464uDgAQGFhIS5cuIB+/fph2rRp0Gq1+O233/Dkk09WWde97lNYWBiOHDmCw4cP480330R8fDzy8vL0M8OOHTvi2WefRUxMjH55otpiARIZsClTpqB3797o27cvAECn08HDwwOJiYl33dbMzAw6nQ4AoFar77leGxsb/ccTJkzAO++8g+joaGzbtq1WB9ssXrwYAwYMwIIFCzBu3DgcO3YMOp0Oc+bMwahRo+66fYcOHfD3339j/fr1+PTTT6t87173KSIiAn/99RfUajWio6Mxbtw45Obm4sUXXwRQOQONjY3Fpk2bsGDBAvzzzz/3zU70L+4DJDJgPj4+CA8Px4YNGwAADg4O8PDwwNatWwFUHsTy736/xo0b60tk48aN+nXY29vf82CaW7duwcvLC4Ig4KeffnqgfJMmTYJGo8Hu3bsRHR2N5cuXo6SkBACQkpKi3ywZExODpUuXIj09Xb//7l/3uk8RERFYtmwZQkND4erqiuzsbGRkZKBJkybQ6XRIS0tDr169MH/+fKSmpj70QT0kTyxAIgM3ffp0ZGRk6D//5ZdfsGTJEoSEhCAoKEj/NoTJkyfj008/Rfv27VFeXq6//cCBA7F69Wr9QTB3mjNnDgYOHIgOHTrAx8fngbIpFArMnj0b8+fPR58+fTBkyBB07twZbdq0wbPPPouysjIAQL9+/bBjxw4MGTKk2vXUdJ9atWqF0tJS/SbPVq1aoV27dgAqi3LkyJEIDg5GWFgYZs+eDZVK9UD5Sd54MmwiIpIlzgCJiEiWWIBERCRLLEAiIpIlFiAREckSC5CIiGSJBUhERLLEAiQiIlliARIRkSyxAImISJZYgEREJEssQCIikiUWIBERyRILkIiIZIkFSEREssQCJCIiWWIBEhGRLLEAiYhIlliAREQkSyxAIiKSJRYgERHJEguQiIhkiQVIRESyxAIkIiJZYgESEZEssQCJiEiWWIBERCRLLEAiIpIlFiAREckSC5CIiGSJBUhERLLEAiQiIlliARIRkSyxAImISJZYgEREJEv/DwLiuV7QrhqLAAAAAElFTkSuQmCC</t>
+  </si>
+  <si>
+    <t>https://www.flipkart.com/micromax-x512/p/itmfhwvhrwhxq5tu?pid=MOBG8C3FGAQYHKFK&amp;lid=LSTMOBG8C3FGAQYHKFKLFWUST&amp;marketplace=FLIPKART&amp;q=micromax+x512&amp;store=tyy%2F4io&amp;srno=s_1_2&amp;otracker=search&amp;iid=e532b5ae-9020-461a-a39a-dca423c959b8.MOBG8C3FGAQYHKFK.SEARCH&amp;ssid=0udxp3g2jk0000001689862408205&amp;qH=8aab057c4a7cd0c3</t>
+  </si>
+  <si>
+    <t>₹1,100</t>
+  </si>
+  <si>
+    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAcAAAAFQCAYAAAAoQ64wAAAAOXRFWHRTb2Z0d2FyZQBNYXRwbG90bGliIHZlcnNpb24zLjYuMSwgaHR0cHM6Ly9tYXRwbG90bGliLm9yZy/av/WaAAAACXBIWXMAAArEAAAKxAFmbYLUAABKA0lEQVR4nO3deVxU9f7H8dew74uCuAHuOwgKKoK5prmWGmppN29lP1u0bmrdytKbLbeuN03Nsky9WmqpaZl2w1001wS3zJ1NUEQW2WFmzu8PblNuiMzAmeXzfDx6BM453/nMAeY953vO+RyNoigKQgghhI2xU7sAIYQQQg0SgEIIIWySBKAQQgibJAEohBDCJkkACiGEsEkSgEIIIWySBKAQQgibJAEohBDCJkkACiGEsEkSgEIIIWySBKAQQgibJAEohBDCJkkACiGEsEkSgEIIIWySBKAQQgibJAEohBDCJkkACiGEsEkSgEIIIWySBKAQQgibJAEohBDCJkkACiGEsEkSgEIIIWySBKAQQgibJAFo5Xr16sWXX35ZI2NrNBrS0tJqZOzqSElJwcfHR+0yzNpXX33F0KFDq/24uZk5cyZPPfXUHR/38PAgPT29FiuqXE3+PYp7JwFYy5o0aYKbmxseHh40bNiQyZMno9PpauW5ly1bRr9+/aq0bEpKCh4eHnh4eODu7o5GozF87+HhUcOVVk9QUBC5ublql2HWxo4dy8aNGw3f3/wh5ubHzc29fugqKCigYcOGNVhR7ZMQNR0JQBXExcVRUFBAfHw869at44svvlC7pFsEBQVRUFBAQUEB58+fBzB8X1BQUGPPq9Vqa2xsc2Dtr8+WKIqCXq9XuwxhBAlAFTVv3pzo6GgSExMN/7Z27Vrat29PnTp1GDZsGJmZmQBcvXqVgQMH4uPjg5+fH4888ggAO3fupEWLFjeMe7tPyRcuXGDixIns3LkTDw8P2rdvb5LXsHHjRpo2bYqfnx/vvfee4d91Oh0zZswgODiYgIAApkyZcsc3/169evHGG28QERGBu7s75eXl7Nq1i86dO+Pj40OvXr0MIfzUU0/xj3/844b1mzVrxp49e0hKSsLBwcHw79nZ2Tz66KPUq1ePZs2a8Z///AeAs2fP3rBX0L9/f/r06WP4vmHDhpw9e/aO2/xm58+f57777sPHx4eGDRvy2muvGR5btmwZvXv35v/+7//w9vZm6dKld6zrdjQaDfPnzycoKIj69evzr3/9y/BYSUkJzz33HPXr1ycoKIi33nrL8Ia8f/9+wsPD8fLyolGjRsyZM8dQz++zAP379wegdevWeHh4EB8ff8PjlW1r4I4/o9tZuHAhzZo1w9/fn3HjxpGXlwf88fv71ltvUadOHZo0acJPP/102zFuVy9AcXExsbGxeHp60rVrVy5evHjD9vv9b2HJkiUEBwfj6elJ69at2blz5z1v8/Hjx/P888/Tp08f3NzcOH/+PPHx8YSHh+Pj40PPnj05deqUYflDhw4RGhqKl5cXEydOvCEwx48fz9tvv234/uYZmu3btxMREYGXlxctW7YkPj6eWbNmER8fz1NPPYWHhwfvvvvuHbe5qAJF1Krg4GAlPj5eURRFOX36tFK/fn1l9uzZiqIoyoEDB5RGjRopx44dU8rKypRp06YpI0eOVBRFUV555RXlmWeeUcrLy5WSkhJl7969iqIoyo4dO5TmzZvf8ByAkpqaqiiKovTs2VNZsWKFoiiKsnTpUqVv3743LPvee+8pgwcPrrTmjIwM5Xa/KoDy8MMPK/n5+crx48cVZ2dn5dy5c4qiKMoHH3yg9O7dW8nMzFRycnKUXr16KfPnz7/t+D179lSaN2+unD17VikuLlZSUlIUPz8/Zffu3YpWq1XmzZunREREKIqiKHFxcUq7du0M6x44cEBp3LixotfrlYsXLyr29vaGxwYNGqRMmTJFKSkpUU6dOqU0aNBAOXr0qKIoihIQEKCcO3dO0Wq1SmBgoNKoUSOlrKxMOXfunBIQEFDpNr/ZuXPnlJ07dyrl5eXKmTNnlMDAQGX9+vWGbW5vb68sXbpU0el0SlFRUaV13W4b9+/fX8nLy1NOnTql1K9fX9m6dauiKIry2muvKT179lSys7OV5ORkpWXLlsrSpUsVRVGUrl27Kl9++aWiKIqSnZ2tHDlyxFDPn38H/vy7cvPjlW3ryn5GN4uLi1Pq16+vnDx5UikoKFBGjBihPP7444qiVPz+2tvbK//85z+V8vJyZdGiRUpQUNBtx7ldvTNmzFBcXV2V7du3K+Xl5cpjjz2m/OUvf7ll+YKCAsXT01M5c+aMoiiKkpSUpFy4cOGet/njjz+u1K1bVzl8+LBSXl6uXL58WfHx8VHWrVunlJWVKR988IHSokULpby8XCktLVUaN26sLFy4UCkrK1PmzZun2NvbG/4eH3/8cWXWrFm33fbnz59XPD09lY0bNyparVZJTk5Wzp49qyjKjX/TwjiyB6iCgQMH4uHhQevWrenevTvPPfccUPEJ9dlnnyUkJARHR0feeOMNvvvuO7RaLY6OjmRkZJCamoqzszPdu3c3SS1///vf+eGHH4xa38PDgw4dOhAaGsrx48cB+OKLL3j77bfx9/fHx8eHKVOmsHbt2juO8+STT9KiRQtcXFz46quvGD58OD169MDe3p5JkyaRlJREUlISffr04erVq5w8eRKAb775htjYWDQazQ3jXb58mZ07d/Lee+/h7OxMmzZtePTRR/n2228B6NGjB7t37yYhIYHQ0FDCwsI4cuQI8fHxxMTEAFR5mzdv3pyePXvi4OBAy5YtGTt2rGEv6ffHx48fj52dHXl5eZXWdTuvvvoqXl5etGnThieffJKvv/4agNWrVzNjxgx8fX0JCgpiypQprFq1ylD7uXPnyM7OxtfXl/Dw8Ep/jrdT2bau7Gd0s9WrV/P000/Trl073N3deffdd/n6669RFAUAd3d3pk2bhoODA+PGjSMlJeWejuX27duX3r174+DgwJgxYzh69Ohtl9NoNJw8eZLS0lKCg4Np2rTpHce80zYHGDlyJJ07d8bBwYG4uDhCQ0MZMWIEjo6OTJkyhaKiIg4dOsS+fftwcHDgmWeewdHRkeeff54GDRpU6TWtWrWKoUOHMmTIEOzt7QkKCrplpkcYTwJQBT/++CP5+fls2LCBw4cPG46ppaSk8M477+Dj44OPjw+BgYE4ODhw+fJlpk2bRlBQED179qRNmzZmc9wwICDA8LWbm9sNr+X36UMfHx/Gjh1rmM69ncaNGxu+TklJYcWKFYZ1fXx8KCws5NKlS9jb2/Pwww8b3kDXrFnD6NGjbxkvJSWFkpISQwD7+PiwaNEiLl++DFQEYHx8vCHw/vx9jx49AKq8zS9dusTw4cOpX78+3t7ezJ07l2vXrt3xtVVW1+0EBgbe8HVGRgYA6enpBAUFGR4LDg42nPG4ePFiTp48SYsWLYiJiWHfvn13HP9OKtvWlf2Mbna7OktKSsjOzgbA398fO7uKtyI3NzeAezrOfKffwT9zd3dn1apVzJs3j4CAAGJjYys9O/RO2xxu/Hne/Nrs7OwIDAwkPT2djIyMG5bVaDQ3fF+ZtLS0SgNamIYEoEo0Gg0PPvgg/fr1MxwHaNSoEbNmzSI3N9fwX3FxMY0bN8bLy4uPPvqIlJQUli1bxqRJk7hw4QLu7u4UFxcbxr1y5Uqlz1lbGjVqxI4dOwyvIy8vj19//bVKtTVq1IgJEybcsB2KioqIjo4GYPTo0XzzzTfs378fOzs7unbtetvn9/DwICcnxzBGfn4+n376KfDHHuCePXvo0aMHPXr0YM+ePezZs8ewB3inbX6z6dOn4+vry5kzZ8jLy+PFF1807N3c7rVVVtftpKam3vD173sRDRs2JCUlxfBYSkqK4dhm69at+eabb8jMzGTMmDF3PH55N3fa1nf7Gf3Z7ep0cXGhTp061aqpugYNGsT27dtJS0vD2dn5hmO1N7vTNocbf543vzZFUUhNTaVhw4Y0aNDglmPxf/6+sr/dwMDA2+5N3/z8wjgSgCqbOnUqixcvJisri7/+9a8sWLDAMIWTnZ3Nd999B8CmTZu4cOECiqLg7e2NRqPB3t6eVq1akZOTw65duygtLWXWrFl3fK569eqRlpZWK2ciPvHEE0yfPp2MjAwURSEpKYldu3ZVad1HH32UNWvWEB8fj16vJz8//4bp0x49epCfn8/06dMZNWrUbcdo1KgRUVFRTJ8+naKiIrRaLUeOHDGEcMeOHbl69Srx8fFERkYSERHBvn37yMjIICwsDLjzNr9Zfn4+np6eeHh4cOLEiUpPUb9bXbfz/vvvc/36dU6fPs2SJUsMr3n06NHMmjWLnJwcUlNT+fDDDxkzZgxQcT3ftWvXcHBwwNPT87Z1Q8XvxJ3eaOHO2/puP6M/Gz16NJ9//jmnTp2isLCQ119/nVGjRlXrjfxu9d7JlStX+OGHHyguLsbZ2Rk3N7c7bhO48za/2cCBAzl69KjhUMWcOXNwdXUlIiKCqKgoysvL+eyzzygvL+fjjz++YU+yY8eObNq0ievXr3PhwoUbZhgeeeQRNm7cyObNm9Hr9aSmphpOMqruNhC3kgBUWdu2benZsycfffQR3bt3Z/bs2fzlL3/By8uLTp06sXfvXgDOnDlD79698fT0ZPDgwcydO5fg4GC8vb356KOPGDVqFE2bNiUyMvKOz9WnTx+aNGmCv78/oaGhALz77rsMHDjQ5K9r2rRpREVFER0djbe3N0OHDr3hU3VlmjZtyurVq5k2bRp16tShTZs2hg8CUDHNFBsby/bt2+/4xgQVIZCWlkazZs2oV68eL774ouETt52dHd27d6dNmzY4OTnh5OREu3bt6Natm+GN8U7b/GZvvvkmO3bswMvLi8mTJzNy5MhKX19ldd3OoEGD6NChA/fddx+TJ082nCn4xhtv0Lp1a9q0aUNUVBRjxozh8ccfB2Dz5s20bt0aT09P5s2bx/Lly2879ptvvsnIkSPx8fG54bjl7+60re/2M/qz/v378+qrrzJo0CCCg4NxdHRk7ty5lW6jO7lbvXei1+v54IMPCAgIoF69ely6dOmGMzBvdqdtfjM/Pz82bNjAjBkzqFu3LuvXr2fDhg04Ojri5OTEunXrmD9/PnXr1uXYsWM3HEd+7LHHaN68OY0bN+aRRx65YS+9adOmrFu3jtdffx1vb2/69u1rCM9JkyaxbNkyfHx8+Oc//1nlbSBupVH+PFcjhDArGo2G1NTUKh87EsaTbW47ZA9QCCGETZIAFEIIYZNkClQIIYRNkj1AIYQQNkkCUAghhE2SABRCCGGTJACFEELYJAlAIYQQNkkCUAghhE2SABRCCGGTJACFEELYJAlAIYQQNkkCUAghhE2SABRCCGGTJACFEELYJAlAIYQQNkkCUAghhE1yULsAIcydTq+QmV9Cem4Jl/NKuJpfQnZhGdcKy7hWUEZOURmlWj06vWL4T6v/3/eKgk6noNUraDTg6eKIj6sj3q6OeLtV/N/H1Qkftz/+rZ6nM838PHB1slf7pQth1eR+gEL8T0m5jrNXCjiVcZ1fM67z2+XrpFwrIjO/FK2+dv9MNBpo4OVCM38Pmvu708zfg2b+7jT396CBtwsajaZW6xHCGkkACpuUmV/CqYx8TmVcN/x34WphrQdddbg62tPM350ODb3pFOxD52Bfmvt7SCgKcY8kAIVNyC8p5+fz19hzNov4s1dJulakdkkm5e3qSKcgH7o2q0tUs7p0aOSNvZ0EohCVkQAUVkmnV0hMzWH3mSz2nMviaGquRezdmYqniwNdm9YhpoUfAzrUp4G3q9olCWF2JACF1cgrLufH4xls/y2TfReukV+iVbsks6DRQHigD4NCGjAwpAGNfCQMhQAJQGHhynV6dp6+yvqENLaeyqRMq1e7JLOm0UDHxj4MCqnPwA4NCKzjpnZJQqhGAlBYpISUHNYnXOKHYxlkF5apXY7FCm3szeCQBozs3Bg/D2e1yxGiVkkACouRllPE+iOXWJ9wiQtZhWqXY1WcHOwYEtKAx7s3oWOgj9rlCFErJACF2Tt4MZvF8RfYeuoKNnQei2rCAn0Y370Jg0Ia4OQgzaKE9ZIAFGZJq9Oz6XgGS/Zc5Ghantrl2CQ/D2ce7RrEuK5B1PNyUbscIUxOAlCYlVKtjm8Op/HZ7vOkZherXY4AHO01DOzQgEl9WtAywFPtcoQwGQlAYRYKS7V8dSCZxfEXycwvVbsccRt2Ghge3pi/3d+Sxr5y9qiwfBKAQlU6vcKqgynM3XqGrAI5m9MSONnb8WjXIJ7v00LOHBUWTQJQqCb+7FXe/uEUp6/kq12KqAZ3J3ueiGnKhPua4eXiqHY5QtwzCUBR685lFvDu5lNs/y1T7VKECfi4OfJMz+Y83r0JLo5yCydhOSQARa3JLSpj7tazfLk/2ab6ctqKRj6u/GNYe/q1C1C7FCGqRAJQ1DitTs9/9iUzb9tZ8orL1S5H1LAB7QOYOay9NOAWZk8CUNSoc5n5vPTNUY7JtXw2xd3Jnin9WzO+exPs5LZMwkxJAIoaodcrfLHnIrPjTlMqDaptVudgXz54OJTm/h5qlyLELSQAhcmlZhcxZc1RDl7MVrsUYQacHez42/2tmNCjmdykV5gVCUBhUl8dSObdTacoLNOpXYowMx0DfVjwSLjcgkmYDQlAYRJXrpfw8tpj7DpzVe1ShBnzdnXk37Ed5UxRYRYkAIXRtv56hSlrjsoZnqJKNBr4v/uaM21Aa5kSFaqSABTVpigK87efY87WM8hvkbhXXZvWYf6j4dTzlDtNCHVIAIpqKSrTMnXNUTYfv6x2KcKC+Xs6M29MOFHN66pdirBBEoDinqVmFzFh+WF+uyw9PIXx7O00vHR/K57t1RyNRqZERe2RABT35OfzWTz31RFyiuR4nzCt/u0CmPdIuPQTFbVGAlBU2bK9F3l70ynp4ylqTGQTXxb/JRJvN7m7hKh5EoDirrQ6PdM3nGD1oVS1SxE2oFWAB8uf6Ep9bzk5RtQsCUBRqVKtjudXJrDl1ytqlyJsSCMfV/7zRBda1JMWaqLmSACKOyos1fL0isPsPXdN7VKEDfJ1c+SL8ZF0CvJVuxRhpSQAxW3lFpUxfukhElNz1S5F2DBXR3sWju1E7zb11C5FWCEJQHGL7MIyxi4+wKmM62qXIgQOdhreHxnKyM6N1S5FWBkJQHGDawWljF18QK7xE2ZFo4E5o8J4KLyR2qUIK2KndgHCfGQVlPLI5/sl/ITZURSYuuYoW+VkLGFCEoACgLyich79fD9nrhSoXYoQt6XVKzy38gj7zstJWcI0JAAFpVodE5YflvATZq9Uq2fC8sMcS8tVuxRhBSQAbZyiKEz55igHk+Tu7cIyFJRqeXzJQc5lylS9MI4EoI1778ff+OFYhtplCHFPcorKGbf4IKnZRWqXIiyYBKANW7b3Ip/tvqB2GUJUy+XrJTz2xQGu5peqXYqwUBKANuq/Jy7z1g+/ql2GEEZJulbEk/85REm5Tu1ShAWSALRBvyTn8OLXCchNHYQ1OJaWx6vfHle7DGGBJABtTPK1QiYsP0xJuV7tUoQwmfUJl/hs93m1yxAWRgLQhpRqdTzz5RGyC8vULkUIk3v/v6fZdeaq2mUICyIBaEPe/uEUv0p/T2GldHqFF1YncCm3WO1ShIWQALQR/z2RwYr9yWqXIUSNyi0q59mvjlCmlSl+cXcSgDYgNbuIl9ceU7sMIWrF0dRc3t4kZziLu5MAtHLlOj2TViVwvUSrdilC1Jrl+5LZeDRd7TKEmZMAtHIf/Pc3uamtsEnTN5wg83qJ2mUIMyYBaMW2/3aFxXsuql2GEKrIKy7ntfVyfaC4MwlAK5V5vYQp3xxFbncsbNnWU5lsSLikdhnCTEkAWql/bPyVnKJytcsQQnUzN56UfqHitiQArdDO05lsOi53eBACKi6NeGPDCbXLEGaoxgPQwcGBsLAwOnToQGxsLEVF93b7kk8//ZSvv/4agGXLlpGZmWl4bNCgQRQXq3vR61NPPcX58+bTgqmkXMcb38kfuxB/9t+Tl+WsUHELjaLU7FEiPz8/srKyABg7diydO3fmpZdeqtZYvXr1YsGCBXTo0MGUJRrodDrs7e1rZOza8sF/f2PhTvMJZCHMRR13J7b87T7qejirXYowE7U6BdqjRw/OnTtHVlYWQ4cOJTQ0lF69epGUlATA6tWradu2LR07duTBBx8EYObMmSxYsID169dz+PBhHn74YSIiIgBo0qQJBQUFvPLKKyxZssTwPE888QTr169Hp9MxZcoUIiMj6dixI1999dUtNe3cuZM+ffowaNAgoqOjKSwsZPz48URGRtK5c2e2bNmCXq+nefPmFBYWAlBcXExwcDBarZZevXpx4kTFHtdPP/1EVFQU4eHhjBs3jrKyMlauXMnrr78OwGuvvUbfvn0B+P7775k8eTI6nY5x48bRrl07QkJCWLp0abW379kr+XweL/f3E+J2sgvLePP7k2qXIcxIrQWgVqvlxx9/JCQkhJkzZ9KjRw+OHTvGM888w+TJkwF45513+P777zl69CjLly+/Yf3hw4cTERHB2rVrOXz48A2PxcbGsmbNGsPzbNu2jYEDB/LFF1/QoEEDDh06xP79+/nggw+4du3aLbX98ssvLF68mP379/POO+8wZMgQDh06xE8//cSkSZPQaDQMHDiQH374AYDNmzfTv39/HBwcDGNkZWXxr3/9i+3bt5OQkECzZs34/PPPiYmJYc+ePQAcOnSIwsJCtFote/bsISYmhsTERC5evMivv/7K8ePHGTFiRLW2r6IovL7+BOU6Oe1TiDvZdCyDveey1C5DmIkaD8Dc3FzCwsKIiIggODiYJ598kj179jBu3DgARo0axcGDBwGIjo7m6aefZvHixdzLzGxERAQXLlwgJyeHbdu2ER0djYuLC3FxcSxevJiwsDCioqLIy8vjwoVb95Cio6Np2LAhAHFxcbz11luEhYXRr18/CgsLuXLlyg0hu3btWmJjY28YY//+/Rw7doyoqCjCwsJYs2YNFy9eJCgoiCtXrlBQUIBOpyMqKoqEhAT27t1LdHQ0zZo1Iz09neeee464uDi8vb2rtZ3XHE7jYFJ2tdYVwpa89+Ope3p/EdbL4e6LGMfHx4fExMRKl9FoNAB88skn7N+/n40bNxIREcHx41W/iPWhhx5iw4YN/Pzzz4Zw0uv1LFq0iJ49e1a6rpubm+FrvV7Pxo0bCQ4OvmGZevXq8cQTT3Dt2jX279/PihUrbnhcr9czePDg205hdurUic8++4zOnTvTrVs3tm3bRlZWFo0aNQLg+PHjbN68mTlz5hAXF8fs2bOr/LoBcgrLeO/HU/e0jhC26sSl63yXmM5D4Y3ULkWoTJXLIGJiYli5ciVQsTfVpUsXAC5cuEBUVBTvvPMOTk5Ot0xXenp6kp+ff9sxY2NjWbVqFVu3bmXgwIEA9O/fn4ULF6LT6QA4ceKE4es76d+/P/PmzTN8/3t429nZMXDgQCZNmkS/fv1umP4EiIqKYseOHSQnV9xx4fr161y8eNHweufMmUN0dDQxMTF8/PHHREZGAhVTp3q9nlGjRjFz5sy7fli4nY+2nZVr/oS4B//66TSl2srfC4T1q/E9wNuZOXMm48ePZ/ny5dSpU4dly5YBMHXqVM6dO4eiKAwfPpzGjRvfsN748eMZP348np6etxwHjIiI4Ny5c0RFReHi4gLAhAkTuHjxIuHh4ej1eho0aMCPP/5YaW1vvPEGL7zwAqGhoWi1Wjp16sSXX34JVIRsr169+Omnn25Zz9/fn88//5yRI0dSVlaGnZ0dc+fOpWnTpsTExJCWlkb37t2pV68erq6uREdHA3Dp0iXGjx+PXq/HwcGBuXPn3tO2TMspYuWBlHtaRwhbdym3mP/8nMTT9zVXuxShohq/DELUrKlrjrL2lzS1yxDC4ni7OrJ7Wm+83RzVLkWoRDrBWLBzmfmslz6HQlRLXnE5C3acVbsMoSIJQAs2Z8tZdHrZgReiuv6zL5m0nHvrTiWshwSghTpzJZ/NJ6TfpxDGKNPq+XDLGbXLECqRALRQ87efk1sdCWEC3yemk5Gnbk9hoQ4JQAt0/moBm45JY18hTEGrV1j2c5LaZQgVSABaoI93nEMO/QlhOqsOpFBUplW7DFHLJAAtTFZBKT8clWN/QpjS9RItaw7L5US2RgLQwnxzOJUynV7tMoSwOkv3XkQvUys2RQLQguj1CqsOStcXIWpC0rUitp66onYZohZJAFqQXWevkpotZ6sJUVO+2HNR7RJELZIAtCBf7U9WuwQhrNqBi9mcuJSndhmilkgAWohLucVs/y1T7TKEsHpL9speoK2QALQQqw+myKUPQtSC/564LJdE2AgJQAug1elZfShV7TKEsAlFZTr+e+Ky2mWIWiABaAG2/HqFq/mlapchhM2Qu6zYBglAC/D9UWl7JkRt2nsui8zrJWqXIWqYBKCZKynXsevMVbXLEMKm6BXYeEw6Llk7CUAzt+dsFkVlOrXLEMLmbD4uAWjtHNQuQFQu7lfzPhh//dAGCo7GAQouTcLw7fs0V1a9iq4wF42DIwD1x83GztGZ7G2fU5KUiGuzzvj2fgKA3PgvcQkKxSU4VMVXIcStjqTkkJFXTANvV7VLETVEAtCM6fQK206Z77V/uqI88o/8QMMnF4KdPVdW/p2y9N8A8H/o7zj5NzEsqy8poOzKeRo++TGXV/4dfWkh+rISyrMv4dNjnEqvQIg7UxT48fhlnohpqnYpoobIFKgZO5yUzbXCMrXLqJSi16Foy0CvQ9FrsXPzuf2CGjvQaFAUPWg0gIa8n1fhE/1obZYrxD358YRMg1oz2QM0Y3G/mndjXns3b7y6jCDtk7+isbPHI2wgjr4NAMjaOBs0dni0741Xl+HYObvh2iScjKWTcW97H9rrmaCxx9EvUOVXIcSdHUnJJb+kHE8XR7VLETVAAtCMmfvxP11JAcXnDtJo4hI0Dk5krplBSeoJ/IZOxcHTD31pIZnrZuFQtzFuzSPxjhqFd9QoAK5+9z51+j1N7p6VlF9Nwr19L9xadVf5FQlxI51e4eDFbPq2DVC7FFEDZArUTP2aft3s7/xQkpSIg29D7F09sXN0xrV5JKXpv+Hg6QeAnbM77m1iKMs4c8N6xUmJOPoFoS8tQnv9Kn4P/Z3rh79X4yUIcVc/n7+mdgmihkgAmqndZ83/2j8HTz9KL51C0Zah6HWUphzHsU5jdEUV3fQVXTnFF37B0S/YsI6iKOQf/g6vLsNRyktBrwU06EsKVHoVQlRunwSg1ZIpUDN1OClH7RLuyrlRG1ybR5C+dDIajR0uTTriEhzGlZWvoOh1oNfj2qILbq2jDesUntyBW6so7BxdcKzXFEVbRsYXz+Ee0k/FVyLEnZ26fJ3cojJ83JzULkWYmEZRFLnHgBnqPGuL2Z8BKoSt+HRcJx7o0EDtMoSJyRSoGUrKKpTwE8KMyHFA6yQBaIaOpJj/9KcQtkSOA1onCUAzJAEohHk5m1kgtySzQhKAZuiX5Fy1SxBC3ORwUrbaJQgTkwA0M4WlWs5cyVe7DCHETU7L36XVkQA0M4mpuej0cmKuEObm7BW5VtXaSACamQQ5/ieEWZKZGesjAWhmTsunTCHMUtK1Qsp1erXLECYkAWhmLlyVABTCHJXrFC5mFapdhjAhCUAzoijyByaEOTt9WaZBrYkEoBm5fL2EojKd2mUIIe7grBwHtCoSgGbk4lXZ+xPCnJ2RY/RWRQLQjKRkF6ldghCiEmcyZQ/QmkgAmpG0HPO+Aa4Qtk7+Rq2LBKAZScuRPUAhzFmZVk9+SbnaZQgTkQA0I5dy5dOlEOYuW25VZjUkAM1Iem6J2iUIIe4iq0AC0FpIAJqR6zK1IoTZkz1A6yEBaEYKS7VqlyCEuItrBXJfQGshAWgmisq0yE0ghDB/12QP0GpIAJqJghLZ+xPCElyTY4BWQwLQTOTL9KcQFiG7UKZArYUEoJmQPUAhLINMgVoPCUAzUSB7gEJYhNJyuSegtZAANBMSgEJYBp0iZ6tZCwlAMyFToEJYBq2crm01JADNRJlOplWEsAR6CUCr4aB2AaKCo718FrFGHQN9qO/lrHYZwoQCfd3ULkGYiASgmXB2kAC0SorCgkc7yQccIcyQ/FWaCScJQKt0NC2P2T+dVrsMIcRtyLuumZA9QOv1WfwF4s9eVbsMIcRN5F3XTMgeoPVSFHjpm6NkSRNlIcyKvOuaCWcHe7VLEDXoan4pU9ccRZFryIQwGxKAZkKmQK3fztNX+WLPRbXLEEL8j7zrmgkJQNvwwX9Pc+JSntplCCGQADQbMgVqG8p0eiatSpCbHwthBiQAzYS3q6PaJYhacjGrkDe/O6l2GULYPAlAM+Ht5oibk+wF2op1R9L4LvGS2mUIYdMkAM1IA28XtUsQtWj6+hOkXCtSuwwhbJa0QjMjDX1cOX+1UO0yRC3JL9UyaXUCaydGmaRV2vnc88Qlx3H0qlxuYS16B/ZmTJsxapdhtSQAzYjsAdqeo6m5/DvuDH8f2MbosZr7NOcZn2fILMpkW8o2tiZv5Zcrv6BTdCaoVKihmXcztUuwahKAZqSBt6vaJQgVLNp9npgWfsS09DPJePXc6vFIm0d4pM0jZJdksyNlB1uSt3Dg8gG0ejn71JLYaeQoVU2SADQjDX1kD9AWVbRKS+THF3pQ18O0t06q41KHka1GMrLVSK6XXWdn6k62JG9hX/o+SnXSms3c2WvkxLiaJAFoRmQP0HZl/q9V2pLxkWg0mhp5Di8nL4Y1H8aw5sMoKi9id9pu4pLj2HNpD8Xa4hp5TmEcezsJwJokAWhGZA/Qtu04fZUle5N4MqZpjT+Xm6MbDzR9gAeaPkCJtoS9l/ayJWULu1J3UVBeUOPPL6rG3dFd7RKsmgSgGZE9QPH+j7/RtWkdOjTyNm6g0nxI+BJa9oe6zStd1MXBhb7Bfekb3JdyXTn7MvaxJXkLO1J3kFdqOW3bTk85jZ2rHRqNBnt3e5q80oS0T9IouVRCnV51qHt/XQDSvkjDf7A/zvVNO91cE3ycfdQuwapJAJoRd2cHGni7kJFXonYpQiVlOj2TVyfww6QY3JyM+PN09gSNPczvBAEdoO0waDcM6rWtdDVHe0fua3wf9zW+D61ey6HLh9iavJVtKdu4VnKt+vXUkmbTm2HvUjFtWJxSjMZBQ4u3W3B+xnnq3l+X4uRi7F3sLSL8AHydfdUuwarJKUZmpl0DL7VLECq7cLWQGaZoldb1aWg9CK6cgJ3vwsJusCASts2CjKN3Xd3BzoGohlG8EfUG20dtZ+mApYxtO5YAtwDja6sFGntNxfWQOtA4VBxXvfr9VfyH+atcWdX5uPioXYJV0yhyxaxZmf3TaRbsOKd2GcIMzHsknGEdGxo3SFE2fBIN+em3PubbBNoOhbYPQuMIqOLJN4qicDzrOFuTt7IleQtpBWnG1Wgip6eext7dHo2dhrr318Wnuw/pK9IpOlNE3f51cfB2oCSlBP8hlhOA3z30nVwLWIMkAM3M5uMZPPvVEbXLEGbA08WBzZN7EFjHzbiBLsbD8mGg6O+8jFej/4XhMAiKAruqTw6dunaKLclb2JqylYt56t3vsDynHEdfR8pzy0n6IInAZwJxCaw4sUzRKyTPTSbouSAur7mMNkdL3QF1cW9l3ieZ7B69G18XmQatKRKAZiYpq5Bes3eqXYYwE+FBPqz5vygcjG2Vtm0WxM+u2rLu9aDN4Ipjhk3uA/uqH4s8n3ueLclb2JK8hTM5Z6pZrPEur76McyNnfHtUhEf2rmw0DhocvB0oPl+M3wN+pMxPocnUJqrVeDd2GjsSHkuQi+FrkGxZMxNc101ujSQMElJy+XCLCYKk16sQ2LVqyxZmwi9LYcVwmN0CNjwHZ34CbdldV23u05yJHSeybtg6Ng3fxIudXqRD3Q5GFn93+lI9uuKKlm+6Eh0FpwpwbuRseCz/SD4+3X1QShUUbcVnfl2RebeI83LykvCrYbIHaIYe++IA8Wez1C5DmAk7DXz5ZFe6tzCyVVpuCnwSA9W9tMHZG1oNqNgzbNEPHKt+2U5GQQZbUyqOGSZmJqJg2redsswyUuanABXTnb49ffHrX7G9Mr/LxK2lGx7tPNCX6Umek4w2T4v/MH98uvmYtA5TauLVhI3DN6pdhlWTADRDH8adZt52ORFG/CHAy5kfX7iPOu5Oxg104ltY+1fjC3J0h5b9Ko4ZthpQcdlFFV0tumpo1n34ymFp1n0HXRt0ZXH/xWqXYdUkAM3QtlNXePI/h9UuQ5iZvm3q8cX4SOMH+u55SFhh/Di/c3CB5n0qwrD1QHD1qfKqOSU57EjdQVxyHAcypFn3n41qNYo3ot5QuwyrJhPMZig8yLeqZ6QLG7Ltt0yW7jXBWZYDPwC/VsaP8zttCZzeDBsmwr9awIoR8MsyKLz7NL6viy8jWo7g036fsmv0Lt6NeZfegb1xtreMC9VrUpBX0D2vo9FomD59uuH7qVOnsmzZsmo9/86dOzl48OA9rzd+/Hh++OGH2/57s2bN6NixI6GhoWzbtq1adX366ad8/fXX1Vr3ZhKAZqiOuxMhxrbCElbpvR9/49f068YN4uQGDy+BmggZfTmc3wYbX4DZrWDZEDj4OVzPuOuqXk5eDG0+lHl95rF79G7+1fNf9A/uj6uDbbYIDPYKvud1PDw8+Oqrr8jPzzf6+SsLQJ2uetPW8+bN4+jRo3z44YdMnDixWmNMnDiR0aNHV2vdm0kAmqlereupXYIwQ2VaPZNWHaG4zMjjZvVD4P63TFPUnSg6SIqHzVPhw7bwRX/4eUHFyTh34eboxgNNHuDfvf7N7tG7mdt7LkOaDcHTserHGi1ddfYAnZ2dGTt2LAsXLrzlsfPnzzNgwAAiIiLo06cPSUlJAPTq1YsTJ04AcOLECXr16kVqaiqffvop//znPwkLCyMxMZHx48fzzDPP0KVLF/75z3+yYcMGunTpQnh4OIMHDyY3N7fKdcbExJCW9kcDhffff5/IyEhCQ0OZPbvicp3Ro0ezfft2wzJ9+vQhISGBmTNnsmDBgju+pvT0dKKjowGIi4vD1dWVsrIycnNzCQ8PB2Du3Lm0bt1aAtBc9W5tOd0qRO06f7WQmd+boFVat4nQ6gHjx6kSBVIPQNzrMDcEPusF8R/CtfN3XdPFwYW+QX15r8d77Bq9i4/7fszwFsOtulG0k50TQZ73HoAAL7zwAp999hklJTf2FH722WdZtGgRhw8fZvr06UybNu2OYwQGBjJx4kT+/ve/k5iYSFhYGADXrl3jwIEDvP766/Ts2ZMDBw6QkJDAgAED+Pjjj6tc46ZNmxg2bBhQEVJpaWkcPHiQhIQENm/ezIkTJ4iNjWXNmjUAZGZmkp6ebgiwyl5Tw4YNycnJobS0lD179tCuXTt++eUXfv75Z6KiogB46623OHLkiDTDNlcdG/tQx92J7MK7X3slbM/Xh1Pp0cqPIaFGtkp7cCF8Gg35d5+iNKn0hIr/tv0D6rWvuLSi7TAIaFfpajc36z585bChWXdWsfVcOtTEuwkOdtV7e/b392fIkCEsWbLE8G8FBQXEx8fz0EMPARXt7Nzd770LzsMPP2y4X2VKSgqxsbFcuXKF4uJiuna9+3WmkydP5qWXXiIlJYW9e/cCFQG4adMm4uPjAcjPz+fMmTMMGjSIl19+GZ1Ox/r16xkxYsQNY1X2miIiIjh48CAHDhxgypQp7Nmzh5ycHMOeYZcuXRg3bpwEoLmys9NwX0s/NiTepoejEMCr3x6nY2Mf41qludeF4YtgxUOVt0qrSZknK/7b+R7UbflHGDYMq3Q1BzsHujXoRrcG3Xit62skZCawNXkrW1O2crnwcu3UXkNa+LQwav2pU6fSr18/Bg4cCIBerycgIIDExMRblnVwcECvr/jZl5aWVjqum9sfv2uTJ0/m9ddfp3///vzwww9VOtlm3rx5DBkyhDlz5jBhwgSOHDmCXq9nxowZPP7447csHxkZye7du1m7di0ffPDBDY9V9ppiYmLYtWsXpaWl9O/fnwkTJpCdnc3TTz8NVOyB7ty5U6ZAzZkcBxSVyS/R8sLqBLQ6I4OrWU+IftEkNRnt2lmI/zd81hPmhkLcdEg9BHe5WstOY0fngM680uUV4kbGsXLQSv7a4a8EegbWUuGm1dK3pVHrBwYGEh0dzbp16wDw8vIiICCAjRsrLqzX6XSG437BwcGGEPn2228NY3h6elZ6Ms3169dp1KgRiqKwfPnye6rvxRdfRKvVEhcXR//+/Vm8eDFFRUUAJCUlkZdX0awhNjaWTz75hLS0tFumPyt7TTExMSxatIiwsDD8/PzIysoiPT2dJk2aoNfrSU1NpW/fvhKA5qxnK3/s5HIIUYkjKbnM3XrW+IF6vw6NTXCNoSnlJsPP8+GLfjCnPWx+GZL2gL7ywNdoNIT4h/BS55fYPGIza4au4enQpy3qrgpt6rQxeoxXXnmF9PQ/ZpBWrlzJ/Pnz6dixIyEhIYbLEF566SU++OADOnfuTFnZH4dchg4dyqpVqwwnwdxsxowZDB06lMjISAID7+2Dhkaj4c0332T27Nk88MADDB8+nG7dutGhQwfGjRtnOH45aNAgNm/ezPDhw287zp1eU9u2bSkuLjZMebZt25ZOnToBFUE5duxYQkND5UJ4czd84V4SUnLVLkOYMTsNfPVUN6Ka1zVuoJxk+LRH9Vul1RYjmnVfyL1gaNZ9Oud0DRZZffYae/aM2YOHk4fapVg9CUAzN2/bWdM0QxZWrb6XCz++0ANfY1ulHV8L6540TVG1wdW34qa/bYdB897gUPVrG1Ovp7IlZQtbk7dyPOt4DRZ5b9rWacs3Q79RuwybIAFo5i5mFdJbbo8kqqBf2wAWPx5h/EAbnoPEL40fp7Y5e1X0JW37v2bdTlU/Oehy4WXDDX4TryaiV+uEIGBc23G80uUV1Z7flkgAWoDYT3/mUFKO2mUIC/CPYe15vHsT4wYpK4RFPStOSLFUjm4VIdjuwXtu1p1VnMW25G1sSdnC4cu136z7w14fcn/w/bX6nLZKAtACfHMolZfXHVO7DGEBnB3s2PBcNG0beBk3UMYxWNwPdJWfFm8R7J0rmnW3+71Zd9XvsJ5bkntDs+5yfXkNFlph56id1HU18niuqBIJQAtQWKol8p2tFBnb/krYhBb1PNj4fAyuTvbGDbRvIfz0qmmKMhd2jtC0R8U0aZsh4FH1jkv5ZfnsTN3J1uSt7E3fS2kNfDiQewDWLglACzF1zVHW/pJ29wWFAB7pEsh7I0KNH+irUXD2J+PHMUcaewjuXhGGbYeCV4Mqr1pUXsTuS7vZmryV+LR4irRFJilpZMuRzOw+0yRjibuTALQQBy5cY/Rn+9UuQ1iQhWM7MSik6m/qt1WYBZ9EQ4Fld1a5O03FdZDthlUcN/Speh/OUl0pey/tZWvyVnam7SS/rPp3Yng35l2GNh9a7fXFvZEAtCC9/rWDpGum+aQprJ+XiwM/vngfjXyMvJ3QhZ2wYrh6rdLU0CDsfy3ZHgS/qrclK9eXsz99P1tTtrIjZQc5pVU/eU2Dhi0PbyHAPaAaBYvqkAC0IAu2n2V2nFwTKKouItiXr/8vCntjWwptmQF755qkJotTr13FXmEVmnX/mU6v4/CVw2xJ3lKlZt3t67Zn9ZDVxlYr7oEEoAXJyCsm+p/b0ctPTNyDyX1a8FL/1sYNotPCkgFw6bBpirJUdVtUBGG7YdAw/O7L/49e0ZOYmWgIw4zCW+++MSl8Ek+HPm3KasVdSABamGe+/IUfT1j78RhhSnYaWDmhG92aGXlqffZFWHQflBp5R3pr4RP0vzB8sOL4oabqe9knsk4QlxzH1uStpOanAvDtsG+NboIt7o0EoIU5cSmPIfP3qF2GsDANvCtapfm42VirtNri2RDaDqkIxODuYFf1S1BOZ59mX/o+xncYX3P1iduSALRAjy85yK4zV9UuQ1iYAe0DWPSYCVqlrX8Gjq40fhxr5e5f0ay77TBo2vOemnWL2iUBaIEOXsxm1KJ9apchLNCshzrwWLdg4wYpLai4X9+1c6Ypypq5+FQ06243rKIbzT006xY1TwLQQo36dB8Hk7LVLkNYGGcHO75/PobW9aveG/O20hPhi/tBV3bXRcX/OHlW9CVtNwxa3H9PzbpFzZAAtFA7T2cyfukhtcsQFqhVgAffPx+Di6ORrdJ+XgBxr5umKFvj6AYt+lZcZ9j6gXtq1i1MRwLQgg2dv4fjl8z85qXCLI3tGsQ7w0OMG0RR4KtYOLfFNEXZKnvninsZth0GbQbdU7NuYRwJQAv23xMZTPzyiNplCAv16bjOPNChvnGDFFyFT6Oh4IppirJ1dg7QpAf0ehWCuqpdjdWzU7sAUX0D2tenZT0PtcsQFuqVdcdIzy02bhAPfxj+KWBkp5mbDP+6CN/3r/PwN3+0/jt4SUf7hQW0mJfPW7sq7sSgKApj1hbRYWEB8w78cXeGJ78r5sw1C7x7il4LF3aoXYXNkAC0YBqNhmkDjOzwIWxWXnE5L36diM7Y1kLN+0D3SaYp6n9e6OrE8odu7GH63OZiVo105fTzHmw+q+X4FR3Hruhxstdw/Bl3liZW3KsvIUOHh5OGVnWNPMapFq/GENhF7SpsggSghevfvj7dm8vNM0X1HLyYzfztJrjze983oWEn48f5n15NHPB0/mOvMj1fj1YPoQH22NtpGNPBgR/OaHG0BwXQ6sHZvmL5t+NLeaOnkRf8q6n9Q/fUVUZUnwSgFZg+uB3G9joWtmv+9nMcMvaSGntHePiLilP9a0B6vkIjzz/erhp52nEpX087f3u8nSHy80ImRjjy49lyIhva4+dmwW9t7UeoXYHNsODfEvG7dg29GBURqHYZwkLp9Aovrk4kr6jcuIHqNIMhH5qmqHuwYJAriRM9+EtHRxYcKmdSFycm/1jCyG+K2JOirfV6jOLfBhp3VrsKmyEBaCWmDmiNl4u0XBLVcym3mL9/e8z4gUJHQegY48e5SUNPDZfy/7gf4aV8PQ09b3z7WppQzpj2DuxN1eHvpmHFcFdm7S69eSjzFvmU2hXYFAlAK+Hn4cxUOSFGGOHHE5f56kCy8QMN/jfUaW78OH/S0NMOew0cu6JDp1dYfULL0FZ/fOArKlfYcFrLuFBHisoVynQKigJ5JSYto2Y5eUBH0394EHcm1wFaEb1eYdjHezhxSW5XI6rHxdGOjc/H0DLA2FZpCbD4ftBXb1q13/JCjl7RU1imUMdVw5pYVzQaePL7Ekq0Co+FOjKzl4th+Vm7SokOsqdPUweKyxWGrCoiI1/hzZ7OjOngaNxrqS0RT8CQOWpXYVMkAK3MkZQcRn7yM/JTFdXVpr4nG56LNr5V2t55sOUN0xRlC575GQLaq12FTZEpUCvTKciXsV2D1C5DWLDfLufzzqZTxg/UfRI072v8OLYgKErCTwUSgFbo9UHtaObvrnYZwoKt2J9M3MnLxg2i0VR0iXGvZ5qirJmc/KIKCUAr5Opkz0ejw3G0l4sDRfW9vO4YGXnGtkqrB8M/wdSt0qyKe72KRtii1kkAWqmQxt680Lel2mUIC5ZbVM6LqxPRG9sqrUU/iHrONEVZo87jwcGCO9dYMAlAK/ZsrxZENpFbq4jqO3AxmwU7THDn934zoWG48eNYG2dviHpW7SpslgSgFbOz0/DhqDA8neUCeVF9H207yy/JJmiVNvKLimvdxB+6PSP3/1ORBKCVC6zjxsxhcnaZqD6dXmHyqkTyio1slVa3OQyabZqirIGLj+z9qUwC0AaM7NyYwaEN1C5DWLBLucW8aopWaWGPQOho48exBt2fBxdvtauwaRKANuLdh0IIruumdhnCgm0+fplVB1OMH2jwv8G3qfHjWDLXOtD1GbWrsHkSgDbC282RLx6PwFMaZgsjvLXxV85l5hs3iLNnxa2T7CykRVlNiJ4MznI8VG0SgDakRT1PFjzaCXu5eaCopuJyHc+vTKBUqzNuoEadoc900xRladz9ocvTalchkAC0OT1b+TN9cFu1yxAW7LfL+bxrilZp0S9As97Gj2NpYv4GTtKpyRxIANqgv0Y3lX6hwij/2ZfM1l+vGDeIRgPDF1XsEdkK/zay92dGJABt1D+GtSe6RV21yxAWbNrao1y5buQN9zwD4CEbapU2+N8V10QKsyABaKMc7O1Y+GhnmvnJVIyonhxTtUpreT90s4Hr4ULHQJMYtasQfyIBaMO83RxZ/HgE3q7yiVRUz74L11i400St0hp0NH4cc+XiA/3fVrsKcRMJQBvXzN+D5U90kcsjRLXN3XqWX5JzjBvEwQkeXmq9rdL6vgkeNnSs00JIAAo6Bvqw4smu0jNUVItWr/DC6gSul5igVdrAD0xTlDlp1Bk6/1XtKsRtSAAKAMICfVj2RBc8JARFNaTlFPPqt8eNHyh8LITEGj+OudDYw5A5YCdvteZIfirCoHOwL/95IhJ3J3u1SxEWaNOxDL4+ZIpWaR+CbxPjxzEHXZ627mObFk4CUNygc3Adlj3RRUJQVMvM73/lXGaBcYO4eMHIJZbfKs2vNfSboXYVohISgOIWkU3qsGR8JG4SguIeFZfrmLzKBK3SGneG3q+Zpig12DvByMXg6Kp2JaISEoDitro2qyshKKrl14zrvLf5N+MHivkbNOtl/Dhq6DMdGoSqXYW4CwlAcUfdmtVl5YRu+Hk4qV2KsDDLfk5i2ykTtUpz8zNNUbWlaU+ImqR2FaIKJABFpcICffj2mWjpGCPu2bS1x8g0ulVafctqleZeD0Z8Lmd9Wgj5KYm7CqrrxrpnutM52FftUoQFyS4s48WvTdAqrVV/6DrRNEXVJI0djPy8or9pVVfRaJg+/Y/bQk2dOpVly5aZtKwNGzZw5swZw/dPPfUU58+fN3pcBwcHwsLCaN++PUOHDiU3N7da4wwaNIji4mKj66kOCUBRJb7uTnz1VFceDGuodinCgvx8/hqf7DL+zZb734L6Zn5MrcfUez5m6eHhwVdffUV+vpE3Ga7EzQG4ePFimjdvbvS4Pj4+JCYmcvLkSXx8fPj444+rNc7mzZtxdVXnZCEJQFFlLo72fDQmnGkDWqOxkBkpob45W86QkGKKVmlLwNFMp+Jb9odef7/n1ZydnRk7diwLFy685bHz588zYMAAIiIi6NOnD0lJSQDs27eP9u3bEx4eznPPPcfDDz8MVARdly5dCA8PZ/DgweTm5nLgwAG+//57Jk+eTFhYGJmZmfTq1YsTJ07wySef8Oabbxqe76233mLOnDkAvP/++0RGRhIaGsrs2bPv+jqio6NJS0sD4OrVq4wYMYKIiAiioqJISEggLy+Pli1bGpZPTk4mLCwMgCZNmlBQUHHpzIoVK4iMjKRjx4689NJLALz77rt8/vnnADz66KM8+eSTAMybN48PP/yQgoICHnjgAUJCQggJCeGnn36q8vaXABT37LneLfh0XGc5Q1RUiVavMHl1AvnGtkrzawkD3zdNUaYUEFLRx9Suen8PL7zwAp999hklJTceL3322WdZtGgRhw8fZvr06UybNg2ACRMmsGLFCkOw/K5nz54cOHCAhIQEBgwYwMcff0zXrl0ZNmwY8+bNIzExkXr16hmWHzFiBN9++63h+3Xr1hEbG0tcXBxpaWkcPHiQhIQENm/ezIkTJ+5Yv06nY8uWLQwZMgSAF198kVdffZXDhw+zfPlyJk6ciLe3N61bt+bAgQMArF27ltjYGzv+nDp1iu+++459+/Zx9OhRsrKy2LRpEzExMezZsweoCM7f92b37NlDTEwMP/30E3Xr1uX48eMcO3aMqKioKm97CUBRLQPa1+fbZ7vTsp6VNi8WJpWaXcxr6+/8JlplnR6DDiONH8dUPBvAo1+Dc/X/Dvz9/RkyZAhLliwx/FtBQQHx8fE89NBDhIWF8be//Y1Lly6Rm5tLeXk5nTp1AmD06NGGdVJSUrj//vsJCQlh3rx5/Prrr5U+b0BAAP7+/pw4cYIzZ87g7u5O48aNiYuLY9OmTYSHh9O5c+cbQufPcnNzCQsLIyAggPT0dAYMGADA1q1bmTBhAmFhYcTGxnL58mUAYmNjWbNmDfBH2P7Ztm3b2L9/PxEREYSFhbF//37OnTtHly5dOHToECkpKQQFBeHv78/Vq1c5cuQI4eHhhISEsHv3bl5++WX279+Pl5dXlbe9BKCotjb1vdg4KUbuLi+qZOPRdL45nGr8QEPmgE+w8eMYy9EdHlkN3o2MHmrq1Kl89NFHaLVaAPR6PQEBASQmJpKYmMjRo0f5+eefUZQ7n1A0efJkXn75ZY4fP87cuXMpLS296/OOGjWKNWvWsGbNGkMg6fV6ZsyYYXju8+fPM2LEiFvW/f0YYHJyMhqN5oZp3MOHDxvWT05OBuChhx7i+++/JzU1leLiYlq1anXDeHq9ngkTJhjWO3PmDC+88AIuLi74+vqydu1aYmJiiI6OZsWKFTRu3BhHR0datWpFYmIi7du356WXXmLBggV33+D/IwEojOLiaM87w0P47LHO+LpZeOsqUeNmfn+SS7lGnvHn4g0jvwA7FRu3/37GZ8MwkwwXGBhIdHQ069atA8DLy4uAgAA2btwIVEwznjhxAl9fXxwcHEhMTAQw7FEBXL9+nUaNGqEoCsuXLzf8u6en5x1Psvl9GvTPe2T9+/dn8eLFFBUVAZCUlHTDVOvN3N3dmTdvHv/+97/RarX07t2bTz75xPD40aNHAfD29qZVq1a88sorhuOWf9a3b1++/vprrl27BkBmZiYZGRlAxTHGOXPmEB0dTUxMDHPmzCEmpuLmwunp6bi7u/P444/z4osvGrZNVUgACpPo374+/33xPro3r6t2KcJMuTra89qgtjTyMcEZf4GR0OtV48eprvtnQZvBJh3ylVdeIT093fD9ypUrmT9/Ph07diQkJIRt27YB8NlnnzF27Fg6deqEs7OzYcpvxowZDB06lMjISAIDAw3jjBkzhlmzZhlOgvmzgIAA/Pz8cHFxoXHjxgA88MADDB8+nG7dutGhQwfGjRt3y/HJm0VERBASEsI333zD/Pnz2blzJx07dqRt27asXLnSsFxsbCyrVq26ZfoToH379rz++uv07duX0NBQBg8eTHZ2NgAxMTHk5eUREhJCp06dyM7OJjo6GoDjx48TGRlJWFgYc+fONZw8UxUapbJ9aiHukV6v8Onu88zZcoZynfxqiQohjbyZOyaM5v4mPGas18OKB+HibtONWRURT1RMw6qksLAQd/eKs2Gff/552rRpw/PPP69aPZZM9gCFSdnZaXi2VwvWTuxOk7puapcjVOZgp+G53s359tnupg0/qOi2MvwzcKvFWYd2D8HAf9Xe893Gd999R1hYGO3atePatWuGywLEvZM9QFFjist0fLzjHJ/FX6BMq1e7HFHLujatw6yHOtAqwLNmn+j0f2HV6LsvZ6x2D1Uce7SXm0ZbCwlAUeMuZhUy8/uT7DpzVe1SRC3w83Dm9cFtGB7euPaedPPLcHBRzY0v4WeVJABFrfnp5GXe2vir8WcBCrNkb6dhXNcgpgxojZdLLZ8RrC2Fz/vCleOmH1vCz2pJAIpaVVJeMS26aLdMi1qT8CAfZj3YgQ6NvNUr4uoZ+KwnlBeZbkwJP6smAShUkZRVyMyNJ9l5WqZFLZmfhxNT+7dmdGQgGnNoEPvLf2DjZNOMJeFn9SQAhap+Pp/FvG1n2X8hW+1SxD3w83BmYs9mjO0ajKu59YRdMx5OrjdujA4jK84wlfCzahKAwiwcvJjNvG1n2XMuS+1SRCX8PZ35v/uaMa5bMC6OZhZ8vyvJg09jIDeleuvH/A36zkBueWL9JACFWTmSksO8bWdlatTM1PN0ZmLP5jzaNch8g+/PUg/C0oGg11Z9HTtHGPIhdPpLzdUlzIoEoDBLx9JymbftLFtPZd59YVFjArwqgu+RLhYSfH+261+w4+2qLeviDaNWQLOeNVuTMCsSgMKsnUzPY9neJDYeS6ekXM4arS1dmtbhkS6BDAppgLODhQXf7/R6WD4MkuIrX863CTy6BvxbVb6csDoSgMIi5BWXs+6XNFYeTOFcZoHa5VglXzdHRnZqzJguQbSwlvs8Xk+HT6Kh+A4nWQV2hTErwd2vdusSZkECUFicAxeusfaXNDYfz6CwTKd2ORZNo4FuTevySNcgBrQPsNy9vcr8thlWP3Lrv4fEwrAF4OhS+zUJsyABKCxWUZmWzccvs/aXVA5ezEYvv8lV1sDbhWFhDRkTGURTP3e1y6l5m6bCoc8rvnZwgQfeq7irg7BpEoDCKmQVlLLjt0y2ncpkz7ksCkrv4ew/G9HMz50BHeozoH19Ojb2No8L12tLeQks7lvRMi12GdTvoHZFwgxIAAqrU6bVc+DiNbadymT7b5mkZJuwNZYFcbTX0DnYl16t69G3TT1a1vRdGcxdTnLFrZOcreT4pjCaBKCwemev5LPtt0x2n7nKsbQ8q907tLfT0LKeB+FBvtzX0o+Yln541nZTaiEsiASgsCl6vcL5qwUkpuZyLC2Po2m5/JaRT5nO8i6xaODtQligDx0DfQgL9CG0sTduTtK6S4iqkgAUNq9Uq+NURj7H0nJJTM3lXGYBl3KKuVZYpnZpALg52dPY15VAXzdaBngSFuhDeJAPAV5y9qIQxpAAFOIOist0XMotIjWnmLScYi7lFJOWU1TxdW4xecXlRt3SSaMBFwd73J3t8XJxpJGvK4F13AxhF1jHjUBfV+p6OJvwVQkhficBKIQRyrR6Cku1FJRqKSzTUlqup0ynp1yrp1SnR6dTcHG0x9WpIujcHB0MX7s62tvWmZhCmBkJQCGEEDbJTu0ChBBCCDVIAAohhLBJEoBCCCFskgSgEEIImyQBKIQQwiZJAAohhLBJEoBCCCFskgSgEEIImyQBKIQQwiZJAAohhLBJEoBCCCFskgSgEEIImyQBKIQQwiZJAAohhLBJEoBCCCFskgSgEEIImyQBKIQQwiZJAAohhLBJEoBCCCFskgSgEEIImyQBKIQQwiZJAAohhLBJEoBCCCFskgSgEEIImyQBKIQQwiZJAAohhLBJEoBCCCFskgSgEEIImyQBKIQQwiZJAAohhLBJEoBCCCFskgSgEEIImyQBKIQQwiZJAAohhLBJEoBCCCFskgSgEEIImyQBKIQQwiZJAAohhLBJEoBCCCFskgSgEEIImyQBKIQQwiZJAAohhLBJEoBCCCFskgSgEEIImyQBKIQQwiZJAAohhLBJEoBCCCFs0v8DAqsSUMzEau4AAAAASUVORK5CYII=</t>
+  </si>
+  <si>
+    <t>https://www.flipkart.com/micromax-x512/p/itmfhwvhrwhxq5tu?pid=MOBFHWSYNUXWAGVT&amp;lid=LSTMOBFHWSYNUXWAGVTREGB3S&amp;marketplace=FLIPKART&amp;q=micromax+x512&amp;store=tyy%2F4io&amp;srno=s_1_3&amp;otracker=search&amp;iid=e532b5ae-9020-461a-a39a-dca423c959b8.MOBFHWSYNUXWAGVT.SEARCH&amp;ssid=0udxp3g2jk0000001689862408205&amp;qH=8aab057c4a7cd0c3</t>
+  </si>
+  <si>
+    <t>₹1,174</t>
+  </si>
+  <si>
+    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAcAAAAFQCAYAAAAoQ64wAAAAOXRFWHRTb2Z0d2FyZQBNYXRwbG90bGliIHZlcnNpb24zLjYuMSwgaHR0cHM6Ly9tYXRwbG90bGliLm9yZy/av/WaAAAACXBIWXMAAArEAAAKxAFmbYLUAABCAElEQVR4nO3deVhU9eIG8Hdg2LcR2XdxF0RQUBFMXEJxqVxQS0vLLCsjb2pWmvbTsvJamWWmmZqmZi65dyV33PfdREA2QRBE9m1mzu8PbnNDAQGBMzPn/TwPj4wzc+adw8y8c7bvkQmCIICIiEhiDMQOQEREJAYWIBERSRILkIiIJIkFSEREksQCJCIiSWIBEhGRJLEAiYhIkliAREQkSSxAIiKSJBYgERFJEguQiIgkiQVIRESSxAIkIiJJYgESEZEksQCJiEiSWIBERCRJLEAiIpIkFiAREUkSC5CIiCSJBUhERJLEAiQiIkliARIRkSSxAImISJJYgHouLCwMv/zyS6NMWyaTITU1tVGmXR/JyclQKBRix9Bq69atw5AhQ+p9vbb5+OOP8eqrr1Z7vaWlJdLS0powUc0a8/1IdccCbGJeXl4wNzeHpaUlXFxcEBUVBZVK1SSPvXr1avTr169Wt01OToalpSUsLS1hYWEBmUymuWxpadnISevHw8MDDx48EDuGVhszZgx27typufzwl5iHr9c2df3SVVBQABcXl0ZM1PRYog2HBSiC6OhoFBQUICYmBlu2bMFPP/0kdqRHeHh4oKCgAAUFBYiPjwcAzeWCgoJGe1ylUtlo09YG+v78pEQQBKjVarFj0BNgAYqoZcuWCAkJwcWLFzX/t3nzZvj4+MDW1hbPPPMMMjMzAQD37t1DREQEFAoF7Ozs8PzzzwMADh06hFatWlWablXfkhMSEjBp0iQcOnQIlpaW8PHxaZDnsHPnTrRo0QJ2dnb47LPPNP+vUqkwZ84ceHp6wtHREVOnTq32wz8sLAwfffQRAgMDYWFhgfLychw+fBhdunSBQqFAWFiYpoRfffVV/N///V+l+3t7e+Po0aNITEyEXC7X/P/9+/fxwgsvwMHBAd7e3vj5558BALdu3aq0VBAeHo4+ffpoLru4uODWrVvVzvOHxcfH46mnnoJCoYCLiws+/PBDzXWrV69G79698frrr8PGxgarVq2qNldVZDIZvv32W3h4eMDJyQn//ve/NdeVlJTgrbfegpOTEzw8PDB37lzNB/LJkycREBAAa2truLq64uuvv9bk+XstQHh4OACgbdu2sLS0RExMTKXra5rXAKr9G1Xl+++/h7e3N+zt7TF27Fjk5uYC+N/rd+7cubC1tYWXlxf27t1b5TSqygsAxcXFiIyMhJWVFbp164bbt29Xmn9/vxdWrlwJT09PWFlZoW3btjh06FCd5/n48eMxefJk9OnTB+bm5oiPj0dMTAwCAgKgUCjQq1cv3LhxQ3P7M2fOwM/PD9bW1pg0aVKlwhw/fjw++eQTzeWH19AcOHAAgYGBsLa2RuvWrRETE4N58+YhJiYGr776KiwtLTF//vxq5znVgkBNytPTU4iJiREEQRBu3rwpODk5CQsXLhQEQRBOnToluLq6CpcvXxbKysqE6dOnC8OHDxcEQRBmzJghvPHGG0J5eblQUlIiHDt2TBAEQTh48KDQsmXLSo8BQEhJSREEQRB69eolrF27VhAEQVi1apXQt2/fSrf97LPPhEGDBtWYOT09XajqpQJAGDFihJCfny9cuXJFMDExEeLi4gRBEIQFCxYIvXv3FjIzM4WcnBwhLCxM+Pbbb6ucfq9evYSWLVsKt27dEoqLi4Xk5GTBzs5OOHLkiKBUKoXFixcLgYGBgiAIQnR0tNChQwfNfU+dOiW4ubkJarVauH37tmBoaKi5buDAgcLUqVOFkpIS4caNG4Kzs7Nw6dIlQRAEwdHRUYiLixOUSqXg7u4uuLq6CmVlZUJcXJzg6OhY4zx/WFxcnHDo0CGhvLxciI2NFdzd3YXff/9dM88NDQ2FVatWCSqVSigqKqoxV1XzODw8XMjNzRVu3LghODk5Cfv27RMEQRA+/PBDoVevXsL9+/eFpKQkoXXr1sKqVasEQRCEbt26Cb/88osgCIJw//594fz585o8/3wN/PO18vD1Nc3rmv5GD4uOjhacnJyEa9euCQUFBcKwYcOEcePGCYJQ8fo1NDQUPv/8c6G8vFxYtmyZ4OHhUeV0qso7Z84cwczMTDhw4IBQXl4uvPjii8JLL730yO0LCgoEKysrITY2VhAEQUhMTBQSEhLqPM/HjRsnNG/eXDh79qxQXl4u3L17V1AoFMKWLVuEsrIyYcGCBUKrVq2E8vJyobS0VHBzcxO+//57oaysTFi8eLFgaGioeT+OGzdOmDdvXpXzPj4+XrCyshJ27twpKJVKISkpSbh165YgCJXf0/RkuAQogoiICFhaWqJt27bo0aMH3nrrLQAV31DffPNNdOzYEUZGRvjoo4+wfft2KJVKGBkZIT09HSkpKTAxMUGPHj0aJMv777+PXbt2PdH9LS0t4evrCz8/P1y5cgUA8NNPP+GTTz6Bvb09FAoFpk6dis2bN1c7nQkTJqBVq1YwNTXFunXrMHToUPTs2ROGhoZ4++23kZiYiMTERPTp0wf37t3DtWvXAAC//fYbIiMjIZPJKk3v7t27OHToED777DOYmJigXbt2eOGFF7B161YAQM+ePXHkyBFcuHABfn5+8Pf3x/nz5xETE4PQ0FAAqPU8b9myJXr16gW5XI7WrVtjzJgxmqWkv68fP348DAwMkJubW2OuqnzwwQewtrZGu3btMGHCBGzcuBEA8Ouvv2LOnDlo1qwZPDw8MHXqVGzYsEGTPS4uDvfv30ezZs0QEBBQ49+xKjXN65r+Rg/79ddf8dprr6FDhw6wsLDA/PnzsXHjRgiCAACwsLDA9OnTIZfLMXbsWCQnJ9dpW27fvn3Ru3dvyOVyjB49GpcuXarydjKZDNeuXUNpaSk8PT3RokWLaqdZ3TwHgOHDh6NLly6Qy+WIjo6Gn58fhg0bBiMjI0ydOhVFRUU4c+YMTpw4AblcjjfeeANGRkaYPHkynJ2da/WcNmzYgCFDhmDw4MEwNDSEh4fHI2t66MmxAEXwxx9/ID8/H9u2bcPZs2c129SSk5Px6aefQqFQQKFQwN3dHXK5HHfv3sX06dPh4eGBXr16oV27dlqz3dDR0VHzu7m5eaXn8vfqQ4VCgTFjxmhW51bFzc1N83tycjLWrl2rua9CoUBhYSHu3LkDQ0NDjBgxQvMBumnTJowaNeqR6SUnJ6OkpERTwAqFAsuWLcPdu3cBVBRgTEyMpvD+eblnz54AUOt5fufOHQwdOhROTk6wsbHBokWLkJ2dXe1zqylXVdzd3Sv9np6eDgBIS0uDh4eH5jpPT0/NHo8rVqzAtWvX0KpVK4SGhuLEiRPVTr86Nc3rmv5GD6sqZ0lJCe7fvw8AsLe3h4FBxUeRubk5ANRpO3N1r8F/srCwwIYNG7B48WI4OjoiMjKyxr1Dq5vnQOW/58PPzcDAAO7u7khLS0N6enql28pkskqXa5KamlpjQVPDYAGKRCaT4dlnn0W/fv002wFcXV0xb948PHjwQPNTXFwMNzc3WFtb45tvvkFycjJWr16Nt99+GwkJCbCwsEBxcbFmuhkZGTU+ZlNxdXXFwYMHNc8jNzcX169fr1U2V1dXTJw4sdJ8KCoqQkhICABg1KhR+O2333Dy5EkYGBigW7duVT6+paUlcnJyNNPIz8/HDz/8AOB/S4BHjx5Fz5490bNnTxw9ehRHjx7VLAFWN88fNmvWLDRr1gyxsbHIzc3FlClTNEs3VT23mnJVJSUlpdLvfy9FuLi4IDk5WXNdcnKyZttm27Zt8dtvvyEzMxOjR4+udvvl41Q3rx/3N/qnqnKamprC1ta2Xpnqa+DAgThw4ABSU1NhYmJSaVvtw6qb50Dlv+fDz00QBKSkpMDFxQXOzs6PbIv/5+Wa3rvu7u5VLk0//Pj0ZFiAIps2bRpWrFiBrKwsvPzyy/juu+80q3Du37+P7du3AwB2796NhIQECIIAGxsbyGQyGBoaok2bNsjJycHhw4dRWlqKefPmVftYDg4OSE1NbZI9EV955RXMmjUL6enpEAQBiYmJOHz4cK3u+8ILL2DTpk2IiYmBWq1Gfn5+pdWnPXv2RH5+PmbNmoWRI0dWOQ1XV1cEBwdj1qxZKCoqglKpxPnz5zUl3KlTJ9y7dw8xMTEICgpCYGAgTpw4gfT0dPj7+wOofp4/LD8/H1ZWVrC0tMTVq1dr3EX9cbmq8sUXXyAvLw83b97EypUrNc951KhRmDdvHnJycpCSkoKvvvoKo0ePBlBxPF92djbkcjmsrKyqzA1UvCaq+6AFqp/Xj/sb/dOoUaPw448/4saNGygsLMTMmTMxcuTIen2QPy5vdTIyMrBr1y4UFxfDxMQE5ubm1c4ToPp5/rCIiAhcunRJs6ni66+/hpmZGQIDAxEcHIzy8nIsX74c5eXlWLJkSaUlyU6dOmH37t3Iy8tDQkJCpTUMzz//PHbu3Ik9e/ZArVYjJSVFs5NRfecBPYoFKLL27dujV69e+Oabb9CjRw8sXLgQL730EqytrdG5c2ccO3YMABAbG4vevXvDysoKgwYNwqJFi+Dp6QkbGxt88803GDlyJFq0aIGgoKBqH6tPnz7w8vKCvb09/Pz8AADz589HREREgz+v6dOnIzg4GCEhIbCxscGQIUMqfauuSYsWLfDrr79i+vTpsLW1Rbt27TRfBICK1UyRkZE4cOBAtR9MQEUJpKamwtvbGw4ODpgyZYrmG7eBgQF69OiBdu3awdjYGMbGxujQoQO6d++u+WCsbp4/bPbs2Th48CCsra0RFRWF4cOH1/j8aspVlYEDB8LX1xdPPfUUoqKiNHsKfvTRR2jbti3atWuH4OBgjB49GuPGjQMA7NmzB23btoWVlRUWL16MNWvWVDnt2bNnY/jw4VAoFJW2W/6tunn9uL/RP4WHh+ODDz7AwIED4enpCSMjIyxatKjGeVSdx+WtjlqtxoIFC+Do6AgHBwfcuXOn0h6YD6tunj/Mzs4O27Ztw5w5c9C8eXP8/vvv2LZtG4yMjGBsbIwtW7bg22+/RfPmzXH58uVK25FffPFFtGzZEm5ubnj++ecrLaW3aNECW7ZswcyZM2FjY4O+fftqyvPtt9/G6tWroVAo8Pnnn9d6HtCjZMI/19UQkVaRyWRISUmp9bYjenKc59LBJUAiIpIkFiAREUkSV4ESEZEkcQmQiIgkiQVIRESSxAIkIiJJYgESEZEksQCJiEiSWIBERCRJLEAiIpIkFiAREUkSC5CIiCSJBUhERJLEAiQiIkliARIRkSSxAImISJJYgEREJElysQMQaaPiMhXScouRkVuC9NwS3M0rQXpuMe7mliK/pBwqtQClWoDqHz9Ktbrid0GASlXxr7HcANamRhU/ZnJYmxpBYW4EO0sTOFibwN7SFPZWJnCwMkEzC2OxnzaRpPB8gCRZhaVKXL2Tiyt3chGXWVBRdLkVRZdXomzyPApzI7RxsEIbJ0u0dbJGW0crtHWygo2ZUZNnIZICFiBJQkm5CtfS8nAl9QEup+bi8p1cJNwrgFoHXv1O1qZo61RRhm0crdDOyQodnK1hYCATOxqRTmMBkl5Kyi7E0bgsXEqpKLy4zAIodaHtasnGzAg9WjZHz9b26NnaDu625mJHItI5LEDSC6VKFU4m3Mehm5k4fPMeErIKxY7UpLyamyO0tR16trZHcMvmsDblalOix2EBks7KLS7H/hsZ+M/Vu4i5lYXicpXYkbSCoYEMndxs0LO1Pfq1d0RHNxuxIxFpJRYg6ZT7hWXYcyUde6/dxcmEbJSr+PJ9nLaOVhjexRXPBbjCwcpU7DhEWoMFSDrh9O37+OVkEv5z9S7KVGqx4+gkQwMZnmpthxFd3NGvgwNM5IZiRyISFQuQtFZ+STm2nr+DdaeSEJtRIHYcvaIwN8IQPxcM7+IGf3eF2HGIRMECJK1z9U4ufjmZhB2X0lBUxu16ja21gyVGBbljVJA7rLjzDEkIC5C0Qkm5CjsupWHdqWRcSnkgdhxJsjKVY2x3T7wS0gL2ViZixyFqdCxAElWpUoX1p5Kx5GA8sgpKxY5DAEzkBhjexQ2vP+UNz+YWYschajQsQBKFSi1g87kULN4fhzsPisWOQ1UwNJDhOX9XRPVtxSIkvcQCpCYlCAJ2Xk7Hoj9jJXewuq6SG8gwNMAVUX1bc8QZ0issQGoy+65n4Ms/Y3EjPU/sKFQPcgMZRgW5Y3r/tlCY88wVpPtYgNTojsdn4d97b+JC8gOxo1ADsLUwxowBbTEy0B0yGQfkJt3FAqRGk5lfgtnbruE/1+6KHYUaQWcPBT55riM6uFiLHYWoXliA1Cg2nknGp7tviHJePWo6hgYyvNjdE1PD2/AYQtI5LEBqUCn3i/D+1ss4FpctdhRqQvZWJpg5sD2eC3AVOwpRrbEAqUGo1QJWHruNL6NjeVYGCevubYt5z/qitaOV2FGIHosFSE8sNiMf722+jIscwYUAGBsa4L0BbfFqT2+xoxDViAVI9VamVGPJwTgsPRTPMzTQI/q1d8TCSD8eMkFaiwVI9ZJyvwhvrjuPK3dyxY5CWszFxhTfvhCALp62YkchegQLkOps3/UMvPvbRe7hSbUiN5DhX0+3wZthLXncIGkVFiDVmkotYMHev7D8SAL4qqG6eqqNPb4a2Ql2ljzTBGkHFiDVSnZBKd5cdx6nbt8XOwrpMAcrEywa7Y8eLe3EjkLEAqTHu5aWi9fWnONZG6hBGMiAKf3aIKpva7GjkMSxAKlGOy+l4b3Nl3lsHzW4kYFumD+0I+SGBmJHIYliAVKVBEHAwuibWHIwXuwopMf6tHPAkhc6w8zYUOwoJEEsQHqESi3g/S2XselcqthRSAL83RVYOT4IthY8XpCaFguQKilXqTFl40XsvpwudhSSEG87C/z8SleecJeaFAuQNErKVXhr3Xns/ytT7CgkQQ5WJlj1chB8XGzEjkISwQIkAEBRmRIT15zlWRxIVFYmcix7sQt6tOJhEtT4WICEvJJyvLzqDM4l5YgdhQjGhgZYOLITnunkInYU0nMsQIm7X1iGl1aewtU7eWJHIdIwkAGLRgewBKlRsQAlLDOvBGNWnMKtzAKxoxA9Qm4gw9KxXfB0B0exo5CeYgFKVFZBKUYsPY7E7CKxoxBVy1hugJ/GBaJna3uxo5Ae4hAMElRcpsKEn8+y/EjrlSnVeG3NOZzmGLTUCFiAEqNWC4j69QIu8eztpCOKy1WY8PMZ/HWX26mpYbEAJWburuv483qG2DGI6iS/RInxK88gjQOyUwNiAUrIipgErD6eKHYMonq5m1eCcStPI7eoXOwopCdYgBLxn6vpmL/nhtgxiJ7IrcwCTPj5DEp4dhJqACxACTifnIMpGy9Czf19SQ+cTcrBrG1XxY5BeoAFqOeSsgsx8eezKClXix2FqMFsPpeKjWeSxY5BOo4FqMdyi8sxftUZZBeWiR2FqMHN3n4N19O4ZyjVHwtQj3249QpuZxWKHYOoUZQq1Xhz3Tnkl3CnGKofFqCe+u1MCnZf4Tn9SL8lZhdh+qbLYscgHcUC1EMJ9wrw8c5rYscgahL/uXYXK2ISxI5BOogFqGfKVWq88+tFFJVxN3GSjs//+AvnkjhcGtUNC1DPLNx7E1fu5Iodg6hJKdUCJq+/gOyCUrGjkA5hAeqRY3FZWM5VQSRR6bklmLLxIniCG6otFqCeuF9Yhn9tvAi+90nKYm5l4bezKWLHIB3BAtQT722+hMx8rv4h+uyPv7gqlGqFBagH1p1Kwr4bmWLHINIKD4rKMW/XdbFjkA5gAeq4rIJSfPHHX2LHINIq2y6m4eitLLFjkJZjAeq4+btvIK9EKXYMIq0za9sVnjWCasQC1GGnErKx9cIdsWMQaaXE7CJ8e+CW2DFIi7EAdZRSpcZH23lKGKKaLD+SgNiMfLFjkJZiAeqo1ccTEZtRIHYMIq1WrhLw4dYrPDaQqsQC1EE5hWVYvJ+rdohq42xSDjac5rGB9CgWoA5atC+WO74Q1cGX0TdRzPFx6SEsQB0Tl1mAdad4JmyiusguLMOaE4lixyAtwwLUMfP33IBSze0ZRHW1/EgCisq45oT+hwWoQ84n5+DAXxzxhag+sgvL8PPxJLFjkBZhAeqQpYfixY5ApNOWH4lHYSmXAqkCC1BHxGXmY9+NDLFjEOm0nKJyrD6eKHYM0hIsQB3xw+EEnuqIqAH8GJOAAi4FEliAOiE9txjbL3LIM6KG8KCoHKuP3RY7BmkBFqAOWBFzG+UqLv4RNZQVR28jv6Rc7BgkMhaglntQVIZfT/O4P6KGVLEUmCh2DBIZC1DLrTmRhEKOYEHU4NaeTIJSpRY7BomIBajFistU3GONqJFk5pci+jr3rJYyFqAW++1sCu4Xlokdg0hvrTvFA+OljAWoxfjmJGpcx+OzkXCPpxWTKhaglrqWlsvz/RE1MkEAB5eXMBagltp+MU3sCESS8PuFOyjnzjCSxALUQmq1gB0sQKImcb+wjIPMSxQLUAudTMjG3bwSsWMQScbmc6liRyARsAC10O8XOOwZUVM6dDOTe1xLEAtQy5SUq/Cfq3fFjkEkKeUqgePtShALUMvsv5GJfI5UT9Tk/rjCL55SwwLUMtv4LZRIFOeTc5BbzAGypYQFqEUeFJXh8M17YscgkiSlWsDRW1lix6AmxALUIn9ez0AZj0ciEs3BmzwcQkpYgFrkRHy22BGIJO1w7D0IAs+9KRUsQC1yIoEFSCSme/mluJaWJ3YMaiIsQC1xO6sQ6bk8+J1IbAc5KoxksAC1xPF4bnwn0gaHYrkjmlSwALXEcW7/I9IKF1Me4EERR4WRAhagljjF7X9EWkGlFnCEh0NIAgtQC9y8m4+sAn7jJNIWR7gaVBJYgFrgBLf/EWmVq3dyxY5ATaDGApTL5fD394evry8iIyNRVFRUp4n/8MMP2LhxIwBg9erVyMz8395VAwcORHFxcT0iN5xXX30V8fHxomYAuP2PSNvEZRagVKkSOwY1MplQw1GfdnZ2yMqqWDoZM2YMunTpgnfffbdeDxQWFobvvvsOvr6+9Uv6GCqVCoaGho0y7cYkCAL85/7JMQiJtMzOyaHo6GYjdgxqRLVeBdqzZ0/ExcUhKysLQ4YMgZ+fH8LCwpCYmAgA+PXXX9G+fXt06tQJzz77LADg448/xnfffYfff/8dZ8+exYgRIxAYGAgA8PLyQkFBAWbMmIGVK1dqHueVV17B77//DpVKhalTpyIoKAidOnXCunXrHsl06NAh9OnTBwMHDkRISAgKCwsxfvx4BAUFoUuXLvjzzz+hVqvRsmVLFBYWAgCKi4vh6ekJpVKJsLAwXL16FQCwd+9eBAcHIyAgAGPHjkVZWRnWr1+PmTNnAgA+/PBD9O3bFwCwY8cOREVFQaVSYezYsejQoQM6duyIVatW1XX+Iym7iOVHpIWup3M1qL6rVQEqlUr88ccf6NixIz7++GP07NkTly9fxhtvvIGoqCgAwKeffoodO3bg0qVLWLNmTaX7Dx06FIGBgdi8eTPOnj1b6brIyEhs2rRJ8zj79+9HREQEfvrpJzg7O+PMmTM4efIkFixYgOzsR1cVnjt3DitWrMDJkyfx6aefYvDgwThz5gz27t2Lt99+GzKZDBEREdi1axcAYM+ePQgPD4dcLtdMIysrC//+979x4MABXLhwAd7e3vjxxx8RGhqKo0ePAgDOnDmDwsJCKJVKHD16FKGhobh48SJu376N69ev48qVKxg2bFht57vGX3fz63wfImp8HBFG/9VYgA8ePIC/vz8CAwPh6emJCRMm4OjRoxg7diwAYOTIkTh9+jQAICQkBK+99hpWrFhRp7H0AgMDkZCQgJycHOzfvx8hISEwNTVFdHQ0VqxYAX9/fwQHByM3NxcJCQmP3D8kJAQuLi4AgOjoaMydOxf+/v7o168fCgsLkZGRUalkN2/ejMjIyErTOHnyJC5fvozg4GD4+/tj06ZNuH37Njw8PJCRkYGCggKoVCoEBwfjwoULOHbsGEJCQuDt7Y20tDS89dZbiI6Oho1N3VeX3GQBEmml6yxAvSev6UqFQoGLFy/WOAGZTAYAWLp0KU6ePImdO3ciMDAQV65cqXWI5557Dtu2bcPx48c15aRWq7Fs2TL06tWrxvuam5trfler1di5cyc8PT0r3cbBwQGvvPIKsrOzcfLkSaxdu7bS9Wq1GoMGDapyFWbnzp2xfPlydOnSBd27d8f+/fuRlZUFV1dXAMCVK1ewZ88efP3114iOjsbChQtr/bwBIDaDBUikjf66mw9BEDSfcaR/6nwYRGhoKNavXw+gYmmqa9euAICEhAQEBwfj008/hbGx8SOrK62srJCfX/WHfWRkJDZs2IB9+/YhIiICABAeHo7vv/8eKlXFnlhXr17V/F6d8PBwLF68WHP57/I2MDBAREQE3n77bfTr16/S6k8ACA4OxsGDB5GUlAQAyMvLw+3btzXP9+uvv0ZISAhCQ0OxZMkSBAUFAahYdapWqzFy5Eh8/PHHj/2yUJW/7vJbJpE2KihVIjG7bnu+k26pcQmwKh9//DHGjx+PNWvWwNbWFqtXrwYATJs2DXFxcRAEAUOHDoWbm1ul+40fPx7jx4+HlZXVI9sBAwMDERcXh+DgYJiamgIAJk6ciNu3byMgIABqtRrOzs74448/asz20Ucf4Z133oGfnx+USiU6d+6MX375BUBFyYaFhWHv3r2P3M/e3h4//vgjhg8fjrKyMhgYGGDRokVo0aIFQkNDkZqaih49esDBwQFmZmYICQkBANy5cwfjx4+HWq2GXC7HokWL6jQvy1VqvsGItNj1tDy0sLMQOwY1khoPg6DGFX+vAH2/PCx2DCKqxlu9W2J6/3Zix6BGwpFgRJSUXSh2BCKqwa2MArEjUCOq8ypQajiJWdq5+jP31FYUXtkHyADr7pGw9OmNu+vfh6rwAWRyIwCA09iFMDAywf39P6Ik8SLMvLugWe9XAAAPYn6BqYcfTD39xHwaRE8sM79U7AjUiFiAIkrUwiXAsnuJKLpxGM7jF0EQBGRs+BDmLSt2+rF/7n0Y23tpbqsuKUBZRjxcJizB3fXvQ11aCHVZCcrv34Gi51iRngFRw7nHAtRrLEARJWnhDjDlWSkwdmkHmdwYMgDGDi1QnHCu6hvLDACZDIKgBmQyADLkHt8ARcgLTRmZqNFkFbAA9Rm3AYoou1D73lxG9p4oTb4CdUkBVCUFKEm5AlVBxSEtWTsXIm1VFPJO/w4AMDAxh5lXANJXRcHMKwDKvExAZggjO3cxnwJRgylVqjlUoR7jEqCI8oqVYkd4hLGdB6wChyDj15mQmZjDxKUtIDOE3ZBpkFvZQV1aiMwt8yBv7gbzlkGwCR4Jm+CRAIB727+Abb/X8ODoepTfS4SFTxjM2/QQ+RkRPZl7+aWwMTMSOwY1Ai4Bikhbv1la+UfAefw3cHr+M8gM5JDbukBuZQcAMDCxgEW7UJSlx1a6T3HiRRjZeUBdWgRl3j3YPfc+8s7uECM+UYPidkD9xQIUiSAIKCjVviVAAFAVPgAAlGenojQ9FmYtOkNVVDEyvqAqR3HCORjZ/W+4OUEQkH92O6y7DoVQXgqolQBkUJdwF3LSffe4HVBvcRWoSApKlVCptXMMgsyt8yCUFkFmZIrmA6dAUJYj87fZENQqQK2GWauuMG8borl94bWDMG8TDAMjUxg5tICgLEP6T2/BomM/EZ8FUcPgEqD+4kgwIknNKULoFwfFjkFEjzGpV0u8H8HRYPQRV4GKRBt3gCGiR3EJUH+xAEWSV6KdO8AQUWXaurMaPTkWoEj4piLSDUq1WuwI1EhYgCLJYwES6QRt3VmNnhwLUCT5JdwGSKQLlCoWoL5iAYrEQCZ2AiL9URR3Gnd+fB13lk9E/qW9EJRlyPh1FtJWvInCm8c0t8vc+glUxfl1mrYuLQHKZDLMmjVLc3natGmak5bX1aFDh3D69Ok632/8+PHYtWtXlf/v7e2NTp06wc/PD/v3769Xrh9++AEbN26s130fxuMARWJiZCh2BGoEzjam6OhqUzE2ODUJtUqJTatXY9Ts5TA2t8TW2S/C290Wdv5d0GnwOOz54i30HzYMiecOwzmwG/wCW9Vp+i3tLRspecOztLTEunXrMGPGDFhZWT3RtA4dOgQ7Ozt07dr1ketUKhUMDev+GbZ48WIMHjwY+/btw6RJk3Dr1q06T2PSpEl1vk91WIAiMTbkwrc+Ss8tAQD093HCwI7OCPRsBgMu7jeq48ePIyu4M355ZyAAwPraUAQFtcZff6kwLdIPievtsOR5fwxZ/xEObdsGExMTkRM3HhMTE4wZMwbff/89ZsyYUem6+Ph4vPnmm8jOzoa1tTVWrlwJLy8vhIWF4bvvvoOvry+uXr2KyZMnY+3atfjhhx8gl8uxYsUKrF69GosWLYKZmRnOnTuHZ599Fj4+Ppg/fz7Ky8vh4uKCdevWQaFQ1CpnaGgoUlNTNZe/+OILbN68GaWlpXjppZcwbdo0jBo1Cq+//jr69OkDAOjTpw++/PJLbN++HXZ2dpg8eXKVz8nY2BiRkZE4duwYoqOj8eyzzyI3NxdFRUXo3bs3Lly4gEWLFmHp0qUsQLGYGLEA9VV6bglWH0/E6uOJsLM0QX8fR0T4OqO7ty3k/OLT4NLS0uDq6qq57OrqirS0NMTGxqJ3796YP38+fvzxR4wbN06vy+9v77zzDrp374533nmn0v+/+eabWLZsGby8vHDgwAFMnz4dmzZtqnIa7u7umDRpkqZo/padnY1Tp05BJpMhJycHzz77LGQyGRYvXowlS5Zg5syZtcq4e/duPPPMMwCA6OhopKam4vTp01Cr1Xj66acxYMAAREZGYtOmTejTpw8yMzORlpaGgIAAbN++/bHPKScnB6WlpTh69Cg6dOiAc+fOIScnB8HBwQCAuXPnIiUlhQUoFi4BSkNWQSnWnUrGulPJaGZuhH7tHTGwozNCWtnBWM7XQGORyWSa7UT5+flYsmQJ1q9fjwkTJiAvLw9z585F+/btRU7ZOOzt7TF48GCsXLlS838FBQWIiYnBc889B6Bi/F4LC4s6T3vEiBGQ/Xf9fnJyMiIjI5GRkYHi4mJ069btsfePiorCu+++i+TkZBw7VrFtNjo6Grt370ZMTAyAir9XbGwsBg4ciPfeew8qlQq///47hg0bVmlaNT2nwMBAnD59GqdOncLUqVNx9OhR5OTkICSkYgjHrl27YuzYsSxAsXAboPTkFJVj07lUbDqXCitTOfq2c8AAX2eEtbWHKV8P9ebi4oI7d+5oLt+5c6fSdqsFCxbgvffew4YNGxAWFoawsDDMmDED69evFyNuk5g2bRr69euHiIgIAIBarYajoyMuXrz4yG3lcjnU/z3WsbS05lFvzM3NNb9HRUVh5syZCA8Px65du2q1s83f2wC//vprTJw4EefPn4darcacOXMwbty4R24fFBSEI0eOYPPmzViwYEGl62p6TqGhoTh8+DBKS0sRHh6OiRMn4v79+3jttdcAVCyBHjp0iHuBisWE3/4lLb9EiW0X0zDpl3PoPO9PvLXuPHZeSkOhlp4hRJt17doVV69exZ07d1BQUIA//vgD/fv3B1CxejQhIQE9e/ZEUVERysrKUFZWhqKiIpFTNy53d3eEhIRgy5YtAABra2s4Ojpi586dACp2Yrl69SoAwNPTU1MiW7du1UzDysoK+fnV7zGbl5cHV1dXCIKANWvW1CnflClToFQqER0djfDwcKxYsULzN0lMTERubsXZZyIjI7F06VKkpqYiICCg0jRqek6hoaFYtmwZ/P39YWdnh6ysLKSlpcHLywtqtRopKSno27cvlwDFwtVf9LeiMhV2X0nH7ivpMJEboGdre0T4OqFfB8cnOxFr1i3g+nYgbh9Qrr8f+HIAXz5tjN6dW0MtCHgv3A3NNw8FAMxddwuz+7oCy57C6LIyPPfpdXw9W4XvRrUElj0lbvD6aDsICJvx+NsBmDFjBn7++WfN5fXr12PSpEmYNWsWysvL8frrr8PX1xfvvvsuRo0ahW+++UazwwkADBkyBCNGjMDGjRurXLqbM2cOhgwZAltbW/Tq1QtJSUm1fhoymQyzZ8/GwoULER0djevXr6N79+5Qq9VQKBTYsmULbGxsMHDgQIwfPx5RUVFVTqe659S+fXsUFxdrVnm2b98eLi4uACqKcsyYMcjPz+fZIMRyLS0XgxYfFTsGaTEjQxl6tLRDhK8Twn2cYGthXL8JlRUBt6KBGzuA2GigrG7HwZEW6TwOeGax2Cn0BgtQJHGZ+ej31RGxY5COMDSQoauXLSI6OmGAjxMcrE3rNyFlKRB/ALi+A7i5Byh50KA5qZEFvgIM/lrsFHqDBSgSng+Q6ksmA7p4NMMAXydEdHSGq8KsfhNSlQO3D1eU4V+7gaKshg1KDa/ra8DAf4udQm+wAEVSplSj7Ud/gHOfnpSfmw0G+DphoK8zvOzqvms7AECtApKOV6wmvbETyE9v2JDUMLq9AUR8LnYKvcECFFG3+fuQkceTbVLDaedkhQhfZ0R0dEIbx3oOhSUIQMrpijK8vgPITW7YkFR/T70H9Kndweb0eCxAEQ1fehznknLEjkF6ytveAhG+TojwdYavq039J5R2oaIIb+wAsuMaLmAj81qUD2sTGQxkQDMzGQ68ZI7ntxTjaqYar3UxQlS3ilFhJmwvxoxQY7RprgPHYkYsALq9LnYKvcHDIETkqjBjAVKjSbhXiCUH47HkYDzcbc0Q4euMAb5OCHBXaEbzqBWXgIqffnOAjGv/K8PM640XvoEcn2ABS+OK53rprgrGhjJcecMCnZcXIqqbCS6kq2BpLNON8gMA8+ZiJ9ArLEARuTWr584LRHWUcr8Yy48kYPmRBDjbmKK/jxMifJ0Q5GVbt8G6HX0qfnp/AGTFATe2VxRi+sVGy95QjAwBAYBSDZgYVjznT2JKsWxwPfeoFYO5rdgJ9ApXgYpo3akkzPz9qtgxSMLsLE0Q7uOICF8nBHs3r/9g3TlJ/9tmmHoGFVUjrhbf5MPWrGIV6JRuJhjjZ4TJe4pxNFmFKd2N4Wghw6UMNd4P1aEBsl8/Ajh3EjuF3mABiuhw7D2MW1n3E04SNQaFuRGebu+IiI5OCG1lX//RivLSKvYkvb4DSD4OCOqGDVpLd/LUcLU2QHq+Gv3WFmHDcDP4OVas6lQLAoZsKMZvI8zwwf5S3MlX41/djRHqoeUrxf51DbBxEzuF3mABiiguswD9vjosdgyiR1iZyNGnvQMifJ0Q1tah/oN1F9wD/tpVsXR4+wigFmes0+nRJfBxMMB4/4rRdH46XwZjQ8DR0gCnUlWY2sMYQzcWYe/Yeh5G0lRmZgBGOrTKVstp+dcd/cZtgKSt8kuV2H4xDdsvpsHc2BBhbe0xwNcZfdo5wNKkDh8blvZA4MsVP8U5wF97Ksow/iCgarxDgArLBKgFwMpEhoIyAQcSlRjpU/F+KyoXsO2mEjtGm2H7TSXKVAIEAfjvuYy1l5EFy6+BcQlQZIGf/ImsgjKxYxDVirHcAE+1tsMAX2c8/SSDdZfmA7F7G22w7oQcNYZurJimSg1M7GyEd7pXbOubd7gUIR6G6NNCjuJyAYM3FCE9X8DsXiYY7fsEg483NhsP4F9XxE6hV1iAIhv2/TGcT34gdgyiOjMylCH478G6OziiuWU9dyYpKwLi/qzYZhi7l4N1V8cjGHjlP2Kn0Cs8J4/IfFye4ABlIhGVqwQcib2HD7ZeQdf5+zF6+Qn8fDwRGXl1XJdobA50eBYY8RPwXjzw/EbAfwxgqmiU3DrLtmWd7yKTyTBr1izN5WnTptXqxLV1sW3bNsTGxmouv/rqq4iPj3/i6crlcvj7+8PHxwdDhgzBgwcP6jWdgQMHori4uMrrWIAi6+jGAiTdp1ILOJlwH3N2XEP3z/Zj+NLjWBGTgNScOq7alJsAbQcAz30PTI8Hxm4FuowHLOwbJbdOsW1R57tYWlpi3bp1NZ7Y9kk9XIArVqxAy5Z1L+uHKRQKXLx4EdeuXYNCocCSJUvqNZ09e/bAzKzq/S1YgCLzYwGSnhEE4FxSDj7ZfQOhXxzEkG+P4vtDcbidVVi3CRnKgVZ9gSHfAFNjgfG7ga6vA1YujRNc2zWve6mYmJhgzJgx+P777x+5Lj4+Hv3790dgYCD69OmDxMREAMCJEyfg4+ODgIAAvPXWWxgxYgSAiqLr2rUrAgICMGjQIDx48ACnTp3Cjh07EBUVBX9/f2RmZiIsLAxXr17F0qVLMXv2bM3jzZ07F19/XXEqpy+++AJBQUHw8/PDwoULH/s8QkJCkJqaCgC4d+8ehg0bhsDAQAQHB+PChQvIzc1F69atNbdPSkqCv78/AMDLywsFBQUAgLVr1yIoKAidOnXCu+++ywIUW2sHK5jVdxdzIh1w5U4uFvznJnovPIQBi45g0b5Y3LxbxyUSAwPAKxQYuAB49zow4U8geDKg8Gic0Nqoeat63e2dd97B8uXLUVJSedX0m2++iWXLluHs2bOYNWsWpk+fDgCYOHEi1q5dqymWv/Xq1QunTp3ChQsX0L9/fyxZsgTdunXDM888g8WLF+PixYtwcHDQ3H7YsGHYunWr5vKWLVsQGRmJ6OhopKam4vTp07hw4QL27NmDq1erHxBEpVLhzz//xODBgwEAU6ZMwQcffICzZ89izZo1mDRpEmxsbNC2bVucOnUKALB582ZERkZWms6NGzewfft2nDhxApcuXUJWVhYPgxCboYEMPi7WOMsxQUkC/rqbj7/u5mPRvlv1H6xbJgPcu1b89P8USLv431FotuvUYN11IjMEmrd+/O2qYG9vj8GDB2PlypWa/ysoKEBMTAyee+45AIAgCLCwsMCDBw9QXl6Ozp07AwBGjRqFn3/+GQCQnJyMyMhIZGRkoLi4GN26davxcR0dHWFvb4+rV6/C2NgYFhYWcHNzw6JFi7B7927ExMQAAPLz8xEbGwtfX99K93/w4AH8/f2RmpqK1q1bo3///gCAffv24dq1a5rb5eRUfHZGRkZi06ZN6NatG7Zs2fLIts79+/fj5MmTCAwMBAAUFRWxALVBgIeCBUiS8/Bg3QN8nDDA1xmdPeo6WLd/xU/f2UDG9f8NyZZ57XH31B22LZ7oGMBp06ahX79+iIiIAACo1Wo4Ojri4sWLlW73d5lUJSoqCjNnzkR4eDh27dpVq51pRo4ciU2bNsHY2FizRKZWqzFnzhyMGzeuxvv+vQ2wsLAQTz/9NL7//ntERUUBAM6ePQu5vHJ9Pffcc/j000/xzjvvoLi4GG3atKl0vVqtxsSJEzFnzhzN/3EVqBYI9OIAtyRtKfeL8WPMbQxfehzBnx3Axzuu4WRCNtTqOh6l5dgBCHsfePM48Pb5ilJ09m+UzE3Kof0T3d3d3R0hISHYsmULAMDa2hqOjo7YuXMngIrVjFevXkWzZs0gl8s1xbhp0ybNNPLy8uDq6gpBELBmzRrN/1tZWVW7k83fq0H/Xv0JAOHh4VixYgWKiip2kEpMTKy0qvVhFhYWWLx4Mb788ksolUr07t0bS5cu1Vx/6dIlAICNjQ3atGmDGTNmaLZb/lPfvn2xceNGZGdnAwAyMzNZgNogyMsWdfnCS6TP7uaVYPXxRIxefhJd5+/DB1uv4EjsPShVdRxTtHlLoOdU4PXDwDuXgfBPAfduAHTwzebQ4YknMWPGDKSlpWkur1+/Ht9++y06deqEjh07Yv/+/QCA5cuXY8yYMejcuTNMTExgbW0NAJgzZw6GDBmCoKAguLu7a6YzevRozJs3T7MTzD85OjrCzs4OpqamcHOrGMN0wIABGDp0KLp37w5fX1+MHTv2ke2TDwsMDETHjh3x22+/4dtvv8WhQ4fQqVMntG/fHuvXr9fcLjIyEhs2bHhk+x8A+Pj4YObMmejbty/8/PwwaNAgHgivLfp+eQjx9+q4lxyRhCjMjdCvfcWZK0Jb28FEXs+dx/LSKwbrvrEDSDoOCKqGDdoYRm8A2g1skocqLCyEhUXFmKiTJ09Gu3btMHny5CZ57KbGAtQS72+5jF/PpIgdg0gnWJnI0bvd/wbrNjOuZxkWZlUM1n3978G6yxs2aIOQAe8lNNm5ANevX48FCxagrKwMnTp1wsqVK6s9jk7XsQC1xI5LaYjacEHsGEQ6x8zo78G6ndC3vWPdBuv+p+Ic4OYfFWUYf6BRB+uuE/v2wFsnxU6hl1iAWqKgVInO8/5EmVKcc6cR6QNjuQF6trLDAF8nhHdwgo35Ew7WfWMHcOvPBh+su04CJwCDvxLv8fUYC1CLvLzqNA7evCd2DCK9YGQoQ3fv5ojwdUa4jyPs6jtYd3lxRQne+O9g3aV5DRv0cYb/BHR8dK9GenIsQC2y8UwyZmzh6U6IGpqhgQxBXs0Q4euMAb5OcLSu5zF1ylIg4VDFatKbuytWmza2d28A1hId/q2RsQC1yP3CMgR9ug+quh77RES1JpMBAe4KTRm625rXb0IqJZB4pKIM/9oFFDbC2huFJzDlcsNPlwCwALXO6OUncDLhvtgxiCSjo6sNBvg6IcLXCd72lvWbiFoNJJ+oGI7txk4gP+3x96mNTi8AQ5c+/nZULyxALbP62G18vPO62DGIJKeFnQUOTgt78gkJApB6FrixvWLp8EFS/af1zLdA55eePBNViSPBaJn+vk4cFYZIBIP9nBtmQjIZ4B4EhH9Ssfry9SMVI9LUZzBr77CGyURV4mDYWsbZxgx+rja4lFr92HhE1PCGdGqkHU2cO1X89J0NZN6oWCq8sQPIqP4UQAAAp47SOt2TCFiAWqi/rxMLkKgJtXG0RBtHq8Z/IIf2FT9hM4Ds+P9uM9wBpFUxCEbbQY2fR+K4ClQLDfRtoFUxRFQrQ/xEOMygeUug57vAa4eAKVeA/vMB9+7QDNbdjgXY2LgTjJZ64ceTOB6fLXYMIr1nIAMOT+9d/8MhGlr+3YoD7zu/KHYSvcclQC01roeX2BGIJKFve0ftKT8AsHJi+TURFqCW6tfeEa4K/RyBnUibvBziJXYEEgkLUEsZGsjwYrCn2DGI9Fo7Jyv0aGkndgwSCQtQi40OcoepEf9ERI1lPDc1SBo/XbWYwtwYz3ZyFTsGkV5qZm6E5wL4/pIyFqCWe6kHV4MSNYbRXT1galTPM8mTXmABajkfFxsEeTUTOwaRXpEbyPASt7FLHgtQB/CQCKKG1d/HCc423Mta6liAOmCAjxOcbep5Ak8iegQPfSCABagT5IYGeLtPPUaSJ6JHdPFshkAvW7FjkBZgAeqIUUHu8La3EDsGkc77cGA7sSOQlmAB6ghDAxne6883LtGT6O/jiC6eXPqjCixAHTLA1wmdPRRixyDSSXIDGWYM4JdI+h8WoI75YGB7sSMQ6aTRXd3hbW8pdgzSIixAHRPkZYt+7R3EjkGkUyyMDTGlXxuxY5CWYQHqoBkD2sHQQCZ2DCKd8dpTLWFnaSJ2DNIyLEAd1NrRCsM7cwxDotpwsDLBxKdaiB2DtBALUEf96+k2PFMEUS1M6dcG5sZysWOQFuInqI5ytjHDxJ7eYscg0mqtHCwxKshd7BikpViAOmxyn1Y8OJ6oGgYy4PNhHbm9nKrFAtRhJnJDfD7MDzK+v4ke8UpICw55RjViAeq4ri1sMaabh9gxiLRKS3sLTOvfVuwYpOVYgHrg/Yj2cOHZIogAVAwb+OVIf57slh6LBagHLE3k+Hw4V4USAcDrT3nD310hdgzSASxAPfFUG3u82J1nuCZpa+toxRFfqNZYgHrkg4j28LbjXqEkTXIDGb4c2QnGcn6sUe3wlaJHzIwN8dUof8i52zdJ0Fu9W8HX1UbsGKRDWIB6xt9dwbPHk+T4uFhjcp9WYscgHcMC1ENRfVuhX3tHsWMQNQkrUzm+fT4ARob8OKO64StGD8lkMiwa7Y/WDjz3Gek3mQz4eqQ/z/NH9cIC1FOWJnL8+FIgbMyMxI5C1Gii+rRGvw5c20H1wwLUY152Fvj2+QCOhUh6qV97B0zpx+3dVH8sQD33VBt7fBDRTuwYRA2qlYMlvhrlDxlHf6AnwAKUgFd7emMYT6BLesLWwhgrxwXB2pSr9+nJsAAlYv7QjujE4aFIxxnLDbD8xS7waG4udhTSAyxAiTA1MsTyF7vAwcpE7ChE9fbF8I48xRE1GBaghDham2LVy0HcM5R00r/6tcHQADexY5AeYQFKjI+LDX6Z0A3WpnKxoxDV2uTerfAO9/ikBsYClKCObjZYM6EbrExYgqT93ghryZPbUqNgAUqUv7sCq18JgoUxTxpK2uv1Xt6YMYCH8VDjYAFKWBdPW6x6uSvMWYKkhSb2bIEPItqLHYP0GAtQ4rq2sMWKcYEwNeJLgbTHhNAWmDmog9gxSM/xU4/Qo6UdVrwUBBOeSJS0wMshXvhoMMuPGh8/8QgAENraDste7MKzaZOoxvfwwpwhPmLHIImQCYIgiB2CtMfZxPt4fe05ZBeWiR2FJOaNsJbc4YWaFAuQHpFyvwivrD6DW5kFYkchCTA2NMBnwzpieBce5E5NiwVIVcorKcdb684j5laW2FFIjzW3MMayF7tweDMSBQuQqqVSC/h4xzWsPZkkdhTSQ20drbBiXCDcbTmwNYmDBUiPtfrYbczbfQMqNV8q1DD6tHPA4ucDYMnRiEhELECqlYM3M/H2+gsoKFWKHYV03ITQFpg5sD0MDHgyWxIXC5Bq7ebdfLyy+gzuPCgWOwrpICNDGeY964vRXT3EjkIEgAVIdfSgqAwztlzG3msZYkchHeKqMMPXo/zRtQV3diHtwQKkell3Kgnzdl1HSbla7Cik5SK7uGH2kA6wMuV5KEm7sACp3uIy8zF5/QX8dTdf7CikhewsjTF/aEeE+ziJHYWoSixAeiKlShW+io7FjzEJ4E6i9LenOzjis2EdYWdpInYUomqxAKlBnEvKwfRNl5CQVSh2FBKRlYkcs4d0QGSgu9hRiB6LBUgNpqRchQX/uYlVx2+Dryrp6e5ti4WRneDWjAe2k25gAVKDO5d0H/+38zoup+aKHYWagKWJHP96ug1eCfGCTMZj+0h3sACpUQiCgK3n7+Dfe2/ibl6J2HGoEchkwIjObnhvQDvYW3FbH+keFiA1quIyFX44HI/lRxJQXK4SOw41kAAPBT4e4oNO7gqxoxDVGwuQmsTd3BIs+M9f+P3iHW4f1GFuzcwwLbwtnvV34epO0nksQGpSl1Ie4JPd13EmMUfsKFQHthbGeKt3K7zY3RPGcgOx4xA1CBYgiWLPlXR89Wcs4njSXa1mbmyIV0Ja4PVe3hzJhfQOC5BEIwgCDt28hx9jEnA8PlvsOPQPTtameKmHJ8Z09YSNOYuP9BMLkLTC1Tu5+Onobey6nIZyFV+SYunoaoMJoS0wyM8ZRoZc1Un6jQVIWuVubglWHb+NDaeSkVfCcw82BQMZ0K+9IyaEtkA37+ZixyFqMixA0kqFpUpsPJOClcduIzWH5x9sDObGhojs4oZXQlvAs7mF2HGImhwLkLSaSi0g5tY97LyUjujrd5HPpcInIpMBXTyaYbCfM4Z2doONGbfvkXSxAElnlCpVOBKbhZ2X0rD/RgYKy3hgfW3IZECAuwKD/FwwqKMznGxMxY5EpBVYgKSTSspV2H8jE7sup+HgzUyemPchMhng767AoI7OGNjRGS4KM7EjEWkdFiDpvMJSJf68noE/rqbjRHy2ZHeeMTSQwc/NBgN9nTHQzxmuLD2iGrEASa+o1QKupuXiRHw2jsdn40zifRTp6apSc2ND+LsrEORliyAvWwR4KGBhIhc7FpHOYAGSXlOq1LienofzSTk4n/wA55NzdHavUjtLYwR62iLQqxmCvGzh42INOY/VI6o3FiBJTmZeCa6l5yExq7DiJ7sIidmFSM0phkot/tvBWG4Ar+bmaGlvCW97C7RysEQnNwW87S3FjkakV1iARP9VrlIjNacYiVmFuJ1ViKTsQtzOLkJWfikKy5QoLFWhsFRZ79M6yQ1kMDM2hLmxIcyN5bC3MoGbwgyuzczg1swMrgpzeNiaw62ZGQwMeKYFosbGAiSqI7VaQGGZEkVlKhSUKlFU+t9/y5QwkFUuOfP//m5mbAgTuaHY0YnoH1iAREQkSdyCTkREksQCJCIiSWIBEhGRJLEAiYhIkliAREQkSSxAIiKSJBYgERFJEguQiIgkiQVIRESSxAIkIiJJYgESEZEksQCJiEiSWIBERCRJLEAiIpIkFiAREUkSC5CIiCSJBUhERJLEAiQiIkliARIRkSSxAImISJJYgEREJEksQCIikiQWIBERSRILkIiIJIkFSEREksQCJCIiSWIBEhGRJLEAiYhIkliAREQkSSxAIiKSJBYgERFJEguQiIgkiQVIRESSxAIkIiJJYgESEZEksQCJiEiSWIBERCRJLEAiIpIkFiAREUkSC5CIiCSJBUhERJLEAiQiIkliARIRkSSxAImISJJYgEREJEksQCIikiQWIBERSdL/Ay30RcVKkW1XAAAAAElFTkSuQmCC</t>
+  </si>
+  <si>
+    <t>https://www.flipkart.com/micromax-x512/p/itmfhwvhrwhxq5tu?pid=MOBFJWWH2D9PTHZQ&amp;lid=LSTMOBFJWWH2D9PTHZQ8WGKHJ&amp;marketplace=FLIPKART&amp;q=micromax+x512&amp;store=tyy%2F4io&amp;srno=s_1_4&amp;otracker=search&amp;iid=e532b5ae-9020-461a-a39a-dca423c959b8.MOBFJWWH2D9PTHZQ.SEARCH&amp;ssid=0udxp3g2jk0000001689862408205&amp;qH=8aab057c4a7cd0c3</t>
+  </si>
+  <si>
+    <t>₹1,150</t>
+  </si>
+  <si>
+    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAcAAAAFQCAYAAAAoQ64wAAAAOXRFWHRTb2Z0d2FyZQBNYXRwbG90bGliIHZlcnNpb24zLjYuMSwgaHR0cHM6Ly9tYXRwbG90bGliLm9yZy/av/WaAAAACXBIWXMAAArEAAAKxAFmbYLUAABIDklEQVR4nO3deVhUdf/G8fcMw76qICgC7ruICiqCiVq4ZeWCVlqa7WXWz6Xdpb3Mp0xLs0VRKyu1LM2eLFPD3Nfcyl1A3AVk3+b7+4PiCQUcEOYwnM/ruroS5sw59xxg7jnb9xiUUgohhBBCZ4xaBxBCCCG0IAUohBBCl6QAhRBC6JIUoBBCCF2SAhRCCKFLUoBCCCF0SQpQCCGELkkBCiGE0CUpQCGEELokBSiEEEKXpACFEELokhSgEEIIXZICFEIIoUtSgEIIIXRJClAIIYQuSQEKIYTQJSlAIYQQuiQFKIQQQpekAIUQQuiSFKAQQghdkgIUQgihS1KAQgghdEkKUAghhC5JAdZwUVFRfPbZZ1Uyb4PBQGJiYpXMuyLi4+Px8vLSOka19vnnnzNw4MAKP17dTJs2jQceeKDUx93c3EhKSrJiorJV5d+jKD8pQCtr2LAhLi4uuLm5Ub9+fcaNG0dBQYFVlh0bG8vNN99s0bTx8fG4ubnh5uaGq6srBoOh6Gs3N7cqTloxgYGBpKSkaB2jWhsxYgQrV64s+vrqDzFXP17dlPdDV3p6OvXr16/CRNYnJVp5pAA1sGbNGtLT04mLi2P58uV8+umnWke6RmBgIOnp6aSnp3Ps2DGAoq/T09OrbLn5+flVNu/qoKa/Pj1RSmE2m7WOIW6AFKCGmjRpQkREBHv27Cn63rJly2jTpg21a9fmtttu4/z58wBcuHCBfv364eXlhbe3N3fddRcA69evp2nTpsXmW9Kn5OPHj/PII4+wfv163NzcaNOmTaW8hpUrV9KoUSO8vb154403ir5fUFDA1KlTCQoKwtfXlwkTJpT65h8VFcXkyZMJDQ3F1dWVvLw8NmzYQKdOnfDy8iIqKqqohB944AFeeumlYs9v3LgxGzdu5OTJk5hMpqLvX758mbvvvpu6devSuHFjFi5cCMCRI0eKbRVER0fTq1evoq/r16/PkSNHSl3nVzt27Bg33XQTXl5e1K9fn+eff77osdjYWHr27MnDDz+Mp6cnCxYsKDVXSQwGA7NnzyYwMBA/Pz/efvvtoseys7N5/PHH8fPzIzAwkJdffrnoDXnLli106NABDw8P/P39effdd4vy/LMXIDo6GoAWLVrg5uZGXFxcscfLWtdAqT+jksyZM4fGjRvj4+PDyJEjSU1NBf73+/vyyy9Tu3ZtGjZsyE8//VTiPErKC5CVlUVMTAzu7u506dKFEydOFFt///wtzJ8/n6CgINzd3WnRogXr168v9zofPXo0Y8eOpVevXri4uHDs2DHi4uLo0KEDXl5e9OjRg0OHDhVNv337doKDg/Hw8OCRRx4pVpijR4/m1VdfLfr66j00v/76K6GhoXh4eNCsWTPi4uJ45ZVXiIuL44EHHsDNzY3XX3+91HUuLKCEVQUFBam4uDillFJ//fWX8vPzUzNmzFBKKbV161bl7++v/vjjD5Wbm6smTZqkhgwZopRS6plnnlGPPvqoysvLU9nZ2er3339XSim1bt061aRJk2LLAFRCQoJSSqkePXqoxYsXK6WUWrBggerdu3exad944w01YMCAMjOfOXNGlfSrAqihQ4eqtLQ0tW/fPuXo6KiOHj2qlFJq+vTpqmfPnur8+fMqOTlZRUVFqdmzZ5c4/x49eqgmTZqoI0eOqKysLBUfH6+8vb3Vb7/9pvLz89WsWbNUaGioUkqpNWvWqNatWxc9d+vWrapBgwbKbDarEydOKDs7u6LH+vfvryZMmKCys7PVoUOHVL169dTevXuVUkr5+vqqo0ePqvz8fBUQEKD8/f1Vbm6uOnr0qPL19S1znV/t6NGjav369SovL08dPnxYBQQEqG+//bZondvZ2akFCxaogoIClZmZWWauktZxdHS0Sk1NVYcOHVJ+fn7ql19+UUop9fzzz6sePXqoy5cvq1OnTqlmzZqpBQsWKKWU6tKli/rss8+UUkpdvnxZ7dq1qyjPv38H/v27cvXjZa3rsn5GV1uzZo3y8/NTBw4cUOnp6Wrw4MFq1KhRSqnC3187Ozv15ptvqry8PDVv3jwVGBhY4nxKyjt16lTl7Oysfv31V5WXl6fuuecede+9914zfXp6unJ3d1eHDx9WSil18uRJdfz48XKv81GjRqk6deqoHTt2qLy8PHX27Fnl5eWlli9frnJzc9X06dNV06ZNVV5ensrJyVENGjRQc+bMUbm5uWrWrFnKzs6u6O9x1KhR6pVXXilx3R87dky5u7urlStXqvz8fHXq1Cl15MgRpVTxv2lxY2QLUAP9+vXDzc2NFi1a0K1bNx5//HGg8BPqY489Rrt27bC3t2fy5Ml899135OfnY29vz5kzZ0hISMDR0ZFu3bpVSpZnn32WVatW3dDz3dzcaNu2LcHBwezbtw+ATz/9lFdffRUfHx+8vLyYMGECy5YtK3U+999/P02bNsXJyYnPP/+cQYMG0b17d+zs7HjiiSc4efIkJ0+epFevXly4cIEDBw4A8PXXXxMTE4PBYCg2v7Nnz7J+/XreeOMNHB0dadmyJXfffTfffPMNAN27d+e3335j9+7dBAcHExISwq5du4iLiyMyMhLA4nXepEkTevTogclkolmzZowYMaJoK+mfx0ePHo3RaCQ1NbXMXCV57rnn8PDwoGXLltx///189dVXAHz55ZdMnTqVWrVqERgYyIQJE1iyZElR9qNHj3L58mVq1apFhw4dyvw5lqSsdV3Wz+hqX375JQ899BCtW7fG1dWV119/na+++gqlFACurq5MmjQJk8nEyJEjiY+PL9ex3N69e9OzZ09MJhN33nkne/fuLXE6g8HAgQMHyMnJISgoiEaNGpU6z9LWOcCQIUPo1KkTJpOJNWvWEBwczODBg7G3t2fChAlkZmayfft2Nm/ejMlk4tFHH8Xe3p6xY8dSr149i17TkiVLGDhwILfeeit2dnYEBgZes6dH3DgpQA38+OOPpKWlsWLFCnbs2FF0TC0+Pp7XXnsNLy8vvLy8CAgIwGQycfbsWSZNmkRgYCA9evSgZcuW1ea4oa+vb9G/XVxcir2Wf3Yfenl5MWLEiKLduSVp0KBB0b/j4+NZvHhx0XO9vLzIyMjg9OnT2NnZMXTo0KI30KVLlzJ8+PBr5hcfH092dnZRAXt5eTFv3jzOnj0LFBZgXFxcUeH9++vu3bsDWLzOT58+zaBBg/Dz88PT05OZM2dy6dKlUl9bWblKEhAQUOzfZ86cASApKYnAwMCix4KCgorOePzkk084cOAATZs2JTIyks2bN5c6/9KUta7L+hldraSc2dnZXL58GQAfHx+MxsK3IhcXF4ByHWcu7Xfw31xdXVmyZAmzZs3C19eXmJiYMs8OLW2dQ/Gf59WvzWg0EhAQQFJSEmfOnCk2rcFgKPZ1WRITE8ssaFE5pAA1YjAYuP3227n55puLjgP4+/vzyiuvkJKSUvRfVlYWDRo0wMPDg/fee4/4+HhiY2N54oknOH78OK6urmRlZRXN99y5c2Uu01r8/f1Zt25d0etITU3l4MGDFmXz9/fnwQcfLLYeMjMziYiIAGD48OF8/fXXbNmyBaPRSJcuXUpcvpubG8nJyUXzSEtL48MPPwT+twW4ceNGunfvTvfu3dm4cSMbN24s2gIsbZ1f7cUXX6RWrVocPnyY1NRUnnrqqaKtm5JeW1m5SpKQkFDs3/9sRdSvX5/4+Piix+Lj44uObbZo0YKvv/6a8+fPc+edd5Z6/PJ6SlvX1/sZ/VtJOZ2cnKhdu3aFMlVU//79+fXXX0lMTMTR0bHYsdqrlbbOofjP8+rXppQiISGB+vXrU69evWuOxf/767L+dgMCAkrcmr56+eLGSAFqbOLEiXzyySdcvHiR++67j/fff79oF87ly5f57rvvAPjhhx84fvw4Sik8PT0xGAzY2dnRvHlzkpOT2bBhAzk5ObzyyiulLqtu3bokJiZa5UzEMWPG8OKLL3LmzBmUUpw8eZINGzZY9Ny7776bpUuXEhcXh9lsJi0trdju0+7du5OWlsaLL77IsGHDSpyHv78/4eHhvPjii2RmZpKfn8+uXbuKSrh9+/ZcuHCBuLg4wsLCCA0NZfPmzZw5c4aQkBCg9HV+tbS0NNzd3XFzc2P//v1lnqJ+vVwleeutt7hy5Qp//fUX8+fPL3rNw4cP55VXXiE5OZmEhATeeecd7rzzTqDwer5Lly5hMplwd3cvMTcU/k6U9kYLpa/r6/2M/m348OF8/PHHHDp0iIyMDF544QWGDRtWoTfy6+Utzblz51i1ahVZWVk4Ojri4uJS6jqB0tf51fr168fevXuLDlW8++67ODs7ExoaSnh4OHl5eXz00Ufk5eXxwQcfFNuSbN++PT/88ANXrlzh+PHjxfYw3HXXXaxcuZLVq1djNptJSEgoOsmooutAXEsKUGOtWrWiR48evPfee3Tr1o0ZM2Zw77334uHhQceOHfn9998BOHz4MD179sTd3Z0BAwYwc+ZMgoKC8PT05L333mPYsGE0atSIsLCwUpfVq1cvGjZsiI+PD8HBwQC8/vrr9OvXr9Jf16RJkwgPDyciIgJPT08GDhxY7FN1WRo1asSXX37JpEmTqF27Ni1btiz6IACFu5liYmL49ddfS31jgsISSExMpHHjxtStW5ennnqq6BO30WikW7dutGzZEgcHBxwcHGjdujVdu3YtemMsbZ1fbcqUKaxbtw4PDw/GjRvHkCFDynx9ZeUqSf/+/Wnbti033XQT48aNKzpTcPLkybRo0YKWLVsSHh7OnXfeyahRowBYvXo1LVq0wN3dnVmzZrFo0aIS5z1lyhSGDBmCl5dXseOW/yhtXV/vZ/Rv0dHRPPfcc/Tv35+goCDs7e2ZOXNmmeuoNNfLWxqz2cz06dPx9fWlbt26nD59utgZmFcrbZ1fzdvbmxUrVjB16lTq1KnDt99+y4oVK7C3t8fBwYHly5cze/Zs6tSpwx9//FHsOPI999xDkyZNaNCgAXfddVexrfRGjRqxfPlyXnjhBTw9Pendu3dReT7xxBPExsbi5eXFm2++afE6ENcyqH/vqxFCVCsGg4GEhASLjx2JGyfrXD9kC1AIIYQuSQEKIYTQJdkFKoQQQpdkC1AIIYQuSQEKIYTQJSlAIYQQuiQFKIQQQpekAIUQQuiSFKAQQghdkgIUQgihS1KAQgghdEkKUAghhC5JAQohhNAlKUAhhBC6JAUohBBCl6QAhRBC6JIUoBBCCF0yaR1ACFuWm28m/nIm8ZczOHclh+TMXFIy80jOyCU5M4+UzFxSsvLIyS8gv0CRV6AwK4UBMBjAaDDg6mjC3env/xzt//63PbVc7Knv5UyDWs40qO2Cn4cTdkaD1i9ZiBpD7gdYhUwmE23btiU/P59WrVqxcOFCXFxcLH7+hx9+SK1atRg+fDixsbH079+funXrAtC/f3+WL1+Os7NzVcW/rgceeIDnnnuOJk2aaJbBWlKz8tiXmMqhM1c4cSmDU5cyOHkxkzOpWZit9Bdkb2fAz9MJfy9nmvi40aa+J23qe9DCzx0nezvrhBCiBpECrELe3t5cvHgRgBEjRtCpUyfGjx9foXlFRUXx/vvv07Zt28qMWKSgoAA7O3kTBcjOK+BAUip7E1LZm5jCH4mpnLyUQXX9SzEZDX8Xogdt/D3p0qg2ret5YJStRSHKJMcAraR79+4cPXqUixcvMnDgQIKDg4mKiuLkyZMAfPnll7Rq1Yr27dtz++23AzBt2jTef/99vv32W3bs2MHQoUMJDQ0FoGHDhqSnp/PMM88wf/78ouWMGTOGb7/9loKCAiZMmEBYWBjt27fn888/vybT+vXr6dWrF/379yciIoKMjAxGjx5NWFgYnTp14ueff8ZsNtOkSRMyMjIAyMrKIigoiPz8fKKioti/fz8AP/30E+Hh4XTo0IGRI0eSm5vLF198wQsvvADA888/T+/evQH4/vvvGTduHAUFBYwcOZLWrVvTrl07FixYUDUr/zqUUhxISmXu+mPc9dEWgqetYcjczby86iDf7UnixMXqW34A+WbFX+fS+Gb3aV5ZdZBbZ2+k46s/88jinSzefJJjF9K1jihEtSTHAK0gPz+fH3/8kb59+zJt2jS6d+/OypUr+eqrrxg3bhzff/89r732Gt9//z3NmjUjNTW12PMHDRpEaGhoiVuAMTExTJ48mTFjxpCfn8/atWuZM2cOn376KfXq1WP79u1kZWXRtWtX+vbtS506dYo9f+fOnRw6dIj69evz/PPPc+uttxIbG8vFixeJjIzk0KFD9OvXj1WrVjF8+HBWr15NdHQ0JtP/fnUuXrzI22+/za+//oqzszNTpkzh448/ZuDAgcybNw+A7du3k5GRQX5+Phs3biQyMpI9e/Zw4sQJDh48CHDN665KqZl5rD98ng2HLxB35CIX0nKstmxrSMnM478HzvLfA2cB8PNwonszb/q3q0dkM2/s7eSzrxBSgFUoJSWFkJAQAG666Sbuv/9+OnfuzOrVqwEYNmwYTz75JAARERE89NBDjBgxgqFDh1q8jNDQUI4fP05ycjLbtm0jIiICJycn1qxZw/79+/nss8+AwnI5fvz4NQUYERFB/fr1AVizZg2rVq3i1VdfBSAjI4Nz584RExPD7NmzGT58OMuWLeO+++4rNo8tW7bwxx9/EB4eDkBOTg4DBgwgMDCQc+fOkZ6eTkFBAeHh4ezevZvff/+dJ598EhcXF5KSknj88ce5/fbbiY6OLucaLp+s3AJ+PnSO7/ec5rfDF8ktMFfp8qqTs1eyWbozkaU7E/FwMnFLaz8GBPsR2dQHB5OUodAnKcAq5OXlxZ49e8qcxmAoPE4zd+5ctmzZwsqVKwkNDWXfvn0WL+eOO+5gxYoVbNq0iZiYGADMZjPz5s2jR48eZT733yflmM1mVq5cSVBQULFp6taty5gxY7h06RJbtmxh8eLFxR43m80MGDCgxF2YHTt25KOPPqJTp0507dqVtWvXcvHiRfz9/QHYt28fq1ev5t1332XNmjXMmDHD4tdtibwCM78dvsD3e5P4+eA5MnMLKnX+tuhKdj7LdyWyfFdhGUa38SOmUwO6NK5z/ScLUYPIRz8ri4yM5IsvvgBg2bJldO7cGYDjx48THh7Oa6+9hoODA5cuXSr2PHd3d9LS0kqcZ0xMDEuWLOGXX36hX79+AERHRzNnzhwKCgrf8Pfv31/079JER0cza9asoq//KW+j0Ui/fv144oknuPnmm4vt/gQIDw9n3bp1nDp1CoArV65w4sSJotf77rvvEhERQWRkJB988AFhYWFA4a5Ts9nMsGHDmDZt2nU/LJTHmdQs3v7pT7q+vpb7F+7guz1JUn4luJKdz7KdiQz/aAu3vLOBBb+f4Ep2ntaxhLAK2QK0smnTpjF69GgWLVpE7dq1iY2NBWDixIkcPXoUpRSDBg2iQYMGxZ43evRoRo8ejbu7Ozt27Cj2WGhoKEePHiU8PBwnJycAHnzwQU6cOEGHDh0wm83Uq1ePH3/8scxskydP5sknnyQ4OJj8/Hw6duxYtAs1JiaGqKgofvrpp2ue5+Pjw8cff8yQIUPIzc3FaDQyc+ZMGjVqRGRkJImJiXTr1o26devi7OxMREQEAKdPn2b06NGYzWZMJhMzZ86syCotZuvxSyzcfJI1B86Rb63rE2qII+fTeWnlQab/9y9uDa7HyK5BtA/w0jqWEFVGLoMQNi8338y3uxOJ3XSKQ2euaB2nRgkNqsXYXk2JalFX6yhCVDopQGGz8grMLN2RyAfrjnI6JUvrODVacANPHu/ZlOjWvkXHrYWwdVKAwubkF5hZtjOR99cdJTFZis+aWvq5M7ZXU/q3rScX2gubJwUobIbZrFi+K5HZvx4l/nKm1nF0raWfO8/3b8VNzX20jiJEhUkBCpuw+dglXl51UI7xVTPdm3nz4oDWtPBz1zqKEOUmBSiqtdMpWbz2w0FW7zurdRRRCjujgZFdAhl/Sws8Xey1jiOExaQARbWUV2Dm47jjzF57lKw8uX7PFtR2deDZfi0ZFhqgdRQhLCIFKKqdPQkpTFy6l6PnZRBnW9SjuQ9vDG5HfS/tbtUlhCWkAEW1kVdg5r1fjjB3wzEK5CJ2m+buaOL5Aa24q3Og1lGEKJUUoKgW/jqbxviv93AgSU5yqUkim3rz5pB2NKhl+Y2ghbAWKUChKbNZ8VHccd75+TC5+fq5O4OeuDrY8frgdtwe4q91FCGKkQIUmrmYnsMTX+xm8/FL159Y2LwRXQKZMrA1jiY7raMIAUgBCo3sjk/msc93cSY1W+sowora+XsyZ0RHAmrLLlGhPSlAYXWfbTnFyysP6uqGtOJ/PJxMzIhpT3QbP62jCJ2TAhRWk51XwOQV+1m6M1HrKKIaeLxnEyZGt5DBtYVmpACFVVxIy+H+hdv5IzFV6yiiGrmtfX3ejgmW44JCE1KAosqduJjBqPnbZABrUaLODWvz0b2d8HJx0DqK0BkpQFGl9iakMCZ2O5cycrWOIqqxxj6uLLyvs5wcI6xKClBUmfV/neexz3eRmStjeYrr83Zz4JNRYYQEeGkdReiEFKCoEst2JvLs8j/IlyHNRDm4OZpYOCaMTkG1tY4idEAKUFS6r7bH8+w3+5DfLFERbo4mYu8LI7ShlKCoWkatA4iaZfnORJ6T8hM3ID0nn1Hzt7H95GWto4gaTgpQVJrv9pxm0rK9yF5PcaMycgsYPX8bW2WYPFGFpABFpVi97wwTvpbyE5UnI7eA+2K3y5agqDJSgOKG/XLwHE9+uVtOeBGVLjO3gAcW7uDo+TSto4gaSApQ3JA9CSmMXbKLvAIpP1E1UrPyGDV/O+evyMDponJJAYoKS0zO5IGFO8jOk0GtRdU6nZLF6AXbSc/J1zqKqEGkAEWFpGXnMSZ2OxfTc7SOInTi4JkrPPrZTvLkLiKikkgBinLLLzDz2Oe7OHwuXesoQmfijlzkuW/2aR1D1BBSgKLcJn93gLgjF7WOIXRq2c5EFm0+qXUMUQNIAYpy+XJbPEu2xWsdQ+jcq6sOsTs+WesYwsZJAQqL/Xn2CtNWHtA6hhDkFph5/PNdXJa7jIgbIAUoLJKZm8/jn++SMz5FtZGUms2TX+7GLNefigqSAhQWefHb/Ry7kKF1DCGKiTtykZm/HNY6hrBRUoDiur7ensA3u09rHUOIEs1ed1TGDBUVIgUoynT8QjpTv5fjfqL6UgqeXv4HmblykbwoH7kfoCiVUorh87awzcYGI85LOculH9/DnJECBiN+I6dz9otnix7PTzmHV+QIPMJu5/Laj8k+uQfnxp2o1XMMAClxn+EUGIxTULBGr0BUxL3hQbx8e1utYwgbYtI6gKi+Fm85ZXPlB3Bp9Uy8uo/EKaAtBVlpGOydqH/fbKCw1E9/OAbnZl0wZ6eTe+4Y9e//gLNfPIs5JwNzbjZ5l0/j1X2kxq9ClNfiLafo29aPbk28tY4ibITsAhUlOp2SxfT//qV1jHLLvXAKg9EOp4DCLQE7Z3cMRruix3NO/4mday3svfzAYASDAaXMYDAABlI3LcEr4m6N0osboRQ8vewPMmS8UGEhKUBRoue/2WeTAw/nJydhcHDm/LKXOBP7JKmbvy72eOafcbi27A6A0dEF54YdOLNgHM4NO5B/5TwY7LD3DtAiuqgEiclZvL76kNYxhI2QAhTXWL4zkQ2HL2gdo0KUuYCchAPUjn4Mv5EzyDq5m6wTuwsfU4rMw5tw+bsAATzDh1F/zPt4hg8jddNXeEXcScrGL7jw7etkHt6k1csQN+CLbfEySoywiBSgKCY1K4/XbPgTtMm9Dg5+TTF5+GAw2ePcOJTc88cByEk8gMmjLiaPa48RZZ3cg713IOacTPKvXMD7jme5suN7a8cXlUApmPr9AblAXlyXFKAo5r1fjtj08FIO9ZpTkJlKQXY6SpnJSdiPfZ3CXZqZf27EpVX3a56jlCJtx3d4dB6EyssBcz5gwJwtd7uwVX8kpvLl9gStY4hqTgpQFDl2IZ3FW05qHeOGGIx21LrpXs59/gxn5o/FVKs+Lk07o5SZzMObcWkRcc1zMg6sw6V5OEZ7J+zrNkLl53Lm08dxbdNLg1cgKss7P/9FWnae1jFENSbXAYoiDyzcwS+HzmkdQ4hK83CPxjzXr5XWMUQ1JVuAAoCtxy9J+YkaZ8HvJ0m4nKl1DFFNSQEKAN748U+tIwhR6XLzzXyw7qjWMUQ1JQUoWHvoHHsSUrSOIUSVWL4rkcRk2QoU15ICFLwvn5BFDZZXoPhg3TGtY4hqSApQ5zYdu8ju+BStYwhRpZbvTOR0SpbWMUQ1IwWoc3Pkk7HQgdwCM3PXy54OUZwUoI7tTUhh49GLWscQwiq+3p7ImVTZChT/IwWoY3J2nNCT3AIzn205pXUMUY1IAerUyYsZ/CzX/Qmd+Wp7Irn5Zq1jiGpCClCnlmyPR8YAEnpzMT2HH/ef0TqGqCakAHUor8DM8p2JWscQQhOLN8tuUFFIClCHfj54jovptnvHByFuxI5TyRw6c0XrGKIakALUoSXb4rWOIISmFslWoEAKUHcSLmfKpQ9C91buTSI7r0DrGEJjUoA68/WOBDn5Reheek4+6/+6oHUMoTEpQJ354Q85A04IgJV/JGkdQWhMClBH/jqbxvGLGVrHEKJa+PXQeTJz87WOITQkBagjcv2TEP+TlVfA2kPntY4hNCQFqCP/3X9W6whCVCsr98puUD2TAtSJkxcz+PNsmtYxhKhW1h++ILtBdUwKUCd+lK0/Ia6Rm29m6/HLWscQGpEC1Il1f8mxDiFKEndErovVKylAHcjOK2CP3PVdiBJtPCrXA+qVFKAO7DyVTG6B3AJGiJIcPpfO+SvZWscQGpAC1IEtxy9pHUGIak2GB9QnKUAd2HxMClCIsmyU44C6JAVYw2XlFrA3MUXrGEJUa9tOypmgeiQFWMPtik8mr0BGvxaiLInJWaRkyj0y9UYKsIbbdzpV6whC2AT5W9EfKcAaTu58LYRl/kiUAtQbKcAaTgpQCMvsly1A3ZECrMFy8gs4fkFufySEJWQXqP5IAdZgR86lk2+WE2CEsIScCKM/UoA12EHZ/SlEucgNo/VFCrAGO3o+XesIQtiUhMuZWkcQViQFWIOdTs7SOoIQNiX+khSgnkgB1mCnU6QAhSiPhGQpQD2RAqzBkqQAhSiXeNkFqitSgDVUbr6ZC+k5WscQwqYkXJYPjXoiBVhDnU3NRskVEEKUy5nULArk0iHdkAKsoZJS5ZOsEOVlVpCWnad1DGElUoA11KV0uaBXiIpIzZIC1AspwBoqIydf6whC2CQpQP2QAqyh0qUAhagQKUD9kAKsoWQLUIiKkQLUDynAGio9VwpQiIqQAtQPKcAaSrYAhagY+dvRDynAGiozp0DrCELYpAKz1gmEtUgB1lByH0AhKsYsI0johknrAKJqGAxaJxClcXcyEdWirtYxRCma+LhpHUFYiRRgDSX9V3090aspD93UROsYQuie7AKtoYxGqcDqqEEtZ0Z1a6h1DCEEUoA1loOd/Giro0l9WuBostM6hhACKcAay8EkP9rqpp2/J7e1r691DCHE3+RdsoZylAKsdp7r3xKDnJ0kRLUh75I1lKezvdYRxL/0almXbk28tY4hhPgXKcAaqraro9YRxN/sjAae69dS6xhCiKtIAdZQtV0dtI4g/hbTqQHNfN21jiGEuIoUYA1Vx00KsDpwcbBj/C3NtY4hhCiBFGANJVuA1cMD3RtT18NJ6xhCiBJIAdZQdaQANeft5sjDNzXWOoYQohRSgDWUp7O9XAyvsaduboaro4w2KER1Je+QNZTBYKBBbWetY+hWEx9X7gwL0DqGEKIMUoA1WGNvV60j6Naz/Vphki1wIao1+QutwRpJAWqic6Pa3NLaV+sYQojrkAKswRrLfc2szmCAF/q30jqGEMICUoA1mGwBWt+AdvVoH+CldQwhhAWkAGswOQZoXQ52Rp7pK0OeCWErpABrsLoeTni5yKDY1nJPeBABtV20jiGEsJBcpFTDtW/gxYbDF7SOUeN5OJl4oldTqyxr57mdfHf0O6ssS5SPt7M34zqO0zqGsJAUYA0XEiAFaA2P92yKl4t1Rt/p5NuJ3xJ/Y/7++VZZnrBcE88mUoA2RHaB1nAdAr20jlDj+Xs5MzqioVWX+X+d/o8nOz5p1WWK67Mz2mkdQZSDFGANFyJnJFa5SX1a4Giy/hvfA+0e4MUuL2JA7jJfXdgZpABtiRRgDefl4iCXQ1Shtv4e3B5SX7PlD285nNe7v47JIEczqgOTUX4OtkQKUAc6yFZglXm+XysMBm23wG5tfCvvRL2Dg1HuAKI1J5Pc+sqWSAHqQHiTOlpHqJF6tvChW1NvrWMA0DOwJ3NunoOLSS7D0FIdJ/lbsyVSgDoQ1aIuGm+k1Dh2RgPPVbMhz7rU68LH0R/j4eChdRTd8nauHh+IhGWkAHXAx92RNvXlTbEyDe3YgOa+7tZZmFKQnWrRpME+wSzou0DeiDUi6922SAHqRFTzulpHqDGc7e0YH93cegvcvxzm94W0sxZN3rxWcxb1XYS/m38VBxNXkwK0LVKAOtGzpY/WEWqMB7s3wtfDSic75OfA2pfg/MHCEkw+ZdHTAjwCiO0bSyPPRlUcUPybFKBtkQLUiZCAWng6y7igN8rbzZGHezSx3gK3fQQp8YX/Tj5RWIIX/rLoqX6ufizsu5BWtavXscqaTArQtkgB6oSd0UDPFrIVeKOevLkZro5WutYrKxl+m1H8e2lJsKAfJO22aBa1nGrxaZ9P6Vi3YxUEFFer4yxngdoSKUAduT1EjgndiMY+rtwVFmC9Bf42A7JTrv1+5iVYeBuc2mTRbNwd3Jl3yzwi/CMqN58oxs5gR22n2lrHEOUgBagj3Zt5U8dVLpauqGf7tsRkZ6U/meRTsO3j0h/PuQKLB8ORny2anZPJidm9ZhMdFF1JAcXVajvVxmiQt1RbIj8tHTHZGbk1uJ7WMWxS54a1iW7jZ70Frn0ZCnLKniY/C5bcBfu/sWiW9kZ7pt80nUFNB1VCQHG1QI9ArSOIcpIC1Jk7Oshu0Ip4foAVTyRJ2l146YMlzHmw/H7YudCiye2MdrzU7SXuaX3PDQQUJZGTjWyPFKDOdAisRcM6MlxWeQwIrmfdu2qsmQwoy6dXZlg5Dja9b9HkBoOBp8Oe5rGQxyqWT5SoZe2WWkcQ5SRDl+vQHR38mfnLEa1j2AQHOyPP9LHiG9tf/4WTcRV77poXCkeM6fWCRZM/2v5R3O3dmb59Oqo8hXuDTs06RcafGbi1diNwbCDmHDPx78eTeyEXg9FA7Z61qXNL4dmUZ5acIf1AOu5t3fG7s3AX9LlvzuHayhW3Vm5Wy2wJKUDbI1uAOnRnWCAmowwOaomRXYMItNYWs7kAfpl6Y/P4bTr8+Ezh8GkWGNl6JC91e8mq97Grc0sdGjzYoNj3fAb40PzN5jSe0phLay+Rcy6HgowCsk5m0ezVZmSeyKQgs4C85Dxyz+ZWu/KzN9rT2Kux1jFEOUkB6pCfpxP92snJMNfj4WRiXO+m1lvg7sVw4c8bn8/WD2HFY4WFaoFBzQbxdo+3sTdaZ6AEt1ZuGJ3+99ZjdDTi2rLwnpV2TnY41nMkPyUfjIW7a5VZFd5yygDnvzuPzx3V73rWpl5Nrbb+ROWRAtSp+yIaah2h2nusZ1O8XKx02UhuBqx7vfLmt/cLWDoK8nMtmvyWoFt4v9f7OJucKy9DBeReyiU7IRvnhs7YOdvh2saVY1OP4drGlbxLeRiMBpzqV7977rWqIyfA2CIpQJ3qGFjLuid22Bh/L2dGd2tovQVumg3p5yp3nodWwpLhkJtp0eTd/Lsx75Z5uNtb6S4XVzHnmUmYm4DfcD+MjoVvTXUH1qXpK02pO7Au578/T93b63J+xXni34/nys4rmuQsiRz/s01SgDomW4Glm9inOU72VjoulnausACrwrFfYfEdkJVi0eQd6nbg0z6fWn1EE6UUiR8n4h7sjmeY5zWPpx9Mx8nfiYKsAnIv5RLwWAAX11y0asayyCUQtkkKUMcGtKuHn7XuamBD2tT34A5rDhu3/g3ITa+6+SdshYW3QvoFiyZvVacVsX1j8XXxrbpMVzm39BxGByN1b7v2tl1KKS79dAnvvt6Yc8yofAUGKMiw7BhnVTMZTDSvZcXbY4lKIwWoYyY7Iw/eJGeuXe35/q0KT7qwhgt/wa5FVb+cs/tgQV9ITbRo8kaejVjUbxFBHkGVHuXE9BMkzEkg7Y80/vy/P8n4K4OLqy+SdTyLo5OPcnTyUdL2pRVNn7IpBY9OHhgdjTgFOqHyFEdfOEqtiFqVnq0i2tdtj4u9XFtriwxKWXi+tKiRsvMKiHp7PWevZGsdpVqIauFD7H2drbfAL+6Ewz9ab3meAXDvd1DHsls6Xcy6yMM/P8zh5MNVHMx2/V+n/2NM2zFaxxAVIFuAOudkb8fjvax4qn81Zmc08Fw/Kx7LObnRuuUHkJpQeE/Bs/ssmtzb2Zv5feYT7BNcxcFsV3f/7lpHEBUkBSi4MyyABrW0Pf29OhjS0Z8WflY6A1Kpv4c800DGeYgdAAnbLJrc09GTj2/5mC71ulRxMNtTz7UezWo10zqGqCApQIG9nZFxvfX9R+xsb8eE6BbWW+D+5ZC0y3rLu1p2Kiy6A46ts2hyF3sX5vSeQ6+AXlWby8bI1p9tkwIUAAzp2IDG3q5ax9DMA90b4WutM2Lzcwtvd6S1vAz4YjgcWmXR5A52Dvwn6j8MbDywioPZju4NpABtmRSgAAqPfz3dV58X83q7OfBwD8tOCqkU2z6ClFPWW15ZCnLg63thzxKLJjcZTbwW+Rp3trizioNVfw5GB9ktbOOkAEWRvm39iGzqrXUMq3uydzPcHK10Y5SsFIibYZ1lWUoVwIpHYetHFk1uMBh4oesLPNjuwSoOVr2F+YVpPnScuDFSgKKYabe11tWdIhr7uHJXZyveyTtuBmQlW295FlPw4yTY8LbFzxjXcRz/1+n/qjBT9Sa7P22fFKAopmldd8ZENtI6htU807clJjsr/Rkkn7J4K0sz616FNS9aPPmYtmOYEj4Fo0FfbyV2BjtuCbpF6xjiBunrt1ZY5Kmbm1Hfs+YPkRbWsBZ92vhZb4G/vlJ4zK262zQbvh8HZrNFk8c0j+HN7m9iMujn/trh9cOp63LtsG3CtkgBimu4OJiYdlsbrWNUuef7W/Gi96TdsG+Z9ZZ3o3YthOX3Q0GeRZP3a9SPmT1n4mjnWMXBqofbm96udQRRCaQARYmi2/gxsH19rWNUmQHt6tEh0IpjSa6ZDNjYqIMHvoEv74a8LIsm7xHQg7k3z8XVvmZfTuPh4GHx9ZAGg4EXX/zfLuWJEycSGxtboeWuX7+ebdssG7zg30aPHs2qVdde6jJ69GgaN25M+/btCQ4OZu3atRXK9eGHH/LVV19V6LlakwIUpXr19rbUq4G7Qh3sjDzd14oXvR/+CU7GWW95lenIGvhsKOSkXX9aCs+M/CT6E7wcvao2l4YGNB6Ag51lN0p2c3Pj888/Jy3NsvVXlrIKsKCgYnfGmDVrFnv37uWdd97hkUceqdA8HnnkEYYPH16h52pNClCUytPFnreHtsdaN0awlhFdAwmqY6WtFHMB/DzVOsuqKqc2wsKBkHnZosnberdlQZ8F1HWumcfIhrew/M3e0dGRESNGMGfOnGseO3bsGH369CE0NJRevXpx8uRJAKKioti/fz8A+/fvJyoqioSEBD788EPefPNNQkJC2LNnD6NHj+bRRx+lc+fOvPnmm6xYsYLOnTvToUMHBgwYQEpKisU5IyMjSUz8351C3nrrLcLCwggODmbGjMLLdoYPH86vv/5aNE2vXr3YvXs306ZN4/333y/1NSUlJREREQHAmjVrcHZ2Jjc3l5SUFDp06ADAzJkzadGiBe3bt+fRRx+1OPeNkgIUZYps5s2o8IZax6g07k4mxvWy4rBvuz+DC4est7yqkrQbFvSDK2csmrxprabE9ovF382K91W0glDfUJp4lW/QhCeffJKPPvqI7Ozid1x57LHHmDdvHjt27ODFF19k0qRJpc4jICCARx55hGeffZY9e/YQEhICwKVLl9i6dSsvvPACPXr0YOvWrezevZs+ffrwwQcfWJzxhx9+4LbbbgMKSyoxMZFt27axe/duVq9ezf79+4mJiWHp0qUAnD9/nqSkpKICK+s11a9fn+TkZHJycti4cSOtW7dm586dbNq0ifDwcABefvlldu3axd69e3nzzTctzn2j9HPalqiwZ/u1ZOPRixw9X4U3bbWSx6KaUsvVst1XNyw3A9a9bp1lWcOFP2F+n8LbKdW+/qUyAe4BLOq3iIfWPMSx1GNWCFj1hrcs/64+Hx8fbr31VubPn1/0vfT0dOLi4rjjjjuAwpv+urqWf6/E0KFDi+5dGR8fT0xMDOfOnSMrK4suXa4/Ss24ceMYP3488fHx/P7770BhAf7www/ExRXutk9LS+Pw4cP079+fp59+moKCAr799lsGDx5cbF5lvabQ0FC2bdvG1q1bmTBhAhs3biQ5Obloy7Bz586MHDmSmJiYoudbg2wBiutysrdj5vAQHEy2/evi7+XMfRENrbfATe9D+lnrLc8aUk4Vbgmet2yrtq5LXWL7xtKmju2fVezj7EPvwN4Veu7EiRN57733yM/PB8BsNuPr68uePXvYs2cPe/fuZdOmTQCYTCbMf1+CkpNT9mUzLi7/uxHvuHHjePrpp9m3bx8zZ8687nOh8Bjg4cOHeeONN3jwwQeLsk2dOrUo27Fjxxg8eDAuLi6EhYXx22+/sWzZMmJiYorNq6zXFBkZyYYNG8jJySE6OppNmzbx+++/FxXgDz/8wNixY9m8eTM9evSwZJVWCtt+RxNW09bfk1dvb6t1jBsyIbo5TvZ21llY+nnYNMs6y7K2tDOwoD+c3mnR5F5OXnza51NCfUOrOFjVGtl6JPZG+wo9NyAggIiICJYvXw6Ah4cHvr6+rFy5Eig8ieWf435BQUHs2bMHgG+++aZoHu7u7mWeTHPlyhX8/f1RSrFo0aJy5XvqqafIz89nzZo1REdH88knn5CZmQnAyZMnSU1NBSAmJoa5c+eSmJh4ze7Psl5TZGQk8+bNIyQkBG9vby5evEhSUhINGzbEbDaTkJBA7969mTFjBvHx8RU+qae8pACFxYaFBTCyqxWHDatEret5MKiDFY9HrX8Dcm1/l3Gpsi7DwtsLb+prAVd7V+bePNdmbx9U26k2d7W864bm8cwzz5CUlFT09RdffMHs2bNp37497dq1K7oMYfz48UyfPp1OnTqRm5tbNP3AgQNZsmRJ0UkwV5s6dSoDBw4kLCyMgICAcmUzGAxMmTKFGTNm0LdvXwYNGkTXrl1p27YtI0eOLDp+2b9/f1avXs2gQYNKnE9pr6lVq1ZkZWUVbfG1atWKjh07AoVFOWLECIKDgwkNDWXKlCnY2Vnng6pBKWVjFycJLeUVmLnroy3sOFUdx7Ms3Wf3dyGymZUG+r5wGOaGgznfOsvTkskJhi2C5n0smjzPnMfzcc/z35P/reJglWtS6CTubXOv1jFEJZMtQFEu9nZG5ozsiK+H7Yz40aO5j/XKD+CXqfooP4D8bPhyhMWj3Ngb7XnrprcY0mxIFQerPD7OPhU6+UVUf1KAotzqujsxd2QnmzgpxmiA5/pb8T6HJ3+Hv1Zbb3nVgTkPvnkQdiywaHKjwci0btMY3WZ01eaqJPe3u183Q7zpTfV/BxPVUsfAWrw7LITqfuekIR0b0NLPwzoLUwp+nmydZVU3ygyrnoLf37P4KRNCJ/BEhyeqLlMl8HP1I6Z5zPUnFDZJClBU2IDgerxUjQfNdra3Y0K0FYc8O/CNxWdG1lg/T4FfXrJ48oeCH+K5zs9hoHp+knqw3YMWD3smbI8UoLgh94Q3ZFxvK46sUg73RzbCz1pjmebnluuNv0bb+A78MLFwi9gCd7e6m1cjX8XOYKVLVCzk7+bPoGYln+0oagYpQHHDxt/SnBFdqtflEd5uDjwSVb4hq27I9o8LLxIXhbZ/DN8+AgWWnQx0W5Pb+E+P/+BgrD5bWw8HP1zh6/6EbZACFJXildvb0r+dFW8uex3jejfDzdFKI/1lpcBvb1tnWbbkjy9h6SjIt+wmwL2DevN+7/dxNjlXcbDrC/EJ4Y6md2gdQ1QxKUBRKYxGA+/d2aFalGBjb1fu7mzFLdK4/0CWbV0XaTV/roLPYwrHRbVAeP1wPrrlI9wd3Ks4WOnsjfZMDZ9aNMamqLmkAEWlsbczMvuujtYdcaUET/dticnOSr/aKfGwdZ51lmWrTmyARbdb/CEhpG4IC/osoI5TnSoOVrL72t5H01pNNVm2sC4pQFGp7IwG/hPTnrs6l28opsoS1rAWfdtacSt07StQYNkuPl1L3A6xtxaOkWqBFrVbsLDfQuq51qviYMU19GjIw8EPW3WZQjtSgKLSGY0GXh/UjtHdGlp92c/1b2W9hSXtgX1Lrbc8W3duP8zvCykJFk0e5BHEon6LaOjRsGpz/c2AganhU+WyBx2RAhRVwmAwMO22Noztab1dSf3b+dExsJbVlld40bsMpVsul48VluDFIxZN7ufqR2zfWFrWrvrRfAY3G0yon23fsUKUjxSgqFIT+7Rg+pBg7O2q9oQCezsDT/ex4pBnh9fAid+st7ya5Epi4T0Fz/xh0eR1nOvwaZ9PCfEJqbJI3s7ejA8dX2XzF9WTFKCocsPCAlh8fxe8XKrumqoRXYJo6F3+O2pXiLmgcMQTUXEZFwqPCcZvsWhyDwcP5t0yj/B64VUS55nOz+DhYKUh80S1IQUorKJr4zqseCyCxj6VX1LuTibrjkaz53O4YNkd0UUZclJh8SA4utaiyV3sXfig9wfcHHhzpca4rclt9G3Yt1LnKWyDFKCwmobernz7WAQRTSv39PZHo5pQ29VKJy7kZsK6162zLD3Iy4Qld8LB7yya3N7Onhk9ZnBbk9sqZfEtarVgcledDmAupACFdXk627Pwvs48FtWkUu4kUd/TiTERjW58Rpba/D6knbHe8vSgIBeW3ge7P7NocjujHa9GvMqIViNuaLHuDu68G/UuTiYrjRcrqh0pQGF1JjsjT/dtyaIxXfB2u7H7rE2IboGTvZUGUU6/UK7b/YhyUAXw3VjYMteiyQ0GA892frbC1+wZMPBaxGsEeGhzvaqoHqQAhWYim3nz45Pd6V7Bu7W3rudh3VFn1r8BuenWW57uKPjvs7D+TYufMbbDWCaGTiz3ku5vdz89A3uW+3miZpECFJrycXdk0ZjOPNO3JaZy7hN9rn9LjNa6I+/FI7BroXWWVYKEVDNRsRm0/iCd4LnpLD2QB8Crv+UQ+G4a3tPTik0//qds2s1NZ9Ka7KLvTVmXzboTlt2dQVPr34D/Pm/x5KPajGJa+DSMBsvezrrU68LYkLEVTSdqEClAoTmDwcCjUU1Y8XgEbepbdir6Tc196N7Mp4qT/cvPU8GsXXmYjDCzrxMHH3djzT0uPPVTNhm5ij5NTGx9oPiZtSnZip1nCtj3qBvbkgpIzVYkpZk5fMlMz0ZWukPGjdryQeEuUbPZosmHNB/CWze9hclY9uvzdfFl+k3TsTNWr3sPCm1IAYpqo62/J989HsGz/VriZF/6r6bRAM/3t+JF76c2wV8/WG95JajnbiTEr/BN28/NiLeLgctZijB/O+q5F19XdobCdWRWCuPf/355Qw5Te9zY8Var270Ylt1XeLNhC/Rt2JdZPWfhZFfySS0ORgf+E/UfajvVrsyUwoZJAYpqxWRn5JEeTfjpqZtKvVxicMcGtPSz4kXLa6rXafI7kwooMEOAZ8l/vu6OBm5pbKLDvAxuaWziVKoZOwO08rHBrZ6DK+DLuyAvy6LJuzfozoe3fIibvVux7xsNRt666S3a+7SvgpDCVhmUUjKYoai2lu5I4PXVh0jOLDzm5WRvZP3Envh5WunU9f3fFG6FVBOXsxTdF2Tw8UAnugX8b3ef9/Q0Lj5d8j30hi/LZFZfJz7ckce+8wWMaGfPoFY2dqfzwG5w91fgZNkHnwOXDvDoz4+SnFN4C6bJXSczrMWwqkwobJBsAYpqLSY0gPWTevJg90Y42Bm5P7KR9covPxfWvmSdZVkgJ19xx5eZPBvhUKz8yrL2eD5tfexIzVHEp5r5OsaZmVst26VYrcRvgoW3QsYliyZvU6cNsX1jqetSl8dCHpPyEyWykSPiQs88ne15YUBrRnYNst6ILwDbP4Hkk9ZbXhmUUoz+Lotejey4p71l60ApxcytuXw11JnDl8zkmsEAJGfZ6E6fM3sLB9G+dwV41L/u5I29GrNs4DJqOVnxDiHCpsguUCFKkp0K74VA1mWtkwCwMT6fmxZkEuz7v502iwc58/WBPBbsyeNMuqKem4Hx4Q6MDy882WXx3lzyzDCmgwNKKYYty+LgBTP3hdgzsZuNnRDzb16BcM8KqNNE6yTCxkkBClGSn6fIqC/VmZtvYQn6ttY6ibBhcgxQiKulJMDWeVqnEGVJPwex/SFxh9ZJhA2TAhTiar++AvnZ159OaCsrGRbdDsc3aJ1E2CgpQCH+7cxe+ONrrVMIS+Wmw+cx8OdqrZMIGyQFKMS/rZkMyGFxm1KQA1/fIx9cRLlJAQrxjyM/wwnZnWaTzPnwzUOFl64IYSEpQCGgcNDln6donULcEAU/TIBDq7QOImyEFKAQAHs+h/MHtU4hblTzvtC8j9YphI2QAhQiNxPWvaZ1CnGjGveEYYvAzsbGORWakQIUYvMHkHZG6xTiRjTsDnctAZMNj3AjrE4KUOhb+gUZ8cXWtRoII5aBvbPWSYSNkQIU+rbhTchN0zqFqKjQMRCzCOytdIcQUaPI3SCEfl08AjtjtU4hKirqeYh6RusUwoZJAQr9+mVa4fVjwrYY7GDAfyC0+tyoWNgmKUChT6c2w59yvZjNMTnB0PnQcoDWSUQNIAUo9OnnyVonEOXl5lt4mUNgV62TiBpCClDoz4FvIXG71ilEeTTsDkM+BXdfrZOIGkQKUOhLfi788pLWKYTFDNB9PPR8AYx2WocRNYwUoNCXHZ9C8gmtUwhLONeCQR9B82itk4gaSgpQ6Ed2KmyYrnUKYQn/UIiJBa8ArZOIGkwKUOhH3DuQdVnrFKIsBiN0eQRufglMDlqnETWcFKDQh5QE2Pqh1ilEWXxawm2zIaCz1kmETkgBCn349VXIz9Y6hSiJnQN0nwCR42WrT1iVFKCo+c78Afu+1jqFKElAl8KtPp8WWicROiQFKGq+nyeDMmudQvybowf0ngJhD4DBoHUaoVNSgKJmO/ILHF+vdQrxD4MddBgBUc+BR32t0widkwIUNdvpnYVnFsoWoMYM0Po26DUZvJtpHUYIAAxKKaV1CCGq1LkDsPZlOPxfrZPoU+OecPNUqN9B6yRCFCMFKPQjfkvhhfDH1mqdRB/8QwuLr9FNWicRokRSgEJ/zh+CzR/AH19DQY7WaWoYAzTpBV0fhWa3aB1GiDJJAQr9Sr8A2z+G7Z9C5kWt09g2B3cIuQs6PwzeTbVOI4RFpACFyMuGP76EzXPg4l9ap7EttZtA54cg5G5w8tA6jRDlIgUoxL8lbId9SwvvGZhxXus01ZPJGZrdDB3uLdzNKdfxCRslBShEScwFhdcP7lsGf66CnCtaJ9LWP6XX+g5o3hcc3bROJMQNkwIU4nrysuHIT4VleOxXyE3XOpF1mJyg6c3QZpCUnqiRpACFKI+C/MKL609sgOMbIHF7zTmT1GAE37YQFAENIwqv35PSEzWYFKAQNyIvC+I3F5bhid/gzF5QBVqnsozRBPXaQ1A3CIqEwK7g7KV1KiGsRgpQiMqUl114Jun5Q4Uj0Jw/WPjvK6e1zWXvUnjHhbqtoW6rwi29BmGyhSd0TQpQCGvISi4swgt/QdrZwjNM0//57xxkXIC8zIrN294VXGqDc62//1+7cKDpOk0KL1Oo0wQ8/OVsTSGuIgUoRHWRk15YhrkZhYN3KzMo9a9///2fwQBOnoVF51IbTI5aJxfCJkkBCiGE0CWj1gGEEEIILUgBCiGE0CUpQCF0xmAw8OKLLxZ9PXHiRGJjYyt1GStWrODw4cNFXz/wwAMcO3bshudrMpkICQmhTZs2DBw4kJSUlArNp3///mRlZd1wHmHbpACF0Bk3Nzc+//xz0tLSqmwZVxfgJ598QpMmTW54vl5eXuzZs4cDBw7g5eXFBx98UKH5rF69Gmdn5xvOI2ybFKAQOuPo6MiIESOYM2fONY8dO3aMPn36EBoaSq9evTh58iQAmzdvpk2bNnTo0IHHH3+coUOHAoVF17lzZzp06MCAAQNISUlh69atfP/994wbN46QkBDOnz9PVFQU+/fvZ+7cuUyZMqVoeS+//DLvvvsuAG+99RZhYWEEBwczY8aM676OiIgIEhMTAbhw4QKDBw8mNDSU8PBwdu/eTWpqKs2aNSua/tSpU4SEhADQsGFD0tMLh7RbvHgxYWFhtG/fnvHjxwPw+uuv8/HHHwNw9913c//99wMwa9Ys3nnnHdLT0+nbty/t2rWjXbt2/PTTTxavf1GNKCGErtSpU0edP39eNW7cWGVlZakJEyaoBQsWKKWUio6OVidOnFBKKbV27Vo1dOhQpZRSbdq0UTt37lRKKTVixAg1ZMgQpZRSly9fVmazWSml1HvvvadeffVVpZRSo0aNUitXrixaZo8ePdS+ffvU2bNnVZs2bYq+HxwcrBISEtRPP/2kxo4dq8xms8rPz1c9e/ZU+/btKzG7Ukrl5+erwYMHq1WrVimllLr77rvVtm3blFJKHT58WHXu3FkppdSAAQPUli1blFJKzZgxoyhfUFCQSktLUwcPHlRDhgxReXl5Siml7rnnHrVq1Sq1YcMGde+99yqllOrWrZuKjIxUSikVExOjtm7dqpYtW6buvvtupZRSZrNZpaamlvfHIKoBk9YFLISwPh8fH2699Vbmz59f9L309HTi4uK44447AFBK4erqSkpKCnl5eXTs2BGA4cOHs3DhQgDi4+OJiYnh3LlzZGVl0aVLlzKX6+vri4+PD/v378fBwQFXV1caNGjAzJkz+eGHH4iLiwMgLS2Nw4cP07Zt22LPT0lJISQkhMTERJo1a0afPn0A+OWXXzhw4EDRdMnJyQDExMSwdOlSunTpwvLly6851rl27Vq2bNlCaGgoAJmZmXTq1ImHH36YRx55hPj4eAIDA8nJyeHChQvs2rWLDh064OXlxVNPPcXTTz/NoEGDCA8PL8/qF9WEFKAQOjVx4kRuvvlm+vXrB4DZbMbX15c9e/YUm+6fMinJuHHjeOGFF4iOjmbVqlUWnUwzbNgwli5dioODAzExMUXLnjp1KqNGjSrzuf8cA8zIyOCWW25hzpw5jBs3DoAdO3ZgMhV/S7vjjjt47bXXePLJJ8nKyqJ58+bFHjebzTz44INMnTr1mmXVqlWLZcuWERkZSXZ2NosXL6ZBgwbY29vTvHlz9uzZw6pVqxg/fjwjRoxg7Nix133tonqRY4BC6FRAQAAREREsX74cAA8PD3x9fVm5ciUABQUF7N+/n1q1amEymYqKcenSpUXzuHLlCv7+/iilWLRoUdH33d3dSz3JZvDgwXzzzTcsX768qACjo6P55JNPyMwsHA7u5MmTpKamlprd1dWVWbNm8Z///If8/Hx69uzJ3Llzix7fu3cvAJ6enjRv3pxnnnmm6Ljlv/Xu3ZuvvvqKS5cuAXD+/HnOnDkDFB5jfPfdd4mIiCAyMpJ3332XyMhIAJKSknB1dWXUqFE89dRT13xoELZBClAIHXvmmWdISkoq+vqLL75g9uzZtG/fnnbt2rF27VoAPvroI0aMGEHHjh1xdHTEw8MDgKlTpzJw4EDCwsIICAgoms+dd97JK6+8UnQSzL/5+vri7e2Nk5MTDRo0AKBv374MGjSIrl270rZtW0aOHEl2dnaZ2UNDQ2nXrh1ff/01s2fPZv369bRv355WrVrxxRdfFE0XExPDkiVLisr239q0acMLL7xA7969CQ4OZsCAAVy+fBmAyMhIUlNTadeuHR07duTy5ctEREQAsG/fPsLCwggJCWHmzJlFJ88I2yJDoQkhrisjIwNXV1cAxo4dS8uWLWWXn7B5sgUohLiu7777jpCQEFq3bs2lS5eKLgsQwpbJFqAQQghdki1AIYQQuiQFKIQQQpekAIUQQuiSFKAQQghdkgIUQgihS1KAQgghdEkKUAghhC5JAQohhNAlKUAhhBC6JAUohBBCl6QAhRBC6JIUoBBCCF2SAhRCCKFLUoBCCCF0SQpQCCGELkkBCiGE0CUpQCGEELokBSiEEEKXpACFEELokhSgEEIIXZICFEIIoUtSgEIIIXRJClAIIYQuSQEKIYTQJSlAIYQQuiQFKIQQQpekAIUQQuiSFKAQQghdkgIUQgihS1KAQgghdEkKUAghhC5JAQohhNAlKUAhhBC6JAUohBBCl/4flUJRdjVEMqYAAAAASUVORK5CYII=</t>
   </si>
 </sst>
 </file>
@@ -406,76 +397,76 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>